<commit_message>
Fix Serial2 CTS/RTS pin numbers
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kurte\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB5F2FE-B9F0-45F9-9E83-28B429CC94DE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF92A8D-DC33-48C1-BA0C-455DA9BDB9E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19170" yWindow="1365" windowWidth="18705" windowHeight="18105" xr2:uid="{AA7C3FBA-D3AB-4A4A-A49A-E3C6F380265F}"/>
+    <workbookView xWindow="18825" yWindow="2625" windowWidth="21270" windowHeight="17985" xr2:uid="{AA7C3FBA-D3AB-4A4A-A49A-E3C6F380265F}"/>
   </bookViews>
   <sheets>
     <sheet name="More Card Like" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1451" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1435" uniqueCount="374">
   <si>
     <t>Column1</t>
   </si>
@@ -1167,6 +1167,9 @@
   </si>
   <si>
     <t>SPI2(1) CS1</t>
+  </si>
+  <si>
+    <t>Serial3(2) RTS</t>
   </si>
 </sst>
 </file>
@@ -1828,7 +1831,7 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2630,7 +2633,7 @@
         <v>167</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>331</v>
+        <v>373</v>
       </c>
       <c r="E21" s="14" t="s">
         <v>366</v>
@@ -2668,8 +2671,8 @@
       <c r="C22" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>13</v>
+      <c r="D22" s="14" t="s">
+        <v>331</v>
       </c>
       <c r="E22" s="17" t="s">
         <v>367</v>
@@ -3508,7 +3511,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5295,7 +5298,7 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
T4.x - Add possible bottom pins and reorder..
Guessing on final pin numbers
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61610A1B-D4E7-4815-983D-15A5608463F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45278FF2-CDCC-466D-83B2-F8931C2CEA6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="2145" windowWidth="22500" windowHeight="17340" xr2:uid="{AA7C3FBA-D3AB-4A4A-A49A-E3C6F380265F}"/>
+    <workbookView xWindow="6420" yWindow="2055" windowWidth="22500" windowHeight="17340" xr2:uid="{AA7C3FBA-D3AB-4A4A-A49A-E3C6F380265F}"/>
   </bookViews>
   <sheets>
     <sheet name="More Card Like" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1919" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="458">
   <si>
     <t>Column1</t>
   </si>
@@ -1267,13 +1267,169 @@
   </si>
   <si>
     <t>3:13</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Bottom Memory Connectors</t>
+  </si>
+  <si>
+    <t>EMC_22</t>
+  </si>
+  <si>
+    <t>EMC_25</t>
+  </si>
+  <si>
+    <t>EMC_26</t>
+  </si>
+  <si>
+    <t>EMC_27</t>
+  </si>
+  <si>
+    <t>EMC_28</t>
+  </si>
+  <si>
+    <t>EMC_29</t>
+  </si>
+  <si>
+    <t>4:22</t>
+  </si>
+  <si>
+    <t>4:24</t>
+  </si>
+  <si>
+    <t>4:25</t>
+  </si>
+  <si>
+    <t>4:26</t>
+  </si>
+  <si>
+    <t>4:27</t>
+  </si>
+  <si>
+    <t>4:28</t>
+  </si>
+  <si>
+    <t>4:29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serial8(5) RX </t>
+  </si>
+  <si>
+    <t>Serial8(5) CTS</t>
+  </si>
+  <si>
+    <t>Serial8(5) RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serial1(6) TX </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serial1(6) RX </t>
+  </si>
+  <si>
+    <t>Serial1(6) RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPI2(1) SCK </t>
+  </si>
+  <si>
+    <t>1:12</t>
+  </si>
+  <si>
+    <t>1:13</t>
+  </si>
+  <si>
+    <t>1:14</t>
+  </si>
+  <si>
+    <t>1:15</t>
+  </si>
+  <si>
+    <t>PWM3_A0</t>
+  </si>
+  <si>
+    <t>PWM2_B,QT4_2</t>
+  </si>
+  <si>
+    <t>PWM2_A2, QT4_1</t>
+  </si>
+  <si>
+    <t>PWM3_B3, QT2_3</t>
+  </si>
+  <si>
+    <t>PWM2_B2, QT4_2</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>SD Pins - Cable connector(T4 34-39)</t>
+  </si>
+  <si>
+    <t>Warning Guessing on actual pin number ordering Here</t>
+  </si>
+  <si>
+    <t>New Top Pins(Pin numbers from Forum posting)</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1309,6 +1465,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1612,8 +1774,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M52" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:M52" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M61" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A1:M61" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="13"/>
@@ -1979,7 +2141,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1990,7 +2152,7 @@
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
@@ -2292,12 +2454,10 @@
       <c r="F8" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="23" t="s">
-        <v>91</v>
-      </c>
+      <c r="G8" s="17" t="s">
+        <v>439</v>
+      </c>
+      <c r="H8" s="23"/>
       <c r="I8" s="23" t="s">
         <v>92</v>
       </c>
@@ -2402,11 +2562,9 @@
         <v>13</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>98</v>
-      </c>
+        <v>441</v>
+      </c>
+      <c r="H11" s="17"/>
       <c r="I11" s="17" t="s">
         <v>99</v>
       </c>
@@ -3615,11 +3773,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D0C246-03A0-4FFF-AF38-F7B7F6DA7DF4}">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3630,7 +3788,7 @@
     <col min="4" max="4" width="14.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="3" bestFit="1" customWidth="1"/>
@@ -3928,10 +4086,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>91</v>
+        <v>439</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>92</v>
@@ -4030,10 +4185,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>98</v>
+        <v>438</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>99</v>
@@ -4840,7 +4992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:12">
       <c r="A33" s="3" t="s">
         <v>252</v>
       </c>
@@ -4875,7 +5027,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:12">
       <c r="A34" s="3" t="s">
         <v>257</v>
       </c>
@@ -4910,7 +5062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:12">
       <c r="A35" s="3" t="s">
         <v>262</v>
       </c>
@@ -4948,7 +5100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:12">
       <c r="A36" s="3" t="s">
         <v>268</v>
       </c>
@@ -4986,308 +5138,493 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
-      <c r="A38" s="3" t="s">
+    <row r="37" spans="1:12">
+      <c r="A37" s="5" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="5" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B39" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2.29</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2.19</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1.28</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="C44" s="3">
+        <v>1.29</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="C45" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="C46" s="3">
+        <v>1.21</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="J38" s="3" t="s">
+      <c r="J56" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="M38" s="3" t="s">
+      <c r="M56" s="3" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
-      <c r="A39" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="B39" s="3" t="s">
+    <row r="57" spans="1:13">
+      <c r="A57" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="J39" s="3" t="s">
+      <c r="J57" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="M39" s="3" t="s">
+      <c r="M57" s="3" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
-      <c r="A40" s="3">
-        <v>36</v>
-      </c>
-      <c r="B40" s="3" t="s">
+    <row r="58" spans="1:13">
+      <c r="A58" s="3" t="s">
+        <v>454</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="J40" s="3" t="s">
+      <c r="J58" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="M40" s="3" t="s">
+      <c r="M58" s="3" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
-      <c r="A41" s="3">
-        <v>37</v>
-      </c>
-      <c r="B41" s="3" t="s">
+    <row r="59" spans="1:13">
+      <c r="A59" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C59" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E59" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F59" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="J59" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="M41" s="3" t="s">
+      <c r="M59" s="3" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
-      <c r="A42" s="3">
-        <v>38</v>
-      </c>
-      <c r="B42" s="3" t="s">
+    <row r="60" spans="1:13">
+      <c r="A60" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C60" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D60" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="J42" s="3" t="s">
+      <c r="J60" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="M42" s="3" t="s">
+      <c r="M60" s="3" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
-      <c r="A43" s="3">
-        <v>39</v>
-      </c>
-      <c r="B43" s="3" t="s">
+    <row r="61" spans="1:13">
+      <c r="A61" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C61" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D61" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="G43" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="J43" s="3" t="s">
+      <c r="J61" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="M43" s="3" t="s">
+      <c r="M61" s="3" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
-      <c r="B45" s="3" t="s">
-        <v>374</v>
-      </c>
-      <c r="C45" s="3">
-        <v>2.29</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13">
-      <c r="B46" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="C46" s="3">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13">
-      <c r="B47" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="C47" s="3">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="J47" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="K47" s="3" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13">
-      <c r="B48" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="C48" s="3">
-        <v>2.19</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K48" s="3" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="49" spans="2:12">
-      <c r="B49" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="C49" s="3">
-        <v>1.28</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="K49" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="50" spans="2:12">
-      <c r="B50" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="C50" s="3">
-        <v>1.29</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="K50" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="L50" s="3" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="51" spans="2:12">
-      <c r="B51" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="C51" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="K51" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="L51" s="3" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="52" spans="2:12">
-      <c r="B52" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="C52" s="3">
-        <v>1.21</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="K52" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="L52" s="3" t="s">
-        <v>401</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -5299,8 +5636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA9E33D-55F9-4A4A-B5CD-11BD9F30F4BE}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
T4.1 - more info on pins
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45278FF2-CDCC-466D-83B2-F8931C2CEA6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90EE714-2DF7-4FC8-ADA8-BF4137F49691}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="2055" windowWidth="22500" windowHeight="17340" xr2:uid="{AA7C3FBA-D3AB-4A4A-A49A-E3C6F380265F}"/>
+    <workbookView xWindow="12360" yWindow="1965" windowWidth="26040" windowHeight="17835" activeTab="1" xr2:uid="{AA7C3FBA-D3AB-4A4A-A49A-E3C6F380265F}"/>
   </bookViews>
   <sheets>
     <sheet name="More Card Like" sheetId="3" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1983" uniqueCount="470">
   <si>
     <t>Column1</t>
   </si>
@@ -1347,9 +1347,6 @@
     <t>Serial1(6) RTS</t>
   </si>
   <si>
-    <t xml:space="preserve">SPI2(1) SCK </t>
-  </si>
-  <si>
     <t>1:12</t>
   </si>
   <si>
@@ -1423,13 +1420,52 @@
   </si>
   <si>
     <t>54</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA0</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA1</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA2</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA3</t>
+  </si>
+  <si>
+    <t>USDHC2_CMD</t>
+  </si>
+  <si>
+    <t>USDHC2_CLK</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_SS1_B</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_SS0_B</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_SCLK</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_DATA00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FLEXSPI2_A_DATA01, SPI2(1) SCK  </t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_DATA02, SPI2(1) MOSI</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_DATA03, SPI2(1) MISO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1474,6 +1510,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1539,7 +1580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1581,11 +1622,53 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="43">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1630,45 +1713,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -1774,45 +1818,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M61" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M61" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
   <autoFilter ref="A1:M61" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{F9478000-D09D-4158-8962-151C792B9115}" name="GPIO" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{EEB23B63-7C82-4BC1-80FE-826F4A02B99D}" name="Serial" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{1D7F4122-4922-476A-8C8E-378628CB944B}" name="I2C" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{8B2BA30D-AD74-4591-9119-1A5E4B5E627D}" name="SPI" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{50F13DDA-AECC-4873-B8BF-BF29B9FA3A1D}" name="PWM" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{99EA318C-72FB-4EFD-9E14-9B5211643911}" name="CAN" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{DC6B9277-B97B-4891-B766-22B3DE725408}" name="Audio" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{1446B065-9F8B-426F-A535-611F882183B3}" name="XBAR" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{DC1C2DEB-A4BD-44FE-B52D-E7ABF3D565E7}" name="FlexIO" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{2A37AD20-1A78-4C16-9F5C-DBB6ECB30C3F}" name="Analog" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{E0FD363E-BD42-46D9-8D08-5AE1FF584E61}" name="SD" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="40"/>
+    <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{F9478000-D09D-4158-8962-151C792B9115}" name="GPIO" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{EEB23B63-7C82-4BC1-80FE-826F4A02B99D}" name="Serial" dataDxfId="37"/>
+    <tableColumn id="5" xr3:uid="{1D7F4122-4922-476A-8C8E-378628CB944B}" name="I2C" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{8B2BA30D-AD74-4591-9119-1A5E4B5E627D}" name="SPI" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{50F13DDA-AECC-4873-B8BF-BF29B9FA3A1D}" name="PWM" dataDxfId="34"/>
+    <tableColumn id="8" xr3:uid="{99EA318C-72FB-4EFD-9E14-9B5211643911}" name="CAN" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{DC6B9277-B97B-4891-B766-22B3DE725408}" name="Audio" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{1446B065-9F8B-426F-A535-611F882183B3}" name="XBAR" dataDxfId="31"/>
+    <tableColumn id="11" xr3:uid="{DC1C2DEB-A4BD-44FE-B52D-E7ABF3D565E7}" name="FlexIO" dataDxfId="30"/>
+    <tableColumn id="12" xr3:uid="{2A37AD20-1A78-4C16-9F5C-DBB6ECB30C3F}" name="Analog" dataDxfId="29"/>
+    <tableColumn id="13" xr3:uid="{E0FD363E-BD42-46D9-8D08-5AE1FF584E61}" name="SD" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{023DA8D0-5E82-4C9F-9484-155B8CC8D730}" name="T4B1_Pins3" displayName="T4B1_Pins3" ref="A1:N45" tableType="queryTable" totalsRowShown="0" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{023DA8D0-5E82-4C9F-9484-155B8CC8D730}" name="T4B1_Pins3" displayName="T4B1_Pins3" ref="A1:N45" tableType="queryTable" totalsRowShown="0" dataDxfId="27">
   <autoFilter ref="A1:N45" xr:uid="{320CEFA1-BC1B-4B93-8E6E-6A70204175E7}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2F64AA19-A241-4640-AFED-5DA8184AC327}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{80F4066A-3DFC-4F69-9419-FCA11E958D1E}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{4927449B-3DC7-4281-A213-4A6CE448FA0E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{BED0BD81-44AE-4B92-B7E6-A2A31C4E4502}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{12DB1949-C671-402C-B15C-53628F6F84BF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{EFBEA00A-A2B7-4AC1-AB6F-E166CE862C32}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{54FF7319-2BEE-4665-99E8-962C8C352D10}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{93B10B9E-BCB4-4434-BECC-9FC1BE60EA79}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{AD1D3450-5A15-467D-B28F-B2E9987390C2}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{E444F2CD-EE99-4C86-AF7F-76E4E3B8DCC6}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{B3E65604-8821-49DB-9955-1D2A15E6FE77}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{7DA5B48E-6DEC-475F-9D0B-195A255BF499}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{9014155F-0103-4411-925A-A668210083BB}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{B6022C8D-0D7B-46D8-A988-07F25C4E041C}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{2F64AA19-A241-4640-AFED-5DA8184AC327}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{80F4066A-3DFC-4F69-9419-FCA11E958D1E}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{4927449B-3DC7-4281-A213-4A6CE448FA0E}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{BED0BD81-44AE-4B92-B7E6-A2A31C4E4502}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{12DB1949-C671-402C-B15C-53628F6F84BF}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{EFBEA00A-A2B7-4AC1-AB6F-E166CE862C32}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{54FF7319-2BEE-4665-99E8-962C8C352D10}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{93B10B9E-BCB4-4434-BECC-9FC1BE60EA79}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{AD1D3450-5A15-467D-B28F-B2E9987390C2}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{E444F2CD-EE99-4C86-AF7F-76E4E3B8DCC6}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{B3E65604-8821-49DB-9955-1D2A15E6FE77}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{7DA5B48E-6DEC-475F-9D0B-195A255BF499}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{9014155F-0103-4411-925A-A668210083BB}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{B6022C8D-0D7B-46D8-A988-07F25C4E041C}" uniqueName="14" name="Column14" queryTableFieldId="14" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1822,19 +1866,19 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D207FBA2-3C66-4700-8D56-05F7E4D05F28}" name="T4B1_Pins" displayName="T4B1_Pins" ref="A1:M36" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:M36" xr:uid="{EFCB34B0-91F3-438F-AC17-137591FE744E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{4E4A7209-6511-46A1-AEB7-11C0D4BB58C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{4898CD4D-4C0D-4F97-9935-0A44E5BEC830}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{DE2F03FB-F1BB-4B34-8C4F-D21BC4CB8E93}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{D3942DB0-E199-4257-9BF0-E8E61DFCD2BF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{CA40BB47-FBDF-4F2C-9517-118613D5C272}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{4DD3DE24-C943-46CC-B510-CA40170BE355}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{8296D93B-C81D-49E6-8182-CE2FD163C97C}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{0A79940A-BF61-4C78-BC45-334277B7B082}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{CC57B938-7FC6-4598-8A7E-A43623C58E41}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{B4483E8F-7FA3-4067-BB65-C37C0A7AA37B}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{891F856C-305A-446E-B7FB-71B76A8F1D4B}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{302BE5EF-E716-4AE4-9B77-F67D6ED69E52}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{0242AAD0-9BB3-48C4-8502-B93007DAC024}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{4E4A7209-6511-46A1-AEB7-11C0D4BB58C5}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{4898CD4D-4C0D-4F97-9935-0A44E5BEC830}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{DE2F03FB-F1BB-4B34-8C4F-D21BC4CB8E93}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{D3942DB0-E199-4257-9BF0-E8E61DFCD2BF}" uniqueName="4" name="Column4" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{CA40BB47-FBDF-4F2C-9517-118613D5C272}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{4DD3DE24-C943-46CC-B510-CA40170BE355}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{8296D93B-C81D-49E6-8182-CE2FD163C97C}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{0A79940A-BF61-4C78-BC45-334277B7B082}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{CC57B938-7FC6-4598-8A7E-A43623C58E41}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{B4483E8F-7FA3-4067-BB65-C37C0A7AA37B}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{891F856C-305A-446E-B7FB-71B76A8F1D4B}" uniqueName="11" name="Column11" queryTableFieldId="11" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{302BE5EF-E716-4AE4-9B77-F67D6ED69E52}" uniqueName="12" name="Column12" queryTableFieldId="12" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{0242AAD0-9BB3-48C4-8502-B93007DAC024}" uniqueName="13" name="Column13" queryTableFieldId="13" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2139,9 +2183,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4A98D7-59ED-43A9-B01B-8AE7AF7474EA}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2455,7 +2499,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="23" t="s">
@@ -2562,7 +2606,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17" t="s">
@@ -3775,9 +3819,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D0C246-03A0-4FFF-AF38-F7B7F6DA7DF4}">
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D42" sqref="D42"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47:XFD54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3787,14 +3831,14 @@
     <col min="3" max="3" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -4086,7 +4130,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>92</v>
@@ -4185,7 +4229,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>99</v>
@@ -4384,7 +4428,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
         <v>138</v>
       </c>
@@ -4422,7 +4466,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
         <v>147</v>
       </c>
@@ -4459,8 +4503,11 @@
       <c r="L18" s="3" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="M18" s="37" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="3" t="s">
         <v>156</v>
       </c>
@@ -4497,8 +4544,11 @@
       <c r="L19" s="3" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="37" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="3" t="s">
         <v>165</v>
       </c>
@@ -4536,7 +4586,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
         <v>174</v>
       </c>
@@ -4574,7 +4624,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:13">
       <c r="A22" s="3" t="s">
         <v>182</v>
       </c>
@@ -4612,7 +4662,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:13">
       <c r="A23" s="3" t="s">
         <v>190</v>
       </c>
@@ -4650,7 +4700,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:13">
       <c r="A24" s="3" t="s">
         <v>198</v>
       </c>
@@ -4687,8 +4737,11 @@
       <c r="L24" s="3" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="M24" s="37" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="3" t="s">
         <v>205</v>
       </c>
@@ -4725,8 +4778,11 @@
       <c r="L25" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="M25" s="37" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="3" t="s">
         <v>26</v>
       </c>
@@ -4764,7 +4820,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27" s="3" t="s">
         <v>214</v>
       </c>
@@ -4802,7 +4858,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28" s="3" t="s">
         <v>221</v>
       </c>
@@ -4840,7 +4896,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29" s="3" t="s">
         <v>229</v>
       </c>
@@ -4878,7 +4934,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30" s="3" t="s">
         <v>235</v>
       </c>
@@ -4916,7 +4972,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13">
       <c r="A31" s="3" t="s">
         <v>241</v>
       </c>
@@ -4954,7 +5010,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13">
       <c r="A32" s="3" t="s">
         <v>246</v>
       </c>
@@ -4992,7 +5048,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:13">
       <c r="A33" s="3" t="s">
         <v>252</v>
       </c>
@@ -5027,7 +5083,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:13">
       <c r="A34" s="3" t="s">
         <v>257</v>
       </c>
@@ -5062,7 +5118,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:13">
       <c r="A35" s="3" t="s">
         <v>262</v>
       </c>
@@ -5100,7 +5156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:13">
       <c r="A36" s="3" t="s">
         <v>268</v>
       </c>
@@ -5138,17 +5194,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:13">
       <c r="A37" s="5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="5" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
-      <c r="A38" s="5" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
         <v>286</v>
       </c>
@@ -5165,7 +5221,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:13">
       <c r="A40" s="3" t="s">
         <v>287</v>
       </c>
@@ -5182,7 +5238,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:13">
       <c r="A41" s="3" t="s">
         <v>406</v>
       </c>
@@ -5208,7 +5264,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:13">
       <c r="A42" s="3" t="s">
         <v>407</v>
       </c>
@@ -5234,7 +5290,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:13">
       <c r="A43" s="3" t="s">
         <v>408</v>
       </c>
@@ -5257,7 +5313,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:13">
       <c r="A44" s="3" t="s">
         <v>409</v>
       </c>
@@ -5280,7 +5336,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:13">
       <c r="A45" s="3" t="s">
         <v>410</v>
       </c>
@@ -5296,8 +5352,11 @@
       <c r="L45" s="3" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="M45" s="37" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="3" t="s">
         <v>411</v>
       </c>
@@ -5316,15 +5375,18 @@
       <c r="L46" s="3" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="M46" s="37" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="5" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:13">
       <c r="A48" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>413</v>
@@ -5335,13 +5397,16 @@
       <c r="E48" s="3" t="s">
         <v>369</v>
       </c>
+      <c r="F48" s="3" t="s">
+        <v>463</v>
+      </c>
       <c r="G48" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>253</v>
@@ -5352,13 +5417,16 @@
       <c r="D49" s="3" t="s">
         <v>426</v>
       </c>
+      <c r="F49" s="3" t="s">
+        <v>464</v>
+      </c>
       <c r="G49" s="3" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>414</v>
@@ -5369,13 +5437,16 @@
       <c r="D50" s="3" t="s">
         <v>429</v>
       </c>
+      <c r="F50" s="3" t="s">
+        <v>465</v>
+      </c>
       <c r="G50" s="3" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>415</v>
@@ -5386,16 +5457,19 @@
       <c r="D51" s="3" t="s">
         <v>430</v>
       </c>
+      <c r="F51" s="3" t="s">
+        <v>466</v>
+      </c>
       <c r="G51" s="3" t="s">
         <v>319</v>
       </c>
       <c r="K51" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="52" spans="1:13">
       <c r="A52" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>416</v>
@@ -5407,18 +5481,18 @@
         <v>428</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>432</v>
+        <v>467</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>320</v>
       </c>
       <c r="K52" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>417</v>
@@ -5430,18 +5504,18 @@
         <v>427</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>351</v>
+        <v>468</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>321</v>
       </c>
       <c r="K53" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>418</v>
@@ -5453,23 +5527,23 @@
         <v>431</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>350</v>
+        <v>469</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K54" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="5" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>299</v>
@@ -5495,7 +5569,7 @@
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>298</v>
@@ -5521,7 +5595,7 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>297</v>
@@ -5547,7 +5621,7 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>296</v>
@@ -5573,7 +5647,7 @@
     </row>
     <row r="60" spans="1:13">
       <c r="A60" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>301</v>
@@ -5599,7 +5673,7 @@
     </row>
     <row r="61" spans="1:13">
       <c r="A61" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>300</v>
@@ -5626,8 +5700,9 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update T4.1 card look to show bottom pins
As always a work in progress...
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28975D4D-5484-452F-B858-2D417E7FD20D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18A6F6D6-50A6-4EF4-BCE8-AEE4CDB8134E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19185" yWindow="-15" windowWidth="19230" windowHeight="21030" activeTab="1" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19200" windowHeight="21030" activeTab="2" xr2:uid="{1AD796A4-1014-4F0D-8283-38C416C6C8D7}"/>
+    <workbookView xWindow="15240" yWindow="1230" windowWidth="23100" windowHeight="18465" activeTab="2" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2240" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="581">
   <si>
     <t>Column1</t>
   </si>
@@ -1779,6 +1778,21 @@
   </si>
   <si>
     <t>CS1-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Back Memory Chips</t>
+  </si>
+  <si>
+    <t>(pin 1)</t>
+  </si>
+  <si>
+    <t>CTS3</t>
+  </si>
+  <si>
+    <t>CTS8</t>
   </si>
 </sst>
 </file>
@@ -1862,7 +1876,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2031,6 +2045,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -2093,7 +2119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2255,6 +2281,12 @@
     <xf numFmtId="0" fontId="9" fillId="27" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2264,12 +2296,14 @@
     <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="9" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2892,7 +2926,6 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4528,10 +4561,10 @@
   </sheetPr>
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6421,13 +6454,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD25"/>
+  <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6442,14 +6473,16 @@
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="18" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="3" bestFit="1" customWidth="1"/>
@@ -6567,19 +6600,19 @@
       <c r="I2" s="48"/>
       <c r="J2" s="48"/>
       <c r="K2" s="48"/>
-      <c r="L2" s="77" t="s">
+      <c r="L2" s="79" t="s">
         <v>469</v>
       </c>
-      <c r="M2" s="77"/>
-      <c r="N2" s="77"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="79"/>
       <c r="O2" s="49"/>
       <c r="P2" s="49"/>
-      <c r="Q2" s="78" t="s">
+      <c r="Q2" s="80" t="s">
         <v>470</v>
       </c>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
       <c r="U2" s="48"/>
       <c r="V2" s="48"/>
       <c r="W2" s="48"/>
@@ -6624,12 +6657,12 @@
       </c>
       <c r="O3" s="49"/>
       <c r="P3" s="49"/>
-      <c r="Q3" s="78" t="s">
+      <c r="Q3" s="80" t="s">
         <v>469</v>
       </c>
-      <c r="R3" s="78"/>
-      <c r="S3" s="78"/>
-      <c r="T3" s="78"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
       <c r="U3" s="48"/>
       <c r="V3" s="48"/>
       <c r="W3" s="48"/>
@@ -6676,12 +6709,12 @@
       </c>
       <c r="O4" s="49"/>
       <c r="P4" s="49"/>
-      <c r="Q4" s="78" t="s">
+      <c r="Q4" s="80" t="s">
         <v>473</v>
       </c>
-      <c r="R4" s="78"/>
-      <c r="S4" s="78"/>
-      <c r="T4" s="78"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="80"/>
+      <c r="T4" s="80"/>
       <c r="U4" s="48"/>
       <c r="V4" s="48"/>
       <c r="W4" s="48"/>
@@ -7371,10 +7404,10 @@
       <c r="Q15" s="54">
         <v>13</v>
       </c>
-      <c r="R15" s="79" t="s">
+      <c r="R15" s="81" t="s">
         <v>496</v>
       </c>
-      <c r="S15" s="79"/>
+      <c r="S15" s="81"/>
       <c r="T15" s="48"/>
       <c r="U15" s="50" t="s">
         <v>497</v>
@@ -7413,19 +7446,19 @@
       <c r="I16" s="48"/>
       <c r="J16" s="48"/>
       <c r="K16" s="48"/>
-      <c r="L16" s="77" t="s">
+      <c r="L16" s="79" t="s">
         <v>498</v>
       </c>
-      <c r="M16" s="77"/>
-      <c r="N16" s="77"/>
+      <c r="M16" s="79"/>
+      <c r="N16" s="79"/>
       <c r="O16" s="49"/>
       <c r="P16" s="49"/>
-      <c r="Q16" s="78" t="s">
+      <c r="Q16" s="80" t="s">
         <v>469</v>
       </c>
-      <c r="R16" s="78"/>
-      <c r="S16" s="78"/>
-      <c r="T16" s="78"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
+      <c r="T16" s="80"/>
       <c r="U16" s="48"/>
       <c r="V16" s="48"/>
       <c r="W16" s="48"/>
@@ -7568,13 +7601,15 @@
       <c r="J19" s="50" t="s">
         <v>529</v>
       </c>
-      <c r="K19" s="48"/>
+      <c r="K19" s="48" t="s">
+        <v>579</v>
+      </c>
       <c r="L19" s="55" t="s">
         <v>532</v>
       </c>
       <c r="M19" s="48"/>
-      <c r="N19" s="52">
-        <v>26</v>
+      <c r="N19" s="52" t="s">
+        <v>576</v>
       </c>
       <c r="O19" s="49"/>
       <c r="P19" s="49"/>
@@ -7590,7 +7625,7 @@
       <c r="T19" s="62" t="s">
         <v>516</v>
       </c>
-      <c r="U19" s="81" t="s">
+      <c r="U19" s="78" t="s">
         <v>528</v>
       </c>
       <c r="V19" s="48"/>
@@ -7650,7 +7685,7 @@
       <c r="T20" s="62" t="s">
         <v>515</v>
       </c>
-      <c r="U20" s="81" t="s">
+      <c r="U20" s="78" t="s">
         <v>575</v>
       </c>
       <c r="V20" s="48"/>
@@ -7706,7 +7741,7 @@
       </c>
       <c r="S21" s="48"/>
       <c r="T21" s="48"/>
-      <c r="U21" s="80" t="s">
+      <c r="U21" s="77" t="s">
         <v>574</v>
       </c>
       <c r="V21" s="48"/>
@@ -7762,7 +7797,7 @@
       </c>
       <c r="S22" s="48"/>
       <c r="T22" s="48"/>
-      <c r="U22" s="80" t="s">
+      <c r="U22" s="77" t="s">
         <v>573</v>
       </c>
       <c r="V22" s="48"/>
@@ -7951,8 +7986,529 @@
       <c r="AC25" s="48"/>
       <c r="AD25" s="48"/>
     </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="82"/>
+      <c r="B26" s="82"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="82"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="82"/>
+      <c r="M26" s="82"/>
+      <c r="N26" s="82"/>
+      <c r="O26" s="82"/>
+      <c r="P26" s="82"/>
+      <c r="Q26" s="82"/>
+      <c r="R26" s="82"/>
+      <c r="S26" s="82"/>
+      <c r="T26" s="82"/>
+      <c r="U26" s="82"/>
+      <c r="V26" s="82"/>
+      <c r="W26" s="82"/>
+      <c r="X26" s="82"/>
+      <c r="Y26" s="82"/>
+      <c r="Z26" s="82"/>
+      <c r="AA26" s="82"/>
+      <c r="AB26" s="82"/>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27" s="82"/>
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="82" t="s">
+        <v>577</v>
+      </c>
+      <c r="P27" s="82"/>
+      <c r="Q27" s="82"/>
+      <c r="R27" s="82"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="82"/>
+      <c r="U27" s="82"/>
+      <c r="V27" s="82"/>
+      <c r="W27" s="82"/>
+      <c r="X27" s="82"/>
+      <c r="Y27" s="82"/>
+      <c r="Z27" s="82"/>
+      <c r="AA27" s="82"/>
+      <c r="AB27" s="82"/>
+    </row>
+    <row r="28" spans="1:30">
+      <c r="A28" s="82"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="82"/>
+      <c r="E28" s="82"/>
+      <c r="F28" s="82"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="82"/>
+      <c r="L28" s="82"/>
+      <c r="M28" s="82"/>
+      <c r="N28" s="82"/>
+      <c r="O28" s="82"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="82"/>
+      <c r="S28" s="82"/>
+      <c r="T28" s="82"/>
+      <c r="U28" s="82"/>
+      <c r="V28" s="82"/>
+      <c r="W28" s="82"/>
+      <c r="X28" s="82"/>
+      <c r="Y28" s="82"/>
+      <c r="Z28" s="82"/>
+      <c r="AA28" s="82"/>
+      <c r="AB28" s="82"/>
+    </row>
+    <row r="29" spans="1:30">
+      <c r="A29" s="82"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82" t="s">
+        <v>409</v>
+      </c>
+      <c r="D29" s="82">
+        <v>4.26</v>
+      </c>
+      <c r="E29" s="82"/>
+      <c r="F29" s="89">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="82"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="84" t="s">
+        <v>471</v>
+      </c>
+      <c r="L29" s="82"/>
+      <c r="M29" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="N29" s="83">
+        <v>52</v>
+      </c>
+      <c r="O29" s="82"/>
+      <c r="P29" s="82"/>
+      <c r="Q29" s="80" t="s">
+        <v>469</v>
+      </c>
+      <c r="R29" s="80"/>
+      <c r="S29" s="80"/>
+      <c r="T29" s="80"/>
+      <c r="U29" s="82"/>
+      <c r="V29" s="82"/>
+      <c r="W29" s="82"/>
+      <c r="X29" s="82"/>
+      <c r="Y29" s="82"/>
+      <c r="Z29" s="82"/>
+      <c r="AA29" s="82"/>
+      <c r="AB29" s="82"/>
+    </row>
+    <row r="30" spans="1:30">
+      <c r="A30" s="82"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="D30" s="82">
+        <v>4.25</v>
+      </c>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="82"/>
+      <c r="I30" s="82"/>
+      <c r="J30" s="82"/>
+      <c r="K30" s="84" t="s">
+        <v>472</v>
+      </c>
+      <c r="L30" s="82"/>
+      <c r="M30" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="N30" s="83">
+        <v>53</v>
+      </c>
+      <c r="O30" s="82"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="83">
+        <v>50</v>
+      </c>
+      <c r="R30" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="S30" s="82"/>
+      <c r="T30" s="85" t="s">
+        <v>580</v>
+      </c>
+      <c r="U30" s="87" t="s">
+        <v>529</v>
+      </c>
+      <c r="V30" s="82"/>
+      <c r="W30" s="82"/>
+      <c r="X30" s="82"/>
+      <c r="Y30" s="89">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="Z30" s="82"/>
+      <c r="AA30" s="82">
+        <v>4.28</v>
+      </c>
+      <c r="AB30" s="82" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" s="82"/>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82" t="s">
+        <v>412</v>
+      </c>
+      <c r="D31" s="82">
+        <v>4.29</v>
+      </c>
+      <c r="E31" s="82"/>
+      <c r="F31" s="89">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="G31" s="82"/>
+      <c r="H31" s="82"/>
+      <c r="I31" s="82"/>
+      <c r="J31" s="87" t="s">
+        <v>529</v>
+      </c>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="N31" s="83">
+        <v>54</v>
+      </c>
+      <c r="O31" s="82"/>
+      <c r="P31" s="82" t="s">
+        <v>578</v>
+      </c>
+      <c r="Q31" s="83">
+        <v>49</v>
+      </c>
+      <c r="R31" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="S31" s="82"/>
+      <c r="T31" s="82"/>
+      <c r="U31" s="87" t="s">
+        <v>506</v>
+      </c>
+      <c r="V31" s="82"/>
+      <c r="W31" s="82"/>
+      <c r="X31" s="82"/>
+      <c r="Y31" s="89">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="Z31" s="82"/>
+      <c r="AA31" s="82">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="AB31" s="82" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" s="82"/>
+      <c r="B32" s="82"/>
+      <c r="C32" s="82"/>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="82"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="M32" s="79"/>
+      <c r="N32" s="79"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="83">
+        <v>51</v>
+      </c>
+      <c r="R32" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="S32" s="82"/>
+      <c r="T32" s="82"/>
+      <c r="U32" s="82"/>
+      <c r="V32" s="82"/>
+      <c r="W32" s="88" t="s">
+        <v>502</v>
+      </c>
+      <c r="X32" s="82"/>
+      <c r="Y32" s="82"/>
+      <c r="Z32" s="82"/>
+      <c r="AA32" s="82">
+        <v>4.22</v>
+      </c>
+      <c r="AB32" s="82" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28">
+      <c r="A33" s="82"/>
+      <c r="B33" s="82"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="82"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="82"/>
+      <c r="R33" s="82"/>
+      <c r="S33" s="82"/>
+      <c r="T33" s="82"/>
+      <c r="U33" s="82"/>
+      <c r="V33" s="82"/>
+      <c r="W33" s="82"/>
+      <c r="X33" s="82"/>
+      <c r="Y33" s="82"/>
+      <c r="Z33" s="82"/>
+      <c r="AA33" s="82"/>
+      <c r="AB33" s="82"/>
+    </row>
+    <row r="34" spans="1:28">
+      <c r="A34" s="82"/>
+      <c r="B34" s="82"/>
+      <c r="C34" s="82" t="s">
+        <v>409</v>
+      </c>
+      <c r="D34" s="82">
+        <v>4.26</v>
+      </c>
+      <c r="E34" s="82"/>
+      <c r="F34" s="89">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="82"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="84" t="s">
+        <v>471</v>
+      </c>
+      <c r="L34" s="82"/>
+      <c r="M34" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="N34" s="83">
+        <v>52</v>
+      </c>
+      <c r="O34" s="82"/>
+      <c r="P34" s="82"/>
+      <c r="Q34" s="80" t="s">
+        <v>469</v>
+      </c>
+      <c r="R34" s="80"/>
+      <c r="S34" s="80"/>
+      <c r="T34" s="80"/>
+      <c r="U34" s="82"/>
+      <c r="V34" s="82"/>
+      <c r="W34" s="82"/>
+      <c r="X34" s="82"/>
+      <c r="Y34" s="82"/>
+      <c r="Z34" s="82"/>
+      <c r="AA34" s="82"/>
+      <c r="AB34" s="82"/>
+    </row>
+    <row r="35" spans="1:28">
+      <c r="A35" s="82"/>
+      <c r="B35" s="82"/>
+      <c r="C35" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="D35" s="82">
+        <v>4.25</v>
+      </c>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="82"/>
+      <c r="I35" s="82"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="84" t="s">
+        <v>472</v>
+      </c>
+      <c r="L35" s="82"/>
+      <c r="M35" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="N35" s="83">
+        <v>53</v>
+      </c>
+      <c r="O35" s="82"/>
+      <c r="P35" s="82"/>
+      <c r="Q35" s="83">
+        <v>50</v>
+      </c>
+      <c r="R35" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="S35" s="82"/>
+      <c r="T35" s="85" t="s">
+        <v>580</v>
+      </c>
+      <c r="U35" s="87" t="s">
+        <v>529</v>
+      </c>
+      <c r="V35" s="82"/>
+      <c r="W35" s="82"/>
+      <c r="X35" s="82"/>
+      <c r="Y35" s="89">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="Z35" s="82"/>
+      <c r="AA35" s="82">
+        <v>4.28</v>
+      </c>
+      <c r="AB35" s="82" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
+      <c r="A36" s="82"/>
+      <c r="B36" s="82"/>
+      <c r="C36" s="82" t="s">
+        <v>412</v>
+      </c>
+      <c r="D36" s="82">
+        <v>4.29</v>
+      </c>
+      <c r="E36" s="82"/>
+      <c r="F36" s="89">
+        <v>5.2083333333333336E-2</v>
+      </c>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="82"/>
+      <c r="J36" s="87" t="s">
+        <v>529</v>
+      </c>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="N36" s="83">
+        <v>54</v>
+      </c>
+      <c r="O36" s="82"/>
+      <c r="P36" s="82"/>
+      <c r="Q36" s="83">
+        <v>49</v>
+      </c>
+      <c r="R36" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="S36" s="82"/>
+      <c r="T36" s="82"/>
+      <c r="U36" s="87" t="s">
+        <v>506</v>
+      </c>
+      <c r="V36" s="82"/>
+      <c r="W36" s="82"/>
+      <c r="X36" s="82"/>
+      <c r="Y36" s="89">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="Z36" s="82"/>
+      <c r="AA36" s="82">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="AB36" s="82" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
+      <c r="A37" s="82"/>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="82"/>
+      <c r="G37" s="82"/>
+      <c r="H37" s="82"/>
+      <c r="I37" s="82"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="79" t="s">
+        <v>498</v>
+      </c>
+      <c r="M37" s="79"/>
+      <c r="N37" s="79"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="82" t="s">
+        <v>578</v>
+      </c>
+      <c r="Q37" s="83">
+        <v>48</v>
+      </c>
+      <c r="R37" s="53" t="s">
+        <v>474</v>
+      </c>
+      <c r="S37" s="82"/>
+      <c r="T37" s="84" t="s">
+        <v>513</v>
+      </c>
+      <c r="U37" s="82"/>
+      <c r="V37" s="82"/>
+      <c r="W37" s="82"/>
+      <c r="X37" s="82"/>
+      <c r="Y37" s="82"/>
+      <c r="Z37" s="82"/>
+      <c r="AA37" s="82">
+        <v>4.24</v>
+      </c>
+      <c r="AB37" s="86" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
+      <c r="K39" s="82"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="L37:N37"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="Q34:T34"/>
+    <mergeCell ref="Q29:T29"/>
     <mergeCell ref="L16:N16"/>
     <mergeCell ref="Q16:T16"/>
     <mergeCell ref="L2:N2"/>
@@ -7973,7 +8529,6 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -9759,7 +10314,6 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Fixed some of the PWM pins and the like.
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28020FAD-A3B7-44B0-9AD7-96E8BD347064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BD4EE8-F672-48A3-957C-5ECB1AAB1DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="23595" windowHeight="18465" activeTab="2" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="2295" yWindow="0" windowWidth="20175" windowHeight="20415" activeTab="2" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="592">
   <si>
     <t>Column1</t>
   </si>
@@ -1540,9 +1540,6 @@
     <t>A0</t>
   </si>
   <si>
-    <t>(LED)</t>
-  </si>
-  <si>
     <t>SCK0</t>
   </si>
   <si>
@@ -1597,12 +1594,6 @@
     <t>TX8</t>
   </si>
   <si>
-    <t>rx5</t>
-  </si>
-  <si>
-    <t>tx5</t>
-  </si>
-  <si>
     <t>B1_13</t>
   </si>
   <si>
@@ -1832,6 +1823,9 @@
   </si>
   <si>
     <t>1.20</t>
+  </si>
+  <si>
+    <t>LED</t>
   </si>
 </sst>
 </file>
@@ -2183,7 +2177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2297,9 +2291,6 @@
     <xf numFmtId="0" fontId="9" fillId="16" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2364,12 +2355,6 @@
     <xf numFmtId="0" fontId="9" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="30" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2386,6 +2371,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4646,8 +4637,8 @@
   <dimension ref="A1:M61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C46" sqref="C46"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6118,7 +6109,7 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>378</v>
@@ -6141,7 +6132,7 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>379</v>
@@ -6164,19 +6155,19 @@
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="3" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>380</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="K45" s="3" t="s">
         <v>401</v>
       </c>
       <c r="L45" s="3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="M45" s="37" t="s">
         <v>451</v>
@@ -6184,7 +6175,7 @@
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>381</v>
@@ -6199,7 +6190,7 @@
         <v>400</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="M46" s="37" t="s">
         <v>452</v>
@@ -6541,8 +6532,8 @@
   <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6588,19 +6579,19 @@
       <c r="C1" s="39" t="s">
         <v>467</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="72" t="s">
+      <c r="E1" s="71" t="s">
         <v>22</v>
       </c>
       <c r="F1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="69" t="s">
-        <v>549</v>
-      </c>
-      <c r="H1" s="66" t="s">
+      <c r="G1" s="68" t="s">
+        <v>546</v>
+      </c>
+      <c r="H1" s="65" t="s">
         <v>18</v>
       </c>
       <c r="I1" s="41" t="s">
@@ -6641,19 +6632,19 @@
       <c r="V1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="66" t="s">
+      <c r="W1" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="70" t="s">
-        <v>549</v>
+      <c r="X1" s="69" t="s">
+        <v>546</v>
       </c>
       <c r="Y1" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="72" t="s">
+      <c r="Z1" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="101" t="s">
+      <c r="AA1" s="98" t="s">
         <v>16</v>
       </c>
       <c r="AB1" s="39" t="s">
@@ -6668,45 +6659,45 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="47" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>469</v>
       </c>
       <c r="C2" s="47"/>
-      <c r="D2" s="106"/>
+      <c r="D2" s="103"/>
       <c r="E2" s="47"/>
       <c r="F2" s="47"/>
-      <c r="G2" s="68">
+      <c r="G2" s="67">
         <v>17</v>
       </c>
       <c r="H2" s="47"/>
       <c r="I2" s="47"/>
       <c r="J2" s="47"/>
       <c r="K2" s="47"/>
-      <c r="L2" s="98" t="s">
+      <c r="L2" s="104" t="s">
         <v>469</v>
       </c>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
-      <c r="Q2" s="99" t="s">
+      <c r="Q2" s="105" t="s">
         <v>470</v>
       </c>
-      <c r="R2" s="99"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="99"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="105"/>
+      <c r="T2" s="105"/>
       <c r="U2" s="47"/>
       <c r="V2" s="47"/>
       <c r="W2" s="47"/>
       <c r="X2" s="47"/>
       <c r="Y2" s="47"/>
       <c r="Z2" s="47"/>
-      <c r="AA2" s="102"/>
+      <c r="AA2" s="99"/>
       <c r="AB2" s="47"/>
       <c r="AC2" s="47" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="AD2" s="47"/>
     </row>
@@ -6716,20 +6707,20 @@
       <c r="C3" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="102" t="s">
+      <c r="D3" s="99" t="s">
         <v>31</v>
       </c>
       <c r="E3" s="47"/>
       <c r="F3" s="47"/>
-      <c r="G3" s="68">
+      <c r="G3" s="67">
         <v>16</v>
       </c>
       <c r="H3" s="47"/>
-      <c r="I3" s="65" t="s">
+      <c r="I3" s="64" t="s">
         <v>491</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K3" s="50" t="s">
         <v>471</v>
@@ -6741,25 +6732,25 @@
       </c>
       <c r="O3" s="48"/>
       <c r="P3" s="48"/>
-      <c r="Q3" s="99" t="s">
+      <c r="Q3" s="105" t="s">
         <v>469</v>
       </c>
-      <c r="R3" s="99"/>
-      <c r="S3" s="99"/>
-      <c r="T3" s="99"/>
+      <c r="R3" s="105"/>
+      <c r="S3" s="105"/>
+      <c r="T3" s="105"/>
       <c r="U3" s="47"/>
       <c r="V3" s="47"/>
       <c r="W3" s="47"/>
       <c r="X3" s="47"/>
       <c r="Y3" s="47"/>
       <c r="Z3" s="47"/>
-      <c r="AA3" s="102"/>
+      <c r="AA3" s="99"/>
       <c r="AB3" s="47"/>
       <c r="AC3" s="47" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="AD3" s="47" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -6768,20 +6759,20 @@
       <c r="C4" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="102" t="s">
+      <c r="D4" s="99" t="s">
         <v>39</v>
       </c>
       <c r="E4" s="47"/>
       <c r="F4" s="47"/>
-      <c r="G4" s="68">
+      <c r="G4" s="67">
         <v>6</v>
       </c>
       <c r="H4" s="47"/>
-      <c r="I4" s="65" t="s">
+      <c r="I4" s="64" t="s">
         <v>493</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="K4" s="50" t="s">
         <v>472</v>
@@ -6793,22 +6784,22 @@
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="48"/>
-      <c r="Q4" s="99" t="s">
+      <c r="Q4" s="105" t="s">
         <v>473</v>
       </c>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
+      <c r="R4" s="105"/>
+      <c r="S4" s="105"/>
+      <c r="T4" s="105"/>
       <c r="U4" s="47"/>
       <c r="V4" s="47"/>
       <c r="W4" s="47"/>
       <c r="X4" s="47"/>
       <c r="Y4" s="47"/>
       <c r="Z4" s="47"/>
-      <c r="AA4" s="102"/>
+      <c r="AA4" s="99"/>
       <c r="AB4" s="47"/>
       <c r="AC4" s="47" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="AD4" s="47">
         <v>3.3</v>
@@ -6817,21 +6808,21 @@
     <row r="5" spans="1:30">
       <c r="A5" s="47"/>
       <c r="B5" s="47" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="102" t="s">
+      <c r="D5" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="71" t="s">
-        <v>550</v>
-      </c>
-      <c r="F5" s="63" t="s">
+      <c r="E5" s="70" t="s">
+        <v>547</v>
+      </c>
+      <c r="F5" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="67">
         <v>7</v>
       </c>
       <c r="H5" s="47"/>
@@ -6858,46 +6849,46 @@
       </c>
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
-      <c r="V5" s="65" t="s">
+      <c r="V5" s="64" t="s">
         <v>471</v>
       </c>
       <c r="W5" s="47"/>
       <c r="X5" s="47"/>
-      <c r="Y5" s="63" t="s">
+      <c r="Y5" s="62" t="s">
         <v>210</v>
       </c>
-      <c r="Z5" s="73" t="s">
-        <v>558</v>
-      </c>
-      <c r="AA5" s="102">
+      <c r="Z5" s="72" t="s">
+        <v>555</v>
+      </c>
+      <c r="AA5" s="99">
         <v>1.25</v>
       </c>
       <c r="AB5" s="47" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="AC5" s="47"/>
       <c r="AD5" s="47" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="47" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B6" s="47"/>
       <c r="C6" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="103" t="s">
+      <c r="D6" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="E6" s="73" t="s">
-        <v>551</v>
-      </c>
-      <c r="F6" s="63" t="s">
+      <c r="E6" s="72" t="s">
+        <v>548</v>
+      </c>
+      <c r="F6" s="62" t="s">
         <v>58</v>
       </c>
-      <c r="G6" s="68">
+      <c r="G6" s="67">
         <v>8</v>
       </c>
       <c r="H6" s="47"/>
@@ -6924,16 +6915,16 @@
       </c>
       <c r="T6" s="47"/>
       <c r="U6" s="47"/>
-      <c r="V6" s="65" t="s">
+      <c r="V6" s="64" t="s">
         <v>472</v>
       </c>
       <c r="W6" s="47"/>
       <c r="X6" s="47"/>
-      <c r="Y6" s="64">
+      <c r="Y6" s="63">
         <v>0.13055555555555556</v>
       </c>
       <c r="Z6" s="47"/>
-      <c r="AA6" s="102">
+      <c r="AA6" s="99">
         <v>1.24</v>
       </c>
       <c r="AB6" s="47" t="s">
@@ -6944,22 +6935,22 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="47" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="D7" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="E7" s="73" t="s">
-        <v>552</v>
-      </c>
-      <c r="F7" s="63" t="s">
+      <c r="E7" s="72" t="s">
+        <v>549</v>
+      </c>
+      <c r="F7" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="67">
         <v>17</v>
       </c>
       <c r="H7" s="47"/>
@@ -6978,26 +6969,23 @@
       <c r="Q7" s="53">
         <v>21</v>
       </c>
-      <c r="R7" s="52" t="s">
-        <v>474</v>
-      </c>
       <c r="S7" s="54" t="s">
         <v>479</v>
       </c>
       <c r="T7" s="50" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="U7" s="47"/>
       <c r="V7" s="47"/>
       <c r="W7" s="47"/>
       <c r="X7" s="47"/>
-      <c r="Y7" s="64">
+      <c r="Y7" s="63">
         <v>0.13263888888888889</v>
       </c>
-      <c r="Z7" s="71" t="s">
-        <v>559</v>
-      </c>
-      <c r="AA7" s="102">
+      <c r="Z7" s="70" t="s">
+        <v>556</v>
+      </c>
+      <c r="AA7" s="99">
         <v>1.27</v>
       </c>
       <c r="AB7" s="47" t="s">
@@ -7005,26 +6993,26 @@
       </c>
       <c r="AC7" s="47"/>
       <c r="AD7" s="47" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="47" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>269</v>
       </c>
-      <c r="D8" s="102" t="s">
+      <c r="D8" s="99" t="s">
         <v>270</v>
       </c>
-      <c r="E8" s="71" t="s">
-        <v>553</v>
-      </c>
-      <c r="F8" s="63" t="s">
+      <c r="E8" s="70" t="s">
+        <v>550</v>
+      </c>
+      <c r="F8" s="62" t="s">
         <v>273</v>
       </c>
       <c r="G8" s="47"/>
@@ -7044,26 +7032,23 @@
       <c r="Q8" s="53">
         <v>20</v>
       </c>
-      <c r="R8" s="52" t="s">
-        <v>474</v>
-      </c>
       <c r="S8" s="54" t="s">
         <v>481</v>
       </c>
       <c r="T8" s="58" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="U8" s="47"/>
       <c r="V8" s="47"/>
       <c r="W8" s="47"/>
       <c r="X8" s="47"/>
-      <c r="Y8" s="64">
+      <c r="Y8" s="63">
         <v>0.13194444444444445</v>
       </c>
-      <c r="Z8" s="71" t="s">
-        <v>560</v>
-      </c>
-      <c r="AA8" s="102">
+      <c r="Z8" s="70" t="s">
+        <v>557</v>
+      </c>
+      <c r="AA8" s="99">
         <v>1.26</v>
       </c>
       <c r="AB8" s="47" t="s">
@@ -7071,24 +7056,24 @@
       </c>
       <c r="AC8" s="47"/>
       <c r="AD8" s="47" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="47"/>
       <c r="B9" s="47" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C9" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="102" t="s">
+      <c r="D9" s="99" t="s">
         <v>89</v>
       </c>
-      <c r="E9" s="71" t="s">
-        <v>554</v>
-      </c>
-      <c r="F9" s="63" t="s">
+      <c r="E9" s="70" t="s">
+        <v>551</v>
+      </c>
+      <c r="F9" s="62" t="s">
         <v>93</v>
       </c>
       <c r="G9" s="47"/>
@@ -7108,51 +7093,53 @@
       <c r="Q9" s="53">
         <v>19</v>
       </c>
-      <c r="R9" s="47"/>
+      <c r="R9" s="52" t="s">
+        <v>474</v>
+      </c>
       <c r="S9" s="54" t="s">
         <v>482</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="U9" s="47"/>
       <c r="V9" s="47"/>
-      <c r="W9" s="67" t="s">
+      <c r="W9" s="66" t="s">
         <v>483</v>
       </c>
       <c r="X9" s="47"/>
-      <c r="Y9" s="64">
+      <c r="Y9" s="63">
         <v>0.125</v>
       </c>
       <c r="Z9" s="47"/>
-      <c r="AA9" s="103">
+      <c r="AA9" s="100">
         <v>1.1599999999999999</v>
       </c>
       <c r="AB9" s="47" t="s">
         <v>175</v>
       </c>
       <c r="AC9" s="47" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AD9" s="47" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="47"/>
       <c r="B10" s="47" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="102" t="s">
+      <c r="D10" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="71" t="s">
-        <v>555</v>
-      </c>
-      <c r="F10" s="63" t="s">
+      <c r="E10" s="70" t="s">
+        <v>552</v>
+      </c>
+      <c r="F10" s="62" t="s">
         <v>317</v>
       </c>
       <c r="G10" s="47"/>
@@ -7174,32 +7161,34 @@
       <c r="Q10" s="53">
         <v>18</v>
       </c>
-      <c r="R10" s="47"/>
+      <c r="R10" s="52" t="s">
+        <v>474</v>
+      </c>
       <c r="S10" s="54" t="s">
         <v>485</v>
       </c>
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
       <c r="V10" s="47"/>
-      <c r="W10" s="67" t="s">
+      <c r="W10" s="66" t="s">
         <v>486</v>
       </c>
       <c r="X10" s="47"/>
-      <c r="Y10" s="64">
+      <c r="Y10" s="63">
         <v>0.12569444444444444</v>
       </c>
       <c r="Z10" s="47"/>
-      <c r="AA10" s="103">
+      <c r="AA10" s="100">
         <v>1.17</v>
       </c>
       <c r="AB10" s="47" t="s">
         <v>166</v>
       </c>
       <c r="AC10" s="47" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="AD10" s="47" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -7208,17 +7197,17 @@
       <c r="C11" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="102" t="s">
+      <c r="D11" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="E11" s="71" t="s">
-        <v>556</v>
-      </c>
-      <c r="F11" s="63" t="s">
+      <c r="E11" s="70" t="s">
+        <v>553</v>
+      </c>
+      <c r="F11" s="62" t="s">
         <v>316</v>
       </c>
       <c r="G11" s="47"/>
-      <c r="H11" s="67" t="s">
+      <c r="H11" s="66" t="s">
         <v>487</v>
       </c>
       <c r="I11" s="47"/>
@@ -7238,26 +7227,23 @@
       <c r="Q11" s="53">
         <v>17</v>
       </c>
-      <c r="R11" s="52" t="s">
-        <v>474</v>
-      </c>
       <c r="S11" s="54" t="s">
         <v>489</v>
       </c>
       <c r="T11" s="58" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="U11" s="47"/>
       <c r="V11" s="47"/>
-      <c r="W11" s="67" t="s">
-        <v>500</v>
+      <c r="W11" s="66" t="s">
+        <v>499</v>
       </c>
       <c r="X11" s="47"/>
-      <c r="Y11" s="64">
+      <c r="Y11" s="63">
         <v>0.12916666666666668</v>
       </c>
       <c r="Z11" s="47"/>
-      <c r="AA11" s="103">
+      <c r="AA11" s="100">
         <v>1.22</v>
       </c>
       <c r="AB11" s="47" t="s">
@@ -7272,13 +7258,13 @@
       <c r="C12" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="102" t="s">
+      <c r="D12" s="99" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="73" t="s">
-        <v>557</v>
-      </c>
-      <c r="F12" s="63" t="s">
+      <c r="E12" s="72" t="s">
+        <v>554</v>
+      </c>
+      <c r="F12" s="62" t="s">
         <v>100</v>
       </c>
       <c r="G12" s="47"/>
@@ -7298,26 +7284,23 @@
       <c r="Q12" s="53">
         <v>16</v>
       </c>
-      <c r="R12" s="52" t="s">
-        <v>474</v>
-      </c>
       <c r="S12" s="54" t="s">
         <v>492</v>
       </c>
       <c r="T12" s="58" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="U12" s="47"/>
       <c r="V12" s="47"/>
-      <c r="W12" s="67" t="s">
-        <v>502</v>
+      <c r="W12" s="66" t="s">
+        <v>501</v>
       </c>
       <c r="X12" s="47"/>
-      <c r="Y12" s="64">
+      <c r="Y12" s="63">
         <v>0.12986111111111112</v>
       </c>
       <c r="Z12" s="47"/>
-      <c r="AA12" s="103">
+      <c r="AA12" s="100">
         <v>1.23</v>
       </c>
       <c r="AB12" s="47" t="s">
@@ -7328,19 +7311,19 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="47" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47" t="s">
         <v>102</v>
       </c>
-      <c r="D13" s="102" t="s">
+      <c r="D13" s="99" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="71" t="s">
-        <v>565</v>
-      </c>
-      <c r="F13" s="63" t="s">
+      <c r="E13" s="70" t="s">
+        <v>562</v>
+      </c>
+      <c r="F13" s="62" t="s">
         <v>107</v>
       </c>
       <c r="G13" s="47"/>
@@ -7362,7 +7345,9 @@
       <c r="Q13" s="53">
         <v>15</v>
       </c>
-      <c r="R13" s="47"/>
+      <c r="R13" s="52" t="s">
+        <v>474</v>
+      </c>
       <c r="S13" s="54" t="s">
         <v>494</v>
       </c>
@@ -7373,13 +7358,13 @@
       <c r="V13" s="47"/>
       <c r="W13" s="47"/>
       <c r="X13" s="47"/>
-      <c r="Y13" s="64">
+      <c r="Y13" s="63">
         <v>0.12708333333333333</v>
       </c>
       <c r="Z13" s="55" t="s">
-        <v>562</v>
-      </c>
-      <c r="AA13" s="102">
+        <v>559</v>
+      </c>
+      <c r="AA13" s="99">
         <v>1.19</v>
       </c>
       <c r="AB13" s="47" t="s">
@@ -7387,37 +7372,39 @@
       </c>
       <c r="AC13" s="47"/>
       <c r="AD13" s="47" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="47" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>109</v>
       </c>
-      <c r="D14" s="102" t="s">
+      <c r="D14" s="99" t="s">
         <v>110</v>
       </c>
       <c r="E14" s="47"/>
-      <c r="F14" s="63" t="s">
+      <c r="F14" s="62" t="s">
         <v>114</v>
       </c>
       <c r="G14" s="47"/>
       <c r="H14" s="47"/>
-      <c r="I14" s="65" t="s">
+      <c r="I14" s="64" t="s">
         <v>472</v>
       </c>
       <c r="J14" s="49" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="K14" s="47"/>
       <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
+      <c r="M14" s="52" t="s">
+        <v>474</v>
+      </c>
       <c r="N14" s="51">
         <v>11</v>
       </c>
@@ -7439,13 +7426,13 @@
       <c r="V14" s="47"/>
       <c r="W14" s="47"/>
       <c r="X14" s="47"/>
-      <c r="Y14" s="64">
+      <c r="Y14" s="63">
         <v>0.12638888888888888</v>
       </c>
-      <c r="Z14" s="71" t="s">
-        <v>561</v>
-      </c>
-      <c r="AA14" s="102">
+      <c r="Z14" s="70" t="s">
+        <v>558</v>
+      </c>
+      <c r="AA14" s="99">
         <v>1.18</v>
       </c>
       <c r="AB14" s="47" t="s">
@@ -7456,32 +7443,34 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="47" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="E15" s="71" t="s">
-        <v>566</v>
-      </c>
-      <c r="F15" s="63" t="s">
+      <c r="E15" s="70" t="s">
+        <v>563</v>
+      </c>
+      <c r="F15" s="62" t="s">
         <v>121</v>
       </c>
       <c r="G15" s="47"/>
       <c r="H15" s="47"/>
       <c r="I15" s="47"/>
       <c r="J15" s="49" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="K15" s="47"/>
       <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
+      <c r="M15" s="52" t="s">
+        <v>474</v>
+      </c>
       <c r="N15" s="51">
         <v>12</v>
       </c>
@@ -7490,41 +7479,43 @@
       <c r="Q15" s="53">
         <v>13</v>
       </c>
-      <c r="R15" s="100" t="s">
-        <v>496</v>
-      </c>
-      <c r="S15" s="100"/>
+      <c r="R15" s="52" t="s">
+        <v>474</v>
+      </c>
+      <c r="S15" s="97" t="s">
+        <v>591</v>
+      </c>
       <c r="T15" s="47"/>
       <c r="U15" s="49" t="s">
-        <v>497</v>
-      </c>
-      <c r="V15" s="65" t="s">
+        <v>496</v>
+      </c>
+      <c r="V15" s="64" t="s">
         <v>480</v>
       </c>
       <c r="W15" s="47"/>
       <c r="X15" s="47"/>
-      <c r="Y15" s="64">
+      <c r="Y15" s="63">
         <v>8.5416666666666655E-2</v>
       </c>
       <c r="Z15" s="47"/>
-      <c r="AA15" s="102">
+      <c r="AA15" s="99">
         <v>2.2999999999999998</v>
       </c>
       <c r="AB15" s="47" t="s">
         <v>123</v>
       </c>
       <c r="AC15" s="47" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="AD15" s="47" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="16" spans="1:30">
       <c r="A16" s="47"/>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
-      <c r="D16" s="102"/>
+      <c r="D16" s="99"/>
       <c r="E16" s="47"/>
       <c r="F16" s="47"/>
       <c r="G16" s="47"/>
@@ -7532,26 +7523,26 @@
       <c r="I16" s="47"/>
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
-      <c r="L16" s="98" t="s">
-        <v>498</v>
-      </c>
-      <c r="M16" s="98"/>
-      <c r="N16" s="98"/>
+      <c r="L16" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="M16" s="104"/>
+      <c r="N16" s="104"/>
       <c r="O16" s="48"/>
       <c r="P16" s="48"/>
-      <c r="Q16" s="99" t="s">
+      <c r="Q16" s="105" t="s">
         <v>469</v>
       </c>
-      <c r="R16" s="99"/>
-      <c r="S16" s="99"/>
-      <c r="T16" s="99"/>
+      <c r="R16" s="105"/>
+      <c r="S16" s="105"/>
+      <c r="T16" s="105"/>
       <c r="U16" s="47"/>
       <c r="V16" s="47"/>
       <c r="W16" s="47"/>
       <c r="X16" s="47"/>
-      <c r="Y16" s="62"/>
+      <c r="Y16" s="61"/>
       <c r="Z16" s="47"/>
-      <c r="AA16" s="102"/>
+      <c r="AA16" s="99"/>
       <c r="AB16" s="47"/>
       <c r="AC16" s="47"/>
       <c r="AD16" s="47"/>
@@ -7562,22 +7553,22 @@
       <c r="C17" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="D17" s="103" t="s">
+      <c r="D17" s="100" t="s">
         <v>216</v>
       </c>
       <c r="E17" s="47"/>
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
-      <c r="H17" s="67" t="s">
+      <c r="H17" s="66" t="s">
         <v>476</v>
       </c>
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="58" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L17" s="54" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="M17" s="52" t="s">
         <v>474</v>
@@ -7590,24 +7581,26 @@
       <c r="Q17" s="59">
         <v>41</v>
       </c>
-      <c r="R17" s="60"/>
+      <c r="R17" s="52" t="s">
+        <v>474</v>
+      </c>
       <c r="S17" s="54" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T17" s="47"/>
       <c r="U17" s="47"/>
       <c r="V17" s="47"/>
       <c r="W17" s="47"/>
       <c r="X17" s="47"/>
-      <c r="Y17" s="64" t="s">
+      <c r="Y17" s="63" t="s">
         <v>400</v>
       </c>
       <c r="Z17" s="47"/>
-      <c r="AA17" s="102">
+      <c r="AA17" s="99">
         <v>1.21</v>
       </c>
       <c r="AB17" s="47" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="AC17" s="47"/>
       <c r="AD17" s="47"/>
@@ -7618,22 +7611,22 @@
       <c r="C18" s="47" t="s">
         <v>222</v>
       </c>
-      <c r="D18" s="103" t="s">
+      <c r="D18" s="100" t="s">
         <v>223</v>
       </c>
       <c r="E18" s="47"/>
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
-      <c r="H18" s="67" t="s">
+      <c r="H18" s="66" t="s">
         <v>478</v>
       </c>
       <c r="I18" s="47"/>
       <c r="J18" s="47"/>
       <c r="K18" s="58" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="L18" s="54" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="M18" s="52" t="s">
         <v>474</v>
@@ -7648,22 +7641,22 @@
       </c>
       <c r="R18" s="60"/>
       <c r="S18" s="54" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T18" s="47"/>
       <c r="U18" s="47"/>
       <c r="V18" s="47"/>
       <c r="W18" s="47"/>
       <c r="X18" s="47"/>
-      <c r="Y18" s="64" t="s">
+      <c r="Y18" s="63" t="s">
         <v>401</v>
       </c>
       <c r="Z18" s="47"/>
-      <c r="AA18" s="102" t="s">
-        <v>593</v>
+      <c r="AA18" s="99" t="s">
+        <v>590</v>
       </c>
       <c r="AB18" s="47" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="AC18" s="47"/>
       <c r="AD18" s="47"/>
@@ -7674,21 +7667,21 @@
       <c r="C19" s="47" t="s">
         <v>230</v>
       </c>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="100" t="s">
         <v>231</v>
       </c>
       <c r="E19" s="47"/>
-      <c r="F19" s="63" t="s">
+      <c r="F19" s="62" t="s">
         <v>284</v>
       </c>
       <c r="G19" s="47"/>
       <c r="H19" s="47"/>
       <c r="I19" s="47"/>
       <c r="J19" s="49" t="s">
+        <v>526</v>
+      </c>
+      <c r="L19" s="54" t="s">
         <v>529</v>
-      </c>
-      <c r="L19" s="54" t="s">
-        <v>532</v>
       </c>
       <c r="M19" s="47"/>
       <c r="N19" s="51">
@@ -7699,30 +7692,26 @@
       <c r="Q19" s="53">
         <v>39</v>
       </c>
-      <c r="R19" s="52" t="s">
-        <v>474</v>
-      </c>
+      <c r="R19" s="60"/>
       <c r="S19" s="54" t="s">
-        <v>534</v>
-      </c>
-      <c r="T19" s="61" t="s">
-        <v>516</v>
-      </c>
-      <c r="U19" s="75" t="s">
-        <v>528</v>
+        <v>531</v>
+      </c>
+      <c r="T19" s="47"/>
+      <c r="U19" s="74" t="s">
+        <v>525</v>
       </c>
       <c r="V19" s="47"/>
       <c r="W19" s="47"/>
       <c r="X19" s="47"/>
-      <c r="Y19" s="63" t="s">
+      <c r="Y19" s="62" t="s">
         <v>403</v>
       </c>
       <c r="Z19" s="47"/>
-      <c r="AA19" s="103">
+      <c r="AA19" s="100">
         <v>1.29</v>
       </c>
       <c r="AB19" s="47" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="AC19" s="47"/>
       <c r="AD19" s="47"/>
@@ -7733,22 +7722,22 @@
       <c r="C20" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="D20" s="103" t="s">
+      <c r="D20" s="100" t="s">
         <v>237</v>
       </c>
       <c r="E20" s="47"/>
-      <c r="F20" s="63" t="s">
+      <c r="F20" s="62" t="s">
         <v>285</v>
       </c>
       <c r="G20" s="47"/>
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
       <c r="J20" s="49" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K20" s="47"/>
       <c r="L20" s="54" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="M20" s="47"/>
       <c r="N20" s="51">
@@ -7759,32 +7748,28 @@
       <c r="Q20" s="53">
         <v>38</v>
       </c>
-      <c r="R20" s="52" t="s">
-        <v>474</v>
-      </c>
+      <c r="R20" s="60"/>
       <c r="S20" s="54" t="s">
-        <v>535</v>
-      </c>
-      <c r="T20" s="61" t="s">
-        <v>515</v>
-      </c>
-      <c r="U20" s="75" t="s">
-        <v>575</v>
+        <v>532</v>
+      </c>
+      <c r="T20" s="47"/>
+      <c r="U20" s="74" t="s">
+        <v>572</v>
       </c>
       <c r="V20" s="47"/>
       <c r="W20" s="47"/>
-      <c r="X20" s="68">
+      <c r="X20" s="67">
         <v>17</v>
       </c>
-      <c r="Y20" s="63" t="s">
+      <c r="Y20" s="62" t="s">
         <v>402</v>
       </c>
       <c r="Z20" s="47"/>
-      <c r="AA20" s="102">
+      <c r="AA20" s="99">
         <v>1.28</v>
       </c>
       <c r="AB20" s="47" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="AC20" s="47"/>
       <c r="AD20" s="47"/>
@@ -7795,7 +7780,7 @@
       <c r="C21" s="47" t="s">
         <v>242</v>
       </c>
-      <c r="D21" s="103" t="s">
+      <c r="D21" s="100" t="s">
         <v>243</v>
       </c>
       <c r="E21" s="47"/>
@@ -7805,7 +7790,7 @@
       <c r="I21" s="47"/>
       <c r="J21" s="47"/>
       <c r="K21" s="58" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="L21" s="47"/>
       <c r="M21" s="52" t="s">
@@ -7824,23 +7809,23 @@
       </c>
       <c r="S21" s="47"/>
       <c r="T21" s="47"/>
-      <c r="U21" s="74" t="s">
-        <v>574</v>
+      <c r="U21" s="73" t="s">
+        <v>571</v>
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="47"/>
-      <c r="X21" s="68">
+      <c r="X21" s="67">
         <v>16</v>
       </c>
-      <c r="Y21" s="63" t="s">
+      <c r="Y21" s="62" t="s">
         <v>397</v>
       </c>
       <c r="Z21" s="47"/>
-      <c r="AA21" s="102">
+      <c r="AA21" s="99">
         <v>2.19</v>
       </c>
       <c r="AB21" s="47" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="AC21" s="47"/>
       <c r="AD21" s="47"/>
@@ -7851,7 +7836,7 @@
       <c r="C22" s="47" t="s">
         <v>247</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="99" t="s">
         <v>248</v>
       </c>
       <c r="E22" s="47"/>
@@ -7861,7 +7846,7 @@
       <c r="I22" s="47"/>
       <c r="J22" s="47"/>
       <c r="K22" s="58" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="L22" s="47"/>
       <c r="M22" s="52" t="s">
@@ -7880,21 +7865,21 @@
       </c>
       <c r="S22" s="47"/>
       <c r="T22" s="47"/>
-      <c r="U22" s="74" t="s">
-        <v>573</v>
+      <c r="U22" s="73" t="s">
+        <v>570</v>
       </c>
       <c r="V22" s="47"/>
       <c r="W22" s="47"/>
       <c r="X22" s="47"/>
-      <c r="Y22" s="63" t="s">
+      <c r="Y22" s="62" t="s">
         <v>396</v>
       </c>
       <c r="Z22" s="47"/>
-      <c r="AA22" s="102">
+      <c r="AA22" s="99">
         <v>2.1800000000000002</v>
       </c>
       <c r="AB22" s="47" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="AC22" s="47"/>
       <c r="AD22" s="47"/>
@@ -7905,12 +7890,12 @@
       <c r="C23" s="47" t="s">
         <v>274</v>
       </c>
-      <c r="D23" s="102">
+      <c r="D23" s="99">
         <v>3.23</v>
       </c>
       <c r="E23" s="47"/>
       <c r="F23" s="47"/>
-      <c r="G23" s="68">
+      <c r="G23" s="67">
         <v>23</v>
       </c>
       <c r="H23" s="47"/>
@@ -7934,21 +7919,21 @@
       </c>
       <c r="S23" s="47"/>
       <c r="T23" s="50" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="U23" s="47"/>
       <c r="V23" s="47"/>
       <c r="W23" s="47"/>
       <c r="X23" s="47"/>
-      <c r="Y23" s="63" t="s">
+      <c r="Y23" s="62" t="s">
         <v>395</v>
       </c>
       <c r="Z23" s="47"/>
-      <c r="AA23" s="102">
+      <c r="AA23" s="99">
         <v>2.2799999999999998</v>
       </c>
       <c r="AB23" s="47" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="AC23" s="47"/>
       <c r="AD23" s="47"/>
@@ -7959,16 +7944,16 @@
       <c r="C24" s="47" t="s">
         <v>278</v>
       </c>
-      <c r="D24" s="106">
+      <c r="D24" s="103">
         <v>3.22</v>
       </c>
       <c r="E24" s="47"/>
       <c r="F24" s="47"/>
-      <c r="G24" s="68">
+      <c r="G24" s="67">
         <v>22</v>
       </c>
       <c r="H24" s="47"/>
-      <c r="I24" s="65" t="s">
+      <c r="I24" s="64" t="s">
         <v>488</v>
       </c>
       <c r="J24" s="47"/>
@@ -7983,12 +7968,10 @@
       <c r="Q24" s="53">
         <v>34</v>
       </c>
-      <c r="R24" s="52" t="s">
-        <v>474</v>
-      </c>
+      <c r="R24" s="60"/>
       <c r="S24" s="47"/>
       <c r="T24" s="50" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="U24" s="47"/>
       <c r="V24" s="56" t="s">
@@ -7996,15 +7979,15 @@
       </c>
       <c r="W24" s="47"/>
       <c r="X24" s="47"/>
-      <c r="Y24" s="63" t="s">
+      <c r="Y24" s="62" t="s">
         <v>394</v>
       </c>
       <c r="Z24" s="47"/>
-      <c r="AA24" s="102">
+      <c r="AA24" s="99">
         <v>2.29</v>
       </c>
       <c r="AB24" s="47" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="AC24" s="47"/>
       <c r="AD24" s="47"/>
@@ -8015,16 +7998,16 @@
       <c r="C25" s="47" t="s">
         <v>263</v>
       </c>
-      <c r="D25" s="106" t="s">
+      <c r="D25" s="103" t="s">
         <v>264</v>
       </c>
-      <c r="E25" s="71" t="s">
-        <v>563</v>
-      </c>
-      <c r="F25" s="64">
+      <c r="E25" s="70" t="s">
+        <v>560</v>
+      </c>
+      <c r="F25" s="63">
         <v>9.1666666666666674E-2</v>
       </c>
-      <c r="G25" s="68">
+      <c r="G25" s="67">
         <v>10</v>
       </c>
       <c r="H25" s="47"/>
@@ -8051,16 +8034,16 @@
         <v>472</v>
       </c>
       <c r="W25" s="47"/>
-      <c r="X25" s="68">
+      <c r="X25" s="67">
         <v>9</v>
       </c>
-      <c r="Y25" s="63" t="s">
+      <c r="Y25" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="Z25" s="71" t="s">
-        <v>564</v>
-      </c>
-      <c r="AA25" s="102">
+      <c r="Z25" s="70" t="s">
+        <v>561</v>
+      </c>
+      <c r="AA25" s="99">
         <v>4.7</v>
       </c>
       <c r="AB25" s="47" t="s">
@@ -8070,779 +8053,783 @@
       <c r="AD25" s="47"/>
     </row>
     <row r="26" spans="1:30">
-      <c r="A26" s="77"/>
-      <c r="B26" s="77"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="87"/>
-      <c r="E26" s="77"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="77"/>
-      <c r="J26" s="77"/>
-      <c r="K26" s="77"/>
-      <c r="L26" s="77"/>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="77"/>
-      <c r="P26" s="77"/>
-      <c r="Q26" s="77"/>
-      <c r="R26" s="77"/>
-      <c r="S26" s="77"/>
-      <c r="T26" s="77"/>
-      <c r="U26" s="77"/>
-      <c r="V26" s="77"/>
-      <c r="W26" s="77"/>
-      <c r="X26" s="77"/>
-      <c r="Y26" s="77"/>
-      <c r="Z26" s="77"/>
-      <c r="AA26" s="87"/>
-      <c r="AB26" s="77"/>
-      <c r="AC26" s="78"/>
-      <c r="AD26" s="78"/>
-    </row>
-    <row r="27" spans="1:30" s="76" customFormat="1" ht="11.25">
-      <c r="A27" s="77"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="79" t="s">
+      <c r="A26" s="76"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="76"/>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
+      <c r="L26" s="76"/>
+      <c r="M26" s="76"/>
+      <c r="N26" s="76"/>
+      <c r="O26" s="76"/>
+      <c r="P26" s="76"/>
+      <c r="Q26" s="76"/>
+      <c r="R26" s="76"/>
+      <c r="S26" s="76"/>
+      <c r="T26" s="76"/>
+      <c r="U26" s="76"/>
+      <c r="V26" s="76"/>
+      <c r="W26" s="76"/>
+      <c r="X26" s="76"/>
+      <c r="Y26" s="76"/>
+      <c r="Z26" s="76"/>
+      <c r="AA26" s="86"/>
+      <c r="AB26" s="76"/>
+      <c r="AC26" s="77"/>
+      <c r="AD26" s="77"/>
+    </row>
+    <row r="27" spans="1:30" s="75" customFormat="1" ht="11.25">
+      <c r="A27" s="76"/>
+      <c r="B27" s="76"/>
+      <c r="C27" s="78" t="s">
         <v>299</v>
       </c>
-      <c r="D27" s="87">
+      <c r="D27" s="86">
         <v>2.15</v>
       </c>
-      <c r="E27" s="77"/>
-      <c r="F27" s="80" t="s">
+      <c r="E27" s="76"/>
+      <c r="F27" s="79" t="s">
         <v>290</v>
       </c>
-      <c r="G27" s="81">
+      <c r="G27" s="80">
         <v>7</v>
       </c>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="82" t="s">
+      <c r="H27" s="76"/>
+      <c r="I27" s="76"/>
+      <c r="J27" s="81" t="s">
+        <v>580</v>
+      </c>
+      <c r="K27" s="76"/>
+      <c r="L27" s="76"/>
+      <c r="M27" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="N27" s="83">
+        <v>42</v>
+      </c>
+      <c r="O27" s="84" t="s">
+        <v>586</v>
+      </c>
+      <c r="P27" s="76" t="s">
+        <v>577</v>
+      </c>
+      <c r="Q27" s="83">
+        <v>47</v>
+      </c>
+      <c r="R27" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="S27" s="76"/>
+      <c r="T27" s="85" t="s">
+        <v>507</v>
+      </c>
+      <c r="U27" s="76"/>
+      <c r="V27" s="76"/>
+      <c r="W27" s="76"/>
+      <c r="X27" s="80">
+        <v>8</v>
+      </c>
+      <c r="Y27" s="79" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z27" s="76"/>
+      <c r="AA27" s="86">
+        <v>3.16</v>
+      </c>
+      <c r="AB27" s="86" t="s">
+        <v>300</v>
+      </c>
+      <c r="AC27" s="84"/>
+      <c r="AD27" s="84"/>
+    </row>
+    <row r="28" spans="1:30" s="75" customFormat="1" ht="11.25">
+      <c r="A28" s="76"/>
+      <c r="B28" s="76"/>
+      <c r="C28" s="86" t="s">
+        <v>298</v>
+      </c>
+      <c r="D28" s="86">
+        <v>3.14</v>
+      </c>
+      <c r="E28" s="76"/>
+      <c r="F28" s="79" t="s">
+        <v>291</v>
+      </c>
+      <c r="G28" s="80">
+        <v>6</v>
+      </c>
+      <c r="H28" s="76"/>
+      <c r="I28" s="76"/>
+      <c r="J28" s="81" t="s">
+        <v>581</v>
+      </c>
+      <c r="K28" s="85" t="s">
+        <v>579</v>
+      </c>
+      <c r="L28" s="76"/>
+      <c r="M28" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="N28" s="83">
+        <v>43</v>
+      </c>
+      <c r="O28" s="76" t="s">
+        <v>578</v>
+      </c>
+      <c r="P28" s="76" t="s">
+        <v>587</v>
+      </c>
+      <c r="Q28" s="83">
+        <v>46</v>
+      </c>
+      <c r="R28" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="S28" s="76"/>
+      <c r="T28" s="85" t="s">
+        <v>504</v>
+      </c>
+      <c r="U28" s="76"/>
+      <c r="V28" s="76"/>
+      <c r="W28" s="76"/>
+      <c r="X28" s="80">
+        <v>9</v>
+      </c>
+      <c r="Y28" s="79" t="s">
+        <v>294</v>
+      </c>
+      <c r="Z28" s="76"/>
+      <c r="AA28" s="86">
+        <v>3.17</v>
+      </c>
+      <c r="AB28" s="78" t="s">
+        <v>301</v>
+      </c>
+      <c r="AC28" s="84"/>
+      <c r="AD28" s="84"/>
+    </row>
+    <row r="29" spans="1:30" s="75" customFormat="1" ht="11.25">
+      <c r="A29" s="84"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="84"/>
+      <c r="D29" s="101"/>
+      <c r="E29" s="84"/>
+      <c r="F29" s="84"/>
+      <c r="G29" s="76"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="84"/>
+      <c r="J29" s="84"/>
+      <c r="K29" s="84"/>
+      <c r="L29" s="104" t="s">
+        <v>469</v>
+      </c>
+      <c r="M29" s="104"/>
+      <c r="N29" s="104"/>
+      <c r="O29" s="84" t="s">
+        <v>585</v>
+      </c>
+      <c r="P29" s="84" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q29" s="83">
+        <v>45</v>
+      </c>
+      <c r="R29" s="82" t="s">
+        <v>474</v>
+      </c>
+      <c r="S29" s="84"/>
+      <c r="T29" s="84"/>
+      <c r="U29" s="87" t="s">
         <v>583</v>
       </c>
-      <c r="K27" s="77"/>
-      <c r="L27" s="77"/>
-      <c r="M27" s="83" t="s">
+      <c r="V29" s="84"/>
+      <c r="W29" s="84"/>
+      <c r="X29" s="88">
+        <v>4</v>
+      </c>
+      <c r="Y29" s="89" t="s">
+        <v>293</v>
+      </c>
+      <c r="Z29" s="84"/>
+      <c r="AA29" s="101">
+        <v>3.12</v>
+      </c>
+      <c r="AB29" s="86" t="s">
+        <v>296</v>
+      </c>
+      <c r="AC29" s="84"/>
+      <c r="AD29" s="84"/>
+    </row>
+    <row r="30" spans="1:30" s="75" customFormat="1" ht="11.25">
+      <c r="A30" s="84"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="78" t="s">
+        <v>297</v>
+      </c>
+      <c r="D30" s="101">
+        <v>3.13</v>
+      </c>
+      <c r="E30" s="84"/>
+      <c r="F30" s="89" t="s">
+        <v>292</v>
+      </c>
+      <c r="G30" s="80">
+        <v>5</v>
+      </c>
+      <c r="H30" s="84"/>
+      <c r="I30" s="84"/>
+      <c r="J30" s="87" t="s">
+        <v>582</v>
+      </c>
+      <c r="K30" s="84"/>
+      <c r="L30" s="84"/>
+      <c r="M30" s="90" t="s">
         <v>474</v>
       </c>
-      <c r="N27" s="84">
-        <v>42</v>
-      </c>
-      <c r="O27" s="85" t="s">
+      <c r="N30" s="83">
+        <v>44</v>
+      </c>
+      <c r="O30" s="84" t="s">
+        <v>584</v>
+      </c>
+      <c r="P30" s="76" t="s">
         <v>589</v>
       </c>
-      <c r="P27" s="77" t="s">
-        <v>580</v>
-      </c>
-      <c r="Q27" s="84">
-        <v>47</v>
-      </c>
-      <c r="R27" s="83" t="s">
-        <v>474</v>
-      </c>
-      <c r="S27" s="77"/>
-      <c r="T27" s="86" t="s">
-        <v>508</v>
-      </c>
-      <c r="U27" s="77"/>
-      <c r="V27" s="77"/>
-      <c r="W27" s="77"/>
-      <c r="X27" s="81">
-        <v>8</v>
-      </c>
-      <c r="Y27" s="80" t="s">
-        <v>295</v>
-      </c>
-      <c r="Z27" s="77"/>
-      <c r="AA27" s="87">
-        <v>3.16</v>
-      </c>
-      <c r="AB27" s="87" t="s">
-        <v>300</v>
-      </c>
-      <c r="AC27" s="85"/>
-      <c r="AD27" s="85"/>
-    </row>
-    <row r="28" spans="1:30" s="76" customFormat="1" ht="11.25">
-      <c r="A28" s="77"/>
-      <c r="B28" s="77"/>
-      <c r="C28" s="87" t="s">
-        <v>298</v>
-      </c>
-      <c r="D28" s="87">
-        <v>3.14</v>
-      </c>
-      <c r="E28" s="77"/>
-      <c r="F28" s="80" t="s">
-        <v>291</v>
-      </c>
-      <c r="G28" s="81">
-        <v>6</v>
-      </c>
-      <c r="H28" s="77"/>
-      <c r="I28" s="77"/>
-      <c r="J28" s="82" t="s">
-        <v>584</v>
-      </c>
-      <c r="K28" s="86" t="s">
-        <v>582</v>
-      </c>
-      <c r="L28" s="77"/>
-      <c r="M28" s="83" t="s">
-        <v>474</v>
-      </c>
-      <c r="N28" s="84">
-        <v>43</v>
-      </c>
-      <c r="O28" s="77" t="s">
-        <v>581</v>
-      </c>
-      <c r="P28" s="77" t="s">
-        <v>590</v>
-      </c>
-      <c r="Q28" s="84">
-        <v>46</v>
-      </c>
-      <c r="R28" s="83" t="s">
-        <v>474</v>
-      </c>
-      <c r="S28" s="77"/>
-      <c r="T28" s="86" t="s">
-        <v>505</v>
-      </c>
-      <c r="U28" s="77"/>
-      <c r="V28" s="77"/>
-      <c r="W28" s="77"/>
-      <c r="X28" s="81">
-        <v>9</v>
-      </c>
-      <c r="Y28" s="80" t="s">
-        <v>294</v>
-      </c>
-      <c r="Z28" s="77"/>
-      <c r="AA28" s="87">
-        <v>3.17</v>
-      </c>
-      <c r="AB28" s="79" t="s">
-        <v>301</v>
-      </c>
-      <c r="AC28" s="85"/>
-      <c r="AD28" s="85"/>
-    </row>
-    <row r="29" spans="1:30" s="76" customFormat="1" ht="11.25">
-      <c r="A29" s="85"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="85"/>
-      <c r="D29" s="104"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="77"/>
-      <c r="H29" s="85"/>
-      <c r="I29" s="85"/>
-      <c r="J29" s="85"/>
-      <c r="K29" s="85"/>
-      <c r="L29" s="98" t="s">
-        <v>469</v>
-      </c>
-      <c r="M29" s="98"/>
-      <c r="N29" s="98"/>
-      <c r="O29" s="85" t="s">
-        <v>588</v>
-      </c>
-      <c r="P29" s="85" t="s">
-        <v>591</v>
-      </c>
-      <c r="Q29" s="84">
-        <v>45</v>
-      </c>
-      <c r="R29" s="83" t="s">
-        <v>474</v>
-      </c>
-      <c r="S29" s="85"/>
-      <c r="T29" s="85"/>
-      <c r="U29" s="88" t="s">
-        <v>586</v>
-      </c>
-      <c r="V29" s="85"/>
-      <c r="W29" s="85"/>
-      <c r="X29" s="89">
-        <v>4</v>
-      </c>
-      <c r="Y29" s="90" t="s">
-        <v>293</v>
-      </c>
-      <c r="Z29" s="85"/>
-      <c r="AA29" s="104">
-        <v>3.12</v>
-      </c>
-      <c r="AB29" s="87" t="s">
-        <v>296</v>
-      </c>
-      <c r="AC29" s="85"/>
-      <c r="AD29" s="85"/>
-    </row>
-    <row r="30" spans="1:30" s="76" customFormat="1" ht="11.25">
-      <c r="A30" s="85"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="79" t="s">
-        <v>297</v>
-      </c>
-      <c r="D30" s="104">
-        <v>3.13</v>
-      </c>
-      <c r="E30" s="85"/>
-      <c r="F30" s="90" t="s">
-        <v>292</v>
-      </c>
-      <c r="G30" s="81">
-        <v>5</v>
-      </c>
-      <c r="H30" s="85"/>
-      <c r="I30" s="85"/>
-      <c r="J30" s="88" t="s">
-        <v>585</v>
-      </c>
-      <c r="K30" s="85"/>
-      <c r="L30" s="85"/>
-      <c r="M30" s="91" t="s">
-        <v>474</v>
-      </c>
-      <c r="N30" s="84">
-        <v>44</v>
-      </c>
-      <c r="O30" s="85" t="s">
-        <v>587</v>
-      </c>
-      <c r="P30" s="77" t="s">
-        <v>592</v>
-      </c>
-      <c r="Q30" s="98" t="s">
-        <v>498</v>
-      </c>
-      <c r="R30" s="98"/>
-      <c r="S30" s="98"/>
-      <c r="T30" s="85"/>
-      <c r="U30" s="85"/>
-      <c r="V30" s="85"/>
-      <c r="W30" s="85"/>
-      <c r="X30" s="85"/>
-      <c r="Y30" s="85"/>
-      <c r="Z30" s="85"/>
-      <c r="AA30" s="104"/>
-      <c r="AB30" s="85"/>
-      <c r="AC30" s="85"/>
-      <c r="AD30" s="85"/>
+      <c r="Q30" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="R30" s="104"/>
+      <c r="S30" s="104"/>
+      <c r="T30" s="84"/>
+      <c r="U30" s="84"/>
+      <c r="V30" s="84"/>
+      <c r="W30" s="84"/>
+      <c r="X30" s="84"/>
+      <c r="Y30" s="84"/>
+      <c r="Z30" s="84"/>
+      <c r="AA30" s="101"/>
+      <c r="AB30" s="84"/>
+      <c r="AC30" s="84"/>
+      <c r="AD30" s="84"/>
     </row>
     <row r="31" spans="1:30">
-      <c r="A31" s="78"/>
-      <c r="B31" s="78"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="105"/>
-      <c r="E31" s="78"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="78"/>
-      <c r="H31" s="78"/>
-      <c r="I31" s="78"/>
-      <c r="J31" s="78"/>
-      <c r="K31" s="78"/>
-      <c r="L31" s="78"/>
-      <c r="M31" s="78"/>
-      <c r="N31" s="78"/>
-      <c r="O31" s="78"/>
-      <c r="P31" s="78"/>
-      <c r="Q31" s="78"/>
-      <c r="R31" s="78"/>
-      <c r="S31" s="78"/>
-      <c r="T31" s="78"/>
-      <c r="U31" s="78"/>
-      <c r="V31" s="78"/>
-      <c r="W31" s="78"/>
-      <c r="X31" s="78"/>
-      <c r="Y31" s="78"/>
-      <c r="Z31" s="78"/>
-      <c r="AA31" s="105"/>
-      <c r="AB31" s="78"/>
-      <c r="AC31" s="78"/>
-      <c r="AD31" s="78"/>
+      <c r="A31" s="77"/>
+      <c r="B31" s="77"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="102"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="77"/>
+      <c r="J31" s="77"/>
+      <c r="K31" s="77"/>
+      <c r="L31" s="77"/>
+      <c r="M31" s="77"/>
+      <c r="N31" s="77"/>
+      <c r="O31" s="77"/>
+      <c r="P31" s="77"/>
+      <c r="Q31" s="77"/>
+      <c r="R31" s="77"/>
+      <c r="S31" s="77"/>
+      <c r="T31" s="77"/>
+      <c r="U31" s="77"/>
+      <c r="V31" s="77"/>
+      <c r="W31" s="77"/>
+      <c r="X31" s="77"/>
+      <c r="Y31" s="77"/>
+      <c r="Z31" s="77"/>
+      <c r="AA31" s="102"/>
+      <c r="AB31" s="77"/>
+      <c r="AC31" s="77"/>
+      <c r="AD31" s="77"/>
     </row>
     <row r="32" spans="1:30">
-      <c r="A32" s="78"/>
-      <c r="B32" s="78"/>
-      <c r="C32" s="78"/>
-      <c r="D32" s="105"/>
-      <c r="E32" s="78"/>
-      <c r="F32" s="78"/>
-      <c r="G32" s="78"/>
-      <c r="H32" s="78"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="78"/>
-      <c r="K32" s="78"/>
-      <c r="L32" s="78"/>
-      <c r="M32" s="78"/>
-      <c r="N32" s="78"/>
-      <c r="O32" s="77" t="s">
-        <v>576</v>
-      </c>
-      <c r="P32" s="78"/>
-      <c r="Q32" s="78"/>
-      <c r="R32" s="78"/>
-      <c r="S32" s="78"/>
-      <c r="T32" s="78"/>
-      <c r="U32" s="78"/>
-      <c r="V32" s="78"/>
-      <c r="W32" s="78"/>
-      <c r="X32" s="78"/>
-      <c r="Y32" s="78"/>
-      <c r="Z32" s="78"/>
-      <c r="AA32" s="105"/>
-      <c r="AB32" s="78"/>
-      <c r="AC32" s="78"/>
-      <c r="AD32" s="78"/>
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="102"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="76" t="s">
+        <v>573</v>
+      </c>
+      <c r="P32" s="77"/>
+      <c r="Q32" s="77"/>
+      <c r="R32" s="77"/>
+      <c r="S32" s="77"/>
+      <c r="T32" s="77"/>
+      <c r="U32" s="77"/>
+      <c r="V32" s="77"/>
+      <c r="W32" s="77"/>
+      <c r="X32" s="77"/>
+      <c r="Y32" s="77"/>
+      <c r="Z32" s="77"/>
+      <c r="AA32" s="102"/>
+      <c r="AB32" s="77"/>
+      <c r="AC32" s="77"/>
+      <c r="AD32" s="77"/>
     </row>
     <row r="33" spans="1:30">
-      <c r="A33" s="77"/>
-      <c r="B33" s="77"/>
-      <c r="C33" s="77" t="s">
+      <c r="A33" s="76"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="76" t="s">
         <v>409</v>
       </c>
-      <c r="D33" s="87">
+      <c r="D33" s="86">
         <v>4.26</v>
       </c>
-      <c r="E33" s="77"/>
-      <c r="F33" s="92">
+      <c r="E33" s="76"/>
+      <c r="F33" s="91">
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="77"/>
-      <c r="J33" s="77"/>
-      <c r="K33" s="93" t="s">
+      <c r="G33" s="76"/>
+      <c r="H33" s="76"/>
+      <c r="I33" s="76"/>
+      <c r="J33" s="76"/>
+      <c r="K33" s="92" t="s">
         <v>471</v>
       </c>
-      <c r="L33" s="77"/>
+      <c r="L33" s="76"/>
       <c r="M33" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="N33" s="94">
+      <c r="N33" s="93">
         <v>52</v>
       </c>
-      <c r="O33" s="77"/>
-      <c r="P33" s="77"/>
-      <c r="Q33" s="99" t="s">
+      <c r="O33" s="76"/>
+      <c r="P33" s="76"/>
+      <c r="Q33" s="105" t="s">
         <v>469</v>
       </c>
-      <c r="R33" s="99"/>
-      <c r="S33" s="99"/>
-      <c r="T33" s="99"/>
-      <c r="U33" s="77"/>
-      <c r="V33" s="77"/>
-      <c r="W33" s="77"/>
-      <c r="X33" s="77"/>
-      <c r="Y33" s="77"/>
-      <c r="Z33" s="77"/>
-      <c r="AA33" s="87"/>
-      <c r="AB33" s="77"/>
-      <c r="AC33" s="78"/>
-      <c r="AD33" s="78"/>
+      <c r="R33" s="105"/>
+      <c r="S33" s="105"/>
+      <c r="T33" s="105"/>
+      <c r="U33" s="76"/>
+      <c r="V33" s="76"/>
+      <c r="W33" s="76"/>
+      <c r="X33" s="76"/>
+      <c r="Y33" s="76"/>
+      <c r="Z33" s="76"/>
+      <c r="AA33" s="86"/>
+      <c r="AB33" s="76"/>
+      <c r="AC33" s="77"/>
+      <c r="AD33" s="77"/>
     </row>
     <row r="34" spans="1:30">
-      <c r="A34" s="77"/>
-      <c r="B34" s="77"/>
-      <c r="C34" s="77" t="s">
+      <c r="A34" s="76"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="76" t="s">
         <v>408</v>
       </c>
-      <c r="D34" s="87">
+      <c r="D34" s="86">
         <v>4.25</v>
       </c>
-      <c r="E34" s="77"/>
-      <c r="F34" s="77"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="77"/>
-      <c r="I34" s="77"/>
-      <c r="J34" s="77"/>
-      <c r="K34" s="93" t="s">
+      <c r="E34" s="76"/>
+      <c r="F34" s="76"/>
+      <c r="G34" s="76"/>
+      <c r="H34" s="76"/>
+      <c r="I34" s="76"/>
+      <c r="J34" s="76"/>
+      <c r="K34" s="92" t="s">
         <v>472</v>
       </c>
-      <c r="L34" s="77"/>
+      <c r="L34" s="76"/>
       <c r="M34" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="N34" s="94">
+      <c r="N34" s="93">
         <v>53</v>
       </c>
-      <c r="O34" s="77"/>
-      <c r="P34" s="77"/>
-      <c r="Q34" s="94">
+      <c r="O34" s="76"/>
+      <c r="P34" s="76"/>
+      <c r="Q34" s="93">
         <v>50</v>
       </c>
       <c r="R34" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="S34" s="77"/>
-      <c r="T34" s="95" t="s">
-        <v>579</v>
-      </c>
-      <c r="U34" s="96" t="s">
-        <v>584</v>
-      </c>
-      <c r="V34" s="77"/>
-      <c r="W34" s="77"/>
-      <c r="X34" s="77"/>
-      <c r="Y34" s="92">
+      <c r="S34" s="76"/>
+      <c r="T34" s="94" t="s">
+        <v>576</v>
+      </c>
+      <c r="U34" s="95" t="s">
+        <v>581</v>
+      </c>
+      <c r="V34" s="76"/>
+      <c r="W34" s="76"/>
+      <c r="X34" s="76"/>
+      <c r="Y34" s="91">
         <v>5.1388888888888894E-2</v>
       </c>
-      <c r="Z34" s="77"/>
-      <c r="AA34" s="87">
+      <c r="Z34" s="76"/>
+      <c r="AA34" s="86">
         <v>4.28</v>
       </c>
-      <c r="AB34" s="77" t="s">
+      <c r="AB34" s="76" t="s">
         <v>411</v>
       </c>
-      <c r="AC34" s="78"/>
-      <c r="AD34" s="78"/>
+      <c r="AC34" s="77"/>
+      <c r="AD34" s="77"/>
     </row>
     <row r="35" spans="1:30">
-      <c r="A35" s="77"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77" t="s">
+      <c r="A35" s="76"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76" t="s">
         <v>412</v>
       </c>
-      <c r="D35" s="87">
+      <c r="D35" s="86">
         <v>4.29</v>
       </c>
-      <c r="E35" s="77"/>
-      <c r="F35" s="92">
+      <c r="E35" s="76"/>
+      <c r="F35" s="91">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="96" t="s">
-        <v>583</v>
-      </c>
-      <c r="K35" s="77"/>
-      <c r="L35" s="77"/>
+      <c r="G35" s="76"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="76"/>
+      <c r="J35" s="95" t="s">
+        <v>580</v>
+      </c>
+      <c r="K35" s="76"/>
+      <c r="L35" s="76"/>
       <c r="M35" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="N35" s="94">
+      <c r="N35" s="93">
         <v>54</v>
       </c>
-      <c r="O35" s="77"/>
-      <c r="P35" s="77" t="s">
-        <v>577</v>
-      </c>
-      <c r="Q35" s="94">
+      <c r="O35" s="76"/>
+      <c r="P35" s="76" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q35" s="93">
         <v>49</v>
       </c>
       <c r="R35" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="S35" s="77"/>
-      <c r="T35" s="77"/>
-      <c r="U35" s="96" t="s">
-        <v>586</v>
-      </c>
-      <c r="V35" s="77"/>
-      <c r="W35" s="77"/>
-      <c r="X35" s="77"/>
-      <c r="Y35" s="92">
+      <c r="S35" s="76"/>
+      <c r="T35" s="76"/>
+      <c r="U35" s="95" t="s">
+        <v>583</v>
+      </c>
+      <c r="V35" s="76"/>
+      <c r="W35" s="76"/>
+      <c r="X35" s="76"/>
+      <c r="Y35" s="91">
         <v>5.0694444444444452E-2</v>
       </c>
-      <c r="Z35" s="77"/>
-      <c r="AA35" s="87">
+      <c r="Z35" s="76"/>
+      <c r="AA35" s="86">
         <v>4.2699999999999996</v>
       </c>
-      <c r="AB35" s="77" t="s">
+      <c r="AB35" s="76" t="s">
         <v>410</v>
       </c>
-      <c r="AC35" s="78"/>
-      <c r="AD35" s="78"/>
+      <c r="AC35" s="77"/>
+      <c r="AD35" s="77"/>
     </row>
     <row r="36" spans="1:30">
-      <c r="A36" s="77"/>
-      <c r="B36" s="77"/>
-      <c r="C36" s="77"/>
-      <c r="D36" s="87"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="77"/>
-      <c r="L36" s="98" t="s">
-        <v>498</v>
-      </c>
-      <c r="M36" s="98"/>
-      <c r="N36" s="98"/>
-      <c r="O36" s="77"/>
-      <c r="P36" s="77"/>
-      <c r="Q36" s="94">
+      <c r="A36" s="76"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
+      <c r="I36" s="76"/>
+      <c r="J36" s="76"/>
+      <c r="K36" s="76"/>
+      <c r="L36" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="M36" s="104"/>
+      <c r="N36" s="104"/>
+      <c r="O36" s="76"/>
+      <c r="P36" s="76"/>
+      <c r="Q36" s="93">
         <v>51</v>
       </c>
       <c r="R36" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="S36" s="77"/>
-      <c r="T36" s="77"/>
-      <c r="U36" s="77"/>
-      <c r="V36" s="77"/>
-      <c r="W36" s="97" t="s">
-        <v>502</v>
-      </c>
-      <c r="X36" s="77"/>
-      <c r="Y36" s="77"/>
-      <c r="Z36" s="77"/>
-      <c r="AA36" s="87">
+      <c r="S36" s="76"/>
+      <c r="T36" s="76"/>
+      <c r="U36" s="76"/>
+      <c r="V36" s="76"/>
+      <c r="W36" s="96" t="s">
+        <v>501</v>
+      </c>
+      <c r="X36" s="76"/>
+      <c r="Y36" s="76"/>
+      <c r="Z36" s="76"/>
+      <c r="AA36" s="86">
         <v>4.22</v>
       </c>
-      <c r="AB36" s="77" t="s">
+      <c r="AB36" s="76" t="s">
         <v>407</v>
       </c>
-      <c r="AC36" s="78"/>
-      <c r="AD36" s="78"/>
+      <c r="AC36" s="77"/>
+      <c r="AD36" s="77"/>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="77"/>
-      <c r="B37" s="77"/>
-      <c r="C37" s="77"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="77"/>
-      <c r="F37" s="77"/>
-      <c r="G37" s="77"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
-      <c r="K37" s="77"/>
-      <c r="L37" s="77"/>
-      <c r="M37" s="77"/>
-      <c r="N37" s="77"/>
-      <c r="O37" s="77"/>
-      <c r="P37" s="77"/>
-      <c r="Q37" s="77"/>
-      <c r="R37" s="77"/>
-      <c r="S37" s="77"/>
-      <c r="T37" s="77"/>
-      <c r="U37" s="77"/>
-      <c r="V37" s="77"/>
-      <c r="W37" s="77"/>
-      <c r="X37" s="77"/>
-      <c r="Y37" s="77"/>
-      <c r="Z37" s="77"/>
-      <c r="AA37" s="87"/>
-      <c r="AB37" s="77"/>
-      <c r="AC37" s="78"/>
-      <c r="AD37" s="78"/>
+      <c r="A37" s="76"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="76"/>
+      <c r="O37" s="76"/>
+      <c r="P37" s="76"/>
+      <c r="Q37" s="76"/>
+      <c r="R37" s="76"/>
+      <c r="S37" s="76"/>
+      <c r="T37" s="76"/>
+      <c r="U37" s="76"/>
+      <c r="V37" s="76"/>
+      <c r="W37" s="76"/>
+      <c r="X37" s="76"/>
+      <c r="Y37" s="76"/>
+      <c r="Z37" s="76"/>
+      <c r="AA37" s="86"/>
+      <c r="AB37" s="76"/>
+      <c r="AC37" s="77"/>
+      <c r="AD37" s="77"/>
     </row>
     <row r="38" spans="1:30">
-      <c r="A38" s="77"/>
-      <c r="B38" s="77"/>
-      <c r="C38" s="77" t="s">
+      <c r="A38" s="76"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="76" t="s">
         <v>409</v>
       </c>
-      <c r="D38" s="87">
+      <c r="D38" s="86">
         <v>4.26</v>
       </c>
-      <c r="E38" s="77"/>
-      <c r="F38" s="92">
+      <c r="E38" s="76"/>
+      <c r="F38" s="91">
         <v>4.9999999999999996E-2</v>
       </c>
-      <c r="G38" s="77"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="77"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="93" t="s">
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="92" t="s">
         <v>471</v>
       </c>
-      <c r="L38" s="77"/>
+      <c r="L38" s="76"/>
       <c r="M38" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="N38" s="94">
+      <c r="N38" s="93">
         <v>52</v>
       </c>
-      <c r="O38" s="77"/>
-      <c r="P38" s="77"/>
-      <c r="Q38" s="99" t="s">
+      <c r="O38" s="76"/>
+      <c r="P38" s="76"/>
+      <c r="Q38" s="105" t="s">
         <v>469</v>
       </c>
-      <c r="R38" s="99"/>
-      <c r="S38" s="99"/>
-      <c r="T38" s="99"/>
-      <c r="U38" s="77"/>
-      <c r="V38" s="77"/>
-      <c r="W38" s="77"/>
-      <c r="X38" s="77"/>
-      <c r="Y38" s="77"/>
-      <c r="Z38" s="77"/>
-      <c r="AA38" s="87"/>
-      <c r="AB38" s="77"/>
-      <c r="AC38" s="78"/>
-      <c r="AD38" s="78"/>
+      <c r="R38" s="105"/>
+      <c r="S38" s="105"/>
+      <c r="T38" s="105"/>
+      <c r="U38" s="76"/>
+      <c r="V38" s="76"/>
+      <c r="W38" s="76"/>
+      <c r="X38" s="76"/>
+      <c r="Y38" s="76"/>
+      <c r="Z38" s="76"/>
+      <c r="AA38" s="86"/>
+      <c r="AB38" s="76"/>
+      <c r="AC38" s="77"/>
+      <c r="AD38" s="77"/>
     </row>
     <row r="39" spans="1:30">
-      <c r="A39" s="77"/>
-      <c r="B39" s="77"/>
-      <c r="C39" s="77" t="s">
+      <c r="A39" s="76"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="76" t="s">
         <v>408</v>
       </c>
-      <c r="D39" s="87">
+      <c r="D39" s="86">
         <v>4.25</v>
       </c>
-      <c r="E39" s="77"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="77"/>
-      <c r="J39" s="77"/>
-      <c r="K39" s="93" t="s">
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="92" t="s">
         <v>472</v>
       </c>
-      <c r="L39" s="77"/>
+      <c r="L39" s="76"/>
       <c r="M39" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="N39" s="94">
+      <c r="N39" s="93">
         <v>53</v>
       </c>
-      <c r="O39" s="77"/>
-      <c r="P39" s="77"/>
-      <c r="Q39" s="94">
+      <c r="O39" s="76"/>
+      <c r="P39" s="76"/>
+      <c r="Q39" s="93">
         <v>50</v>
       </c>
       <c r="R39" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="S39" s="77"/>
-      <c r="T39" s="95" t="s">
-        <v>579</v>
-      </c>
-      <c r="U39" s="96" t="s">
-        <v>584</v>
-      </c>
-      <c r="V39" s="77"/>
-      <c r="W39" s="77"/>
-      <c r="X39" s="77"/>
-      <c r="Y39" s="92">
+      <c r="S39" s="76"/>
+      <c r="T39" s="94" t="s">
+        <v>576</v>
+      </c>
+      <c r="U39" s="95" t="s">
+        <v>581</v>
+      </c>
+      <c r="V39" s="76"/>
+      <c r="W39" s="76"/>
+      <c r="X39" s="76"/>
+      <c r="Y39" s="91">
         <v>5.1388888888888894E-2</v>
       </c>
-      <c r="Z39" s="77"/>
-      <c r="AA39" s="87">
+      <c r="Z39" s="76"/>
+      <c r="AA39" s="86">
         <v>4.28</v>
       </c>
-      <c r="AB39" s="77" t="s">
+      <c r="AB39" s="76" t="s">
         <v>411</v>
       </c>
-      <c r="AC39" s="78"/>
-      <c r="AD39" s="78"/>
+      <c r="AC39" s="77"/>
+      <c r="AD39" s="77"/>
     </row>
     <row r="40" spans="1:30">
-      <c r="A40" s="77"/>
-      <c r="B40" s="77"/>
-      <c r="C40" s="77" t="s">
+      <c r="A40" s="76"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="76" t="s">
         <v>412</v>
       </c>
-      <c r="D40" s="87">
+      <c r="D40" s="86">
         <v>4.29</v>
       </c>
-      <c r="E40" s="77"/>
-      <c r="F40" s="92">
+      <c r="E40" s="76"/>
+      <c r="F40" s="91">
         <v>5.2083333333333336E-2</v>
       </c>
-      <c r="G40" s="77"/>
-      <c r="H40" s="77"/>
-      <c r="I40" s="77"/>
-      <c r="J40" s="96" t="s">
-        <v>583</v>
-      </c>
-      <c r="K40" s="77"/>
-      <c r="L40" s="77"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="76"/>
+      <c r="J40" s="95" t="s">
+        <v>580</v>
+      </c>
+      <c r="K40" s="76"/>
+      <c r="L40" s="76"/>
       <c r="M40" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="N40" s="94">
+      <c r="N40" s="93">
         <v>54</v>
       </c>
-      <c r="O40" s="77"/>
-      <c r="P40" s="77"/>
-      <c r="Q40" s="94">
+      <c r="O40" s="76"/>
+      <c r="P40" s="76"/>
+      <c r="Q40" s="93">
         <v>49</v>
       </c>
       <c r="R40" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="S40" s="77"/>
-      <c r="T40" s="77"/>
-      <c r="U40" s="96" t="s">
-        <v>586</v>
-      </c>
-      <c r="V40" s="77"/>
-      <c r="W40" s="77"/>
-      <c r="X40" s="77"/>
-      <c r="Y40" s="92">
+      <c r="S40" s="76"/>
+      <c r="T40" s="76"/>
+      <c r="U40" s="95" t="s">
+        <v>583</v>
+      </c>
+      <c r="V40" s="76"/>
+      <c r="W40" s="76"/>
+      <c r="X40" s="76"/>
+      <c r="Y40" s="91">
         <v>5.0694444444444452E-2</v>
       </c>
-      <c r="Z40" s="77"/>
-      <c r="AA40" s="87">
+      <c r="Z40" s="76"/>
+      <c r="AA40" s="86">
         <v>4.2699999999999996</v>
       </c>
-      <c r="AB40" s="77" t="s">
+      <c r="AB40" s="76" t="s">
         <v>410</v>
       </c>
-      <c r="AC40" s="78"/>
-      <c r="AD40" s="78"/>
+      <c r="AC40" s="77"/>
+      <c r="AD40" s="77"/>
     </row>
     <row r="41" spans="1:30">
-      <c r="A41" s="77"/>
-      <c r="B41" s="77"/>
-      <c r="C41" s="77"/>
-      <c r="D41" s="87"/>
-      <c r="E41" s="77"/>
-      <c r="F41" s="77"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="77"/>
-      <c r="I41" s="77"/>
-      <c r="J41" s="77"/>
-      <c r="K41" s="77"/>
-      <c r="L41" s="98" t="s">
-        <v>498</v>
-      </c>
-      <c r="M41" s="98"/>
-      <c r="N41" s="98"/>
-      <c r="O41" s="77"/>
-      <c r="P41" s="77" t="s">
-        <v>577</v>
-      </c>
-      <c r="Q41" s="94">
+      <c r="A41" s="76"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="86"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="104" t="s">
+        <v>497</v>
+      </c>
+      <c r="M41" s="104"/>
+      <c r="N41" s="104"/>
+      <c r="O41" s="76"/>
+      <c r="P41" s="76" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q41" s="93">
         <v>48</v>
       </c>
       <c r="R41" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="S41" s="77"/>
-      <c r="T41" s="93" t="s">
-        <v>513</v>
-      </c>
-      <c r="U41" s="77"/>
-      <c r="V41" s="77"/>
-      <c r="W41" s="77"/>
-      <c r="X41" s="77"/>
-      <c r="Y41" s="77"/>
-      <c r="Z41" s="77"/>
-      <c r="AA41" s="87">
+      <c r="S41" s="76"/>
+      <c r="T41" s="92" t="s">
+        <v>512</v>
+      </c>
+      <c r="U41" s="76"/>
+      <c r="V41" s="76"/>
+      <c r="W41" s="76"/>
+      <c r="X41" s="76"/>
+      <c r="Y41" s="76"/>
+      <c r="Z41" s="76"/>
+      <c r="AA41" s="86">
         <v>4.24</v>
       </c>
-      <c r="AB41" s="87" t="s">
+      <c r="AB41" s="86" t="s">
         <v>253</v>
       </c>
-      <c r="AC41" s="78"/>
-      <c r="AD41" s="78"/>
+      <c r="AC41" s="77"/>
+      <c r="AD41" s="77"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="Q4:T4"/>
     <mergeCell ref="L41:N41"/>
     <mergeCell ref="L36:N36"/>
     <mergeCell ref="Q38:T38"/>
@@ -8851,11 +8838,6 @@
     <mergeCell ref="Q16:T16"/>
     <mergeCell ref="L29:N29"/>
     <mergeCell ref="Q30:S30"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="R15:S15"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
T4 and T4.1 update XBAR pins on card like
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D49BAA-52F7-42CE-B381-469D562E251A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D0F54D-2672-4441-80A5-8B7DE99086E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="0" windowWidth="22650" windowHeight="20415" activeTab="2" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="22605" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="18000" yWindow="720" windowWidth="22605" windowHeight="20415" xr2:uid="{704AA4A8-87AD-42BA-A92F-F9E203ADE002}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
-    <sheet name="T4.1(Larger)" sheetId="6" r:id="rId2"/>
-    <sheet name="T4.1 card like" sheetId="7" r:id="rId3"/>
-    <sheet name="Beta 2" sheetId="1" r:id="rId4"/>
-    <sheet name="Beta 1" sheetId="2" r:id="rId5"/>
+    <sheet name="T4 card like" sheetId="8" r:id="rId2"/>
+    <sheet name="T4.1(Larger)" sheetId="6" r:id="rId3"/>
+    <sheet name="T4.1 card like" sheetId="7" r:id="rId4"/>
+    <sheet name="Beta 2" sheetId="1" r:id="rId5"/>
+    <sheet name="Beta 1" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="4" hidden="1">'Beta 1'!$A$1:$M$36</definedName>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">'Beta 2'!$A$1:$M$45</definedName>
+    <definedName name="ExternalData_1" localSheetId="5" hidden="1">'Beta 1'!$A$1:$M$36</definedName>
+    <definedName name="ExternalData_1" localSheetId="4" hidden="1">'Beta 2'!$A$1:$M$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="595">
   <si>
     <t>Column1</t>
   </si>
@@ -1829,6 +1831,12 @@
   </si>
   <si>
     <t>SDIO Pins</t>
+  </si>
+  <si>
+    <t>Bottom SDIO Pins</t>
+  </si>
+  <si>
+    <t>Bottom SMT Pins</t>
   </si>
 </sst>
 </file>
@@ -2119,7 +2127,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2175,12 +2183,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="164">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2375,6 +2407,144 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="18" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="19" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="20" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2538,6 +2708,159 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>90407</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>249116</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>791025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55B44057-6366-4275-B467-5C9FD4CBDA6D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="3811101" y="997845"/>
+          <a:ext cx="2806211" cy="1308753"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>146539</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>168520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>754672</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>55762</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BDC96FD-E42F-4CD8-831E-C3E4601D5305}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4615962" y="3223847"/>
+          <a:ext cx="1216268" cy="1411242"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>65267</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>131882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>681404</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>132061</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A504D664-1E9C-4447-B31B-C7CA24ECAE80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4534690" y="4711209"/>
+          <a:ext cx="1224272" cy="2344794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3002,7 +3325,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4A98D7-59ED-43A9-B01B-8AE7AF7474EA}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4632,6 +4960,1927 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCC63EF2-98A0-433F-8E4A-255F5D191DD4}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:AD37"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.7109375" customWidth="1"/>
+    <col min="26" max="26" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="30.75">
+      <c r="A1" s="104" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="104" t="s">
+        <v>466</v>
+      </c>
+      <c r="C1" s="105" t="s">
+        <v>467</v>
+      </c>
+      <c r="D1" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="109" t="s">
+        <v>546</v>
+      </c>
+      <c r="H1" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="111" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="112" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="114" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="116" t="s">
+        <v>468</v>
+      </c>
+      <c r="O1" s="105"/>
+      <c r="P1" s="105"/>
+      <c r="Q1" s="116" t="s">
+        <v>468</v>
+      </c>
+      <c r="R1" s="115" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="114" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="113" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="112" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="111" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="110" t="s">
+        <v>18</v>
+      </c>
+      <c r="X1" s="117" t="s">
+        <v>546</v>
+      </c>
+      <c r="Y1" s="108" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="107" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" s="105" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC1" s="104" t="s">
+        <v>466</v>
+      </c>
+      <c r="AD1" s="104" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
+      <c r="A2" s="118" t="s">
+        <v>534</v>
+      </c>
+      <c r="B2" s="118" t="s">
+        <v>469</v>
+      </c>
+      <c r="C2" s="118"/>
+      <c r="D2" s="119"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="118"/>
+      <c r="H2" s="118"/>
+      <c r="I2" s="118"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="118"/>
+      <c r="L2" s="161" t="s">
+        <v>469</v>
+      </c>
+      <c r="M2" s="161"/>
+      <c r="N2" s="161"/>
+      <c r="O2" s="121"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="160" t="s">
+        <v>470</v>
+      </c>
+      <c r="R2" s="160"/>
+      <c r="S2" s="160"/>
+      <c r="T2" s="160"/>
+      <c r="U2" s="118"/>
+      <c r="V2" s="118"/>
+      <c r="W2" s="118"/>
+      <c r="X2" s="118"/>
+      <c r="Y2" s="118"/>
+      <c r="Z2" s="118"/>
+      <c r="AA2" s="122"/>
+      <c r="AB2" s="118"/>
+      <c r="AC2" s="118" t="s">
+        <v>535</v>
+      </c>
+      <c r="AD2" s="118"/>
+    </row>
+    <row r="3" spans="1:30">
+      <c r="A3" s="118"/>
+      <c r="B3" s="118"/>
+      <c r="C3" s="118" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="122" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="120">
+        <v>17</v>
+      </c>
+      <c r="H3" s="118"/>
+      <c r="I3" s="123" t="s">
+        <v>491</v>
+      </c>
+      <c r="J3" s="124" t="s">
+        <v>502</v>
+      </c>
+      <c r="K3" s="125" t="s">
+        <v>471</v>
+      </c>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="126">
+        <v>0</v>
+      </c>
+      <c r="O3" s="121"/>
+      <c r="P3" s="121"/>
+      <c r="Q3" s="160" t="s">
+        <v>469</v>
+      </c>
+      <c r="R3" s="160"/>
+      <c r="S3" s="160"/>
+      <c r="T3" s="160"/>
+      <c r="U3" s="118"/>
+      <c r="V3" s="118"/>
+      <c r="W3" s="118"/>
+      <c r="X3" s="118"/>
+      <c r="Y3" s="118"/>
+      <c r="Z3" s="118"/>
+      <c r="AA3" s="122"/>
+      <c r="AB3" s="118"/>
+      <c r="AC3" s="118" t="s">
+        <v>534</v>
+      </c>
+      <c r="AD3" s="118" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" s="118"/>
+      <c r="B4" s="118"/>
+      <c r="C4" s="118" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="122" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="118"/>
+      <c r="F4" s="118"/>
+      <c r="G4" s="120">
+        <v>16</v>
+      </c>
+      <c r="H4" s="118"/>
+      <c r="I4" s="123" t="s">
+        <v>493</v>
+      </c>
+      <c r="J4" s="124" t="s">
+        <v>525</v>
+      </c>
+      <c r="K4" s="125" t="s">
+        <v>472</v>
+      </c>
+      <c r="L4" s="118"/>
+      <c r="M4" s="118"/>
+      <c r="N4" s="126">
+        <v>1</v>
+      </c>
+      <c r="O4" s="121"/>
+      <c r="P4" s="121"/>
+      <c r="Q4" s="160" t="s">
+        <v>473</v>
+      </c>
+      <c r="R4" s="160"/>
+      <c r="S4" s="160"/>
+      <c r="T4" s="160"/>
+      <c r="U4" s="118"/>
+      <c r="V4" s="118"/>
+      <c r="W4" s="118"/>
+      <c r="X4" s="118"/>
+      <c r="Y4" s="118"/>
+      <c r="Z4" s="118"/>
+      <c r="AA4" s="122"/>
+      <c r="AB4" s="118"/>
+      <c r="AC4" s="118" t="s">
+        <v>536</v>
+      </c>
+      <c r="AD4" s="118">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="A5" s="118"/>
+      <c r="B5" s="118" t="s">
+        <v>541</v>
+      </c>
+      <c r="C5" s="118" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="122" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="127" t="s">
+        <v>547</v>
+      </c>
+      <c r="F5" s="128" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="120">
+        <v>6</v>
+      </c>
+      <c r="H5" s="118"/>
+      <c r="I5" s="118"/>
+      <c r="J5" s="118"/>
+      <c r="K5" s="118"/>
+      <c r="L5" s="118"/>
+      <c r="M5" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N5" s="126">
+        <v>2</v>
+      </c>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="130">
+        <v>23</v>
+      </c>
+      <c r="R5" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S5" s="131" t="s">
+        <v>475</v>
+      </c>
+      <c r="T5" s="118"/>
+      <c r="U5" s="118"/>
+      <c r="V5" s="123" t="s">
+        <v>471</v>
+      </c>
+      <c r="W5" s="118"/>
+      <c r="X5" s="118"/>
+      <c r="Y5" s="128" t="s">
+        <v>210</v>
+      </c>
+      <c r="Z5" s="132" t="s">
+        <v>555</v>
+      </c>
+      <c r="AA5" s="122">
+        <v>1.25</v>
+      </c>
+      <c r="AB5" s="118" t="s">
+        <v>522</v>
+      </c>
+      <c r="AC5" s="118"/>
+      <c r="AD5" s="118" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30">
+      <c r="A6" s="118" t="s">
+        <v>539</v>
+      </c>
+      <c r="B6" s="118"/>
+      <c r="C6" s="118" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="133" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="132" t="s">
+        <v>548</v>
+      </c>
+      <c r="F6" s="128" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="120">
+        <v>7</v>
+      </c>
+      <c r="H6" s="118"/>
+      <c r="I6" s="118"/>
+      <c r="J6" s="118"/>
+      <c r="K6" s="118"/>
+      <c r="L6" s="118"/>
+      <c r="M6" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N6" s="126">
+        <v>3</v>
+      </c>
+      <c r="O6" s="121"/>
+      <c r="P6" s="121"/>
+      <c r="Q6" s="130">
+        <v>22</v>
+      </c>
+      <c r="R6" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S6" s="131" t="s">
+        <v>477</v>
+      </c>
+      <c r="T6" s="118"/>
+      <c r="U6" s="118"/>
+      <c r="V6" s="123" t="s">
+        <v>472</v>
+      </c>
+      <c r="W6" s="118"/>
+      <c r="X6" s="118"/>
+      <c r="Y6" s="134">
+        <v>0.13055555555555556</v>
+      </c>
+      <c r="Z6" s="118"/>
+      <c r="AA6" s="122">
+        <v>1.24</v>
+      </c>
+      <c r="AB6" s="118" t="s">
+        <v>199</v>
+      </c>
+      <c r="AC6" s="118"/>
+      <c r="AD6" s="118"/>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="118" t="s">
+        <v>533</v>
+      </c>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="133" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="132" t="s">
+        <v>549</v>
+      </c>
+      <c r="F7" s="128" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="120">
+        <v>8</v>
+      </c>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N7" s="126">
+        <v>4</v>
+      </c>
+      <c r="O7" s="121"/>
+      <c r="P7" s="121"/>
+      <c r="Q7" s="130">
+        <v>21</v>
+      </c>
+      <c r="R7" s="135"/>
+      <c r="S7" s="131" t="s">
+        <v>479</v>
+      </c>
+      <c r="T7" s="125" t="s">
+        <v>504</v>
+      </c>
+      <c r="U7" s="118"/>
+      <c r="V7" s="118"/>
+      <c r="W7" s="118"/>
+      <c r="X7" s="118"/>
+      <c r="Y7" s="134">
+        <v>0.13263888888888889</v>
+      </c>
+      <c r="Z7" s="127" t="s">
+        <v>556</v>
+      </c>
+      <c r="AA7" s="122">
+        <v>1.27</v>
+      </c>
+      <c r="AB7" s="118" t="s">
+        <v>191</v>
+      </c>
+      <c r="AC7" s="118"/>
+      <c r="AD7" s="118" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" s="118" t="s">
+        <v>533</v>
+      </c>
+      <c r="B8" s="118" t="s">
+        <v>542</v>
+      </c>
+      <c r="C8" s="118" t="s">
+        <v>269</v>
+      </c>
+      <c r="D8" s="122" t="s">
+        <v>270</v>
+      </c>
+      <c r="E8" s="127" t="s">
+        <v>550</v>
+      </c>
+      <c r="F8" s="128" t="s">
+        <v>273</v>
+      </c>
+      <c r="G8" s="120">
+        <v>17</v>
+      </c>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="136"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N8" s="126">
+        <v>5</v>
+      </c>
+      <c r="O8" s="121"/>
+      <c r="P8" s="121"/>
+      <c r="Q8" s="130">
+        <v>20</v>
+      </c>
+      <c r="R8" s="135"/>
+      <c r="S8" s="131" t="s">
+        <v>481</v>
+      </c>
+      <c r="T8" s="137" t="s">
+        <v>507</v>
+      </c>
+      <c r="U8" s="118"/>
+      <c r="V8" s="118"/>
+      <c r="W8" s="118"/>
+      <c r="X8" s="118"/>
+      <c r="Y8" s="134">
+        <v>0.13194444444444445</v>
+      </c>
+      <c r="Z8" s="127" t="s">
+        <v>557</v>
+      </c>
+      <c r="AA8" s="122">
+        <v>1.26</v>
+      </c>
+      <c r="AB8" s="118" t="s">
+        <v>183</v>
+      </c>
+      <c r="AC8" s="118"/>
+      <c r="AD8" s="118" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="118"/>
+      <c r="B9" s="118" t="s">
+        <v>543</v>
+      </c>
+      <c r="C9" s="118" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="122" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" s="127" t="s">
+        <v>551</v>
+      </c>
+      <c r="F9" s="128" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="118"/>
+      <c r="H9" s="118"/>
+      <c r="I9" s="118"/>
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N9" s="126">
+        <v>6</v>
+      </c>
+      <c r="O9" s="121"/>
+      <c r="P9" s="121"/>
+      <c r="Q9" s="130">
+        <v>19</v>
+      </c>
+      <c r="R9" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S9" s="131" t="s">
+        <v>482</v>
+      </c>
+      <c r="T9" s="137" t="s">
+        <v>575</v>
+      </c>
+      <c r="U9" s="118"/>
+      <c r="V9" s="118"/>
+      <c r="W9" s="138" t="s">
+        <v>483</v>
+      </c>
+      <c r="X9" s="118"/>
+      <c r="Y9" s="134">
+        <v>0.125</v>
+      </c>
+      <c r="Z9" s="118"/>
+      <c r="AA9" s="133">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="AB9" s="118" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC9" s="118" t="s">
+        <v>541</v>
+      </c>
+      <c r="AD9" s="118" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="118"/>
+      <c r="B10" s="118" t="s">
+        <v>544</v>
+      </c>
+      <c r="C10" s="118" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="122" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="127" t="s">
+        <v>552</v>
+      </c>
+      <c r="F10" s="128" t="s">
+        <v>317</v>
+      </c>
+      <c r="G10" s="120">
+        <v>15</v>
+      </c>
+      <c r="H10" s="118"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="118"/>
+      <c r="K10" s="125" t="s">
+        <v>491</v>
+      </c>
+      <c r="L10" s="118"/>
+      <c r="M10" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N10" s="126">
+        <v>7</v>
+      </c>
+      <c r="O10" s="121"/>
+      <c r="P10" s="121"/>
+      <c r="Q10" s="130">
+        <v>18</v>
+      </c>
+      <c r="R10" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S10" s="131" t="s">
+        <v>485</v>
+      </c>
+      <c r="T10" s="118"/>
+      <c r="U10" s="118"/>
+      <c r="V10" s="118"/>
+      <c r="W10" s="138" t="s">
+        <v>486</v>
+      </c>
+      <c r="X10" s="118"/>
+      <c r="Y10" s="134">
+        <v>0.12569444444444444</v>
+      </c>
+      <c r="Z10" s="118"/>
+      <c r="AA10" s="133">
+        <v>1.17</v>
+      </c>
+      <c r="AB10" s="118" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC10" s="118" t="s">
+        <v>541</v>
+      </c>
+      <c r="AD10" s="118" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="118"/>
+      <c r="B11" s="118"/>
+      <c r="C11" s="118" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="122" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="127" t="s">
+        <v>553</v>
+      </c>
+      <c r="F11" s="128" t="s">
+        <v>316</v>
+      </c>
+      <c r="G11" s="120">
+        <v>14</v>
+      </c>
+      <c r="H11" s="138" t="s">
+        <v>487</v>
+      </c>
+      <c r="I11" s="118"/>
+      <c r="J11" s="118"/>
+      <c r="K11" s="125" t="s">
+        <v>493</v>
+      </c>
+      <c r="L11" s="118"/>
+      <c r="M11" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N11" s="126">
+        <v>8</v>
+      </c>
+      <c r="O11" s="121"/>
+      <c r="P11" s="121"/>
+      <c r="Q11" s="130">
+        <v>17</v>
+      </c>
+      <c r="R11" s="135"/>
+      <c r="S11" s="131" t="s">
+        <v>489</v>
+      </c>
+      <c r="T11" s="137" t="s">
+        <v>506</v>
+      </c>
+      <c r="U11" s="118"/>
+      <c r="V11" s="118"/>
+      <c r="W11" s="138" t="s">
+        <v>499</v>
+      </c>
+      <c r="X11" s="118"/>
+      <c r="Y11" s="134">
+        <v>0.12916666666666668</v>
+      </c>
+      <c r="Z11" s="118"/>
+      <c r="AA11" s="133">
+        <v>1.22</v>
+      </c>
+      <c r="AB11" s="118" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC11" s="118"/>
+      <c r="AD11" s="118"/>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="118"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="118" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="122" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="132" t="s">
+        <v>554</v>
+      </c>
+      <c r="F12" s="128" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="118"/>
+      <c r="J12" s="118"/>
+      <c r="K12" s="136"/>
+      <c r="L12" s="118"/>
+      <c r="M12" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N12" s="126">
+        <v>9</v>
+      </c>
+      <c r="O12" s="121"/>
+      <c r="P12" s="121"/>
+      <c r="Q12" s="130">
+        <v>16</v>
+      </c>
+      <c r="R12" s="135"/>
+      <c r="S12" s="131" t="s">
+        <v>492</v>
+      </c>
+      <c r="T12" s="137" t="s">
+        <v>503</v>
+      </c>
+      <c r="U12" s="118"/>
+      <c r="V12" s="118"/>
+      <c r="W12" s="138" t="s">
+        <v>501</v>
+      </c>
+      <c r="X12" s="118"/>
+      <c r="Y12" s="134">
+        <v>0.12986111111111112</v>
+      </c>
+      <c r="Z12" s="118"/>
+      <c r="AA12" s="133">
+        <v>1.23</v>
+      </c>
+      <c r="AB12" s="118" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC12" s="118"/>
+      <c r="AD12" s="118"/>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="118" t="s">
+        <v>541</v>
+      </c>
+      <c r="B13" s="118"/>
+      <c r="C13" s="118" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="122" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="127" t="s">
+        <v>562</v>
+      </c>
+      <c r="F13" s="128" t="s">
+        <v>107</v>
+      </c>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
+      <c r="I13" s="118"/>
+      <c r="J13" s="124" t="s">
+        <v>490</v>
+      </c>
+      <c r="K13" s="136"/>
+      <c r="L13" s="118"/>
+      <c r="M13" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N13" s="126">
+        <v>10</v>
+      </c>
+      <c r="O13" s="121"/>
+      <c r="P13" s="121"/>
+      <c r="Q13" s="130">
+        <v>15</v>
+      </c>
+      <c r="R13" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S13" s="131" t="s">
+        <v>494</v>
+      </c>
+      <c r="T13" s="137" t="s">
+        <v>484</v>
+      </c>
+      <c r="U13" s="118"/>
+      <c r="V13" s="118"/>
+      <c r="W13" s="118"/>
+      <c r="X13" s="118"/>
+      <c r="Y13" s="134">
+        <v>0.12708333333333333</v>
+      </c>
+      <c r="Z13" s="139" t="s">
+        <v>559</v>
+      </c>
+      <c r="AA13" s="122">
+        <v>1.19</v>
+      </c>
+      <c r="AB13" s="118" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC13" s="118"/>
+      <c r="AD13" s="118" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="118" t="s">
+        <v>540</v>
+      </c>
+      <c r="B14" s="118" t="s">
+        <v>545</v>
+      </c>
+      <c r="C14" s="118" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="122" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="118"/>
+      <c r="F14" s="128" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="118"/>
+      <c r="H14" s="118"/>
+      <c r="I14" s="123" t="s">
+        <v>472</v>
+      </c>
+      <c r="J14" s="124" t="s">
+        <v>523</v>
+      </c>
+      <c r="K14" s="118"/>
+      <c r="L14" s="118"/>
+      <c r="M14" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N14" s="126">
+        <v>11</v>
+      </c>
+      <c r="O14" s="121"/>
+      <c r="P14" s="121"/>
+      <c r="Q14" s="130">
+        <v>14</v>
+      </c>
+      <c r="R14" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S14" s="131" t="s">
+        <v>495</v>
+      </c>
+      <c r="T14" s="137" t="s">
+        <v>488</v>
+      </c>
+      <c r="U14" s="118"/>
+      <c r="V14" s="118"/>
+      <c r="W14" s="118"/>
+      <c r="X14" s="118"/>
+      <c r="Y14" s="134">
+        <v>0.12638888888888888</v>
+      </c>
+      <c r="Z14" s="127" t="s">
+        <v>558</v>
+      </c>
+      <c r="AA14" s="122">
+        <v>1.18</v>
+      </c>
+      <c r="AB14" s="118" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC14" s="118"/>
+      <c r="AD14" s="118"/>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="118" t="s">
+        <v>540</v>
+      </c>
+      <c r="B15" s="118" t="s">
+        <v>539</v>
+      </c>
+      <c r="C15" s="118" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="122" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" s="127" t="s">
+        <v>563</v>
+      </c>
+      <c r="F15" s="128" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="124" t="s">
+        <v>524</v>
+      </c>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N15" s="126">
+        <v>12</v>
+      </c>
+      <c r="O15" s="121"/>
+      <c r="P15" s="121"/>
+      <c r="Q15" s="130">
+        <v>13</v>
+      </c>
+      <c r="R15" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S15" s="140" t="s">
+        <v>591</v>
+      </c>
+      <c r="T15" s="118"/>
+      <c r="U15" s="124" t="s">
+        <v>496</v>
+      </c>
+      <c r="V15" s="123" t="s">
+        <v>480</v>
+      </c>
+      <c r="W15" s="118"/>
+      <c r="X15" s="118"/>
+      <c r="Y15" s="134">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="Z15" s="118"/>
+      <c r="AA15" s="122">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AB15" s="118" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC15" s="118" t="s">
+        <v>539</v>
+      </c>
+      <c r="AD15" s="118" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="118"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="122"/>
+      <c r="H16" s="122"/>
+      <c r="I16" s="122"/>
+      <c r="J16" s="122"/>
+      <c r="K16" s="122"/>
+      <c r="L16" s="122"/>
+      <c r="M16" s="122"/>
+      <c r="N16" s="122"/>
+      <c r="O16" s="122"/>
+      <c r="P16" s="122"/>
+      <c r="Q16" s="122"/>
+      <c r="R16" s="122"/>
+      <c r="S16" s="122"/>
+      <c r="T16" s="122"/>
+      <c r="U16" s="122"/>
+      <c r="V16" s="122"/>
+      <c r="W16" s="122"/>
+      <c r="X16" s="122"/>
+      <c r="Y16" s="122"/>
+      <c r="Z16" s="122"/>
+      <c r="AA16" s="122"/>
+      <c r="AB16" s="122"/>
+      <c r="AC16" s="118"/>
+      <c r="AD16" s="118"/>
+    </row>
+    <row r="17" spans="1:30">
+      <c r="A17" s="118"/>
+      <c r="B17" s="118"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="122"/>
+      <c r="G17" s="122"/>
+      <c r="H17" s="122"/>
+      <c r="I17" s="122"/>
+      <c r="J17" s="122"/>
+      <c r="K17" s="159" t="s">
+        <v>594</v>
+      </c>
+      <c r="L17" s="122"/>
+      <c r="M17" s="122"/>
+      <c r="N17" s="122"/>
+      <c r="O17" s="122"/>
+      <c r="P17" s="122"/>
+      <c r="Q17" s="122"/>
+      <c r="R17" s="122"/>
+      <c r="S17" s="122"/>
+      <c r="T17" s="122"/>
+      <c r="U17" s="122"/>
+      <c r="V17" s="122"/>
+      <c r="W17" s="122"/>
+      <c r="X17" s="122"/>
+      <c r="Y17" s="122"/>
+      <c r="Z17" s="122"/>
+      <c r="AA17" s="122"/>
+      <c r="AB17" s="122"/>
+      <c r="AC17" s="118"/>
+      <c r="AD17" s="118"/>
+    </row>
+    <row r="18" spans="1:30">
+      <c r="A18" s="118"/>
+      <c r="B18" s="118"/>
+      <c r="C18" s="118" t="s">
+        <v>215</v>
+      </c>
+      <c r="D18" s="133" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" s="118"/>
+      <c r="F18" s="118"/>
+      <c r="G18" s="118"/>
+      <c r="H18" s="138" t="s">
+        <v>476</v>
+      </c>
+      <c r="I18" s="118"/>
+      <c r="J18" s="118"/>
+      <c r="K18" s="137" t="s">
+        <v>508</v>
+      </c>
+      <c r="L18" s="131" t="s">
+        <v>527</v>
+      </c>
+      <c r="M18" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N18" s="126">
+        <v>24</v>
+      </c>
+      <c r="O18" s="122"/>
+      <c r="P18" s="122"/>
+      <c r="Q18" s="126">
+        <v>25</v>
+      </c>
+      <c r="R18" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S18" s="131" t="s">
+        <v>528</v>
+      </c>
+      <c r="T18" s="137" t="s">
+        <v>509</v>
+      </c>
+      <c r="U18" s="122"/>
+      <c r="V18" s="122"/>
+      <c r="W18" s="138" t="s">
+        <v>478</v>
+      </c>
+      <c r="X18" s="122"/>
+      <c r="Y18" s="122"/>
+      <c r="Z18" s="122"/>
+      <c r="AA18" s="133" t="s">
+        <v>223</v>
+      </c>
+      <c r="AB18" s="118" t="s">
+        <v>222</v>
+      </c>
+      <c r="AC18" s="118"/>
+      <c r="AD18" s="118"/>
+    </row>
+    <row r="19" spans="1:30">
+      <c r="A19" s="118"/>
+      <c r="B19" s="118"/>
+      <c r="C19" s="118" t="s">
+        <v>230</v>
+      </c>
+      <c r="D19" s="133" t="s">
+        <v>231</v>
+      </c>
+      <c r="E19" s="118"/>
+      <c r="F19" s="128" t="s">
+        <v>284</v>
+      </c>
+      <c r="G19" s="118"/>
+      <c r="H19" s="118"/>
+      <c r="I19" s="118"/>
+      <c r="J19" s="124" t="s">
+        <v>526</v>
+      </c>
+      <c r="K19" s="135"/>
+      <c r="L19" s="131" t="s">
+        <v>529</v>
+      </c>
+      <c r="M19" s="118"/>
+      <c r="N19" s="126">
+        <v>26</v>
+      </c>
+      <c r="O19" s="121"/>
+      <c r="P19" s="121"/>
+      <c r="Q19" s="126">
+        <v>27</v>
+      </c>
+      <c r="R19" s="141"/>
+      <c r="S19" s="131" t="s">
+        <v>530</v>
+      </c>
+      <c r="T19" s="118"/>
+      <c r="U19" s="124" t="s">
+        <v>505</v>
+      </c>
+      <c r="V19" s="118"/>
+      <c r="W19" s="118"/>
+      <c r="X19" s="118"/>
+      <c r="Y19" s="128" t="s">
+        <v>285</v>
+      </c>
+      <c r="Z19" s="118"/>
+      <c r="AA19" s="133" t="s">
+        <v>237</v>
+      </c>
+      <c r="AB19" s="118" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC19" s="118"/>
+      <c r="AD19" s="118"/>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="A20" s="118"/>
+      <c r="B20" s="118"/>
+      <c r="C20" s="118" t="s">
+        <v>242</v>
+      </c>
+      <c r="D20" s="133" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" s="118"/>
+      <c r="F20" s="118"/>
+      <c r="G20" s="118"/>
+      <c r="H20" s="118"/>
+      <c r="I20" s="118"/>
+      <c r="J20" s="118"/>
+      <c r="K20" s="137" t="s">
+        <v>510</v>
+      </c>
+      <c r="L20" s="118"/>
+      <c r="M20" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="N20" s="126">
+        <v>28</v>
+      </c>
+      <c r="O20" s="121"/>
+      <c r="P20" s="121"/>
+      <c r="Q20" s="126">
+        <v>29</v>
+      </c>
+      <c r="R20" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S20" s="142"/>
+      <c r="T20" s="137" t="s">
+        <v>511</v>
+      </c>
+      <c r="U20" s="118"/>
+      <c r="V20" s="118"/>
+      <c r="W20" s="118"/>
+      <c r="X20" s="118"/>
+      <c r="Y20" s="142"/>
+      <c r="Z20" s="118"/>
+      <c r="AA20" s="122" t="s">
+        <v>248</v>
+      </c>
+      <c r="AB20" s="118" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC20" s="118"/>
+      <c r="AD20" s="118"/>
+    </row>
+    <row r="21" spans="1:30">
+      <c r="A21" s="118"/>
+      <c r="B21" s="118"/>
+      <c r="C21" s="118" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="122">
+        <v>3.23</v>
+      </c>
+      <c r="E21" s="118"/>
+      <c r="F21" s="118"/>
+      <c r="G21" s="120">
+        <v>23</v>
+      </c>
+      <c r="H21" s="118"/>
+      <c r="I21" s="143" t="s">
+        <v>484</v>
+      </c>
+      <c r="J21" s="118"/>
+      <c r="K21" s="118"/>
+      <c r="L21" s="118"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="126">
+        <v>30</v>
+      </c>
+      <c r="O21" s="121"/>
+      <c r="P21" s="121"/>
+      <c r="Q21" s="126">
+        <v>31</v>
+      </c>
+      <c r="R21" s="141"/>
+      <c r="S21" s="142"/>
+      <c r="T21" s="118"/>
+      <c r="U21" s="142"/>
+      <c r="V21" s="123" t="s">
+        <v>488</v>
+      </c>
+      <c r="W21" s="118"/>
+      <c r="X21" s="120">
+        <v>22</v>
+      </c>
+      <c r="Y21" s="142"/>
+      <c r="Z21" s="118"/>
+      <c r="AA21" s="119">
+        <v>3.22</v>
+      </c>
+      <c r="AB21" s="118" t="s">
+        <v>278</v>
+      </c>
+      <c r="AC21" s="118"/>
+      <c r="AD21" s="118"/>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" s="118"/>
+      <c r="B22" s="118"/>
+      <c r="C22" s="118" t="s">
+        <v>263</v>
+      </c>
+      <c r="D22" s="119" t="s">
+        <v>264</v>
+      </c>
+      <c r="E22" s="127" t="s">
+        <v>560</v>
+      </c>
+      <c r="F22" s="134">
+        <v>9.1666666666666674E-2</v>
+      </c>
+      <c r="G22" s="120">
+        <v>10</v>
+      </c>
+      <c r="H22" s="118"/>
+      <c r="I22" s="118"/>
+      <c r="J22" s="118"/>
+      <c r="K22" s="118"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="118"/>
+      <c r="N22" s="126">
+        <v>32</v>
+      </c>
+      <c r="O22" s="121"/>
+      <c r="P22" s="121"/>
+      <c r="Q22" s="130">
+        <v>33</v>
+      </c>
+      <c r="R22" s="129" t="s">
+        <v>474</v>
+      </c>
+      <c r="S22" s="118"/>
+      <c r="T22" s="118"/>
+      <c r="U22" s="118"/>
+      <c r="V22" s="143" t="s">
+        <v>472</v>
+      </c>
+      <c r="W22" s="118"/>
+      <c r="X22" s="120">
+        <v>9</v>
+      </c>
+      <c r="Y22" s="128" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z22" s="127" t="s">
+        <v>561</v>
+      </c>
+      <c r="AA22" s="122">
+        <v>4.7</v>
+      </c>
+      <c r="AB22" s="118" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC22" s="118"/>
+      <c r="AD22" s="118"/>
+    </row>
+    <row r="23" spans="1:30">
+      <c r="A23" s="142"/>
+      <c r="B23" s="142"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="144"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="142"/>
+      <c r="J23" s="142"/>
+      <c r="K23" s="142"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="142"/>
+      <c r="P23" s="142"/>
+      <c r="Q23" s="142"/>
+      <c r="R23" s="142"/>
+      <c r="S23" s="142"/>
+      <c r="T23" s="142"/>
+      <c r="U23" s="142"/>
+      <c r="V23" s="142"/>
+      <c r="W23" s="142"/>
+      <c r="X23" s="142"/>
+      <c r="Y23" s="142"/>
+      <c r="Z23" s="142"/>
+      <c r="AA23" s="144"/>
+      <c r="AB23" s="142"/>
+      <c r="AC23" s="135"/>
+      <c r="AD23" s="135"/>
+    </row>
+    <row r="24" spans="1:30">
+      <c r="A24" s="142"/>
+      <c r="B24" s="142"/>
+      <c r="C24" s="142"/>
+      <c r="D24" s="144"/>
+      <c r="E24" s="142"/>
+      <c r="F24" s="142"/>
+      <c r="G24" s="142"/>
+      <c r="H24" s="142"/>
+      <c r="I24" s="142"/>
+      <c r="J24" s="142"/>
+      <c r="K24" s="142"/>
+      <c r="L24" s="142"/>
+      <c r="M24" s="142"/>
+      <c r="N24" s="142"/>
+      <c r="P24" s="142"/>
+      <c r="Q24" s="142"/>
+      <c r="R24" s="142"/>
+      <c r="S24" s="142"/>
+      <c r="T24" s="142"/>
+      <c r="U24" s="142"/>
+      <c r="V24" s="142"/>
+      <c r="W24" s="142"/>
+      <c r="X24" s="142"/>
+      <c r="Y24" s="142"/>
+      <c r="Z24" s="142"/>
+      <c r="AA24" s="144"/>
+      <c r="AB24" s="142"/>
+      <c r="AC24" s="135"/>
+      <c r="AD24" s="135"/>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25" s="142"/>
+      <c r="B25" s="142"/>
+      <c r="C25" s="142"/>
+      <c r="D25" s="144"/>
+      <c r="E25" s="142"/>
+      <c r="F25" s="142"/>
+      <c r="G25" s="142"/>
+      <c r="H25" s="142"/>
+      <c r="I25" s="142"/>
+      <c r="J25" s="142"/>
+      <c r="K25" s="159" t="s">
+        <v>593</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="N25" s="142"/>
+      <c r="O25" s="142"/>
+      <c r="P25" s="142"/>
+      <c r="Q25" s="142"/>
+      <c r="R25" s="142"/>
+      <c r="S25" s="142"/>
+      <c r="T25" s="142"/>
+      <c r="U25" s="142"/>
+      <c r="V25" s="142"/>
+      <c r="W25" s="142"/>
+      <c r="X25" s="142"/>
+      <c r="Y25" s="142"/>
+      <c r="Z25" s="142"/>
+      <c r="AA25" s="144"/>
+      <c r="AB25" s="142"/>
+      <c r="AC25" s="135"/>
+      <c r="AD25" s="135"/>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="142"/>
+      <c r="B26" s="142"/>
+      <c r="C26" s="142"/>
+      <c r="D26" s="144"/>
+      <c r="E26" s="142"/>
+      <c r="F26" s="142"/>
+      <c r="G26" s="142"/>
+      <c r="H26" s="142"/>
+      <c r="I26" s="142"/>
+      <c r="J26" s="142"/>
+      <c r="K26" s="142"/>
+      <c r="L26" s="142"/>
+      <c r="M26" s="142"/>
+      <c r="N26" s="142"/>
+      <c r="O26" s="142"/>
+      <c r="P26" s="142"/>
+      <c r="Q26" s="142"/>
+      <c r="R26" s="142"/>
+      <c r="S26" s="142"/>
+      <c r="T26" s="142"/>
+      <c r="U26" s="142"/>
+      <c r="V26" s="142"/>
+      <c r="W26" s="142"/>
+      <c r="X26" s="142"/>
+      <c r="Y26" s="142"/>
+      <c r="Z26" s="142"/>
+      <c r="AA26" s="144"/>
+      <c r="AB26" s="142"/>
+      <c r="AC26" s="135"/>
+      <c r="AD26" s="135"/>
+    </row>
+    <row r="27" spans="1:30" s="75" customFormat="1" ht="11.25">
+      <c r="A27" s="142"/>
+      <c r="B27" s="142"/>
+      <c r="C27" s="145" t="s">
+        <v>299</v>
+      </c>
+      <c r="D27" s="144">
+        <v>2.15</v>
+      </c>
+      <c r="E27" s="142"/>
+      <c r="F27" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="G27" s="147">
+        <v>7</v>
+      </c>
+      <c r="H27" s="142"/>
+      <c r="I27" s="142"/>
+      <c r="J27" s="148" t="s">
+        <v>580</v>
+      </c>
+      <c r="K27" s="142"/>
+      <c r="L27" s="142"/>
+      <c r="M27" s="149" t="s">
+        <v>474</v>
+      </c>
+      <c r="N27" s="150">
+        <v>34</v>
+      </c>
+      <c r="O27" s="151" t="s">
+        <v>586</v>
+      </c>
+      <c r="P27" s="142" t="s">
+        <v>577</v>
+      </c>
+      <c r="Q27" s="151"/>
+      <c r="R27" s="151"/>
+      <c r="S27" s="142"/>
+      <c r="T27" s="151"/>
+      <c r="U27" s="142"/>
+      <c r="V27" s="142"/>
+      <c r="W27" s="142"/>
+      <c r="X27" s="151"/>
+      <c r="Y27" s="151"/>
+      <c r="Z27" s="142"/>
+      <c r="AA27" s="151"/>
+      <c r="AB27" s="151"/>
+      <c r="AC27" s="151"/>
+      <c r="AD27" s="151"/>
+    </row>
+    <row r="28" spans="1:30" s="75" customFormat="1" ht="11.25">
+      <c r="A28" s="142"/>
+      <c r="B28" s="142"/>
+      <c r="C28" s="144" t="s">
+        <v>298</v>
+      </c>
+      <c r="D28" s="144">
+        <v>3.14</v>
+      </c>
+      <c r="E28" s="142"/>
+      <c r="F28" s="146" t="s">
+        <v>291</v>
+      </c>
+      <c r="G28" s="147">
+        <v>6</v>
+      </c>
+      <c r="H28" s="142"/>
+      <c r="I28" s="142"/>
+      <c r="J28" s="148" t="s">
+        <v>581</v>
+      </c>
+      <c r="K28" s="152" t="s">
+        <v>579</v>
+      </c>
+      <c r="L28" s="142"/>
+      <c r="M28" s="149" t="s">
+        <v>474</v>
+      </c>
+      <c r="N28" s="150">
+        <v>35</v>
+      </c>
+      <c r="O28" s="142" t="s">
+        <v>578</v>
+      </c>
+      <c r="P28" s="142" t="s">
+        <v>587</v>
+      </c>
+      <c r="Q28" s="151"/>
+      <c r="R28" s="151"/>
+      <c r="S28" s="142"/>
+      <c r="T28" s="151"/>
+      <c r="U28" s="142"/>
+      <c r="V28" s="142"/>
+      <c r="W28" s="142"/>
+      <c r="X28" s="151"/>
+      <c r="Y28" s="151"/>
+      <c r="Z28" s="142"/>
+      <c r="AA28" s="151"/>
+      <c r="AB28" s="151"/>
+      <c r="AC28" s="151"/>
+      <c r="AD28" s="151"/>
+    </row>
+    <row r="29" spans="1:30" s="75" customFormat="1" ht="11.25">
+      <c r="A29" s="151"/>
+      <c r="B29" s="151"/>
+      <c r="C29" s="151"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="151"/>
+      <c r="F29" s="151"/>
+      <c r="G29" s="142"/>
+      <c r="H29" s="151"/>
+      <c r="I29" s="151"/>
+      <c r="J29" s="151"/>
+      <c r="K29" s="151"/>
+      <c r="L29" s="161" t="s">
+        <v>469</v>
+      </c>
+      <c r="M29" s="161"/>
+      <c r="N29" s="161"/>
+      <c r="O29" s="151" t="s">
+        <v>585</v>
+      </c>
+      <c r="P29" s="151" t="s">
+        <v>588</v>
+      </c>
+      <c r="Q29" s="151"/>
+      <c r="R29" s="151"/>
+      <c r="S29" s="151"/>
+      <c r="T29" s="151"/>
+      <c r="U29" s="151"/>
+      <c r="V29" s="151"/>
+      <c r="W29" s="151"/>
+      <c r="X29" s="151"/>
+      <c r="Y29" s="151"/>
+      <c r="Z29" s="151"/>
+      <c r="AA29" s="151"/>
+      <c r="AB29" s="151"/>
+      <c r="AC29" s="151"/>
+      <c r="AD29" s="151"/>
+    </row>
+    <row r="30" spans="1:30" s="75" customFormat="1">
+      <c r="A30" s="151"/>
+      <c r="B30" s="151"/>
+      <c r="C30" s="145" t="s">
+        <v>297</v>
+      </c>
+      <c r="D30" s="153">
+        <v>3.13</v>
+      </c>
+      <c r="E30" s="151"/>
+      <c r="F30" s="154" t="s">
+        <v>292</v>
+      </c>
+      <c r="G30" s="147">
+        <v>5</v>
+      </c>
+      <c r="H30" s="151"/>
+      <c r="I30" s="151"/>
+      <c r="J30" s="155" t="s">
+        <v>582</v>
+      </c>
+      <c r="K30" s="151"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="156" t="s">
+        <v>474</v>
+      </c>
+      <c r="N30" s="150">
+        <v>36</v>
+      </c>
+      <c r="O30" s="151" t="s">
+        <v>584</v>
+      </c>
+      <c r="P30" s="142" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q30" s="135"/>
+      <c r="R30" s="135"/>
+      <c r="S30" s="135"/>
+      <c r="T30" s="151"/>
+      <c r="U30" s="151"/>
+      <c r="V30" s="151"/>
+      <c r="W30" s="151"/>
+      <c r="X30" s="151"/>
+      <c r="Y30" s="151"/>
+      <c r="Z30" s="151"/>
+      <c r="AA30" s="153"/>
+      <c r="AB30" s="151"/>
+      <c r="AC30" s="151"/>
+      <c r="AD30" s="151"/>
+    </row>
+    <row r="31" spans="1:30">
+      <c r="A31" s="135"/>
+      <c r="B31" s="135"/>
+      <c r="L31" s="160" t="s">
+        <v>473</v>
+      </c>
+      <c r="M31" s="160"/>
+      <c r="N31" s="160"/>
+      <c r="O31" s="160"/>
+      <c r="P31" s="135"/>
+      <c r="Q31" s="135"/>
+      <c r="R31" s="135"/>
+      <c r="S31" s="135"/>
+      <c r="T31" s="135"/>
+      <c r="U31" s="135"/>
+      <c r="V31" s="135"/>
+      <c r="W31" s="135"/>
+      <c r="X31" s="135"/>
+      <c r="Y31" s="135"/>
+      <c r="Z31" s="135"/>
+      <c r="AA31" s="157"/>
+      <c r="AB31" s="135"/>
+      <c r="AC31" s="135"/>
+      <c r="AD31" s="135"/>
+    </row>
+    <row r="32" spans="1:30">
+      <c r="A32" s="135"/>
+      <c r="B32" s="135"/>
+      <c r="C32" s="144" t="s">
+        <v>296</v>
+      </c>
+      <c r="D32" s="153">
+        <v>3.12</v>
+      </c>
+      <c r="E32" s="135"/>
+      <c r="F32" s="154" t="s">
+        <v>293</v>
+      </c>
+      <c r="G32" s="158">
+        <v>4</v>
+      </c>
+      <c r="H32" s="135"/>
+      <c r="I32" s="135"/>
+      <c r="J32" s="155" t="s">
+        <v>583</v>
+      </c>
+      <c r="K32" s="135"/>
+      <c r="L32" s="135"/>
+      <c r="M32" s="149" t="s">
+        <v>474</v>
+      </c>
+      <c r="N32" s="150">
+        <v>37</v>
+      </c>
+      <c r="O32" s="135"/>
+      <c r="P32" s="135"/>
+      <c r="Q32" s="135"/>
+      <c r="R32" s="135"/>
+      <c r="S32" s="135"/>
+      <c r="T32" s="135"/>
+      <c r="U32" s="135"/>
+      <c r="V32" s="135"/>
+      <c r="W32" s="135"/>
+      <c r="X32" s="135"/>
+      <c r="Y32" s="135"/>
+      <c r="Z32" s="135"/>
+      <c r="AA32" s="157"/>
+      <c r="AB32" s="135"/>
+      <c r="AC32" s="135"/>
+      <c r="AD32" s="135"/>
+    </row>
+    <row r="33" spans="1:30">
+      <c r="A33" s="135"/>
+      <c r="B33" s="135"/>
+      <c r="C33" s="145" t="s">
+        <v>301</v>
+      </c>
+      <c r="D33" s="144">
+        <v>3.17</v>
+      </c>
+      <c r="E33" s="135"/>
+      <c r="F33" s="146" t="s">
+        <v>294</v>
+      </c>
+      <c r="G33" s="147">
+        <v>9</v>
+      </c>
+      <c r="H33" s="135"/>
+      <c r="I33" s="135"/>
+      <c r="J33" s="135"/>
+      <c r="K33" s="152" t="s">
+        <v>504</v>
+      </c>
+      <c r="L33" s="135"/>
+      <c r="M33" s="149" t="s">
+        <v>474</v>
+      </c>
+      <c r="N33" s="150">
+        <v>38</v>
+      </c>
+      <c r="O33" s="135"/>
+      <c r="P33" s="135"/>
+      <c r="Q33" s="135"/>
+      <c r="R33" s="135"/>
+      <c r="S33" s="135"/>
+      <c r="T33" s="135"/>
+      <c r="U33" s="135"/>
+      <c r="V33" s="135"/>
+      <c r="W33" s="135"/>
+      <c r="X33" s="135"/>
+      <c r="Y33" s="135"/>
+      <c r="Z33" s="135"/>
+      <c r="AA33" s="157"/>
+      <c r="AB33" s="135"/>
+      <c r="AC33" s="135"/>
+      <c r="AD33" s="135"/>
+    </row>
+    <row r="34" spans="1:30">
+      <c r="A34" s="135"/>
+      <c r="B34" s="135"/>
+      <c r="C34" s="144" t="s">
+        <v>300</v>
+      </c>
+      <c r="D34" s="144">
+        <v>3.16</v>
+      </c>
+      <c r="E34" s="135"/>
+      <c r="F34" s="146" t="s">
+        <v>295</v>
+      </c>
+      <c r="G34" s="147">
+        <v>8</v>
+      </c>
+      <c r="H34" s="135"/>
+      <c r="I34" s="135"/>
+      <c r="J34" s="135"/>
+      <c r="K34" s="152" t="s">
+        <v>507</v>
+      </c>
+      <c r="L34" s="135"/>
+      <c r="M34" s="149" t="s">
+        <v>474</v>
+      </c>
+      <c r="N34" s="150">
+        <v>39</v>
+      </c>
+      <c r="O34" s="135"/>
+      <c r="P34" s="135"/>
+      <c r="Q34" s="135"/>
+      <c r="R34" s="135"/>
+      <c r="S34" s="135"/>
+      <c r="T34" s="135"/>
+      <c r="U34" s="135"/>
+      <c r="V34" s="135"/>
+      <c r="W34" s="135"/>
+      <c r="X34" s="135"/>
+      <c r="Y34" s="135"/>
+      <c r="Z34" s="135"/>
+      <c r="AA34" s="157"/>
+      <c r="AB34" s="135"/>
+      <c r="AC34" s="135"/>
+      <c r="AD34" s="135"/>
+    </row>
+    <row r="35" spans="1:30">
+      <c r="A35" s="135"/>
+      <c r="B35" s="135"/>
+      <c r="O35" s="135"/>
+      <c r="P35" s="135"/>
+      <c r="Q35" s="135"/>
+      <c r="R35" s="135"/>
+      <c r="S35" s="135"/>
+      <c r="T35" s="135"/>
+      <c r="U35" s="135"/>
+      <c r="V35" s="135"/>
+      <c r="W35" s="135"/>
+      <c r="X35" s="135"/>
+      <c r="Y35" s="135"/>
+      <c r="Z35" s="135"/>
+      <c r="AA35" s="157"/>
+      <c r="AB35" s="135"/>
+      <c r="AC35" s="135"/>
+      <c r="AD35" s="135"/>
+    </row>
+    <row r="36" spans="1:30">
+      <c r="A36" s="135"/>
+      <c r="B36" s="135"/>
+      <c r="C36" s="135"/>
+      <c r="D36" s="157"/>
+      <c r="E36" s="135"/>
+      <c r="F36" s="135"/>
+      <c r="G36" s="135"/>
+      <c r="H36" s="135"/>
+      <c r="I36" s="135"/>
+      <c r="J36" s="135"/>
+      <c r="K36" s="135"/>
+      <c r="L36" s="135"/>
+      <c r="M36" s="135"/>
+      <c r="N36" s="135"/>
+      <c r="O36" s="135"/>
+      <c r="P36" s="135"/>
+      <c r="Q36" s="135"/>
+      <c r="R36" s="135"/>
+      <c r="S36" s="135"/>
+      <c r="T36" s="135"/>
+      <c r="U36" s="135"/>
+      <c r="V36" s="135"/>
+      <c r="W36" s="135"/>
+      <c r="X36" s="135"/>
+      <c r="Y36" s="135"/>
+      <c r="Z36" s="135"/>
+      <c r="AA36" s="157"/>
+      <c r="AB36" s="135"/>
+      <c r="AC36" s="135"/>
+      <c r="AD36" s="135"/>
+    </row>
+    <row r="37" spans="1:30">
+      <c r="A37" s="135"/>
+      <c r="B37" s="135"/>
+      <c r="C37" s="135"/>
+      <c r="D37" s="157"/>
+      <c r="E37" s="135"/>
+      <c r="F37" s="135"/>
+      <c r="G37" s="135"/>
+      <c r="H37" s="135"/>
+      <c r="I37" s="135"/>
+      <c r="J37" s="135"/>
+      <c r="K37" s="135"/>
+      <c r="L37" s="135"/>
+      <c r="M37" s="135"/>
+      <c r="N37" s="135"/>
+      <c r="O37" s="135"/>
+      <c r="P37" s="135"/>
+      <c r="Q37" s="135"/>
+      <c r="R37" s="135"/>
+      <c r="S37" s="135"/>
+      <c r="T37" s="135"/>
+      <c r="U37" s="135"/>
+      <c r="V37" s="135"/>
+      <c r="W37" s="135"/>
+      <c r="X37" s="135"/>
+      <c r="Y37" s="135"/>
+      <c r="Z37" s="135"/>
+      <c r="AA37" s="157"/>
+      <c r="AB37" s="135"/>
+      <c r="AC37" s="135"/>
+      <c r="AD37" s="135"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="Q4:T4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="78" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60D0C246-03A0-4FFF-AF38-F7B7F6DA7DF4}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4641,6 +6890,9 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+    </sheetView>
+    <sheetView topLeftCell="A25" workbookViewId="1">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6526,7 +8778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946B382E-0C83-4AA1-A09A-F99110E70DA1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6535,8 +8787,9 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W34" sqref="W34"/>
+      <selection pane="bottomLeft" activeCell="X21" sqref="X21"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -6670,26 +8923,23 @@
       <c r="D2" s="103"/>
       <c r="E2" s="47"/>
       <c r="F2" s="47"/>
-      <c r="G2" s="67">
-        <v>17</v>
-      </c>
       <c r="H2" s="47"/>
       <c r="I2" s="47"/>
       <c r="J2" s="47"/>
       <c r="K2" s="47"/>
-      <c r="L2" s="104" t="s">
+      <c r="L2" s="162" t="s">
         <v>469</v>
       </c>
-      <c r="M2" s="104"/>
-      <c r="N2" s="104"/>
+      <c r="M2" s="162"/>
+      <c r="N2" s="162"/>
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
-      <c r="Q2" s="105" t="s">
+      <c r="Q2" s="163" t="s">
         <v>470</v>
       </c>
-      <c r="R2" s="105"/>
-      <c r="S2" s="105"/>
-      <c r="T2" s="105"/>
+      <c r="R2" s="163"/>
+      <c r="S2" s="163"/>
+      <c r="T2" s="163"/>
       <c r="U2" s="47"/>
       <c r="V2" s="47"/>
       <c r="W2" s="47"/>
@@ -6715,7 +8965,7 @@
       <c r="E3" s="47"/>
       <c r="F3" s="47"/>
       <c r="G3" s="67">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="47"/>
       <c r="I3" s="64" t="s">
@@ -6734,12 +8984,12 @@
       </c>
       <c r="O3" s="48"/>
       <c r="P3" s="48"/>
-      <c r="Q3" s="105" t="s">
+      <c r="Q3" s="163" t="s">
         <v>469</v>
       </c>
-      <c r="R3" s="105"/>
-      <c r="S3" s="105"/>
-      <c r="T3" s="105"/>
+      <c r="R3" s="163"/>
+      <c r="S3" s="163"/>
+      <c r="T3" s="163"/>
       <c r="U3" s="47"/>
       <c r="V3" s="47"/>
       <c r="W3" s="47"/>
@@ -6767,7 +9017,7 @@
       <c r="E4" s="47"/>
       <c r="F4" s="47"/>
       <c r="G4" s="67">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="64" t="s">
@@ -6786,12 +9036,12 @@
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="48"/>
-      <c r="Q4" s="105" t="s">
+      <c r="Q4" s="163" t="s">
         <v>473</v>
       </c>
-      <c r="R4" s="105"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="105"/>
+      <c r="R4" s="163"/>
+      <c r="S4" s="163"/>
+      <c r="T4" s="163"/>
       <c r="U4" s="47"/>
       <c r="V4" s="47"/>
       <c r="W4" s="47"/>
@@ -6825,7 +9075,7 @@
         <v>51</v>
       </c>
       <c r="G5" s="67">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" s="47"/>
       <c r="I5" s="47"/>
@@ -6891,7 +9141,7 @@
         <v>58</v>
       </c>
       <c r="G6" s="67">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" s="47"/>
       <c r="I6" s="47"/>
@@ -6953,7 +9203,7 @@
         <v>65</v>
       </c>
       <c r="G7" s="67">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="H7" s="47"/>
       <c r="I7" s="47"/>
@@ -7017,7 +9267,9 @@
       <c r="F8" s="62" t="s">
         <v>273</v>
       </c>
-      <c r="G8" s="47"/>
+      <c r="G8" s="67">
+        <v>17</v>
+      </c>
       <c r="H8" s="47"/>
       <c r="I8" s="47"/>
       <c r="J8" s="47"/>
@@ -7144,7 +9396,9 @@
       <c r="F10" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="G10" s="47"/>
+      <c r="G10" s="67">
+        <v>15</v>
+      </c>
       <c r="H10" s="47"/>
       <c r="I10" s="47"/>
       <c r="J10" s="47"/>
@@ -7208,7 +9462,9 @@
       <c r="F11" s="62" t="s">
         <v>316</v>
       </c>
-      <c r="G11" s="47"/>
+      <c r="G11" s="67">
+        <v>14</v>
+      </c>
       <c r="H11" s="66" t="s">
         <v>487</v>
       </c>
@@ -7525,19 +9781,19 @@
       <c r="I16" s="47"/>
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
-      <c r="L16" s="104" t="s">
+      <c r="L16" s="162" t="s">
         <v>497</v>
       </c>
-      <c r="M16" s="104"/>
-      <c r="N16" s="104"/>
+      <c r="M16" s="162"/>
+      <c r="N16" s="162"/>
       <c r="O16" s="48"/>
       <c r="P16" s="48"/>
-      <c r="Q16" s="105" t="s">
+      <c r="Q16" s="163" t="s">
         <v>469</v>
       </c>
-      <c r="R16" s="105"/>
-      <c r="S16" s="105"/>
-      <c r="T16" s="105"/>
+      <c r="R16" s="163"/>
+      <c r="S16" s="163"/>
+      <c r="T16" s="163"/>
       <c r="U16" s="47"/>
       <c r="V16" s="47"/>
       <c r="W16" s="47"/>
@@ -7760,9 +10016,6 @@
       </c>
       <c r="V20" s="47"/>
       <c r="W20" s="47"/>
-      <c r="X20" s="67">
-        <v>17</v>
-      </c>
       <c r="Y20" s="62" t="s">
         <v>402</v>
       </c>
@@ -7817,7 +10070,7 @@
       <c r="V21" s="47"/>
       <c r="W21" s="47"/>
       <c r="X21" s="67">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Y21" s="62" t="s">
         <v>397</v>
@@ -7872,7 +10125,9 @@
       </c>
       <c r="V22" s="47"/>
       <c r="W22" s="47"/>
-      <c r="X22" s="47"/>
+      <c r="X22" s="67">
+        <v>16</v>
+      </c>
       <c r="Y22" s="62" t="s">
         <v>396</v>
       </c>
@@ -8262,11 +10517,11 @@
       <c r="I30" s="84"/>
       <c r="J30" s="84"/>
       <c r="K30" s="84"/>
-      <c r="L30" s="104" t="s">
+      <c r="L30" s="162" t="s">
         <v>469</v>
       </c>
-      <c r="M30" s="104"/>
-      <c r="N30" s="104"/>
+      <c r="M30" s="162"/>
+      <c r="N30" s="162"/>
       <c r="O30" s="84" t="s">
         <v>585</v>
       </c>
@@ -8337,11 +10592,11 @@
       <c r="P31" s="76" t="s">
         <v>589</v>
       </c>
-      <c r="Q31" s="104" t="s">
+      <c r="Q31" s="162" t="s">
         <v>497</v>
       </c>
-      <c r="R31" s="104"/>
-      <c r="S31" s="104"/>
+      <c r="R31" s="162"/>
+      <c r="S31" s="162"/>
       <c r="T31" s="84"/>
       <c r="U31" s="84"/>
       <c r="V31" s="84"/>
@@ -8449,12 +10704,12 @@
       </c>
       <c r="O34" s="76"/>
       <c r="P34" s="76"/>
-      <c r="Q34" s="105" t="s">
+      <c r="Q34" s="163" t="s">
         <v>469</v>
       </c>
-      <c r="R34" s="105"/>
-      <c r="S34" s="105"/>
-      <c r="T34" s="105"/>
+      <c r="R34" s="163"/>
+      <c r="S34" s="163"/>
+      <c r="T34" s="163"/>
       <c r="U34" s="76"/>
       <c r="V34" s="76"/>
       <c r="W34" s="76"/>
@@ -8589,11 +10844,11 @@
       <c r="I37" s="76"/>
       <c r="J37" s="76"/>
       <c r="K37" s="76"/>
-      <c r="L37" s="104" t="s">
+      <c r="L37" s="162" t="s">
         <v>497</v>
       </c>
-      <c r="M37" s="104"/>
-      <c r="N37" s="104"/>
+      <c r="M37" s="162"/>
+      <c r="N37" s="162"/>
       <c r="O37" s="76"/>
       <c r="P37" s="76" t="s">
         <v>574</v>
@@ -8684,12 +10939,12 @@
       </c>
       <c r="O39" s="76"/>
       <c r="P39" s="76"/>
-      <c r="Q39" s="105" t="s">
+      <c r="Q39" s="163" t="s">
         <v>469</v>
       </c>
-      <c r="R39" s="105"/>
-      <c r="S39" s="105"/>
-      <c r="T39" s="105"/>
+      <c r="R39" s="163"/>
+      <c r="S39" s="163"/>
+      <c r="T39" s="163"/>
       <c r="U39" s="76"/>
       <c r="V39" s="76"/>
       <c r="W39" s="76"/>
@@ -8825,11 +11080,11 @@
       <c r="I42" s="76"/>
       <c r="J42" s="76"/>
       <c r="K42" s="76"/>
-      <c r="L42" s="104" t="s">
+      <c r="L42" s="162" t="s">
         <v>497</v>
       </c>
-      <c r="M42" s="104"/>
-      <c r="N42" s="104"/>
+      <c r="M42" s="162"/>
+      <c r="N42" s="162"/>
       <c r="O42" s="76"/>
       <c r="P42" s="76" t="s">
         <v>574</v>
@@ -8881,11 +11136,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA9E33D-55F9-4A4A-B5CD-11BD9F30F4BE}">
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -10666,11 +12922,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AC36B9-4299-42F4-A6F4-E5E30F812968}">
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Remove comments about guessing...
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D0F54D-2672-4441-80A5-8B7DE99086E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD50B5E-5257-4611-B308-54FAB5423A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15" yWindow="0" windowWidth="22605" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
-    <workbookView xWindow="18000" yWindow="720" windowWidth="22605" windowHeight="20415" xr2:uid="{704AA4A8-87AD-42BA-A92F-F9E203ADE002}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -52,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2582" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="593">
   <si>
     <t>Column1</t>
   </si>
@@ -1381,12 +1380,6 @@
   </si>
   <si>
     <t>SD Pins - Cable connector(T4 34-39)</t>
-  </si>
-  <si>
-    <t>Warning Guessing on actual pin number ordering Here</t>
-  </si>
-  <si>
-    <t>New Top Pins(Pin numbers from Forum posting)</t>
   </si>
   <si>
     <t>49</t>
@@ -2960,8 +2953,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M61" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
-  <autoFilter ref="A1:M61" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M59" totalsRowShown="0" headerRowDxfId="42" dataDxfId="41">
+  <autoFilter ref="A1:M59" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="40"/>
     <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="39"/>
@@ -3328,9 +3321,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A38" sqref="A38"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4968,9 +4958,8 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" sqref="A1:AD35"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5010,10 +4999,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="104" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C1" s="105" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D1" s="106" t="s">
         <v>16</v>
@@ -5025,7 +5014,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="109" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H1" s="110" t="s">
         <v>18</v>
@@ -5046,12 +5035,12 @@
         <v>20</v>
       </c>
       <c r="N1" s="116" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="O1" s="105"/>
       <c r="P1" s="105"/>
       <c r="Q1" s="116" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="R1" s="115" t="s">
         <v>20</v>
@@ -5072,7 +5061,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="117" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="Y1" s="108" t="s">
         <v>24</v>
@@ -5084,10 +5073,10 @@
         <v>16</v>
       </c>
       <c r="AB1" s="105" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="AC1" s="104" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="AD1" s="104" t="s">
         <v>22</v>
@@ -5095,10 +5084,10 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="118" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C2" s="118"/>
       <c r="D2" s="119"/>
@@ -5109,14 +5098,14 @@
       <c r="J2" s="118"/>
       <c r="K2" s="118"/>
       <c r="L2" s="161" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M2" s="161"/>
       <c r="N2" s="161"/>
       <c r="O2" s="121"/>
       <c r="P2" s="121"/>
       <c r="Q2" s="160" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="R2" s="160"/>
       <c r="S2" s="160"/>
@@ -5130,7 +5119,7 @@
       <c r="AA2" s="122"/>
       <c r="AB2" s="118"/>
       <c r="AC2" s="118" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="AD2" s="118"/>
     </row>
@@ -5150,13 +5139,13 @@
       </c>
       <c r="H3" s="118"/>
       <c r="I3" s="123" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J3" s="124" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K3" s="125" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L3" s="118"/>
       <c r="M3" s="118"/>
@@ -5166,7 +5155,7 @@
       <c r="O3" s="121"/>
       <c r="P3" s="121"/>
       <c r="Q3" s="160" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="R3" s="160"/>
       <c r="S3" s="160"/>
@@ -5180,10 +5169,10 @@
       <c r="AA3" s="122"/>
       <c r="AB3" s="118"/>
       <c r="AC3" s="118" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AD3" s="118" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -5202,13 +5191,13 @@
       </c>
       <c r="H4" s="118"/>
       <c r="I4" s="123" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J4" s="124" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="K4" s="125" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="L4" s="118"/>
       <c r="M4" s="118"/>
@@ -5218,7 +5207,7 @@
       <c r="O4" s="121"/>
       <c r="P4" s="121"/>
       <c r="Q4" s="160" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="R4" s="160"/>
       <c r="S4" s="160"/>
@@ -5232,7 +5221,7 @@
       <c r="AA4" s="122"/>
       <c r="AB4" s="118"/>
       <c r="AC4" s="118" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AD4" s="118">
         <v>3.3</v>
@@ -5241,7 +5230,7 @@
     <row r="5" spans="1:30">
       <c r="A5" s="118"/>
       <c r="B5" s="118" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C5" s="118" t="s">
         <v>46</v>
@@ -5250,7 +5239,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="127" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F5" s="128" t="s">
         <v>51</v>
@@ -5264,7 +5253,7 @@
       <c r="K5" s="118"/>
       <c r="L5" s="118"/>
       <c r="M5" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N5" s="126">
         <v>2</v>
@@ -5275,15 +5264,15 @@
         <v>23</v>
       </c>
       <c r="R5" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S5" s="131" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="T5" s="118"/>
       <c r="U5" s="118"/>
       <c r="V5" s="123" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="W5" s="118"/>
       <c r="X5" s="118"/>
@@ -5291,22 +5280,22 @@
         <v>210</v>
       </c>
       <c r="Z5" s="132" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="AA5" s="122">
         <v>1.25</v>
       </c>
       <c r="AB5" s="118" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AC5" s="118"/>
       <c r="AD5" s="118" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="118" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B6" s="118"/>
       <c r="C6" s="118" t="s">
@@ -5316,7 +5305,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="132" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F6" s="128" t="s">
         <v>58</v>
@@ -5330,7 +5319,7 @@
       <c r="K6" s="118"/>
       <c r="L6" s="118"/>
       <c r="M6" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N6" s="126">
         <v>3</v>
@@ -5341,15 +5330,15 @@
         <v>22</v>
       </c>
       <c r="R6" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S6" s="131" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="T6" s="118"/>
       <c r="U6" s="118"/>
       <c r="V6" s="123" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="W6" s="118"/>
       <c r="X6" s="118"/>
@@ -5368,7 +5357,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="118" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B7" s="118"/>
       <c r="C7" s="118" t="s">
@@ -5378,7 +5367,7 @@
         <v>61</v>
       </c>
       <c r="E7" s="132" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F7" s="128" t="s">
         <v>65</v>
@@ -5392,7 +5381,7 @@
       <c r="K7" s="118"/>
       <c r="L7" s="118"/>
       <c r="M7" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N7" s="126">
         <v>4</v>
@@ -5404,10 +5393,10 @@
       </c>
       <c r="R7" s="135"/>
       <c r="S7" s="131" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="T7" s="125" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="U7" s="118"/>
       <c r="V7" s="118"/>
@@ -5417,7 +5406,7 @@
         <v>0.13263888888888889</v>
       </c>
       <c r="Z7" s="127" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="AA7" s="122">
         <v>1.27</v>
@@ -5427,15 +5416,15 @@
       </c>
       <c r="AC7" s="118"/>
       <c r="AD7" s="118" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="118" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B8" s="118" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C8" s="118" t="s">
         <v>269</v>
@@ -5444,7 +5433,7 @@
         <v>270</v>
       </c>
       <c r="E8" s="127" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F8" s="128" t="s">
         <v>273</v>
@@ -5458,7 +5447,7 @@
       <c r="K8" s="136"/>
       <c r="L8" s="118"/>
       <c r="M8" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N8" s="126">
         <v>5</v>
@@ -5470,10 +5459,10 @@
       </c>
       <c r="R8" s="135"/>
       <c r="S8" s="131" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="T8" s="137" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="U8" s="118"/>
       <c r="V8" s="118"/>
@@ -5483,7 +5472,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="Z8" s="127" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="AA8" s="122">
         <v>1.26</v>
@@ -5493,13 +5482,13 @@
       </c>
       <c r="AC8" s="118"/>
       <c r="AD8" s="118" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="118"/>
       <c r="B9" s="118" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C9" s="118" t="s">
         <v>88</v>
@@ -5508,7 +5497,7 @@
         <v>89</v>
       </c>
       <c r="E9" s="127" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F9" s="128" t="s">
         <v>93</v>
@@ -5520,7 +5509,7 @@
       <c r="K9" s="118"/>
       <c r="L9" s="118"/>
       <c r="M9" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N9" s="126">
         <v>6</v>
@@ -5531,18 +5520,18 @@
         <v>19</v>
       </c>
       <c r="R9" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S9" s="131" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="T9" s="137" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="U9" s="118"/>
       <c r="V9" s="118"/>
       <c r="W9" s="138" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="X9" s="118"/>
       <c r="Y9" s="134">
@@ -5556,16 +5545,16 @@
         <v>175</v>
       </c>
       <c r="AC9" s="118" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AD9" s="118" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="118"/>
       <c r="B10" s="118" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C10" s="118" t="s">
         <v>74</v>
@@ -5574,7 +5563,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="127" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F10" s="128" t="s">
         <v>317</v>
@@ -5586,11 +5575,11 @@
       <c r="I10" s="118"/>
       <c r="J10" s="118"/>
       <c r="K10" s="125" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L10" s="118"/>
       <c r="M10" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N10" s="126">
         <v>7</v>
@@ -5601,16 +5590,16 @@
         <v>18</v>
       </c>
       <c r="R10" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S10" s="131" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="T10" s="118"/>
       <c r="U10" s="118"/>
       <c r="V10" s="118"/>
       <c r="W10" s="138" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="X10" s="118"/>
       <c r="Y10" s="134">
@@ -5624,10 +5613,10 @@
         <v>166</v>
       </c>
       <c r="AC10" s="118" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AD10" s="118" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -5640,7 +5629,7 @@
         <v>82</v>
       </c>
       <c r="E11" s="127" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F11" s="128" t="s">
         <v>316</v>
@@ -5649,16 +5638,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="138" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I11" s="118"/>
       <c r="J11" s="118"/>
       <c r="K11" s="125" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L11" s="118"/>
       <c r="M11" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N11" s="126">
         <v>8</v>
@@ -5670,15 +5659,15 @@
       </c>
       <c r="R11" s="135"/>
       <c r="S11" s="131" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="T11" s="137" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="U11" s="118"/>
       <c r="V11" s="118"/>
       <c r="W11" s="138" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="X11" s="118"/>
       <c r="Y11" s="134">
@@ -5704,7 +5693,7 @@
         <v>96</v>
       </c>
       <c r="E12" s="132" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F12" s="128" t="s">
         <v>100</v>
@@ -5716,7 +5705,7 @@
       <c r="K12" s="136"/>
       <c r="L12" s="118"/>
       <c r="M12" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N12" s="126">
         <v>9</v>
@@ -5728,15 +5717,15 @@
       </c>
       <c r="R12" s="135"/>
       <c r="S12" s="131" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="T12" s="137" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="U12" s="118"/>
       <c r="V12" s="118"/>
       <c r="W12" s="138" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="X12" s="118"/>
       <c r="Y12" s="134">
@@ -5754,7 +5743,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="118" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B13" s="118"/>
       <c r="C13" s="118" t="s">
@@ -5764,7 +5753,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="127" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F13" s="128" t="s">
         <v>107</v>
@@ -5773,12 +5762,12 @@
       <c r="H13" s="118"/>
       <c r="I13" s="118"/>
       <c r="J13" s="124" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K13" s="136"/>
       <c r="L13" s="118"/>
       <c r="M13" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N13" s="126">
         <v>10</v>
@@ -5789,13 +5778,13 @@
         <v>15</v>
       </c>
       <c r="R13" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S13" s="131" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="T13" s="137" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="U13" s="118"/>
       <c r="V13" s="118"/>
@@ -5805,7 +5794,7 @@
         <v>0.12708333333333333</v>
       </c>
       <c r="Z13" s="139" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="AA13" s="122">
         <v>1.19</v>
@@ -5815,15 +5804,15 @@
       </c>
       <c r="AC13" s="118"/>
       <c r="AD13" s="118" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="118" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B14" s="118" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C14" s="118" t="s">
         <v>109</v>
@@ -5838,15 +5827,15 @@
       <c r="G14" s="118"/>
       <c r="H14" s="118"/>
       <c r="I14" s="123" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J14" s="124" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="K14" s="118"/>
       <c r="L14" s="118"/>
       <c r="M14" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N14" s="126">
         <v>11</v>
@@ -5857,13 +5846,13 @@
         <v>14</v>
       </c>
       <c r="R14" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S14" s="131" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="T14" s="137" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="U14" s="118"/>
       <c r="V14" s="118"/>
@@ -5873,7 +5862,7 @@
         <v>0.12638888888888888</v>
       </c>
       <c r="Z14" s="127" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="AA14" s="122">
         <v>1.18</v>
@@ -5886,10 +5875,10 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="118" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B15" s="118" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C15" s="118" t="s">
         <v>116</v>
@@ -5898,7 +5887,7 @@
         <v>117</v>
       </c>
       <c r="E15" s="127" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F15" s="128" t="s">
         <v>121</v>
@@ -5907,12 +5896,12 @@
       <c r="H15" s="118"/>
       <c r="I15" s="118"/>
       <c r="J15" s="124" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K15" s="118"/>
       <c r="L15" s="118"/>
       <c r="M15" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N15" s="126">
         <v>12</v>
@@ -5923,17 +5912,17 @@
         <v>13</v>
       </c>
       <c r="R15" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S15" s="140" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="T15" s="118"/>
       <c r="U15" s="124" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="V15" s="123" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="W15" s="118"/>
       <c r="X15" s="118"/>
@@ -5948,10 +5937,10 @@
         <v>123</v>
       </c>
       <c r="AC15" s="118" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AD15" s="118" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -5998,7 +5987,7 @@
       <c r="I17" s="122"/>
       <c r="J17" s="122"/>
       <c r="K17" s="159" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="L17" s="122"/>
       <c r="M17" s="122"/>
@@ -6033,18 +6022,18 @@
       <c r="F18" s="118"/>
       <c r="G18" s="118"/>
       <c r="H18" s="138" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I18" s="118"/>
       <c r="J18" s="118"/>
       <c r="K18" s="137" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="L18" s="131" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="M18" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N18" s="126">
         <v>24</v>
@@ -6055,18 +6044,18 @@
         <v>25</v>
       </c>
       <c r="R18" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S18" s="131" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="T18" s="137" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="U18" s="122"/>
       <c r="V18" s="122"/>
       <c r="W18" s="138" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="X18" s="122"/>
       <c r="Y18" s="122"/>
@@ -6097,11 +6086,11 @@
       <c r="H19" s="118"/>
       <c r="I19" s="118"/>
       <c r="J19" s="124" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="K19" s="135"/>
       <c r="L19" s="131" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="M19" s="118"/>
       <c r="N19" s="126">
@@ -6114,11 +6103,11 @@
       </c>
       <c r="R19" s="141"/>
       <c r="S19" s="131" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="T19" s="118"/>
       <c r="U19" s="124" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="V19" s="118"/>
       <c r="W19" s="118"/>
@@ -6152,11 +6141,11 @@
       <c r="I20" s="118"/>
       <c r="J20" s="118"/>
       <c r="K20" s="137" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="L20" s="118"/>
       <c r="M20" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N20" s="126">
         <v>28</v>
@@ -6167,11 +6156,11 @@
         <v>29</v>
       </c>
       <c r="R20" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S20" s="142"/>
       <c r="T20" s="137" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="U20" s="118"/>
       <c r="V20" s="118"/>
@@ -6204,7 +6193,7 @@
       </c>
       <c r="H21" s="118"/>
       <c r="I21" s="143" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J21" s="118"/>
       <c r="K21" s="118"/>
@@ -6223,7 +6212,7 @@
       <c r="T21" s="118"/>
       <c r="U21" s="142"/>
       <c r="V21" s="123" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="W21" s="118"/>
       <c r="X21" s="120">
@@ -6250,7 +6239,7 @@
         <v>264</v>
       </c>
       <c r="E22" s="127" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F22" s="134">
         <v>9.1666666666666674E-2</v>
@@ -6273,13 +6262,13 @@
         <v>33</v>
       </c>
       <c r="R22" s="129" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S22" s="118"/>
       <c r="T22" s="118"/>
       <c r="U22" s="118"/>
       <c r="V22" s="143" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="W22" s="118"/>
       <c r="X22" s="120">
@@ -6289,7 +6278,7 @@
         <v>72</v>
       </c>
       <c r="Z22" s="127" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="AA22" s="122">
         <v>4.7</v>
@@ -6375,7 +6364,7 @@
       <c r="I25" s="142"/>
       <c r="J25" s="142"/>
       <c r="K25" s="159" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="L25" s="2"/>
       <c r="N25" s="142"/>
@@ -6447,21 +6436,21 @@
       <c r="H27" s="142"/>
       <c r="I27" s="142"/>
       <c r="J27" s="148" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="K27" s="142"/>
       <c r="L27" s="142"/>
       <c r="M27" s="149" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N27" s="150">
         <v>34</v>
       </c>
       <c r="O27" s="151" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="P27" s="142" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="Q27" s="151"/>
       <c r="R27" s="151"/>
@@ -6497,23 +6486,23 @@
       <c r="H28" s="142"/>
       <c r="I28" s="142"/>
       <c r="J28" s="148" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K28" s="152" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L28" s="142"/>
       <c r="M28" s="149" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N28" s="150">
         <v>35</v>
       </c>
       <c r="O28" s="142" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="P28" s="142" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="Q28" s="151"/>
       <c r="R28" s="151"/>
@@ -6543,15 +6532,15 @@
       <c r="J29" s="151"/>
       <c r="K29" s="151"/>
       <c r="L29" s="161" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M29" s="161"/>
       <c r="N29" s="161"/>
       <c r="O29" s="151" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="P29" s="151" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="Q29" s="151"/>
       <c r="R29" s="151"/>
@@ -6587,21 +6576,21 @@
       <c r="H30" s="151"/>
       <c r="I30" s="151"/>
       <c r="J30" s="155" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="K30" s="151"/>
       <c r="L30" s="151"/>
       <c r="M30" s="156" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N30" s="150">
         <v>36</v>
       </c>
       <c r="O30" s="151" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="P30" s="142" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="Q30" s="135"/>
       <c r="R30" s="135"/>
@@ -6622,7 +6611,7 @@
       <c r="A31" s="135"/>
       <c r="B31" s="135"/>
       <c r="L31" s="160" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="M31" s="160"/>
       <c r="N31" s="160"/>
@@ -6662,12 +6651,12 @@
       <c r="H32" s="135"/>
       <c r="I32" s="135"/>
       <c r="J32" s="155" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K32" s="135"/>
       <c r="L32" s="135"/>
       <c r="M32" s="149" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N32" s="150">
         <v>37</v>
@@ -6709,11 +6698,11 @@
       <c r="I33" s="135"/>
       <c r="J33" s="135"/>
       <c r="K33" s="152" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="L33" s="135"/>
       <c r="M33" s="149" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N33" s="150">
         <v>38</v>
@@ -6755,11 +6744,11 @@
       <c r="I34" s="135"/>
       <c r="J34" s="135"/>
       <c r="K34" s="152" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="L34" s="135"/>
       <c r="M34" s="149" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N34" s="150">
         <v>39</v>
@@ -6885,14 +6874,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
-    </sheetView>
-    <sheetView topLeftCell="A25" workbookViewId="1">
-      <selection activeCell="J48" sqref="J48"/>
+      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7575,7 +7561,7 @@
         <v>358</v>
       </c>
       <c r="M18" s="37" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -7616,7 +7602,7 @@
         <v>359</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -7809,7 +7795,7 @@
         <v>364</v>
       </c>
       <c r="M24" s="37" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -7850,7 +7836,7 @@
         <v>365</v>
       </c>
       <c r="M25" s="37" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -8266,99 +8252,135 @@
       </c>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="5" t="s">
-        <v>443</v>
+      <c r="A37" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2.29</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="5" t="s">
-        <v>444</v>
+      <c r="A38" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39" s="3" t="s">
-        <v>286</v>
+        <v>404</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C39" s="3">
-        <v>2.29</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>382</v>
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40" s="3" t="s">
-        <v>287</v>
+        <v>405</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C40" s="3">
-        <v>2.2799999999999998</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>383</v>
+        <v>2.19</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="3" t="s">
-        <v>404</v>
+        <v>562</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C41" s="3">
-        <v>2.1800000000000002</v>
+        <v>1.28</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>384</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>44</v>
+        <v>392</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>396</v>
+        <v>402</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="3" t="s">
-        <v>405</v>
+        <v>563</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C42" s="3">
-        <v>2.19</v>
+        <v>1.29</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>388</v>
+        <v>349</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>36</v>
+        <v>393</v>
       </c>
       <c r="K42" s="3" t="s">
-        <v>397</v>
+        <v>403</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -8366,22 +8388,19 @@
         <v>564</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="C43" s="3">
-        <v>1.28</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>392</v>
+        <v>380</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>588</v>
       </c>
       <c r="K43" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>398</v>
+        <v>566</v>
+      </c>
+      <c r="M43" s="37" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -8389,251 +8408,254 @@
         <v>565</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C44" s="3">
-        <v>1.29</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>393</v>
+        <v>1.21</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>389</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>399</v>
+        <v>567</v>
+      </c>
+      <c r="M44" s="37" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>380</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>568</v>
-      </c>
-      <c r="M45" s="37" t="s">
-        <v>451</v>
+      <c r="A45" s="5" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="3" t="s">
-        <v>567</v>
+        <v>435</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="C46" s="3">
-        <v>1.21</v>
+        <v>299</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>350</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="K46" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>569</v>
-      </c>
-      <c r="M46" s="37" t="s">
-        <v>452</v>
+        <v>319</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="5" t="s">
-        <v>442</v>
+      <c r="A47" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="3" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>336</v>
+        <v>303</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>368</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>319</v>
+        <v>256</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>57</v>
+        <v>314</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="3" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>337</v>
+        <v>302</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>369</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>318</v>
+        <v>261</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>50</v>
+        <v>315</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="3" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>368</v>
+        <v>307</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>335</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>352</v>
+        <v>462</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>256</v>
+        <v>321</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>314</v>
+        <v>71</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="3" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>369</v>
+        <v>306</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>334</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>353</v>
+        <v>463</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>261</v>
+        <v>320</v>
       </c>
       <c r="J51" s="3" t="s">
-        <v>315</v>
+        <v>64</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="J52" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="M52" s="3" t="s">
-        <v>294</v>
+      <c r="A52" s="5" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="3" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>300</v>
+        <v>253</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>306</v>
+        <v>414</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>334</v>
+        <v>420</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="G53" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="G54" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="J53" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="M53" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13">
-      <c r="A54" s="5" t="s">
-        <v>406</v>
+      <c r="K54" s="3" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="3" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>253</v>
+        <v>411</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>256</v>
+        <v>321</v>
+      </c>
+      <c r="K55" s="3" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -8641,22 +8663,19 @@
         <v>445</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>417</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>422</v>
+        <v>413</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>369</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>427</v>
+        <v>433</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -8664,22 +8683,22 @@
         <v>446</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -8687,19 +8706,19 @@
         <v>447</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>369</v>
+        <v>415</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>423</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>457</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>433</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -8707,64 +8726,21 @@
         <v>448</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>319</v>
+        <v>430</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13">
-      <c r="A60" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>459</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13">
-      <c r="A61" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>412</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>463</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="K61" s="3" t="s">
         <v>429</v>
       </c>
     </row>
@@ -8787,9 +8763,8 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X21" sqref="X21"/>
+      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -8829,10 +8804,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D1" s="98" t="s">
         <v>16</v>
@@ -8844,7 +8819,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="68" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>18</v>
@@ -8865,12 +8840,12 @@
         <v>20</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="O1" s="39"/>
       <c r="P1" s="39"/>
       <c r="Q1" s="46" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="R1" s="45" t="s">
         <v>20</v>
@@ -8891,7 +8866,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="69" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="Y1" s="40" t="s">
         <v>24</v>
@@ -8903,10 +8878,10 @@
         <v>16</v>
       </c>
       <c r="AB1" s="39" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="AC1" s="38" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="AD1" s="38" t="s">
         <v>22</v>
@@ -8914,10 +8889,10 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="47" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="103"/>
@@ -8928,14 +8903,14 @@
       <c r="J2" s="47"/>
       <c r="K2" s="47"/>
       <c r="L2" s="162" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M2" s="162"/>
       <c r="N2" s="162"/>
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
       <c r="Q2" s="163" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="R2" s="163"/>
       <c r="S2" s="163"/>
@@ -8949,7 +8924,7 @@
       <c r="AA2" s="99"/>
       <c r="AB2" s="47"/>
       <c r="AC2" s="47" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="AD2" s="47"/>
     </row>
@@ -8969,13 +8944,13 @@
       </c>
       <c r="H3" s="47"/>
       <c r="I3" s="64" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="K3" s="50" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
@@ -8985,7 +8960,7 @@
       <c r="O3" s="48"/>
       <c r="P3" s="48"/>
       <c r="Q3" s="163" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="R3" s="163"/>
       <c r="S3" s="163"/>
@@ -8999,10 +8974,10 @@
       <c r="AA3" s="99"/>
       <c r="AB3" s="47"/>
       <c r="AC3" s="47" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="AD3" s="47" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -9021,13 +8996,13 @@
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="64" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="L4" s="47"/>
       <c r="M4" s="47"/>
@@ -9037,7 +9012,7 @@
       <c r="O4" s="48"/>
       <c r="P4" s="48"/>
       <c r="Q4" s="163" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="R4" s="163"/>
       <c r="S4" s="163"/>
@@ -9051,7 +9026,7 @@
       <c r="AA4" s="99"/>
       <c r="AB4" s="47"/>
       <c r="AC4" s="47" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="AD4" s="47">
         <v>3.3</v>
@@ -9060,7 +9035,7 @@
     <row r="5" spans="1:30">
       <c r="A5" s="47"/>
       <c r="B5" s="47" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>46</v>
@@ -9069,7 +9044,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F5" s="62" t="s">
         <v>51</v>
@@ -9083,7 +9058,7 @@
       <c r="K5" s="47"/>
       <c r="L5" s="47"/>
       <c r="M5" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N5" s="51">
         <v>2</v>
@@ -9094,15 +9069,15 @@
         <v>23</v>
       </c>
       <c r="R5" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S5" s="54" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
       <c r="V5" s="64" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="W5" s="47"/>
       <c r="X5" s="47"/>
@@ -9110,22 +9085,22 @@
         <v>210</v>
       </c>
       <c r="Z5" s="72" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="AA5" s="99">
         <v>1.25</v>
       </c>
       <c r="AB5" s="47" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="AC5" s="47"/>
       <c r="AD5" s="47" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="47" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B6" s="47"/>
       <c r="C6" s="47" t="s">
@@ -9135,7 +9110,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F6" s="62" t="s">
         <v>58</v>
@@ -9149,7 +9124,7 @@
       <c r="K6" s="47"/>
       <c r="L6" s="47"/>
       <c r="M6" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N6" s="51">
         <v>3</v>
@@ -9160,15 +9135,15 @@
         <v>22</v>
       </c>
       <c r="R6" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S6" s="54" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="T6" s="47"/>
       <c r="U6" s="47"/>
       <c r="V6" s="64" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="W6" s="47"/>
       <c r="X6" s="47"/>
@@ -9187,7 +9162,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="47" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="47" t="s">
@@ -9197,7 +9172,7 @@
         <v>61</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F7" s="62" t="s">
         <v>65</v>
@@ -9211,7 +9186,7 @@
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
       <c r="M7" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N7" s="51">
         <v>4</v>
@@ -9222,10 +9197,10 @@
         <v>21</v>
       </c>
       <c r="S7" s="54" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="T7" s="50" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="U7" s="47"/>
       <c r="V7" s="47"/>
@@ -9235,7 +9210,7 @@
         <v>0.13263888888888889</v>
       </c>
       <c r="Z7" s="70" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="AA7" s="99">
         <v>1.27</v>
@@ -9245,15 +9220,15 @@
       </c>
       <c r="AC7" s="47"/>
       <c r="AD7" s="47" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="47" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>269</v>
@@ -9262,7 +9237,7 @@
         <v>270</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F8" s="62" t="s">
         <v>273</v>
@@ -9276,7 +9251,7 @@
       <c r="K8" s="57"/>
       <c r="L8" s="47"/>
       <c r="M8" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N8" s="51">
         <v>5</v>
@@ -9287,10 +9262,10 @@
         <v>20</v>
       </c>
       <c r="S8" s="54" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="T8" s="58" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="U8" s="47"/>
       <c r="V8" s="47"/>
@@ -9300,7 +9275,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="Z8" s="70" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="AA8" s="99">
         <v>1.26</v>
@@ -9310,13 +9285,13 @@
       </c>
       <c r="AC8" s="47"/>
       <c r="AD8" s="47" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="47"/>
       <c r="B9" s="47" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C9" s="47" t="s">
         <v>88</v>
@@ -9325,7 +9300,7 @@
         <v>89</v>
       </c>
       <c r="E9" s="70" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F9" s="62" t="s">
         <v>93</v>
@@ -9337,7 +9312,7 @@
       <c r="K9" s="47"/>
       <c r="L9" s="47"/>
       <c r="M9" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N9" s="51">
         <v>6</v>
@@ -9348,18 +9323,18 @@
         <v>19</v>
       </c>
       <c r="R9" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S9" s="54" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="U9" s="47"/>
       <c r="V9" s="47"/>
       <c r="W9" s="66" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="X9" s="47"/>
       <c r="Y9" s="63">
@@ -9373,16 +9348,16 @@
         <v>175</v>
       </c>
       <c r="AC9" s="47" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AD9" s="47" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="47"/>
       <c r="B10" s="47" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>74</v>
@@ -9391,7 +9366,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F10" s="62" t="s">
         <v>317</v>
@@ -9403,11 +9378,11 @@
       <c r="I10" s="47"/>
       <c r="J10" s="47"/>
       <c r="K10" s="50" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="L10" s="47"/>
       <c r="M10" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N10" s="51">
         <v>7</v>
@@ -9418,16 +9393,16 @@
         <v>18</v>
       </c>
       <c r="R10" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S10" s="54" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
       <c r="V10" s="47"/>
       <c r="W10" s="66" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="X10" s="47"/>
       <c r="Y10" s="63">
@@ -9441,10 +9416,10 @@
         <v>166</v>
       </c>
       <c r="AC10" s="47" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="AD10" s="47" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -9457,7 +9432,7 @@
         <v>82</v>
       </c>
       <c r="E11" s="70" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F11" s="62" t="s">
         <v>316</v>
@@ -9466,16 +9441,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="66" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="50" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="L11" s="47"/>
       <c r="M11" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N11" s="51">
         <v>8</v>
@@ -9486,15 +9461,15 @@
         <v>17</v>
       </c>
       <c r="S11" s="54" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="T11" s="58" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="U11" s="47"/>
       <c r="V11" s="47"/>
       <c r="W11" s="66" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="X11" s="47"/>
       <c r="Y11" s="63">
@@ -9520,7 +9495,7 @@
         <v>96</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F12" s="62" t="s">
         <v>100</v>
@@ -9532,7 +9507,7 @@
       <c r="K12" s="57"/>
       <c r="L12" s="47"/>
       <c r="M12" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N12" s="51">
         <v>9</v>
@@ -9543,15 +9518,15 @@
         <v>16</v>
       </c>
       <c r="S12" s="54" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="T12" s="58" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="U12" s="47"/>
       <c r="V12" s="47"/>
       <c r="W12" s="66" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="X12" s="47"/>
       <c r="Y12" s="63">
@@ -9569,7 +9544,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="47" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47" t="s">
@@ -9579,7 +9554,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="70" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F13" s="62" t="s">
         <v>107</v>
@@ -9588,12 +9563,12 @@
       <c r="H13" s="47"/>
       <c r="I13" s="47"/>
       <c r="J13" s="49" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="K13" s="57"/>
       <c r="L13" s="47"/>
       <c r="M13" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N13" s="51">
         <v>10</v>
@@ -9604,13 +9579,13 @@
         <v>15</v>
       </c>
       <c r="R13" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S13" s="54" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="T13" s="58" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="U13" s="47"/>
       <c r="V13" s="47"/>
@@ -9620,7 +9595,7 @@
         <v>0.12708333333333333</v>
       </c>
       <c r="Z13" s="55" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="AA13" s="99">
         <v>1.19</v>
@@ -9630,15 +9605,15 @@
       </c>
       <c r="AC13" s="47"/>
       <c r="AD13" s="47" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="47" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>109</v>
@@ -9653,15 +9628,15 @@
       <c r="G14" s="47"/>
       <c r="H14" s="47"/>
       <c r="I14" s="64" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J14" s="49" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="K14" s="47"/>
       <c r="L14" s="47"/>
       <c r="M14" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N14" s="51">
         <v>11</v>
@@ -9672,13 +9647,13 @@
         <v>14</v>
       </c>
       <c r="R14" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S14" s="54" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="T14" s="58" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="U14" s="47"/>
       <c r="V14" s="47"/>
@@ -9688,7 +9663,7 @@
         <v>0.12638888888888888</v>
       </c>
       <c r="Z14" s="70" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="AA14" s="99">
         <v>1.18</v>
@@ -9701,10 +9676,10 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="47" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>116</v>
@@ -9713,7 +9688,7 @@
         <v>117</v>
       </c>
       <c r="E15" s="70" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F15" s="62" t="s">
         <v>121</v>
@@ -9722,12 +9697,12 @@
       <c r="H15" s="47"/>
       <c r="I15" s="47"/>
       <c r="J15" s="49" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="K15" s="47"/>
       <c r="L15" s="47"/>
       <c r="M15" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N15" s="51">
         <v>12</v>
@@ -9738,17 +9713,17 @@
         <v>13</v>
       </c>
       <c r="R15" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S15" s="97" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="T15" s="47"/>
       <c r="U15" s="49" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="V15" s="64" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="W15" s="47"/>
       <c r="X15" s="47"/>
@@ -9763,10 +9738,10 @@
         <v>123</v>
       </c>
       <c r="AC15" s="47" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AD15" s="47" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -9782,14 +9757,14 @@
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
       <c r="L16" s="162" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="M16" s="162"/>
       <c r="N16" s="162"/>
       <c r="O16" s="48"/>
       <c r="P16" s="48"/>
       <c r="Q16" s="163" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -9818,18 +9793,18 @@
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="66" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="58" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="L17" s="54" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="M17" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N17" s="51">
         <v>24</v>
@@ -9840,10 +9815,10 @@
         <v>41</v>
       </c>
       <c r="R17" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S17" s="54" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="T17" s="47"/>
       <c r="U17" s="47"/>
@@ -9858,7 +9833,7 @@
         <v>1.21</v>
       </c>
       <c r="AB17" s="47" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="AC17" s="47"/>
       <c r="AD17" s="47"/>
@@ -9876,18 +9851,18 @@
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
       <c r="H18" s="66" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I18" s="47"/>
       <c r="J18" s="47"/>
       <c r="K18" s="58" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="L18" s="54" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="M18" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N18" s="51">
         <v>25</v>
@@ -9899,7 +9874,7 @@
       </c>
       <c r="R18" s="60"/>
       <c r="S18" s="54" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="T18" s="47"/>
       <c r="U18" s="47"/>
@@ -9911,10 +9886,10 @@
       </c>
       <c r="Z18" s="47"/>
       <c r="AA18" s="99" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="AB18" s="47" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="AC18" s="47"/>
       <c r="AD18" s="47"/>
@@ -9936,10 +9911,10 @@
       <c r="H19" s="47"/>
       <c r="I19" s="47"/>
       <c r="J19" s="49" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="L19" s="54" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="M19" s="47"/>
       <c r="N19" s="51">
@@ -9952,11 +9927,11 @@
       </c>
       <c r="R19" s="60"/>
       <c r="S19" s="54" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="T19" s="47"/>
       <c r="U19" s="74" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="V19" s="47"/>
       <c r="W19" s="47"/>
@@ -9969,7 +9944,7 @@
         <v>1.29</v>
       </c>
       <c r="AB19" s="47" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="AC19" s="47"/>
       <c r="AD19" s="47"/>
@@ -9991,11 +9966,11 @@
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
       <c r="J20" s="49" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="K20" s="47"/>
       <c r="L20" s="54" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="M20" s="47"/>
       <c r="N20" s="51">
@@ -10008,11 +9983,11 @@
       </c>
       <c r="R20" s="60"/>
       <c r="S20" s="54" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="T20" s="47"/>
       <c r="U20" s="74" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="V20" s="47"/>
       <c r="W20" s="47"/>
@@ -10024,7 +9999,7 @@
         <v>1.28</v>
       </c>
       <c r="AB20" s="47" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="AC20" s="47"/>
       <c r="AD20" s="47"/>
@@ -10045,11 +10020,11 @@
       <c r="I21" s="47"/>
       <c r="J21" s="47"/>
       <c r="K21" s="58" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="L21" s="47"/>
       <c r="M21" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N21" s="51">
         <v>28</v>
@@ -10060,12 +10035,12 @@
         <v>37</v>
       </c>
       <c r="R21" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S21" s="47"/>
       <c r="T21" s="47"/>
       <c r="U21" s="73" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="47"/>
@@ -10080,7 +10055,7 @@
         <v>2.19</v>
       </c>
       <c r="AB21" s="47" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="AC21" s="47"/>
       <c r="AD21" s="47"/>
@@ -10101,11 +10076,11 @@
       <c r="I22" s="47"/>
       <c r="J22" s="47"/>
       <c r="K22" s="58" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="L22" s="47"/>
       <c r="M22" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N22" s="51">
         <v>29</v>
@@ -10116,12 +10091,12 @@
         <v>36</v>
       </c>
       <c r="R22" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S22" s="47"/>
       <c r="T22" s="47"/>
       <c r="U22" s="73" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="V22" s="47"/>
       <c r="W22" s="47"/>
@@ -10136,7 +10111,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="AB22" s="47" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="AC22" s="47"/>
       <c r="AD22" s="47"/>
@@ -10157,7 +10132,7 @@
       </c>
       <c r="H23" s="47"/>
       <c r="I23" s="56" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J23" s="47"/>
       <c r="K23" s="47"/>
@@ -10172,11 +10147,11 @@
         <v>35</v>
       </c>
       <c r="R23" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S23" s="47"/>
       <c r="T23" s="50" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="U23" s="47"/>
       <c r="V23" s="47"/>
@@ -10190,7 +10165,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="AB23" s="47" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="AC23" s="47"/>
       <c r="AD23" s="47"/>
@@ -10211,7 +10186,7 @@
       </c>
       <c r="H24" s="47"/>
       <c r="I24" s="64" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="J24" s="47"/>
       <c r="K24" s="47"/>
@@ -10228,11 +10203,11 @@
       <c r="R24" s="60"/>
       <c r="S24" s="47"/>
       <c r="T24" s="50" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U24" s="47"/>
       <c r="V24" s="56" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="W24" s="47"/>
       <c r="X24" s="47"/>
@@ -10244,7 +10219,7 @@
         <v>2.29</v>
       </c>
       <c r="AB24" s="47" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="AC24" s="47"/>
       <c r="AD24" s="47"/>
@@ -10259,7 +10234,7 @@
         <v>264</v>
       </c>
       <c r="E25" s="70" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F25" s="63">
         <v>9.1666666666666674E-2</v>
@@ -10282,13 +10257,13 @@
         <v>33</v>
       </c>
       <c r="R25" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S25" s="47"/>
       <c r="T25" s="47"/>
       <c r="U25" s="47"/>
       <c r="V25" s="56" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="W25" s="47"/>
       <c r="X25" s="67">
@@ -10298,7 +10273,7 @@
         <v>72</v>
       </c>
       <c r="Z25" s="70" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="AA25" s="99">
         <v>4.7</v>
@@ -10357,7 +10332,7 @@
       <c r="M27" s="76"/>
       <c r="N27" s="76"/>
       <c r="O27" s="76" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="P27" s="76"/>
       <c r="Q27" s="76"/>
@@ -10394,31 +10369,31 @@
       <c r="H28" s="76"/>
       <c r="I28" s="76"/>
       <c r="J28" s="81" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="K28" s="76"/>
       <c r="L28" s="76"/>
       <c r="M28" s="82" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N28" s="83">
         <v>42</v>
       </c>
       <c r="O28" s="84" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="P28" s="76" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="Q28" s="83">
         <v>47</v>
       </c>
       <c r="R28" s="82" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S28" s="76"/>
       <c r="T28" s="85" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="U28" s="76"/>
       <c r="V28" s="76"/>
@@ -10458,33 +10433,33 @@
       <c r="H29" s="76"/>
       <c r="I29" s="76"/>
       <c r="J29" s="81" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K29" s="85" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="L29" s="76"/>
       <c r="M29" s="82" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N29" s="83">
         <v>43</v>
       </c>
       <c r="O29" s="76" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="P29" s="76" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="Q29" s="83">
         <v>46</v>
       </c>
       <c r="R29" s="82" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S29" s="76"/>
       <c r="T29" s="85" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="U29" s="76"/>
       <c r="V29" s="76"/>
@@ -10518,26 +10493,26 @@
       <c r="J30" s="84"/>
       <c r="K30" s="84"/>
       <c r="L30" s="162" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="M30" s="162"/>
       <c r="N30" s="162"/>
       <c r="O30" s="84" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="P30" s="84" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="Q30" s="83">
         <v>45</v>
       </c>
       <c r="R30" s="82" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S30" s="84"/>
       <c r="T30" s="84"/>
       <c r="U30" s="87" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="V30" s="84"/>
       <c r="W30" s="84"/>
@@ -10576,24 +10551,24 @@
       <c r="H31" s="84"/>
       <c r="I31" s="84"/>
       <c r="J31" s="87" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="K31" s="84"/>
       <c r="L31" s="84"/>
       <c r="M31" s="90" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N31" s="83">
         <v>44</v>
       </c>
       <c r="O31" s="84" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="P31" s="76" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="Q31" s="162" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="R31" s="162"/>
       <c r="S31" s="162"/>
@@ -10657,7 +10632,7 @@
       <c r="M33" s="77"/>
       <c r="N33" s="77"/>
       <c r="O33" s="76" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="P33" s="77"/>
       <c r="Q33" s="77"/>
@@ -10693,11 +10668,11 @@
       <c r="I34" s="76"/>
       <c r="J34" s="76"/>
       <c r="K34" s="92" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L34" s="76"/>
       <c r="M34" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N34" s="93">
         <v>52</v>
@@ -10705,7 +10680,7 @@
       <c r="O34" s="76"/>
       <c r="P34" s="76"/>
       <c r="Q34" s="163" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="R34" s="163"/>
       <c r="S34" s="163"/>
@@ -10737,11 +10712,11 @@
       <c r="I35" s="76"/>
       <c r="J35" s="76"/>
       <c r="K35" s="92" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="L35" s="76"/>
       <c r="M35" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N35" s="93">
         <v>53</v>
@@ -10752,14 +10727,14 @@
         <v>50</v>
       </c>
       <c r="R35" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S35" s="76"/>
       <c r="T35" s="94" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="U35" s="95" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="V35" s="76"/>
       <c r="W35" s="76"/>
@@ -10794,12 +10769,12 @@
       <c r="H36" s="76"/>
       <c r="I36" s="76"/>
       <c r="J36" s="95" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="K36" s="76"/>
       <c r="L36" s="76"/>
       <c r="M36" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N36" s="93">
         <v>54</v>
@@ -10809,12 +10784,12 @@
         <v>49</v>
       </c>
       <c r="R36" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S36" s="76"/>
       <c r="T36" s="76"/>
       <c r="U36" s="95" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="V36" s="76"/>
       <c r="W36" s="76"/>
@@ -10845,26 +10820,26 @@
       <c r="J37" s="76"/>
       <c r="K37" s="76"/>
       <c r="L37" s="162" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="M37" s="162"/>
       <c r="N37" s="162"/>
       <c r="O37" s="76"/>
       <c r="P37" s="76" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="Q37" s="93">
         <v>51</v>
       </c>
       <c r="R37" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S37" s="76"/>
       <c r="T37" s="76"/>
       <c r="U37" s="76"/>
       <c r="V37" s="76"/>
       <c r="W37" s="96" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="X37" s="76"/>
       <c r="Y37" s="76"/>
@@ -10928,11 +10903,11 @@
       <c r="I39" s="76"/>
       <c r="J39" s="76"/>
       <c r="K39" s="92" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L39" s="76"/>
       <c r="M39" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N39" s="93">
         <v>52</v>
@@ -10940,7 +10915,7 @@
       <c r="O39" s="76"/>
       <c r="P39" s="76"/>
       <c r="Q39" s="163" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="R39" s="163"/>
       <c r="S39" s="163"/>
@@ -10972,11 +10947,11 @@
       <c r="I40" s="76"/>
       <c r="J40" s="76"/>
       <c r="K40" s="92" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="L40" s="76"/>
       <c r="M40" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N40" s="93">
         <v>53</v>
@@ -10987,14 +10962,14 @@
         <v>50</v>
       </c>
       <c r="R40" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S40" s="76"/>
       <c r="T40" s="94" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="U40" s="95" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="V40" s="76"/>
       <c r="W40" s="76"/>
@@ -11029,12 +11004,12 @@
       <c r="H41" s="76"/>
       <c r="I41" s="76"/>
       <c r="J41" s="95" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="K41" s="76"/>
       <c r="L41" s="76"/>
       <c r="M41" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="N41" s="93">
         <v>54</v>
@@ -11045,12 +11020,12 @@
         <v>49</v>
       </c>
       <c r="R41" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S41" s="76"/>
       <c r="T41" s="76"/>
       <c r="U41" s="95" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="V41" s="76"/>
       <c r="W41" s="76"/>
@@ -11081,23 +11056,23 @@
       <c r="J42" s="76"/>
       <c r="K42" s="76"/>
       <c r="L42" s="162" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="M42" s="162"/>
       <c r="N42" s="162"/>
       <c r="O42" s="76"/>
       <c r="P42" s="76" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="Q42" s="93">
         <v>48</v>
       </c>
       <c r="R42" s="52" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="S42" s="76"/>
       <c r="T42" s="92" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="U42" s="76"/>
       <c r="V42" s="76"/>
@@ -11141,7 +11116,6 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12927,7 +12901,6 @@
   <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
T4.1 Card - Fix PWM - Change to which timer...
I find that I often wanted more information than just that it can be PWM, but at times which one... As some use same timer.  As each PWM timer may have up to 3 IO pins that they control A, B, X and if two PWM outputs are configured, that use same timer, they can only have one frequency.
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD50B5E-5257-4611-B308-54FAB5423A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94218B71-62EE-481B-99D4-D6660DCEBB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="22605" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="4995" yWindow="480" windowWidth="23535" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2580" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="631">
   <si>
     <t>Column1</t>
   </si>
@@ -1346,9 +1346,6 @@
     <t>PWM3_A0</t>
   </si>
   <si>
-    <t>PWM2_B,QT4_2</t>
-  </si>
-  <si>
     <t>PWM2_A2, QT4_1</t>
   </si>
   <si>
@@ -1830,6 +1827,123 @@
   </si>
   <si>
     <t>Bottom SMT Pins</t>
+  </si>
+  <si>
+    <t>PWM2_B2,QT4_2</t>
+  </si>
+  <si>
+    <t>1X1</t>
+  </si>
+  <si>
+    <t>1X0</t>
+  </si>
+  <si>
+    <t>4A2</t>
+  </si>
+  <si>
+    <t>4B2</t>
+  </si>
+  <si>
+    <t>2A0</t>
+  </si>
+  <si>
+    <t>2A1</t>
+  </si>
+  <si>
+    <t>2A2, Q41</t>
+  </si>
+  <si>
+    <t>1B3</t>
+  </si>
+  <si>
+    <t>1A3</t>
+  </si>
+  <si>
+    <t>2B2,Q42</t>
+  </si>
+  <si>
+    <t>Q10</t>
+  </si>
+  <si>
+    <t>Q12</t>
+  </si>
+  <si>
+    <t>Q11</t>
+  </si>
+  <si>
+    <t>1X3</t>
+  </si>
+  <si>
+    <t>1X2</t>
+  </si>
+  <si>
+    <t>3B1</t>
+  </si>
+  <si>
+    <t>1B1</t>
+  </si>
+  <si>
+    <t>3A1</t>
+  </si>
+  <si>
+    <t>G13</t>
+  </si>
+  <si>
+    <t>G12</t>
+  </si>
+  <si>
+    <t>4A1</t>
+  </si>
+  <si>
+    <t>4A0</t>
+  </si>
+  <si>
+    <t>3A0</t>
+  </si>
+  <si>
+    <t>Q30</t>
+  </si>
+  <si>
+    <t>Q31</t>
+  </si>
+  <si>
+    <t>Q33</t>
+  </si>
+  <si>
+    <t>Q32</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>G21</t>
+  </si>
+  <si>
+    <t>2A3</t>
+  </si>
+  <si>
+    <t>2B3</t>
+  </si>
+  <si>
+    <t>2B0</t>
+  </si>
+  <si>
+    <t>1A1</t>
+  </si>
+  <si>
+    <t>1B0</t>
+  </si>
+  <si>
+    <t>1A0</t>
+  </si>
+  <si>
+    <t>1B2</t>
+  </si>
+  <si>
+    <t>1A2</t>
+  </si>
+  <si>
+    <t>3B3,Q23</t>
   </si>
 </sst>
 </file>
@@ -2864,7 +2978,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>765844</xdr:colOff>
+      <xdr:colOff>765845</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>21981</xdr:rowOff>
     </xdr:to>
@@ -3633,7 +3747,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="23" t="s">
@@ -3740,7 +3854,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H11" s="17"/>
       <c r="I11" s="17" t="s">
@@ -4958,7 +5072,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:AD35"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4999,10 +5113,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="104" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="105" t="s">
         <v>464</v>
-      </c>
-      <c r="C1" s="105" t="s">
-        <v>465</v>
       </c>
       <c r="D1" s="106" t="s">
         <v>16</v>
@@ -5014,7 +5128,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="109" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H1" s="110" t="s">
         <v>18</v>
@@ -5035,12 +5149,12 @@
         <v>20</v>
       </c>
       <c r="N1" s="116" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O1" s="105"/>
       <c r="P1" s="105"/>
       <c r="Q1" s="116" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="R1" s="115" t="s">
         <v>20</v>
@@ -5061,7 +5175,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="117" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Y1" s="108" t="s">
         <v>24</v>
@@ -5073,10 +5187,10 @@
         <v>16</v>
       </c>
       <c r="AB1" s="105" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AC1" s="104" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AD1" s="104" t="s">
         <v>22</v>
@@ -5084,10 +5198,10 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="118" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C2" s="118"/>
       <c r="D2" s="119"/>
@@ -5098,14 +5212,14 @@
       <c r="J2" s="118"/>
       <c r="K2" s="118"/>
       <c r="L2" s="161" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M2" s="161"/>
       <c r="N2" s="161"/>
       <c r="O2" s="121"/>
       <c r="P2" s="121"/>
       <c r="Q2" s="160" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="R2" s="160"/>
       <c r="S2" s="160"/>
@@ -5119,7 +5233,7 @@
       <c r="AA2" s="122"/>
       <c r="AB2" s="118"/>
       <c r="AC2" s="118" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AD2" s="118"/>
     </row>
@@ -5139,23 +5253,25 @@
       </c>
       <c r="H3" s="118"/>
       <c r="I3" s="123" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J3" s="124" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K3" s="125" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L3" s="118"/>
-      <c r="M3" s="118"/>
+      <c r="M3" s="129" t="s">
+        <v>471</v>
+      </c>
       <c r="N3" s="126">
         <v>0</v>
       </c>
       <c r="O3" s="121"/>
       <c r="P3" s="121"/>
       <c r="Q3" s="160" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R3" s="160"/>
       <c r="S3" s="160"/>
@@ -5169,10 +5285,10 @@
       <c r="AA3" s="122"/>
       <c r="AB3" s="118"/>
       <c r="AC3" s="118" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AD3" s="118" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -5191,23 +5307,25 @@
       </c>
       <c r="H4" s="118"/>
       <c r="I4" s="123" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J4" s="124" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K4" s="125" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L4" s="118"/>
-      <c r="M4" s="118"/>
+      <c r="M4" s="129" t="s">
+        <v>471</v>
+      </c>
       <c r="N4" s="126">
         <v>1</v>
       </c>
       <c r="O4" s="121"/>
       <c r="P4" s="121"/>
       <c r="Q4" s="160" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="R4" s="160"/>
       <c r="S4" s="160"/>
@@ -5221,7 +5339,7 @@
       <c r="AA4" s="122"/>
       <c r="AB4" s="118"/>
       <c r="AC4" s="118" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AD4" s="118">
         <v>3.3</v>
@@ -5230,7 +5348,7 @@
     <row r="5" spans="1:30">
       <c r="A5" s="118"/>
       <c r="B5" s="118" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C5" s="118" t="s">
         <v>46</v>
@@ -5239,7 +5357,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="127" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F5" s="128" t="s">
         <v>51</v>
@@ -5253,7 +5371,7 @@
       <c r="K5" s="118"/>
       <c r="L5" s="118"/>
       <c r="M5" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N5" s="126">
         <v>2</v>
@@ -5264,15 +5382,15 @@
         <v>23</v>
       </c>
       <c r="R5" s="129" t="s">
+        <v>471</v>
+      </c>
+      <c r="S5" s="131" t="s">
         <v>472</v>
-      </c>
-      <c r="S5" s="131" t="s">
-        <v>473</v>
       </c>
       <c r="T5" s="118"/>
       <c r="U5" s="118"/>
       <c r="V5" s="123" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="W5" s="118"/>
       <c r="X5" s="118"/>
@@ -5280,22 +5398,22 @@
         <v>210</v>
       </c>
       <c r="Z5" s="132" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AA5" s="122">
         <v>1.25</v>
       </c>
       <c r="AB5" s="118" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AC5" s="118"/>
       <c r="AD5" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="118" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B6" s="118"/>
       <c r="C6" s="118" t="s">
@@ -5305,7 +5423,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="132" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F6" s="128" t="s">
         <v>58</v>
@@ -5319,7 +5437,7 @@
       <c r="K6" s="118"/>
       <c r="L6" s="118"/>
       <c r="M6" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N6" s="126">
         <v>3</v>
@@ -5330,15 +5448,15 @@
         <v>22</v>
       </c>
       <c r="R6" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S6" s="131" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T6" s="118"/>
       <c r="U6" s="118"/>
       <c r="V6" s="123" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="W6" s="118"/>
       <c r="X6" s="118"/>
@@ -5357,7 +5475,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B7" s="118"/>
       <c r="C7" s="118" t="s">
@@ -5367,7 +5485,7 @@
         <v>61</v>
       </c>
       <c r="E7" s="132" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F7" s="128" t="s">
         <v>65</v>
@@ -5381,7 +5499,7 @@
       <c r="K7" s="118"/>
       <c r="L7" s="118"/>
       <c r="M7" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N7" s="126">
         <v>4</v>
@@ -5393,10 +5511,10 @@
       </c>
       <c r="R7" s="135"/>
       <c r="S7" s="131" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="T7" s="125" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="U7" s="118"/>
       <c r="V7" s="118"/>
@@ -5406,7 +5524,7 @@
         <v>0.13263888888888889</v>
       </c>
       <c r="Z7" s="127" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AA7" s="122">
         <v>1.27</v>
@@ -5416,15 +5534,15 @@
       </c>
       <c r="AC7" s="118"/>
       <c r="AD7" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B8" s="118" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C8" s="118" t="s">
         <v>269</v>
@@ -5433,7 +5551,7 @@
         <v>270</v>
       </c>
       <c r="E8" s="127" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F8" s="128" t="s">
         <v>273</v>
@@ -5447,7 +5565,7 @@
       <c r="K8" s="136"/>
       <c r="L8" s="118"/>
       <c r="M8" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N8" s="126">
         <v>5</v>
@@ -5459,10 +5577,10 @@
       </c>
       <c r="R8" s="135"/>
       <c r="S8" s="131" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="T8" s="137" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="U8" s="118"/>
       <c r="V8" s="118"/>
@@ -5472,7 +5590,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="Z8" s="127" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AA8" s="122">
         <v>1.26</v>
@@ -5482,13 +5600,13 @@
       </c>
       <c r="AC8" s="118"/>
       <c r="AD8" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="118"/>
       <c r="B9" s="118" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C9" s="118" t="s">
         <v>88</v>
@@ -5497,7 +5615,7 @@
         <v>89</v>
       </c>
       <c r="E9" s="127" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F9" s="128" t="s">
         <v>93</v>
@@ -5509,7 +5627,7 @@
       <c r="K9" s="118"/>
       <c r="L9" s="118"/>
       <c r="M9" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N9" s="126">
         <v>6</v>
@@ -5520,18 +5638,18 @@
         <v>19</v>
       </c>
       <c r="R9" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S9" s="131" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="T9" s="137" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="U9" s="118"/>
       <c r="V9" s="118"/>
       <c r="W9" s="138" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="X9" s="118"/>
       <c r="Y9" s="134">
@@ -5545,16 +5663,16 @@
         <v>175</v>
       </c>
       <c r="AC9" s="118" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AD9" s="118" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="118"/>
       <c r="B10" s="118" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C10" s="118" t="s">
         <v>74</v>
@@ -5563,7 +5681,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="127" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F10" s="128" t="s">
         <v>317</v>
@@ -5575,11 +5693,11 @@
       <c r="I10" s="118"/>
       <c r="J10" s="118"/>
       <c r="K10" s="125" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L10" s="118"/>
       <c r="M10" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N10" s="126">
         <v>7</v>
@@ -5590,16 +5708,16 @@
         <v>18</v>
       </c>
       <c r="R10" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S10" s="131" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="T10" s="118"/>
       <c r="U10" s="118"/>
       <c r="V10" s="118"/>
       <c r="W10" s="138" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="X10" s="118"/>
       <c r="Y10" s="134">
@@ -5613,10 +5731,10 @@
         <v>166</v>
       </c>
       <c r="AC10" s="118" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AD10" s="118" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -5629,7 +5747,7 @@
         <v>82</v>
       </c>
       <c r="E11" s="127" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F11" s="128" t="s">
         <v>316</v>
@@ -5638,16 +5756,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="138" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I11" s="118"/>
       <c r="J11" s="118"/>
       <c r="K11" s="125" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L11" s="118"/>
       <c r="M11" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N11" s="126">
         <v>8</v>
@@ -5659,15 +5777,15 @@
       </c>
       <c r="R11" s="135"/>
       <c r="S11" s="131" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="T11" s="137" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="U11" s="118"/>
       <c r="V11" s="118"/>
       <c r="W11" s="138" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="X11" s="118"/>
       <c r="Y11" s="134">
@@ -5693,7 +5811,7 @@
         <v>96</v>
       </c>
       <c r="E12" s="132" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F12" s="128" t="s">
         <v>100</v>
@@ -5705,7 +5823,7 @@
       <c r="K12" s="136"/>
       <c r="L12" s="118"/>
       <c r="M12" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N12" s="126">
         <v>9</v>
@@ -5717,15 +5835,15 @@
       </c>
       <c r="R12" s="135"/>
       <c r="S12" s="131" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="T12" s="137" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="U12" s="118"/>
       <c r="V12" s="118"/>
       <c r="W12" s="138" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="X12" s="118"/>
       <c r="Y12" s="134">
@@ -5743,7 +5861,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="118" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B13" s="118"/>
       <c r="C13" s="118" t="s">
@@ -5753,7 +5871,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="127" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F13" s="128" t="s">
         <v>107</v>
@@ -5762,12 +5880,12 @@
       <c r="H13" s="118"/>
       <c r="I13" s="118"/>
       <c r="J13" s="124" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K13" s="136"/>
       <c r="L13" s="118"/>
       <c r="M13" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N13" s="126">
         <v>10</v>
@@ -5778,13 +5896,13 @@
         <v>15</v>
       </c>
       <c r="R13" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S13" s="131" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T13" s="137" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="U13" s="118"/>
       <c r="V13" s="118"/>
@@ -5794,7 +5912,7 @@
         <v>0.12708333333333333</v>
       </c>
       <c r="Z13" s="139" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AA13" s="122">
         <v>1.19</v>
@@ -5804,15 +5922,15 @@
       </c>
       <c r="AC13" s="118"/>
       <c r="AD13" s="118" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="118" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B14" s="118" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C14" s="118" t="s">
         <v>109</v>
@@ -5827,15 +5945,15 @@
       <c r="G14" s="118"/>
       <c r="H14" s="118"/>
       <c r="I14" s="123" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J14" s="124" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K14" s="118"/>
       <c r="L14" s="118"/>
       <c r="M14" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N14" s="126">
         <v>11</v>
@@ -5846,13 +5964,13 @@
         <v>14</v>
       </c>
       <c r="R14" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S14" s="131" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="T14" s="137" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="U14" s="118"/>
       <c r="V14" s="118"/>
@@ -5862,7 +5980,7 @@
         <v>0.12638888888888888</v>
       </c>
       <c r="Z14" s="127" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AA14" s="122">
         <v>1.18</v>
@@ -5875,10 +5993,10 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="118" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B15" s="118" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C15" s="118" t="s">
         <v>116</v>
@@ -5887,7 +6005,7 @@
         <v>117</v>
       </c>
       <c r="E15" s="127" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F15" s="128" t="s">
         <v>121</v>
@@ -5896,12 +6014,12 @@
       <c r="H15" s="118"/>
       <c r="I15" s="118"/>
       <c r="J15" s="124" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K15" s="118"/>
       <c r="L15" s="118"/>
       <c r="M15" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N15" s="126">
         <v>12</v>
@@ -5912,17 +6030,17 @@
         <v>13</v>
       </c>
       <c r="R15" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S15" s="140" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="T15" s="118"/>
       <c r="U15" s="124" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V15" s="123" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="W15" s="118"/>
       <c r="X15" s="118"/>
@@ -5937,10 +6055,10 @@
         <v>123</v>
       </c>
       <c r="AC15" s="118" t="s">
+        <v>536</v>
+      </c>
+      <c r="AD15" s="118" t="s">
         <v>537</v>
-      </c>
-      <c r="AD15" s="118" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -5987,7 +6105,7 @@
       <c r="I17" s="122"/>
       <c r="J17" s="122"/>
       <c r="K17" s="159" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L17" s="122"/>
       <c r="M17" s="122"/>
@@ -6022,18 +6140,18 @@
       <c r="F18" s="118"/>
       <c r="G18" s="118"/>
       <c r="H18" s="138" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I18" s="118"/>
       <c r="J18" s="118"/>
       <c r="K18" s="137" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L18" s="131" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M18" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N18" s="126">
         <v>24</v>
@@ -6044,18 +6162,18 @@
         <v>25</v>
       </c>
       <c r="R18" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S18" s="131" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="T18" s="137" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="U18" s="122"/>
       <c r="V18" s="122"/>
       <c r="W18" s="138" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="X18" s="122"/>
       <c r="Y18" s="122"/>
@@ -6086,11 +6204,11 @@
       <c r="H19" s="118"/>
       <c r="I19" s="118"/>
       <c r="J19" s="124" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K19" s="135"/>
       <c r="L19" s="131" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M19" s="118"/>
       <c r="N19" s="126">
@@ -6103,11 +6221,11 @@
       </c>
       <c r="R19" s="141"/>
       <c r="S19" s="131" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="T19" s="118"/>
       <c r="U19" s="124" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="V19" s="118"/>
       <c r="W19" s="118"/>
@@ -6141,11 +6259,11 @@
       <c r="I20" s="118"/>
       <c r="J20" s="118"/>
       <c r="K20" s="137" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L20" s="118"/>
       <c r="M20" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N20" s="126">
         <v>28</v>
@@ -6156,11 +6274,11 @@
         <v>29</v>
       </c>
       <c r="R20" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S20" s="142"/>
       <c r="T20" s="137" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="U20" s="118"/>
       <c r="V20" s="118"/>
@@ -6193,7 +6311,7 @@
       </c>
       <c r="H21" s="118"/>
       <c r="I21" s="143" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J21" s="118"/>
       <c r="K21" s="118"/>
@@ -6212,7 +6330,7 @@
       <c r="T21" s="118"/>
       <c r="U21" s="142"/>
       <c r="V21" s="123" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="W21" s="118"/>
       <c r="X21" s="120">
@@ -6239,7 +6357,7 @@
         <v>264</v>
       </c>
       <c r="E22" s="127" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F22" s="134">
         <v>9.1666666666666674E-2</v>
@@ -6262,13 +6380,13 @@
         <v>33</v>
       </c>
       <c r="R22" s="129" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="S22" s="118"/>
       <c r="T22" s="118"/>
       <c r="U22" s="118"/>
       <c r="V22" s="143" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="W22" s="118"/>
       <c r="X22" s="120">
@@ -6278,7 +6396,7 @@
         <v>72</v>
       </c>
       <c r="Z22" s="127" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AA22" s="122">
         <v>4.7</v>
@@ -6364,7 +6482,7 @@
       <c r="I25" s="142"/>
       <c r="J25" s="142"/>
       <c r="K25" s="159" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L25" s="2"/>
       <c r="N25" s="142"/>
@@ -6436,21 +6554,21 @@
       <c r="H27" s="142"/>
       <c r="I27" s="142"/>
       <c r="J27" s="148" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K27" s="142"/>
       <c r="L27" s="142"/>
       <c r="M27" s="149" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N27" s="150">
         <v>34</v>
       </c>
       <c r="O27" s="151" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="P27" s="142" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="Q27" s="151"/>
       <c r="R27" s="151"/>
@@ -6486,23 +6604,23 @@
       <c r="H28" s="142"/>
       <c r="I28" s="142"/>
       <c r="J28" s="148" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K28" s="152" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L28" s="142"/>
       <c r="M28" s="149" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N28" s="150">
         <v>35</v>
       </c>
       <c r="O28" s="142" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P28" s="142" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Q28" s="151"/>
       <c r="R28" s="151"/>
@@ -6532,15 +6650,15 @@
       <c r="J29" s="151"/>
       <c r="K29" s="151"/>
       <c r="L29" s="161" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M29" s="161"/>
       <c r="N29" s="161"/>
       <c r="O29" s="151" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="P29" s="151" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Q29" s="151"/>
       <c r="R29" s="151"/>
@@ -6576,21 +6694,21 @@
       <c r="H30" s="151"/>
       <c r="I30" s="151"/>
       <c r="J30" s="155" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="K30" s="151"/>
       <c r="L30" s="151"/>
       <c r="M30" s="156" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N30" s="150">
         <v>36</v>
       </c>
       <c r="O30" s="151" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="P30" s="142" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="Q30" s="135"/>
       <c r="R30" s="135"/>
@@ -6611,7 +6729,7 @@
       <c r="A31" s="135"/>
       <c r="B31" s="135"/>
       <c r="L31" s="160" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="M31" s="160"/>
       <c r="N31" s="160"/>
@@ -6651,12 +6769,12 @@
       <c r="H32" s="135"/>
       <c r="I32" s="135"/>
       <c r="J32" s="155" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K32" s="135"/>
       <c r="L32" s="135"/>
       <c r="M32" s="149" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N32" s="150">
         <v>37</v>
@@ -6698,11 +6816,11 @@
       <c r="I33" s="135"/>
       <c r="J33" s="135"/>
       <c r="K33" s="152" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="L33" s="135"/>
       <c r="M33" s="149" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N33" s="150">
         <v>38</v>
@@ -6744,11 +6862,11 @@
       <c r="I34" s="135"/>
       <c r="J34" s="135"/>
       <c r="K34" s="152" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L34" s="135"/>
       <c r="M34" s="149" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="N34" s="150">
         <v>39</v>
@@ -7187,7 +7305,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>92</v>
@@ -7286,7 +7404,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>431</v>
+        <v>592</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>99</v>
@@ -7561,7 +7679,7 @@
         <v>358</v>
       </c>
       <c r="M18" s="37" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -7602,7 +7720,7 @@
         <v>359</v>
       </c>
       <c r="M19" s="37" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -7795,7 +7913,7 @@
         <v>364</v>
       </c>
       <c r="M24" s="37" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -7836,7 +7954,7 @@
         <v>365</v>
       </c>
       <c r="M25" s="37" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -8339,7 +8457,7 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>378</v>
@@ -8362,7 +8480,7 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>379</v>
@@ -8385,27 +8503,27 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>380</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>401</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M43" s="37" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>381</v>
@@ -8420,20 +8538,20 @@
         <v>400</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="M44" s="37" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45" s="5" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46" s="3" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>299</v>
@@ -8459,7 +8577,7 @@
     </row>
     <row r="47" spans="1:13">
       <c r="A47" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>298</v>
@@ -8485,7 +8603,7 @@
     </row>
     <row r="48" spans="1:13">
       <c r="A48" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>297</v>
@@ -8511,7 +8629,7 @@
     </row>
     <row r="49" spans="1:13">
       <c r="A49" s="3" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>296</v>
@@ -8537,7 +8655,7 @@
     </row>
     <row r="50" spans="1:13">
       <c r="A50" s="3" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>301</v>
@@ -8549,7 +8667,7 @@
         <v>335</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>321</v>
@@ -8563,7 +8681,7 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="3" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>300</v>
@@ -8575,7 +8693,7 @@
         <v>334</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>320</v>
@@ -8594,7 +8712,7 @@
     </row>
     <row r="53" spans="1:13">
       <c r="A53" s="3" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>253</v>
@@ -8606,7 +8724,7 @@
         <v>420</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>256</v>
@@ -8614,7 +8732,7 @@
     </row>
     <row r="54" spans="1:13">
       <c r="A54" s="3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>410</v>
@@ -8626,7 +8744,7 @@
         <v>422</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>320</v>
@@ -8637,7 +8755,7 @@
     </row>
     <row r="55" spans="1:13">
       <c r="A55" s="3" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>411</v>
@@ -8649,7 +8767,7 @@
         <v>421</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G55" s="3" t="s">
         <v>321</v>
@@ -8660,7 +8778,7 @@
     </row>
     <row r="56" spans="1:13">
       <c r="A56" s="3" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>407</v>
@@ -8672,15 +8790,15 @@
         <v>369</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="57" spans="1:13">
       <c r="A57" s="3" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>409</v>
@@ -8692,7 +8810,7 @@
         <v>424</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>319</v>
@@ -8703,7 +8821,7 @@
     </row>
     <row r="58" spans="1:13">
       <c r="A58" s="3" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>408</v>
@@ -8715,7 +8833,7 @@
         <v>423</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G58" s="3" t="s">
         <v>318</v>
@@ -8723,7 +8841,7 @@
     </row>
     <row r="59" spans="1:13">
       <c r="A59" s="3" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>412</v>
@@ -8735,7 +8853,7 @@
         <v>425</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G59" s="3" t="s">
         <v>430</v>
@@ -8761,9 +8879,9 @@
   </sheetPr>
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O27" sqref="O27"/>
+      <selection pane="bottomLeft" activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8780,11 +8898,11 @@
     <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
     <col min="17" max="17" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -8804,10 +8922,10 @@
         <v>22</v>
       </c>
       <c r="B1" s="38" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="39" t="s">
         <v>464</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>465</v>
       </c>
       <c r="D1" s="98" t="s">
         <v>16</v>
@@ -8819,7 +8937,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="68" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>18</v>
@@ -8840,12 +8958,12 @@
         <v>20</v>
       </c>
       <c r="N1" s="46" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="O1" s="39"/>
       <c r="P1" s="39"/>
       <c r="Q1" s="46" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="R1" s="45" t="s">
         <v>20</v>
@@ -8866,7 +8984,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="69" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="Y1" s="40" t="s">
         <v>24</v>
@@ -8878,10 +8996,10 @@
         <v>16</v>
       </c>
       <c r="AB1" s="39" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AC1" s="38" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AD1" s="38" t="s">
         <v>22</v>
@@ -8889,10 +9007,10 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="47" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="103"/>
@@ -8903,14 +9021,14 @@
       <c r="J2" s="47"/>
       <c r="K2" s="47"/>
       <c r="L2" s="162" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M2" s="162"/>
       <c r="N2" s="162"/>
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
       <c r="Q2" s="163" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="R2" s="163"/>
       <c r="S2" s="163"/>
@@ -8924,7 +9042,7 @@
       <c r="AA2" s="99"/>
       <c r="AB2" s="47"/>
       <c r="AC2" s="47" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AD2" s="47"/>
     </row>
@@ -8944,23 +9062,25 @@
       </c>
       <c r="H3" s="47"/>
       <c r="I3" s="64" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="K3" s="50" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
+      <c r="M3" s="129" t="s">
+        <v>593</v>
+      </c>
       <c r="N3" s="51">
         <v>0</v>
       </c>
       <c r="O3" s="48"/>
       <c r="P3" s="48"/>
       <c r="Q3" s="163" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R3" s="163"/>
       <c r="S3" s="163"/>
@@ -8974,10 +9094,10 @@
       <c r="AA3" s="99"/>
       <c r="AB3" s="47"/>
       <c r="AC3" s="47" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AD3" s="47" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -8996,23 +9116,25 @@
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="64" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K4" s="50" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
+      <c r="M4" s="129" t="s">
+        <v>594</v>
+      </c>
       <c r="N4" s="51">
         <v>1</v>
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="48"/>
       <c r="Q4" s="163" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="R4" s="163"/>
       <c r="S4" s="163"/>
@@ -9026,7 +9148,7 @@
       <c r="AA4" s="99"/>
       <c r="AB4" s="47"/>
       <c r="AC4" s="47" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AD4" s="47">
         <v>3.3</v>
@@ -9035,7 +9157,7 @@
     <row r="5" spans="1:30">
       <c r="A5" s="47"/>
       <c r="B5" s="47" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>46</v>
@@ -9044,7 +9166,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F5" s="62" t="s">
         <v>51</v>
@@ -9058,7 +9180,7 @@
       <c r="K5" s="47"/>
       <c r="L5" s="47"/>
       <c r="M5" s="52" t="s">
-        <v>472</v>
+        <v>595</v>
       </c>
       <c r="N5" s="51">
         <v>2</v>
@@ -9069,15 +9191,15 @@
         <v>23</v>
       </c>
       <c r="R5" s="52" t="s">
+        <v>613</v>
+      </c>
+      <c r="S5" s="54" t="s">
         <v>472</v>
-      </c>
-      <c r="S5" s="54" t="s">
-        <v>473</v>
       </c>
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
       <c r="V5" s="64" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="W5" s="47"/>
       <c r="X5" s="47"/>
@@ -9085,22 +9207,22 @@
         <v>210</v>
       </c>
       <c r="Z5" s="72" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AA5" s="99">
         <v>1.25</v>
       </c>
       <c r="AB5" s="47" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="AC5" s="47"/>
       <c r="AD5" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="47" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B6" s="47"/>
       <c r="C6" s="47" t="s">
@@ -9110,7 +9232,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F6" s="62" t="s">
         <v>58</v>
@@ -9124,7 +9246,7 @@
       <c r="K6" s="47"/>
       <c r="L6" s="47"/>
       <c r="M6" s="52" t="s">
-        <v>472</v>
+        <v>596</v>
       </c>
       <c r="N6" s="51">
         <v>3</v>
@@ -9135,15 +9257,15 @@
         <v>22</v>
       </c>
       <c r="R6" s="52" t="s">
-        <v>472</v>
+        <v>614</v>
       </c>
       <c r="S6" s="54" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T6" s="47"/>
       <c r="U6" s="47"/>
       <c r="V6" s="64" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="W6" s="47"/>
       <c r="X6" s="47"/>
@@ -9162,7 +9284,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="47" t="s">
@@ -9172,7 +9294,7 @@
         <v>61</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F7" s="62" t="s">
         <v>65</v>
@@ -9186,7 +9308,7 @@
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
       <c r="M7" s="52" t="s">
-        <v>472</v>
+        <v>597</v>
       </c>
       <c r="N7" s="51">
         <v>4</v>
@@ -9197,10 +9319,10 @@
         <v>21</v>
       </c>
       <c r="S7" s="54" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="T7" s="50" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="U7" s="47"/>
       <c r="V7" s="47"/>
@@ -9210,7 +9332,7 @@
         <v>0.13263888888888889</v>
       </c>
       <c r="Z7" s="70" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AA7" s="99">
         <v>1.27</v>
@@ -9220,15 +9342,15 @@
       </c>
       <c r="AC7" s="47"/>
       <c r="AD7" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>269</v>
@@ -9237,7 +9359,7 @@
         <v>270</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F8" s="62" t="s">
         <v>273</v>
@@ -9251,7 +9373,7 @@
       <c r="K8" s="57"/>
       <c r="L8" s="47"/>
       <c r="M8" s="52" t="s">
-        <v>472</v>
+        <v>598</v>
       </c>
       <c r="N8" s="51">
         <v>5</v>
@@ -9262,10 +9384,10 @@
         <v>20</v>
       </c>
       <c r="S8" s="54" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="T8" s="58" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="U8" s="47"/>
       <c r="V8" s="47"/>
@@ -9275,7 +9397,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="Z8" s="70" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AA8" s="99">
         <v>1.26</v>
@@ -9285,13 +9407,13 @@
       </c>
       <c r="AC8" s="47"/>
       <c r="AD8" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="47"/>
       <c r="B9" s="47" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C9" s="47" t="s">
         <v>88</v>
@@ -9300,7 +9422,7 @@
         <v>89</v>
       </c>
       <c r="E9" s="70" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F9" s="62" t="s">
         <v>93</v>
@@ -9312,7 +9434,7 @@
       <c r="K9" s="47"/>
       <c r="L9" s="47"/>
       <c r="M9" s="52" t="s">
-        <v>472</v>
+        <v>599</v>
       </c>
       <c r="N9" s="51">
         <v>6</v>
@@ -9323,18 +9445,18 @@
         <v>19</v>
       </c>
       <c r="R9" s="52" t="s">
-        <v>472</v>
+        <v>616</v>
       </c>
       <c r="S9" s="54" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="U9" s="47"/>
       <c r="V9" s="47"/>
       <c r="W9" s="66" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="X9" s="47"/>
       <c r="Y9" s="63">
@@ -9348,16 +9470,16 @@
         <v>175</v>
       </c>
       <c r="AC9" s="47" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AD9" s="47" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="47"/>
       <c r="B10" s="47" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>74</v>
@@ -9366,7 +9488,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F10" s="62" t="s">
         <v>317</v>
@@ -9378,11 +9500,11 @@
       <c r="I10" s="47"/>
       <c r="J10" s="47"/>
       <c r="K10" s="50" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="L10" s="47"/>
       <c r="M10" s="52" t="s">
-        <v>472</v>
+        <v>600</v>
       </c>
       <c r="N10" s="51">
         <v>7</v>
@@ -9393,16 +9515,16 @@
         <v>18</v>
       </c>
       <c r="R10" s="52" t="s">
-        <v>472</v>
+        <v>617</v>
       </c>
       <c r="S10" s="54" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
       <c r="V10" s="47"/>
       <c r="W10" s="66" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="X10" s="47"/>
       <c r="Y10" s="63">
@@ -9416,10 +9538,10 @@
         <v>166</v>
       </c>
       <c r="AC10" s="47" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="AD10" s="47" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -9432,7 +9554,7 @@
         <v>82</v>
       </c>
       <c r="E11" s="70" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F11" s="62" t="s">
         <v>316</v>
@@ -9441,16 +9563,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="66" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="50" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="L11" s="47"/>
       <c r="M11" s="52" t="s">
-        <v>472</v>
+        <v>601</v>
       </c>
       <c r="N11" s="51">
         <v>8</v>
@@ -9461,15 +9583,15 @@
         <v>17</v>
       </c>
       <c r="S11" s="54" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="T11" s="58" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="U11" s="47"/>
       <c r="V11" s="47"/>
       <c r="W11" s="66" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="X11" s="47"/>
       <c r="Y11" s="63">
@@ -9495,7 +9617,7 @@
         <v>96</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F12" s="62" t="s">
         <v>100</v>
@@ -9507,7 +9629,7 @@
       <c r="K12" s="57"/>
       <c r="L12" s="47"/>
       <c r="M12" s="52" t="s">
-        <v>472</v>
+        <v>602</v>
       </c>
       <c r="N12" s="51">
         <v>9</v>
@@ -9518,15 +9640,15 @@
         <v>16</v>
       </c>
       <c r="S12" s="54" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="T12" s="58" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="U12" s="47"/>
       <c r="V12" s="47"/>
       <c r="W12" s="66" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="X12" s="47"/>
       <c r="Y12" s="63">
@@ -9544,7 +9666,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="47" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47" t="s">
@@ -9554,7 +9676,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="70" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F13" s="62" t="s">
         <v>107</v>
@@ -9563,12 +9685,12 @@
       <c r="H13" s="47"/>
       <c r="I13" s="47"/>
       <c r="J13" s="49" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K13" s="57"/>
       <c r="L13" s="47"/>
       <c r="M13" s="52" t="s">
-        <v>472</v>
+        <v>603</v>
       </c>
       <c r="N13" s="51">
         <v>10</v>
@@ -9579,13 +9701,13 @@
         <v>15</v>
       </c>
       <c r="R13" s="52" t="s">
-        <v>472</v>
+        <v>618</v>
       </c>
       <c r="S13" s="54" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T13" s="58" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="U13" s="47"/>
       <c r="V13" s="47"/>
@@ -9595,7 +9717,7 @@
         <v>0.12708333333333333</v>
       </c>
       <c r="Z13" s="55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="AA13" s="99">
         <v>1.19</v>
@@ -9605,15 +9727,15 @@
       </c>
       <c r="AC13" s="47"/>
       <c r="AD13" s="47" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>109</v>
@@ -9628,15 +9750,15 @@
       <c r="G14" s="47"/>
       <c r="H14" s="47"/>
       <c r="I14" s="64" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J14" s="49" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K14" s="47"/>
       <c r="L14" s="47"/>
       <c r="M14" s="52" t="s">
-        <v>472</v>
+        <v>604</v>
       </c>
       <c r="N14" s="51">
         <v>11</v>
@@ -9647,13 +9769,13 @@
         <v>14</v>
       </c>
       <c r="R14" s="52" t="s">
-        <v>472</v>
+        <v>619</v>
       </c>
       <c r="S14" s="54" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="T14" s="58" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="U14" s="47"/>
       <c r="V14" s="47"/>
@@ -9663,7 +9785,7 @@
         <v>0.12638888888888888</v>
       </c>
       <c r="Z14" s="70" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AA14" s="99">
         <v>1.18</v>
@@ -9676,10 +9798,10 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>116</v>
@@ -9688,7 +9810,7 @@
         <v>117</v>
       </c>
       <c r="E15" s="70" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F15" s="62" t="s">
         <v>121</v>
@@ -9697,12 +9819,12 @@
       <c r="H15" s="47"/>
       <c r="I15" s="47"/>
       <c r="J15" s="49" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K15" s="47"/>
       <c r="L15" s="47"/>
       <c r="M15" s="52" t="s">
-        <v>472</v>
+        <v>605</v>
       </c>
       <c r="N15" s="51">
         <v>12</v>
@@ -9713,17 +9835,17 @@
         <v>13</v>
       </c>
       <c r="R15" s="52" t="s">
-        <v>472</v>
+        <v>620</v>
       </c>
       <c r="S15" s="97" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="T15" s="47"/>
       <c r="U15" s="49" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="V15" s="64" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="W15" s="47"/>
       <c r="X15" s="47"/>
@@ -9738,10 +9860,10 @@
         <v>123</v>
       </c>
       <c r="AC15" s="47" t="s">
+        <v>536</v>
+      </c>
+      <c r="AD15" s="47" t="s">
         <v>537</v>
-      </c>
-      <c r="AD15" s="47" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -9757,14 +9879,14 @@
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
       <c r="L16" s="162" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M16" s="162"/>
       <c r="N16" s="162"/>
       <c r="O16" s="48"/>
       <c r="P16" s="48"/>
       <c r="Q16" s="163" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R16" s="163"/>
       <c r="S16" s="163"/>
@@ -9793,18 +9915,18 @@
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="66" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="58" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L17" s="54" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M17" s="52" t="s">
-        <v>472</v>
+        <v>607</v>
       </c>
       <c r="N17" s="51">
         <v>24</v>
@@ -9814,11 +9936,11 @@
       <c r="Q17" s="59">
         <v>41</v>
       </c>
-      <c r="R17" s="52" t="s">
-        <v>472</v>
+      <c r="R17" s="60" t="s">
+        <v>621</v>
       </c>
       <c r="S17" s="54" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="T17" s="47"/>
       <c r="U17" s="47"/>
@@ -9833,7 +9955,7 @@
         <v>1.21</v>
       </c>
       <c r="AB17" s="47" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AC17" s="47"/>
       <c r="AD17" s="47"/>
@@ -9851,18 +9973,18 @@
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
       <c r="H18" s="66" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I18" s="47"/>
       <c r="J18" s="47"/>
       <c r="K18" s="58" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L18" s="54" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M18" s="52" t="s">
-        <v>472</v>
+        <v>606</v>
       </c>
       <c r="N18" s="51">
         <v>25</v>
@@ -9874,7 +9996,7 @@
       </c>
       <c r="R18" s="60"/>
       <c r="S18" s="54" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T18" s="47"/>
       <c r="U18" s="47"/>
@@ -9886,10 +10008,10 @@
       </c>
       <c r="Z18" s="47"/>
       <c r="AA18" s="99" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="AB18" s="47" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AC18" s="47"/>
       <c r="AD18" s="47"/>
@@ -9911,10 +10033,10 @@
       <c r="H19" s="47"/>
       <c r="I19" s="47"/>
       <c r="J19" s="49" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="L19" s="54" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M19" s="47"/>
       <c r="N19" s="51">
@@ -9927,11 +10049,11 @@
       </c>
       <c r="R19" s="60"/>
       <c r="S19" s="54" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="T19" s="47"/>
       <c r="U19" s="74" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="V19" s="47"/>
       <c r="W19" s="47"/>
@@ -9944,7 +10066,7 @@
         <v>1.29</v>
       </c>
       <c r="AB19" s="47" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AC19" s="47"/>
       <c r="AD19" s="47"/>
@@ -9966,11 +10088,11 @@
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
       <c r="J20" s="49" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="K20" s="47"/>
       <c r="L20" s="54" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="M20" s="47"/>
       <c r="N20" s="51">
@@ -9983,11 +10105,11 @@
       </c>
       <c r="R20" s="60"/>
       <c r="S20" s="54" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="T20" s="47"/>
       <c r="U20" s="74" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="V20" s="47"/>
       <c r="W20" s="47"/>
@@ -9999,7 +10121,7 @@
         <v>1.28</v>
       </c>
       <c r="AB20" s="47" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AC20" s="47"/>
       <c r="AD20" s="47"/>
@@ -10020,11 +10142,11 @@
       <c r="I21" s="47"/>
       <c r="J21" s="47"/>
       <c r="K21" s="58" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L21" s="47"/>
       <c r="M21" s="52" t="s">
-        <v>472</v>
+        <v>608</v>
       </c>
       <c r="N21" s="51">
         <v>28</v>
@@ -10035,12 +10157,12 @@
         <v>37</v>
       </c>
       <c r="R21" s="52" t="s">
-        <v>472</v>
+        <v>623</v>
       </c>
       <c r="S21" s="47"/>
       <c r="T21" s="47"/>
       <c r="U21" s="73" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="47"/>
@@ -10055,7 +10177,7 @@
         <v>2.19</v>
       </c>
       <c r="AB21" s="47" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AC21" s="47"/>
       <c r="AD21" s="47"/>
@@ -10076,11 +10198,11 @@
       <c r="I22" s="47"/>
       <c r="J22" s="47"/>
       <c r="K22" s="58" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="L22" s="47"/>
       <c r="M22" s="52" t="s">
-        <v>472</v>
+        <v>610</v>
       </c>
       <c r="N22" s="51">
         <v>29</v>
@@ -10091,12 +10213,12 @@
         <v>36</v>
       </c>
       <c r="R22" s="52" t="s">
-        <v>472</v>
+        <v>622</v>
       </c>
       <c r="S22" s="47"/>
       <c r="T22" s="47"/>
       <c r="U22" s="73" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="V22" s="47"/>
       <c r="W22" s="47"/>
@@ -10111,7 +10233,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="AB22" s="47" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AC22" s="47"/>
       <c r="AD22" s="47"/>
@@ -10132,12 +10254,14 @@
       </c>
       <c r="H23" s="47"/>
       <c r="I23" s="56" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="J23" s="47"/>
       <c r="K23" s="47"/>
       <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
+      <c r="M23" s="47" t="s">
+        <v>611</v>
+      </c>
       <c r="N23" s="51">
         <v>30</v>
       </c>
@@ -10146,12 +10270,10 @@
       <c r="Q23" s="53">
         <v>35</v>
       </c>
-      <c r="R23" s="52" t="s">
-        <v>472</v>
-      </c>
+      <c r="R23" s="60"/>
       <c r="S23" s="47"/>
       <c r="T23" s="50" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="U23" s="47"/>
       <c r="V23" s="47"/>
@@ -10165,7 +10287,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="AB23" s="47" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AC23" s="47"/>
       <c r="AD23" s="47"/>
@@ -10186,12 +10308,14 @@
       </c>
       <c r="H24" s="47"/>
       <c r="I24" s="64" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J24" s="47"/>
       <c r="K24" s="47"/>
       <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
+      <c r="M24" s="47" t="s">
+        <v>612</v>
+      </c>
       <c r="N24" s="51">
         <v>31</v>
       </c>
@@ -10203,11 +10327,11 @@
       <c r="R24" s="60"/>
       <c r="S24" s="47"/>
       <c r="T24" s="50" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="U24" s="47"/>
       <c r="V24" s="56" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="W24" s="47"/>
       <c r="X24" s="47"/>
@@ -10219,7 +10343,7 @@
         <v>2.29</v>
       </c>
       <c r="AB24" s="47" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AC24" s="47"/>
       <c r="AD24" s="47"/>
@@ -10234,7 +10358,7 @@
         <v>264</v>
       </c>
       <c r="E25" s="70" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F25" s="63">
         <v>9.1666666666666674E-2</v>
@@ -10257,13 +10381,13 @@
         <v>33</v>
       </c>
       <c r="R25" s="52" t="s">
-        <v>472</v>
+        <v>624</v>
       </c>
       <c r="S25" s="47"/>
       <c r="T25" s="47"/>
       <c r="U25" s="47"/>
       <c r="V25" s="56" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="W25" s="47"/>
       <c r="X25" s="67">
@@ -10273,7 +10397,7 @@
         <v>72</v>
       </c>
       <c r="Z25" s="70" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AA25" s="99">
         <v>4.7</v>
@@ -10332,7 +10456,7 @@
       <c r="M27" s="76"/>
       <c r="N27" s="76"/>
       <c r="O27" s="76" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="P27" s="76"/>
       <c r="Q27" s="76"/>
@@ -10369,31 +10493,31 @@
       <c r="H28" s="76"/>
       <c r="I28" s="76"/>
       <c r="J28" s="81" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K28" s="76"/>
       <c r="L28" s="76"/>
       <c r="M28" s="82" t="s">
-        <v>472</v>
+        <v>609</v>
       </c>
       <c r="N28" s="83">
         <v>42</v>
       </c>
       <c r="O28" s="84" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="P28" s="76" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="Q28" s="83">
         <v>47</v>
       </c>
       <c r="R28" s="82" t="s">
-        <v>472</v>
+        <v>629</v>
       </c>
       <c r="S28" s="76"/>
       <c r="T28" s="85" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="U28" s="76"/>
       <c r="V28" s="76"/>
@@ -10433,33 +10557,33 @@
       <c r="H29" s="76"/>
       <c r="I29" s="76"/>
       <c r="J29" s="81" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K29" s="85" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="L29" s="76"/>
       <c r="M29" s="82" t="s">
-        <v>472</v>
+        <v>625</v>
       </c>
       <c r="N29" s="83">
         <v>43</v>
       </c>
       <c r="O29" s="76" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="P29" s="76" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Q29" s="83">
         <v>46</v>
       </c>
       <c r="R29" s="82" t="s">
-        <v>472</v>
+        <v>628</v>
       </c>
       <c r="S29" s="76"/>
       <c r="T29" s="85" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="U29" s="76"/>
       <c r="V29" s="76"/>
@@ -10493,26 +10617,26 @@
       <c r="J30" s="84"/>
       <c r="K30" s="84"/>
       <c r="L30" s="162" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="M30" s="162"/>
       <c r="N30" s="162"/>
       <c r="O30" s="84" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="P30" s="84" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Q30" s="83">
         <v>45</v>
       </c>
       <c r="R30" s="82" t="s">
-        <v>472</v>
+        <v>627</v>
       </c>
       <c r="S30" s="84"/>
       <c r="T30" s="84"/>
       <c r="U30" s="87" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="V30" s="84"/>
       <c r="W30" s="84"/>
@@ -10551,24 +10675,24 @@
       <c r="H31" s="84"/>
       <c r="I31" s="84"/>
       <c r="J31" s="87" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="K31" s="84"/>
       <c r="L31" s="84"/>
       <c r="M31" s="90" t="s">
-        <v>472</v>
+        <v>626</v>
       </c>
       <c r="N31" s="83">
         <v>44</v>
       </c>
       <c r="O31" s="84" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="P31" s="76" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="Q31" s="162" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="R31" s="162"/>
       <c r="S31" s="162"/>
@@ -10632,7 +10756,7 @@
       <c r="M33" s="77"/>
       <c r="N33" s="77"/>
       <c r="O33" s="76" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="P33" s="77"/>
       <c r="Q33" s="77"/>
@@ -10668,11 +10792,11 @@
       <c r="I34" s="76"/>
       <c r="J34" s="76"/>
       <c r="K34" s="92" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L34" s="76"/>
       <c r="M34" s="52" t="s">
-        <v>472</v>
+        <v>609</v>
       </c>
       <c r="N34" s="93">
         <v>52</v>
@@ -10680,7 +10804,7 @@
       <c r="O34" s="76"/>
       <c r="P34" s="76"/>
       <c r="Q34" s="163" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R34" s="163"/>
       <c r="S34" s="163"/>
@@ -10712,11 +10836,11 @@
       <c r="I35" s="76"/>
       <c r="J35" s="76"/>
       <c r="K35" s="92" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L35" s="76"/>
       <c r="M35" s="52" t="s">
-        <v>472</v>
+        <v>625</v>
       </c>
       <c r="N35" s="93">
         <v>53</v>
@@ -10727,14 +10851,14 @@
         <v>50</v>
       </c>
       <c r="R35" s="52" t="s">
-        <v>472</v>
+        <v>628</v>
       </c>
       <c r="S35" s="76"/>
       <c r="T35" s="94" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="U35" s="95" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="V35" s="76"/>
       <c r="W35" s="76"/>
@@ -10769,12 +10893,12 @@
       <c r="H36" s="76"/>
       <c r="I36" s="76"/>
       <c r="J36" s="95" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K36" s="76"/>
       <c r="L36" s="76"/>
       <c r="M36" s="52" t="s">
-        <v>472</v>
+        <v>615</v>
       </c>
       <c r="N36" s="93">
         <v>54</v>
@@ -10784,12 +10908,12 @@
         <v>49</v>
       </c>
       <c r="R36" s="52" t="s">
-        <v>472</v>
+        <v>629</v>
       </c>
       <c r="S36" s="76"/>
       <c r="T36" s="76"/>
       <c r="U36" s="95" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="V36" s="76"/>
       <c r="W36" s="76"/>
@@ -10820,26 +10944,26 @@
       <c r="J37" s="76"/>
       <c r="K37" s="76"/>
       <c r="L37" s="162" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M37" s="162"/>
       <c r="N37" s="162"/>
       <c r="O37" s="76"/>
       <c r="P37" s="76" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="Q37" s="93">
         <v>51</v>
       </c>
       <c r="R37" s="52" t="s">
-        <v>472</v>
+        <v>630</v>
       </c>
       <c r="S37" s="76"/>
       <c r="T37" s="76"/>
       <c r="U37" s="76"/>
       <c r="V37" s="76"/>
       <c r="W37" s="96" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="X37" s="76"/>
       <c r="Y37" s="76"/>
@@ -10903,11 +11027,11 @@
       <c r="I39" s="76"/>
       <c r="J39" s="76"/>
       <c r="K39" s="92" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="L39" s="76"/>
       <c r="M39" s="52" t="s">
-        <v>472</v>
+        <v>609</v>
       </c>
       <c r="N39" s="93">
         <v>52</v>
@@ -10915,7 +11039,7 @@
       <c r="O39" s="76"/>
       <c r="P39" s="76"/>
       <c r="Q39" s="163" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="R39" s="163"/>
       <c r="S39" s="163"/>
@@ -10947,11 +11071,11 @@
       <c r="I40" s="76"/>
       <c r="J40" s="76"/>
       <c r="K40" s="92" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="L40" s="76"/>
       <c r="M40" s="52" t="s">
-        <v>472</v>
+        <v>625</v>
       </c>
       <c r="N40" s="93">
         <v>53</v>
@@ -10962,14 +11086,14 @@
         <v>50</v>
       </c>
       <c r="R40" s="52" t="s">
-        <v>472</v>
+        <v>628</v>
       </c>
       <c r="S40" s="76"/>
       <c r="T40" s="94" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="U40" s="95" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="V40" s="76"/>
       <c r="W40" s="76"/>
@@ -11004,12 +11128,12 @@
       <c r="H41" s="76"/>
       <c r="I41" s="76"/>
       <c r="J41" s="95" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K41" s="76"/>
       <c r="L41" s="76"/>
       <c r="M41" s="52" t="s">
-        <v>472</v>
+        <v>615</v>
       </c>
       <c r="N41" s="93">
         <v>54</v>
@@ -11020,12 +11144,12 @@
         <v>49</v>
       </c>
       <c r="R41" s="52" t="s">
-        <v>472</v>
+        <v>629</v>
       </c>
       <c r="S41" s="76"/>
       <c r="T41" s="76"/>
       <c r="U41" s="95" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="V41" s="76"/>
       <c r="W41" s="76"/>
@@ -11056,23 +11180,23 @@
       <c r="J42" s="76"/>
       <c r="K42" s="76"/>
       <c r="L42" s="162" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M42" s="162"/>
       <c r="N42" s="162"/>
       <c r="O42" s="76"/>
       <c r="P42" s="76" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="Q42" s="93">
         <v>48</v>
       </c>
       <c r="R42" s="52" t="s">
-        <v>472</v>
+        <v>626</v>
       </c>
       <c r="S42" s="76"/>
       <c r="T42" s="92" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="U42" s="76"/>
       <c r="V42" s="76"/>

</xml_diff>

<commit_message>
T4 PWM pins updated to same data as T4.1
Added the Timer info instead of just P not P...

Also updated PDF print outs for both
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94218B71-62EE-481B-99D4-D6660DCEBB96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7DBC01-141D-4042-AB3F-3F06F9088D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="480" windowWidth="23535" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="2880" yWindow="0" windowWidth="23655" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2599" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="630">
   <si>
     <t>Column1</t>
   </si>
@@ -1464,9 +1464,6 @@
   </si>
   <si>
     <t>3.3V 250mA max</t>
-  </si>
-  <si>
-    <t>P</t>
   </si>
   <si>
     <t>A9</t>
@@ -2319,7 +2316,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="164">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2635,14 +2632,12 @@
     <xf numFmtId="0" fontId="9" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="31" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2825,7 +2820,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>791025</xdr:colOff>
+      <xdr:colOff>791026</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2874,7 +2869,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>754672</xdr:colOff>
+      <xdr:colOff>754673</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>55762</xdr:rowOff>
     </xdr:to>
@@ -2924,7 +2919,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>681404</xdr:colOff>
+      <xdr:colOff>681405</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>132061</xdr:rowOff>
     </xdr:to>
@@ -5072,7 +5067,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M4" sqref="M4"/>
+      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5089,11 +5084,11 @@
     <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
     <col min="17" max="17" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -5128,7 +5123,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="109" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H1" s="110" t="s">
         <v>18</v>
@@ -5175,7 +5170,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="117" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="Y1" s="108" t="s">
         <v>24</v>
@@ -5198,7 +5193,7 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B2" s="118" t="s">
         <v>466</v>
@@ -5211,19 +5206,19 @@
       <c r="I2" s="118"/>
       <c r="J2" s="118"/>
       <c r="K2" s="118"/>
-      <c r="L2" s="161" t="s">
+      <c r="L2" s="159" t="s">
         <v>466</v>
       </c>
-      <c r="M2" s="161"/>
-      <c r="N2" s="161"/>
+      <c r="M2" s="159"/>
+      <c r="N2" s="159"/>
       <c r="O2" s="121"/>
       <c r="P2" s="121"/>
-      <c r="Q2" s="160" t="s">
+      <c r="Q2" s="158" t="s">
         <v>467</v>
       </c>
-      <c r="R2" s="160"/>
-      <c r="S2" s="160"/>
-      <c r="T2" s="160"/>
+      <c r="R2" s="158"/>
+      <c r="S2" s="158"/>
+      <c r="T2" s="158"/>
       <c r="U2" s="118"/>
       <c r="V2" s="118"/>
       <c r="W2" s="118"/>
@@ -5233,7 +5228,7 @@
       <c r="AA2" s="122"/>
       <c r="AB2" s="118"/>
       <c r="AC2" s="118" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AD2" s="118"/>
     </row>
@@ -5253,29 +5248,29 @@
       </c>
       <c r="H3" s="118"/>
       <c r="I3" s="123" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J3" s="124" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K3" s="125" t="s">
         <v>468</v>
       </c>
       <c r="L3" s="118"/>
       <c r="M3" s="129" t="s">
-        <v>471</v>
+        <v>592</v>
       </c>
       <c r="N3" s="126">
         <v>0</v>
       </c>
       <c r="O3" s="121"/>
       <c r="P3" s="121"/>
-      <c r="Q3" s="160" t="s">
+      <c r="Q3" s="158" t="s">
         <v>466</v>
       </c>
-      <c r="R3" s="160"/>
-      <c r="S3" s="160"/>
-      <c r="T3" s="160"/>
+      <c r="R3" s="158"/>
+      <c r="S3" s="158"/>
+      <c r="T3" s="158"/>
       <c r="U3" s="118"/>
       <c r="V3" s="118"/>
       <c r="W3" s="118"/>
@@ -5285,10 +5280,10 @@
       <c r="AA3" s="122"/>
       <c r="AB3" s="118"/>
       <c r="AC3" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AD3" s="118" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -5307,29 +5302,29 @@
       </c>
       <c r="H4" s="118"/>
       <c r="I4" s="123" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J4" s="124" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K4" s="125" t="s">
         <v>469</v>
       </c>
       <c r="L4" s="118"/>
       <c r="M4" s="129" t="s">
-        <v>471</v>
+        <v>593</v>
       </c>
       <c r="N4" s="126">
         <v>1</v>
       </c>
       <c r="O4" s="121"/>
       <c r="P4" s="121"/>
-      <c r="Q4" s="160" t="s">
+      <c r="Q4" s="158" t="s">
         <v>470</v>
       </c>
-      <c r="R4" s="160"/>
-      <c r="S4" s="160"/>
-      <c r="T4" s="160"/>
+      <c r="R4" s="158"/>
+      <c r="S4" s="158"/>
+      <c r="T4" s="158"/>
       <c r="U4" s="118"/>
       <c r="V4" s="118"/>
       <c r="W4" s="118"/>
@@ -5339,7 +5334,7 @@
       <c r="AA4" s="122"/>
       <c r="AB4" s="118"/>
       <c r="AC4" s="118" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AD4" s="118">
         <v>3.3</v>
@@ -5348,7 +5343,7 @@
     <row r="5" spans="1:30">
       <c r="A5" s="118"/>
       <c r="B5" s="118" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C5" s="118" t="s">
         <v>46</v>
@@ -5357,7 +5352,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="127" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F5" s="128" t="s">
         <v>51</v>
@@ -5370,8 +5365,8 @@
       <c r="J5" s="118"/>
       <c r="K5" s="118"/>
       <c r="L5" s="118"/>
-      <c r="M5" s="129" t="s">
-        <v>471</v>
+      <c r="M5" s="52" t="s">
+        <v>594</v>
       </c>
       <c r="N5" s="126">
         <v>2</v>
@@ -5381,11 +5376,11 @@
       <c r="Q5" s="130">
         <v>23</v>
       </c>
-      <c r="R5" s="129" t="s">
+      <c r="R5" s="52" t="s">
+        <v>612</v>
+      </c>
+      <c r="S5" s="131" t="s">
         <v>471</v>
-      </c>
-      <c r="S5" s="131" t="s">
-        <v>472</v>
       </c>
       <c r="T5" s="118"/>
       <c r="U5" s="118"/>
@@ -5398,22 +5393,22 @@
         <v>210</v>
       </c>
       <c r="Z5" s="132" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AA5" s="122">
         <v>1.25</v>
       </c>
       <c r="AB5" s="118" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AC5" s="118"/>
       <c r="AD5" s="118" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="118" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B6" s="118"/>
       <c r="C6" s="118" t="s">
@@ -5423,7 +5418,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="132" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F6" s="128" t="s">
         <v>58</v>
@@ -5436,8 +5431,8 @@
       <c r="J6" s="118"/>
       <c r="K6" s="118"/>
       <c r="L6" s="118"/>
-      <c r="M6" s="129" t="s">
-        <v>471</v>
+      <c r="M6" s="52" t="s">
+        <v>595</v>
       </c>
       <c r="N6" s="126">
         <v>3</v>
@@ -5447,11 +5442,11 @@
       <c r="Q6" s="130">
         <v>22</v>
       </c>
-      <c r="R6" s="129" t="s">
-        <v>471</v>
+      <c r="R6" s="52" t="s">
+        <v>613</v>
       </c>
       <c r="S6" s="131" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="T6" s="118"/>
       <c r="U6" s="118"/>
@@ -5475,7 +5470,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="118" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B7" s="118"/>
       <c r="C7" s="118" t="s">
@@ -5485,7 +5480,7 @@
         <v>61</v>
       </c>
       <c r="E7" s="132" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F7" s="128" t="s">
         <v>65</v>
@@ -5498,8 +5493,8 @@
       <c r="J7" s="118"/>
       <c r="K7" s="118"/>
       <c r="L7" s="118"/>
-      <c r="M7" s="129" t="s">
-        <v>471</v>
+      <c r="M7" s="52" t="s">
+        <v>596</v>
       </c>
       <c r="N7" s="126">
         <v>4</v>
@@ -5509,12 +5504,11 @@
       <c r="Q7" s="130">
         <v>21</v>
       </c>
-      <c r="R7" s="135"/>
       <c r="S7" s="131" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="T7" s="125" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="U7" s="118"/>
       <c r="V7" s="118"/>
@@ -5524,7 +5518,7 @@
         <v>0.13263888888888889</v>
       </c>
       <c r="Z7" s="127" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AA7" s="122">
         <v>1.27</v>
@@ -5534,15 +5528,15 @@
       </c>
       <c r="AC7" s="118"/>
       <c r="AD7" s="118" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="118" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B8" s="118" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C8" s="118" t="s">
         <v>269</v>
@@ -5551,7 +5545,7 @@
         <v>270</v>
       </c>
       <c r="E8" s="127" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F8" s="128" t="s">
         <v>273</v>
@@ -5564,8 +5558,8 @@
       <c r="J8" s="118"/>
       <c r="K8" s="136"/>
       <c r="L8" s="118"/>
-      <c r="M8" s="129" t="s">
-        <v>471</v>
+      <c r="M8" s="52" t="s">
+        <v>597</v>
       </c>
       <c r="N8" s="126">
         <v>5</v>
@@ -5575,12 +5569,11 @@
       <c r="Q8" s="130">
         <v>20</v>
       </c>
-      <c r="R8" s="135"/>
       <c r="S8" s="131" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="T8" s="137" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="U8" s="118"/>
       <c r="V8" s="118"/>
@@ -5590,7 +5583,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="Z8" s="127" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AA8" s="122">
         <v>1.26</v>
@@ -5600,13 +5593,13 @@
       </c>
       <c r="AC8" s="118"/>
       <c r="AD8" s="118" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="118"/>
       <c r="B9" s="118" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C9" s="118" t="s">
         <v>88</v>
@@ -5615,7 +5608,7 @@
         <v>89</v>
       </c>
       <c r="E9" s="127" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F9" s="128" t="s">
         <v>93</v>
@@ -5626,8 +5619,8 @@
       <c r="J9" s="118"/>
       <c r="K9" s="118"/>
       <c r="L9" s="118"/>
-      <c r="M9" s="129" t="s">
-        <v>471</v>
+      <c r="M9" s="52" t="s">
+        <v>598</v>
       </c>
       <c r="N9" s="126">
         <v>6</v>
@@ -5637,19 +5630,19 @@
       <c r="Q9" s="130">
         <v>19</v>
       </c>
-      <c r="R9" s="129" t="s">
-        <v>471</v>
+      <c r="R9" s="52" t="s">
+        <v>615</v>
       </c>
       <c r="S9" s="131" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="T9" s="137" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="U9" s="118"/>
       <c r="V9" s="118"/>
       <c r="W9" s="138" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="X9" s="118"/>
       <c r="Y9" s="134">
@@ -5663,16 +5656,16 @@
         <v>175</v>
       </c>
       <c r="AC9" s="118" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AD9" s="118" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="118"/>
       <c r="B10" s="118" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C10" s="118" t="s">
         <v>74</v>
@@ -5681,7 +5674,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="127" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F10" s="128" t="s">
         <v>317</v>
@@ -5693,11 +5686,11 @@
       <c r="I10" s="118"/>
       <c r="J10" s="118"/>
       <c r="K10" s="125" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="L10" s="118"/>
-      <c r="M10" s="129" t="s">
-        <v>471</v>
+      <c r="M10" s="52" t="s">
+        <v>599</v>
       </c>
       <c r="N10" s="126">
         <v>7</v>
@@ -5707,17 +5700,17 @@
       <c r="Q10" s="130">
         <v>18</v>
       </c>
-      <c r="R10" s="129" t="s">
-        <v>471</v>
+      <c r="R10" s="52" t="s">
+        <v>616</v>
       </c>
       <c r="S10" s="131" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="T10" s="118"/>
       <c r="U10" s="118"/>
       <c r="V10" s="118"/>
       <c r="W10" s="138" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="X10" s="118"/>
       <c r="Y10" s="134">
@@ -5731,10 +5724,10 @@
         <v>166</v>
       </c>
       <c r="AC10" s="118" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AD10" s="118" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -5747,7 +5740,7 @@
         <v>82</v>
       </c>
       <c r="E11" s="127" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F11" s="128" t="s">
         <v>316</v>
@@ -5756,16 +5749,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="138" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I11" s="118"/>
       <c r="J11" s="118"/>
       <c r="K11" s="125" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L11" s="118"/>
-      <c r="M11" s="129" t="s">
-        <v>471</v>
+      <c r="M11" s="52" t="s">
+        <v>600</v>
       </c>
       <c r="N11" s="126">
         <v>8</v>
@@ -5775,17 +5768,16 @@
       <c r="Q11" s="130">
         <v>17</v>
       </c>
-      <c r="R11" s="135"/>
       <c r="S11" s="131" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="T11" s="137" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U11" s="118"/>
       <c r="V11" s="118"/>
       <c r="W11" s="138" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="X11" s="118"/>
       <c r="Y11" s="134">
@@ -5811,7 +5803,7 @@
         <v>96</v>
       </c>
       <c r="E12" s="132" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F12" s="128" t="s">
         <v>100</v>
@@ -5822,8 +5814,8 @@
       <c r="J12" s="118"/>
       <c r="K12" s="136"/>
       <c r="L12" s="118"/>
-      <c r="M12" s="129" t="s">
-        <v>471</v>
+      <c r="M12" s="52" t="s">
+        <v>601</v>
       </c>
       <c r="N12" s="126">
         <v>9</v>
@@ -5833,17 +5825,16 @@
       <c r="Q12" s="130">
         <v>16</v>
       </c>
-      <c r="R12" s="135"/>
       <c r="S12" s="131" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="T12" s="137" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="U12" s="118"/>
       <c r="V12" s="118"/>
       <c r="W12" s="138" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="X12" s="118"/>
       <c r="Y12" s="134">
@@ -5861,7 +5852,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="118" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B13" s="118"/>
       <c r="C13" s="118" t="s">
@@ -5871,7 +5862,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="127" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F13" s="128" t="s">
         <v>107</v>
@@ -5880,12 +5871,12 @@
       <c r="H13" s="118"/>
       <c r="I13" s="118"/>
       <c r="J13" s="124" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K13" s="136"/>
       <c r="L13" s="118"/>
-      <c r="M13" s="129" t="s">
-        <v>471</v>
+      <c r="M13" s="52" t="s">
+        <v>602</v>
       </c>
       <c r="N13" s="126">
         <v>10</v>
@@ -5895,14 +5886,14 @@
       <c r="Q13" s="130">
         <v>15</v>
       </c>
-      <c r="R13" s="129" t="s">
-        <v>471</v>
+      <c r="R13" s="52" t="s">
+        <v>617</v>
       </c>
       <c r="S13" s="131" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="T13" s="137" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="U13" s="118"/>
       <c r="V13" s="118"/>
@@ -5912,7 +5903,7 @@
         <v>0.12708333333333333</v>
       </c>
       <c r="Z13" s="139" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AA13" s="122">
         <v>1.19</v>
@@ -5922,15 +5913,15 @@
       </c>
       <c r="AC13" s="118"/>
       <c r="AD13" s="118" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="118" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B14" s="118" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C14" s="118" t="s">
         <v>109</v>
@@ -5948,12 +5939,12 @@
         <v>469</v>
       </c>
       <c r="J14" s="124" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K14" s="118"/>
       <c r="L14" s="118"/>
-      <c r="M14" s="129" t="s">
-        <v>471</v>
+      <c r="M14" s="52" t="s">
+        <v>603</v>
       </c>
       <c r="N14" s="126">
         <v>11</v>
@@ -5963,14 +5954,14 @@
       <c r="Q14" s="130">
         <v>14</v>
       </c>
-      <c r="R14" s="129" t="s">
-        <v>471</v>
+      <c r="R14" s="52" t="s">
+        <v>618</v>
       </c>
       <c r="S14" s="131" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T14" s="137" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="U14" s="118"/>
       <c r="V14" s="118"/>
@@ -5980,7 +5971,7 @@
         <v>0.12638888888888888</v>
       </c>
       <c r="Z14" s="127" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AA14" s="122">
         <v>1.18</v>
@@ -5993,10 +5984,10 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="118" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B15" s="118" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C15" s="118" t="s">
         <v>116</v>
@@ -6005,7 +5996,7 @@
         <v>117</v>
       </c>
       <c r="E15" s="127" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F15" s="128" t="s">
         <v>121</v>
@@ -6014,12 +6005,12 @@
       <c r="H15" s="118"/>
       <c r="I15" s="118"/>
       <c r="J15" s="124" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K15" s="118"/>
       <c r="L15" s="118"/>
-      <c r="M15" s="129" t="s">
-        <v>471</v>
+      <c r="M15" s="52" t="s">
+        <v>604</v>
       </c>
       <c r="N15" s="126">
         <v>12</v>
@@ -6029,18 +6020,18 @@
       <c r="Q15" s="130">
         <v>13</v>
       </c>
-      <c r="R15" s="129" t="s">
-        <v>471</v>
+      <c r="R15" s="52" t="s">
+        <v>619</v>
       </c>
       <c r="S15" s="140" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="T15" s="118"/>
       <c r="U15" s="124" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="V15" s="123" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="W15" s="118"/>
       <c r="X15" s="118"/>
@@ -6055,10 +6046,10 @@
         <v>123</v>
       </c>
       <c r="AC15" s="118" t="s">
+        <v>535</v>
+      </c>
+      <c r="AD15" s="118" t="s">
         <v>536</v>
-      </c>
-      <c r="AD15" s="118" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -6104,8 +6095,8 @@
       <c r="H17" s="122"/>
       <c r="I17" s="122"/>
       <c r="J17" s="122"/>
-      <c r="K17" s="159" t="s">
-        <v>591</v>
+      <c r="K17" s="157" t="s">
+        <v>590</v>
       </c>
       <c r="L17" s="122"/>
       <c r="M17" s="122"/>
@@ -6140,18 +6131,18 @@
       <c r="F18" s="118"/>
       <c r="G18" s="118"/>
       <c r="H18" s="138" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I18" s="118"/>
       <c r="J18" s="118"/>
       <c r="K18" s="137" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L18" s="131" t="s">
-        <v>524</v>
-      </c>
-      <c r="M18" s="129" t="s">
-        <v>471</v>
+        <v>523</v>
+      </c>
+      <c r="M18" s="52" t="s">
+        <v>606</v>
       </c>
       <c r="N18" s="126">
         <v>24</v>
@@ -6161,19 +6152,19 @@
       <c r="Q18" s="126">
         <v>25</v>
       </c>
-      <c r="R18" s="129" t="s">
-        <v>471</v>
+      <c r="R18" s="52" t="s">
+        <v>605</v>
       </c>
       <c r="S18" s="131" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="T18" s="137" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="U18" s="122"/>
       <c r="V18" s="122"/>
       <c r="W18" s="138" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="X18" s="122"/>
       <c r="Y18" s="122"/>
@@ -6204,11 +6195,11 @@
       <c r="H19" s="118"/>
       <c r="I19" s="118"/>
       <c r="J19" s="124" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K19" s="135"/>
       <c r="L19" s="131" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M19" s="118"/>
       <c r="N19" s="126">
@@ -6221,11 +6212,11 @@
       </c>
       <c r="R19" s="141"/>
       <c r="S19" s="131" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="T19" s="118"/>
       <c r="U19" s="124" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="V19" s="118"/>
       <c r="W19" s="118"/>
@@ -6259,11 +6250,11 @@
       <c r="I20" s="118"/>
       <c r="J20" s="118"/>
       <c r="K20" s="137" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L20" s="118"/>
-      <c r="M20" s="129" t="s">
-        <v>471</v>
+      <c r="M20" s="52" t="s">
+        <v>607</v>
       </c>
       <c r="N20" s="126">
         <v>28</v>
@@ -6273,12 +6264,12 @@
       <c r="Q20" s="126">
         <v>29</v>
       </c>
-      <c r="R20" s="129" t="s">
-        <v>471</v>
+      <c r="R20" s="52" t="s">
+        <v>609</v>
       </c>
       <c r="S20" s="142"/>
       <c r="T20" s="137" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="U20" s="118"/>
       <c r="V20" s="118"/>
@@ -6311,12 +6302,14 @@
       </c>
       <c r="H21" s="118"/>
       <c r="I21" s="143" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J21" s="118"/>
       <c r="K21" s="118"/>
       <c r="L21" s="118"/>
-      <c r="M21" s="118"/>
+      <c r="M21" s="47" t="s">
+        <v>610</v>
+      </c>
       <c r="N21" s="126">
         <v>30</v>
       </c>
@@ -6325,12 +6318,14 @@
       <c r="Q21" s="126">
         <v>31</v>
       </c>
-      <c r="R21" s="141"/>
+      <c r="R21" s="47" t="s">
+        <v>611</v>
+      </c>
       <c r="S21" s="142"/>
       <c r="T21" s="118"/>
       <c r="U21" s="142"/>
       <c r="V21" s="123" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="W21" s="118"/>
       <c r="X21" s="120">
@@ -6357,7 +6352,7 @@
         <v>264</v>
       </c>
       <c r="E22" s="127" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F22" s="134">
         <v>9.1666666666666674E-2</v>
@@ -6379,8 +6374,8 @@
       <c r="Q22" s="130">
         <v>33</v>
       </c>
-      <c r="R22" s="129" t="s">
-        <v>471</v>
+      <c r="R22" s="52" t="s">
+        <v>623</v>
       </c>
       <c r="S22" s="118"/>
       <c r="T22" s="118"/>
@@ -6396,7 +6391,7 @@
         <v>72</v>
       </c>
       <c r="Z22" s="127" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AA22" s="122">
         <v>4.7</v>
@@ -6481,8 +6476,8 @@
       <c r="H25" s="142"/>
       <c r="I25" s="142"/>
       <c r="J25" s="142"/>
-      <c r="K25" s="159" t="s">
-        <v>590</v>
+      <c r="K25" s="157" t="s">
+        <v>589</v>
       </c>
       <c r="L25" s="2"/>
       <c r="N25" s="142"/>
@@ -6554,36 +6549,36 @@
       <c r="H27" s="142"/>
       <c r="I27" s="142"/>
       <c r="J27" s="148" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K27" s="142"/>
       <c r="L27" s="142"/>
-      <c r="M27" s="149" t="s">
-        <v>471</v>
-      </c>
-      <c r="N27" s="150">
+      <c r="M27" s="82" t="s">
+        <v>608</v>
+      </c>
+      <c r="N27" s="149">
         <v>34</v>
       </c>
-      <c r="O27" s="151" t="s">
-        <v>583</v>
+      <c r="O27" s="150" t="s">
+        <v>582</v>
       </c>
       <c r="P27" s="142" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q27" s="151"/>
-      <c r="R27" s="151"/>
+        <v>573</v>
+      </c>
+      <c r="Q27" s="150"/>
+      <c r="R27" s="150"/>
       <c r="S27" s="142"/>
-      <c r="T27" s="151"/>
+      <c r="T27" s="150"/>
       <c r="U27" s="142"/>
       <c r="V27" s="142"/>
       <c r="W27" s="142"/>
-      <c r="X27" s="151"/>
-      <c r="Y27" s="151"/>
+      <c r="X27" s="150"/>
+      <c r="Y27" s="150"/>
       <c r="Z27" s="142"/>
-      <c r="AA27" s="151"/>
-      <c r="AB27" s="151"/>
-      <c r="AC27" s="151"/>
-      <c r="AD27" s="151"/>
+      <c r="AA27" s="150"/>
+      <c r="AB27" s="150"/>
+      <c r="AC27" s="150"/>
+      <c r="AD27" s="150"/>
     </row>
     <row r="28" spans="1:30" s="75" customFormat="1" ht="11.25">
       <c r="A28" s="142"/>
@@ -6604,136 +6599,136 @@
       <c r="H28" s="142"/>
       <c r="I28" s="142"/>
       <c r="J28" s="148" t="s">
-        <v>578</v>
-      </c>
-      <c r="K28" s="152" t="s">
-        <v>576</v>
+        <v>577</v>
+      </c>
+      <c r="K28" s="151" t="s">
+        <v>575</v>
       </c>
       <c r="L28" s="142"/>
-      <c r="M28" s="149" t="s">
-        <v>471</v>
-      </c>
-      <c r="N28" s="150">
+      <c r="M28" s="82" t="s">
+        <v>624</v>
+      </c>
+      <c r="N28" s="149">
         <v>35</v>
       </c>
       <c r="O28" s="142" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="P28" s="142" t="s">
-        <v>584</v>
-      </c>
-      <c r="Q28" s="151"/>
-      <c r="R28" s="151"/>
+        <v>583</v>
+      </c>
+      <c r="Q28" s="150"/>
+      <c r="R28" s="150"/>
       <c r="S28" s="142"/>
-      <c r="T28" s="151"/>
+      <c r="T28" s="150"/>
       <c r="U28" s="142"/>
       <c r="V28" s="142"/>
       <c r="W28" s="142"/>
-      <c r="X28" s="151"/>
-      <c r="Y28" s="151"/>
+      <c r="X28" s="150"/>
+      <c r="Y28" s="150"/>
       <c r="Z28" s="142"/>
-      <c r="AA28" s="151"/>
-      <c r="AB28" s="151"/>
-      <c r="AC28" s="151"/>
-      <c r="AD28" s="151"/>
+      <c r="AA28" s="150"/>
+      <c r="AB28" s="150"/>
+      <c r="AC28" s="150"/>
+      <c r="AD28" s="150"/>
     </row>
     <row r="29" spans="1:30" s="75" customFormat="1" ht="11.25">
-      <c r="A29" s="151"/>
-      <c r="B29" s="151"/>
-      <c r="C29" s="151"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="151"/>
-      <c r="F29" s="151"/>
+      <c r="A29" s="150"/>
+      <c r="B29" s="150"/>
+      <c r="C29" s="150"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="150"/>
+      <c r="F29" s="150"/>
       <c r="G29" s="142"/>
-      <c r="H29" s="151"/>
-      <c r="I29" s="151"/>
-      <c r="J29" s="151"/>
-      <c r="K29" s="151"/>
-      <c r="L29" s="161" t="s">
+      <c r="H29" s="150"/>
+      <c r="I29" s="150"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="159" t="s">
         <v>466</v>
       </c>
-      <c r="M29" s="161"/>
-      <c r="N29" s="161"/>
-      <c r="O29" s="151" t="s">
-        <v>582</v>
-      </c>
-      <c r="P29" s="151" t="s">
-        <v>585</v>
-      </c>
-      <c r="Q29" s="151"/>
-      <c r="R29" s="151"/>
-      <c r="S29" s="151"/>
-      <c r="T29" s="151"/>
-      <c r="U29" s="151"/>
-      <c r="V29" s="151"/>
-      <c r="W29" s="151"/>
-      <c r="X29" s="151"/>
-      <c r="Y29" s="151"/>
-      <c r="Z29" s="151"/>
-      <c r="AA29" s="151"/>
-      <c r="AB29" s="151"/>
-      <c r="AC29" s="151"/>
-      <c r="AD29" s="151"/>
+      <c r="M29" s="159"/>
+      <c r="N29" s="159"/>
+      <c r="O29" s="150" t="s">
+        <v>581</v>
+      </c>
+      <c r="P29" s="150" t="s">
+        <v>584</v>
+      </c>
+      <c r="Q29" s="150"/>
+      <c r="R29" s="150"/>
+      <c r="S29" s="150"/>
+      <c r="T29" s="150"/>
+      <c r="U29" s="150"/>
+      <c r="V29" s="150"/>
+      <c r="W29" s="150"/>
+      <c r="X29" s="150"/>
+      <c r="Y29" s="150"/>
+      <c r="Z29" s="150"/>
+      <c r="AA29" s="150"/>
+      <c r="AB29" s="150"/>
+      <c r="AC29" s="150"/>
+      <c r="AD29" s="150"/>
     </row>
     <row r="30" spans="1:30" s="75" customFormat="1">
-      <c r="A30" s="151"/>
-      <c r="B30" s="151"/>
+      <c r="A30" s="150"/>
+      <c r="B30" s="150"/>
       <c r="C30" s="145" t="s">
         <v>297</v>
       </c>
-      <c r="D30" s="153">
+      <c r="D30" s="152">
         <v>3.13</v>
       </c>
-      <c r="E30" s="151"/>
-      <c r="F30" s="154" t="s">
+      <c r="E30" s="150"/>
+      <c r="F30" s="153" t="s">
         <v>292</v>
       </c>
       <c r="G30" s="147">
         <v>5</v>
       </c>
-      <c r="H30" s="151"/>
-      <c r="I30" s="151"/>
-      <c r="J30" s="155" t="s">
-        <v>579</v>
-      </c>
-      <c r="K30" s="151"/>
-      <c r="L30" s="151"/>
-      <c r="M30" s="156" t="s">
-        <v>471</v>
-      </c>
-      <c r="N30" s="150">
+      <c r="H30" s="150"/>
+      <c r="I30" s="150"/>
+      <c r="J30" s="154" t="s">
+        <v>578</v>
+      </c>
+      <c r="K30" s="150"/>
+      <c r="L30" s="150"/>
+      <c r="M30" s="90" t="s">
+        <v>625</v>
+      </c>
+      <c r="N30" s="149">
         <v>36</v>
       </c>
-      <c r="O30" s="151" t="s">
-        <v>581</v>
+      <c r="O30" s="150" t="s">
+        <v>580</v>
       </c>
       <c r="P30" s="142" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Q30" s="135"/>
       <c r="R30" s="135"/>
       <c r="S30" s="135"/>
-      <c r="T30" s="151"/>
-      <c r="U30" s="151"/>
-      <c r="V30" s="151"/>
-      <c r="W30" s="151"/>
-      <c r="X30" s="151"/>
-      <c r="Y30" s="151"/>
-      <c r="Z30" s="151"/>
-      <c r="AA30" s="153"/>
-      <c r="AB30" s="151"/>
-      <c r="AC30" s="151"/>
-      <c r="AD30" s="151"/>
+      <c r="T30" s="150"/>
+      <c r="U30" s="150"/>
+      <c r="V30" s="150"/>
+      <c r="W30" s="150"/>
+      <c r="X30" s="150"/>
+      <c r="Y30" s="150"/>
+      <c r="Z30" s="150"/>
+      <c r="AA30" s="152"/>
+      <c r="AB30" s="150"/>
+      <c r="AC30" s="150"/>
+      <c r="AD30" s="150"/>
     </row>
     <row r="31" spans="1:30">
       <c r="A31" s="135"/>
       <c r="B31" s="135"/>
-      <c r="L31" s="160" t="s">
+      <c r="L31" s="158" t="s">
         <v>470</v>
       </c>
-      <c r="M31" s="160"/>
-      <c r="N31" s="160"/>
-      <c r="O31" s="160"/>
+      <c r="M31" s="158"/>
+      <c r="N31" s="158"/>
+      <c r="O31" s="158"/>
       <c r="P31" s="135"/>
       <c r="Q31" s="135"/>
       <c r="R31" s="135"/>
@@ -6745,7 +6740,7 @@
       <c r="X31" s="135"/>
       <c r="Y31" s="135"/>
       <c r="Z31" s="135"/>
-      <c r="AA31" s="157"/>
+      <c r="AA31" s="155"/>
       <c r="AB31" s="135"/>
       <c r="AC31" s="135"/>
       <c r="AD31" s="135"/>
@@ -6756,27 +6751,27 @@
       <c r="C32" s="144" t="s">
         <v>296</v>
       </c>
-      <c r="D32" s="153">
+      <c r="D32" s="152">
         <v>3.12</v>
       </c>
       <c r="E32" s="135"/>
-      <c r="F32" s="154" t="s">
+      <c r="F32" s="153" t="s">
         <v>293</v>
       </c>
-      <c r="G32" s="158">
+      <c r="G32" s="156">
         <v>4</v>
       </c>
       <c r="H32" s="135"/>
       <c r="I32" s="135"/>
-      <c r="J32" s="155" t="s">
-        <v>580</v>
+      <c r="J32" s="154" t="s">
+        <v>579</v>
       </c>
       <c r="K32" s="135"/>
       <c r="L32" s="135"/>
-      <c r="M32" s="149" t="s">
-        <v>471</v>
-      </c>
-      <c r="N32" s="150">
+      <c r="M32" s="82" t="s">
+        <v>626</v>
+      </c>
+      <c r="N32" s="149">
         <v>37</v>
       </c>
       <c r="O32" s="135"/>
@@ -6791,7 +6786,7 @@
       <c r="X32" s="135"/>
       <c r="Y32" s="135"/>
       <c r="Z32" s="135"/>
-      <c r="AA32" s="157"/>
+      <c r="AA32" s="155"/>
       <c r="AB32" s="135"/>
       <c r="AC32" s="135"/>
       <c r="AD32" s="135"/>
@@ -6815,14 +6810,14 @@
       <c r="H33" s="135"/>
       <c r="I33" s="135"/>
       <c r="J33" s="135"/>
-      <c r="K33" s="152" t="s">
-        <v>501</v>
+      <c r="K33" s="151" t="s">
+        <v>500</v>
       </c>
       <c r="L33" s="135"/>
-      <c r="M33" s="149" t="s">
-        <v>471</v>
-      </c>
-      <c r="N33" s="150">
+      <c r="M33" s="82" t="s">
+        <v>627</v>
+      </c>
+      <c r="N33" s="149">
         <v>38</v>
       </c>
       <c r="O33" s="135"/>
@@ -6837,7 +6832,7 @@
       <c r="X33" s="135"/>
       <c r="Y33" s="135"/>
       <c r="Z33" s="135"/>
-      <c r="AA33" s="157"/>
+      <c r="AA33" s="155"/>
       <c r="AB33" s="135"/>
       <c r="AC33" s="135"/>
       <c r="AD33" s="135"/>
@@ -6861,14 +6856,14 @@
       <c r="H34" s="135"/>
       <c r="I34" s="135"/>
       <c r="J34" s="135"/>
-      <c r="K34" s="152" t="s">
-        <v>504</v>
+      <c r="K34" s="151" t="s">
+        <v>503</v>
       </c>
       <c r="L34" s="135"/>
-      <c r="M34" s="149" t="s">
-        <v>471</v>
-      </c>
-      <c r="N34" s="150">
+      <c r="M34" s="82" t="s">
+        <v>628</v>
+      </c>
+      <c r="N34" s="149">
         <v>39</v>
       </c>
       <c r="O34" s="135"/>
@@ -6883,7 +6878,7 @@
       <c r="X34" s="135"/>
       <c r="Y34" s="135"/>
       <c r="Z34" s="135"/>
-      <c r="AA34" s="157"/>
+      <c r="AA34" s="155"/>
       <c r="AB34" s="135"/>
       <c r="AC34" s="135"/>
       <c r="AD34" s="135"/>
@@ -6903,7 +6898,7 @@
       <c r="X35" s="135"/>
       <c r="Y35" s="135"/>
       <c r="Z35" s="135"/>
-      <c r="AA35" s="157"/>
+      <c r="AA35" s="155"/>
       <c r="AB35" s="135"/>
       <c r="AC35" s="135"/>
       <c r="AD35" s="135"/>
@@ -6912,7 +6907,7 @@
       <c r="A36" s="135"/>
       <c r="B36" s="135"/>
       <c r="C36" s="135"/>
-      <c r="D36" s="157"/>
+      <c r="D36" s="155"/>
       <c r="E36" s="135"/>
       <c r="F36" s="135"/>
       <c r="G36" s="135"/>
@@ -6935,7 +6930,7 @@
       <c r="X36" s="135"/>
       <c r="Y36" s="135"/>
       <c r="Z36" s="135"/>
-      <c r="AA36" s="157"/>
+      <c r="AA36" s="155"/>
       <c r="AB36" s="135"/>
       <c r="AC36" s="135"/>
       <c r="AD36" s="135"/>
@@ -6944,7 +6939,7 @@
       <c r="A37" s="135"/>
       <c r="B37" s="135"/>
       <c r="C37" s="135"/>
-      <c r="D37" s="157"/>
+      <c r="D37" s="155"/>
       <c r="E37" s="135"/>
       <c r="F37" s="135"/>
       <c r="G37" s="135"/>
@@ -6967,7 +6962,7 @@
       <c r="X37" s="135"/>
       <c r="Y37" s="135"/>
       <c r="Z37" s="135"/>
-      <c r="AA37" s="157"/>
+      <c r="AA37" s="155"/>
       <c r="AB37" s="135"/>
       <c r="AC37" s="135"/>
       <c r="AD37" s="135"/>
@@ -7404,7 +7399,7 @@
         <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>99</v>
@@ -8457,7 +8452,7 @@
     </row>
     <row r="41" spans="1:13">
       <c r="A41" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>378</v>
@@ -8480,7 +8475,7 @@
     </row>
     <row r="42" spans="1:13">
       <c r="A42" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>379</v>
@@ -8503,19 +8498,19 @@
     </row>
     <row r="43" spans="1:13">
       <c r="A43" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>380</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="K43" s="3" t="s">
         <v>401</v>
       </c>
       <c r="L43" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="M43" s="37" t="s">
         <v>448</v>
@@ -8523,7 +8518,7 @@
     </row>
     <row r="44" spans="1:13">
       <c r="A44" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>381</v>
@@ -8538,7 +8533,7 @@
         <v>400</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="M44" s="37" t="s">
         <v>449</v>
@@ -8881,7 +8876,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W28" sqref="W28"/>
+      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8937,7 +8932,7 @@
         <v>24</v>
       </c>
       <c r="G1" s="68" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="H1" s="65" t="s">
         <v>18</v>
@@ -8984,7 +8979,7 @@
         <v>18</v>
       </c>
       <c r="X1" s="69" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="Y1" s="40" t="s">
         <v>24</v>
@@ -9007,7 +9002,7 @@
     </row>
     <row r="2" spans="1:30">
       <c r="A2" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B2" s="47" t="s">
         <v>466</v>
@@ -9020,19 +9015,19 @@
       <c r="I2" s="47"/>
       <c r="J2" s="47"/>
       <c r="K2" s="47"/>
-      <c r="L2" s="162" t="s">
+      <c r="L2" s="160" t="s">
         <v>466</v>
       </c>
-      <c r="M2" s="162"/>
-      <c r="N2" s="162"/>
+      <c r="M2" s="160"/>
+      <c r="N2" s="160"/>
       <c r="O2" s="48"/>
       <c r="P2" s="48"/>
-      <c r="Q2" s="163" t="s">
+      <c r="Q2" s="161" t="s">
         <v>467</v>
       </c>
-      <c r="R2" s="163"/>
-      <c r="S2" s="163"/>
-      <c r="T2" s="163"/>
+      <c r="R2" s="161"/>
+      <c r="S2" s="161"/>
+      <c r="T2" s="161"/>
       <c r="U2" s="47"/>
       <c r="V2" s="47"/>
       <c r="W2" s="47"/>
@@ -9042,7 +9037,7 @@
       <c r="AA2" s="99"/>
       <c r="AB2" s="47"/>
       <c r="AC2" s="47" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="AD2" s="47"/>
     </row>
@@ -9062,29 +9057,29 @@
       </c>
       <c r="H3" s="47"/>
       <c r="I3" s="64" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J3" s="49" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="K3" s="50" t="s">
         <v>468</v>
       </c>
       <c r="L3" s="47"/>
       <c r="M3" s="129" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="N3" s="51">
         <v>0</v>
       </c>
       <c r="O3" s="48"/>
       <c r="P3" s="48"/>
-      <c r="Q3" s="163" t="s">
+      <c r="Q3" s="161" t="s">
         <v>466</v>
       </c>
-      <c r="R3" s="163"/>
-      <c r="S3" s="163"/>
-      <c r="T3" s="163"/>
+      <c r="R3" s="161"/>
+      <c r="S3" s="161"/>
+      <c r="T3" s="161"/>
       <c r="U3" s="47"/>
       <c r="V3" s="47"/>
       <c r="W3" s="47"/>
@@ -9094,10 +9089,10 @@
       <c r="AA3" s="99"/>
       <c r="AB3" s="47"/>
       <c r="AC3" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="AD3" s="47" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="4" spans="1:30">
@@ -9116,29 +9111,29 @@
       </c>
       <c r="H4" s="47"/>
       <c r="I4" s="64" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J4" s="49" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K4" s="50" t="s">
         <v>469</v>
       </c>
       <c r="L4" s="47"/>
       <c r="M4" s="129" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="N4" s="51">
         <v>1</v>
       </c>
       <c r="O4" s="48"/>
       <c r="P4" s="48"/>
-      <c r="Q4" s="163" t="s">
+      <c r="Q4" s="161" t="s">
         <v>470</v>
       </c>
-      <c r="R4" s="163"/>
-      <c r="S4" s="163"/>
-      <c r="T4" s="163"/>
+      <c r="R4" s="161"/>
+      <c r="S4" s="161"/>
+      <c r="T4" s="161"/>
       <c r="U4" s="47"/>
       <c r="V4" s="47"/>
       <c r="W4" s="47"/>
@@ -9148,7 +9143,7 @@
       <c r="AA4" s="99"/>
       <c r="AB4" s="47"/>
       <c r="AC4" s="47" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AD4" s="47">
         <v>3.3</v>
@@ -9157,7 +9152,7 @@
     <row r="5" spans="1:30">
       <c r="A5" s="47"/>
       <c r="B5" s="47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C5" s="47" t="s">
         <v>46</v>
@@ -9166,7 +9161,7 @@
         <v>47</v>
       </c>
       <c r="E5" s="70" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F5" s="62" t="s">
         <v>51</v>
@@ -9180,7 +9175,7 @@
       <c r="K5" s="47"/>
       <c r="L5" s="47"/>
       <c r="M5" s="52" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="N5" s="51">
         <v>2</v>
@@ -9191,10 +9186,10 @@
         <v>23</v>
       </c>
       <c r="R5" s="52" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="S5" s="54" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
@@ -9207,22 +9202,22 @@
         <v>210</v>
       </c>
       <c r="Z5" s="72" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="AA5" s="99">
         <v>1.25</v>
       </c>
       <c r="AB5" s="47" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="AC5" s="47"/>
       <c r="AD5" s="47" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="6" spans="1:30">
       <c r="A6" s="47" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B6" s="47"/>
       <c r="C6" s="47" t="s">
@@ -9232,7 +9227,7 @@
         <v>54</v>
       </c>
       <c r="E6" s="72" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F6" s="62" t="s">
         <v>58</v>
@@ -9246,7 +9241,7 @@
       <c r="K6" s="47"/>
       <c r="L6" s="47"/>
       <c r="M6" s="52" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="N6" s="51">
         <v>3</v>
@@ -9257,10 +9252,10 @@
         <v>22</v>
       </c>
       <c r="R6" s="52" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="S6" s="54" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="T6" s="47"/>
       <c r="U6" s="47"/>
@@ -9284,7 +9279,7 @@
     </row>
     <row r="7" spans="1:30">
       <c r="A7" s="47" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="47" t="s">
@@ -9294,7 +9289,7 @@
         <v>61</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F7" s="62" t="s">
         <v>65</v>
@@ -9308,7 +9303,7 @@
       <c r="K7" s="47"/>
       <c r="L7" s="47"/>
       <c r="M7" s="52" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="N7" s="51">
         <v>4</v>
@@ -9319,10 +9314,10 @@
         <v>21</v>
       </c>
       <c r="S7" s="54" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="T7" s="50" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="U7" s="47"/>
       <c r="V7" s="47"/>
@@ -9332,7 +9327,7 @@
         <v>0.13263888888888889</v>
       </c>
       <c r="Z7" s="70" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="AA7" s="99">
         <v>1.27</v>
@@ -9342,15 +9337,15 @@
       </c>
       <c r="AC7" s="47"/>
       <c r="AD7" s="47" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="47" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B8" s="47" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>269</v>
@@ -9359,7 +9354,7 @@
         <v>270</v>
       </c>
       <c r="E8" s="70" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F8" s="62" t="s">
         <v>273</v>
@@ -9373,7 +9368,7 @@
       <c r="K8" s="57"/>
       <c r="L8" s="47"/>
       <c r="M8" s="52" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="N8" s="51">
         <v>5</v>
@@ -9384,10 +9379,10 @@
         <v>20</v>
       </c>
       <c r="S8" s="54" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="T8" s="58" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="U8" s="47"/>
       <c r="V8" s="47"/>
@@ -9397,7 +9392,7 @@
         <v>0.13194444444444445</v>
       </c>
       <c r="Z8" s="70" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="AA8" s="99">
         <v>1.26</v>
@@ -9407,13 +9402,13 @@
       </c>
       <c r="AC8" s="47"/>
       <c r="AD8" s="47" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="47"/>
       <c r="B9" s="47" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C9" s="47" t="s">
         <v>88</v>
@@ -9422,7 +9417,7 @@
         <v>89</v>
       </c>
       <c r="E9" s="70" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F9" s="62" t="s">
         <v>93</v>
@@ -9434,7 +9429,7 @@
       <c r="K9" s="47"/>
       <c r="L9" s="47"/>
       <c r="M9" s="52" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="N9" s="51">
         <v>6</v>
@@ -9445,18 +9440,18 @@
         <v>19</v>
       </c>
       <c r="R9" s="52" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="S9" s="54" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="T9" s="58" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="U9" s="47"/>
       <c r="V9" s="47"/>
       <c r="W9" s="66" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="X9" s="47"/>
       <c r="Y9" s="63">
@@ -9470,16 +9465,16 @@
         <v>175</v>
       </c>
       <c r="AC9" s="47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AD9" s="47" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="47"/>
       <c r="B10" s="47" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C10" s="47" t="s">
         <v>74</v>
@@ -9488,7 +9483,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="70" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F10" s="62" t="s">
         <v>317</v>
@@ -9500,11 +9495,11 @@
       <c r="I10" s="47"/>
       <c r="J10" s="47"/>
       <c r="K10" s="50" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="L10" s="47"/>
       <c r="M10" s="52" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="N10" s="51">
         <v>7</v>
@@ -9515,16 +9510,16 @@
         <v>18</v>
       </c>
       <c r="R10" s="52" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="S10" s="54" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="T10" s="47"/>
       <c r="U10" s="47"/>
       <c r="V10" s="47"/>
       <c r="W10" s="66" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="X10" s="47"/>
       <c r="Y10" s="63">
@@ -9538,10 +9533,10 @@
         <v>166</v>
       </c>
       <c r="AC10" s="47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="AD10" s="47" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="11" spans="1:30">
@@ -9554,7 +9549,7 @@
         <v>82</v>
       </c>
       <c r="E11" s="70" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F11" s="62" t="s">
         <v>316</v>
@@ -9563,16 +9558,16 @@
         <v>14</v>
       </c>
       <c r="H11" s="66" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I11" s="47"/>
       <c r="J11" s="47"/>
       <c r="K11" s="50" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L11" s="47"/>
       <c r="M11" s="52" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="N11" s="51">
         <v>8</v>
@@ -9583,15 +9578,15 @@
         <v>17</v>
       </c>
       <c r="S11" s="54" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="T11" s="58" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="U11" s="47"/>
       <c r="V11" s="47"/>
       <c r="W11" s="66" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="X11" s="47"/>
       <c r="Y11" s="63">
@@ -9617,7 +9612,7 @@
         <v>96</v>
       </c>
       <c r="E12" s="72" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F12" s="62" t="s">
         <v>100</v>
@@ -9629,7 +9624,7 @@
       <c r="K12" s="57"/>
       <c r="L12" s="47"/>
       <c r="M12" s="52" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="N12" s="51">
         <v>9</v>
@@ -9640,15 +9635,15 @@
         <v>16</v>
       </c>
       <c r="S12" s="54" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="T12" s="58" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="U12" s="47"/>
       <c r="V12" s="47"/>
       <c r="W12" s="66" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="X12" s="47"/>
       <c r="Y12" s="63">
@@ -9666,7 +9661,7 @@
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="47" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B13" s="47"/>
       <c r="C13" s="47" t="s">
@@ -9676,7 +9671,7 @@
         <v>103</v>
       </c>
       <c r="E13" s="70" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F13" s="62" t="s">
         <v>107</v>
@@ -9685,12 +9680,12 @@
       <c r="H13" s="47"/>
       <c r="I13" s="47"/>
       <c r="J13" s="49" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K13" s="57"/>
       <c r="L13" s="47"/>
       <c r="M13" s="52" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="N13" s="51">
         <v>10</v>
@@ -9701,13 +9696,13 @@
         <v>15</v>
       </c>
       <c r="R13" s="52" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="S13" s="54" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="T13" s="58" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="U13" s="47"/>
       <c r="V13" s="47"/>
@@ -9717,7 +9712,7 @@
         <v>0.12708333333333333</v>
       </c>
       <c r="Z13" s="55" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AA13" s="99">
         <v>1.19</v>
@@ -9727,15 +9722,15 @@
       </c>
       <c r="AC13" s="47"/>
       <c r="AD13" s="47" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="14" spans="1:30">
       <c r="A14" s="47" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B14" s="47" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C14" s="47" t="s">
         <v>109</v>
@@ -9753,12 +9748,12 @@
         <v>469</v>
       </c>
       <c r="J14" s="49" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K14" s="47"/>
       <c r="L14" s="47"/>
       <c r="M14" s="52" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="N14" s="51">
         <v>11</v>
@@ -9769,13 +9764,13 @@
         <v>14</v>
       </c>
       <c r="R14" s="52" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="S14" s="54" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="T14" s="58" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="U14" s="47"/>
       <c r="V14" s="47"/>
@@ -9785,7 +9780,7 @@
         <v>0.12638888888888888</v>
       </c>
       <c r="Z14" s="70" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="AA14" s="99">
         <v>1.18</v>
@@ -9798,10 +9793,10 @@
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="47" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>116</v>
@@ -9810,7 +9805,7 @@
         <v>117</v>
       </c>
       <c r="E15" s="70" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F15" s="62" t="s">
         <v>121</v>
@@ -9819,12 +9814,12 @@
       <c r="H15" s="47"/>
       <c r="I15" s="47"/>
       <c r="J15" s="49" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K15" s="47"/>
       <c r="L15" s="47"/>
       <c r="M15" s="52" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N15" s="51">
         <v>12</v>
@@ -9835,17 +9830,17 @@
         <v>13</v>
       </c>
       <c r="R15" s="52" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="S15" s="97" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="T15" s="47"/>
       <c r="U15" s="49" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="V15" s="64" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="W15" s="47"/>
       <c r="X15" s="47"/>
@@ -9860,10 +9855,10 @@
         <v>123</v>
       </c>
       <c r="AC15" s="47" t="s">
+        <v>535</v>
+      </c>
+      <c r="AD15" s="47" t="s">
         <v>536</v>
-      </c>
-      <c r="AD15" s="47" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="16" spans="1:30">
@@ -9878,19 +9873,19 @@
       <c r="I16" s="47"/>
       <c r="J16" s="47"/>
       <c r="K16" s="47"/>
-      <c r="L16" s="162" t="s">
-        <v>494</v>
-      </c>
-      <c r="M16" s="162"/>
-      <c r="N16" s="162"/>
+      <c r="L16" s="160" t="s">
+        <v>493</v>
+      </c>
+      <c r="M16" s="160"/>
+      <c r="N16" s="160"/>
       <c r="O16" s="48"/>
       <c r="P16" s="48"/>
-      <c r="Q16" s="163" t="s">
+      <c r="Q16" s="161" t="s">
         <v>466</v>
       </c>
-      <c r="R16" s="163"/>
-      <c r="S16" s="163"/>
-      <c r="T16" s="163"/>
+      <c r="R16" s="161"/>
+      <c r="S16" s="161"/>
+      <c r="T16" s="161"/>
       <c r="U16" s="47"/>
       <c r="V16" s="47"/>
       <c r="W16" s="47"/>
@@ -9915,18 +9910,18 @@
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="66" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I17" s="47"/>
       <c r="J17" s="47"/>
       <c r="K17" s="58" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="L17" s="54" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="M17" s="52" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="N17" s="51">
         <v>24</v>
@@ -9937,10 +9932,10 @@
         <v>41</v>
       </c>
       <c r="R17" s="60" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="S17" s="54" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T17" s="47"/>
       <c r="U17" s="47"/>
@@ -9955,7 +9950,7 @@
         <v>1.21</v>
       </c>
       <c r="AB17" s="47" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="AC17" s="47"/>
       <c r="AD17" s="47"/>
@@ -9973,18 +9968,18 @@
       <c r="F18" s="47"/>
       <c r="G18" s="47"/>
       <c r="H18" s="66" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I18" s="47"/>
       <c r="J18" s="47"/>
       <c r="K18" s="58" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="L18" s="54" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M18" s="52" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="N18" s="51">
         <v>25</v>
@@ -9996,7 +9991,7 @@
       </c>
       <c r="R18" s="60"/>
       <c r="S18" s="54" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T18" s="47"/>
       <c r="U18" s="47"/>
@@ -10008,10 +10003,10 @@
       </c>
       <c r="Z18" s="47"/>
       <c r="AA18" s="99" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AB18" s="47" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="AC18" s="47"/>
       <c r="AD18" s="47"/>
@@ -10033,10 +10028,10 @@
       <c r="H19" s="47"/>
       <c r="I19" s="47"/>
       <c r="J19" s="49" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="L19" s="54" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M19" s="47"/>
       <c r="N19" s="51">
@@ -10049,11 +10044,11 @@
       </c>
       <c r="R19" s="60"/>
       <c r="S19" s="54" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="T19" s="47"/>
       <c r="U19" s="74" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="V19" s="47"/>
       <c r="W19" s="47"/>
@@ -10066,7 +10061,7 @@
         <v>1.29</v>
       </c>
       <c r="AB19" s="47" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="AC19" s="47"/>
       <c r="AD19" s="47"/>
@@ -10088,11 +10083,11 @@
       <c r="H20" s="47"/>
       <c r="I20" s="47"/>
       <c r="J20" s="49" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="K20" s="47"/>
       <c r="L20" s="54" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="M20" s="47"/>
       <c r="N20" s="51">
@@ -10105,11 +10100,11 @@
       </c>
       <c r="R20" s="60"/>
       <c r="S20" s="54" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="T20" s="47"/>
       <c r="U20" s="74" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="V20" s="47"/>
       <c r="W20" s="47"/>
@@ -10121,7 +10116,7 @@
         <v>1.28</v>
       </c>
       <c r="AB20" s="47" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="AC20" s="47"/>
       <c r="AD20" s="47"/>
@@ -10142,11 +10137,11 @@
       <c r="I21" s="47"/>
       <c r="J21" s="47"/>
       <c r="K21" s="58" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="L21" s="47"/>
       <c r="M21" s="52" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="N21" s="51">
         <v>28</v>
@@ -10157,12 +10152,12 @@
         <v>37</v>
       </c>
       <c r="R21" s="52" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="S21" s="47"/>
       <c r="T21" s="47"/>
       <c r="U21" s="73" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="V21" s="47"/>
       <c r="W21" s="47"/>
@@ -10177,7 +10172,7 @@
         <v>2.19</v>
       </c>
       <c r="AB21" s="47" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="AC21" s="47"/>
       <c r="AD21" s="47"/>
@@ -10198,11 +10193,11 @@
       <c r="I22" s="47"/>
       <c r="J22" s="47"/>
       <c r="K22" s="58" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L22" s="47"/>
       <c r="M22" s="52" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="N22" s="51">
         <v>29</v>
@@ -10213,12 +10208,12 @@
         <v>36</v>
       </c>
       <c r="R22" s="52" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="S22" s="47"/>
       <c r="T22" s="47"/>
       <c r="U22" s="73" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="V22" s="47"/>
       <c r="W22" s="47"/>
@@ -10233,7 +10228,7 @@
         <v>2.1800000000000002</v>
       </c>
       <c r="AB22" s="47" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="AC22" s="47"/>
       <c r="AD22" s="47"/>
@@ -10254,13 +10249,13 @@
       </c>
       <c r="H23" s="47"/>
       <c r="I23" s="56" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="J23" s="47"/>
       <c r="K23" s="47"/>
       <c r="L23" s="47"/>
       <c r="M23" s="47" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="N23" s="51">
         <v>30</v>
@@ -10273,7 +10268,7 @@
       <c r="R23" s="60"/>
       <c r="S23" s="47"/>
       <c r="T23" s="50" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="U23" s="47"/>
       <c r="V23" s="47"/>
@@ -10287,7 +10282,7 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="AB23" s="47" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="AC23" s="47"/>
       <c r="AD23" s="47"/>
@@ -10308,13 +10303,13 @@
       </c>
       <c r="H24" s="47"/>
       <c r="I24" s="64" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="J24" s="47"/>
       <c r="K24" s="47"/>
       <c r="L24" s="47"/>
       <c r="M24" s="47" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="N24" s="51">
         <v>31</v>
@@ -10327,7 +10322,7 @@
       <c r="R24" s="60"/>
       <c r="S24" s="47"/>
       <c r="T24" s="50" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="U24" s="47"/>
       <c r="V24" s="56" t="s">
@@ -10343,7 +10338,7 @@
         <v>2.29</v>
       </c>
       <c r="AB24" s="47" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="AC24" s="47"/>
       <c r="AD24" s="47"/>
@@ -10358,7 +10353,7 @@
         <v>264</v>
       </c>
       <c r="E25" s="70" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F25" s="63">
         <v>9.1666666666666674E-2</v>
@@ -10381,7 +10376,7 @@
         <v>33</v>
       </c>
       <c r="R25" s="52" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="S25" s="47"/>
       <c r="T25" s="47"/>
@@ -10397,7 +10392,7 @@
         <v>72</v>
       </c>
       <c r="Z25" s="70" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="AA25" s="99">
         <v>4.7</v>
@@ -10456,7 +10451,7 @@
       <c r="M27" s="76"/>
       <c r="N27" s="76"/>
       <c r="O27" s="76" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="P27" s="76"/>
       <c r="Q27" s="76"/>
@@ -10493,31 +10488,31 @@
       <c r="H28" s="76"/>
       <c r="I28" s="76"/>
       <c r="J28" s="81" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K28" s="76"/>
       <c r="L28" s="76"/>
       <c r="M28" s="82" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N28" s="83">
         <v>42</v>
       </c>
       <c r="O28" s="84" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="P28" s="76" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="Q28" s="83">
         <v>47</v>
       </c>
       <c r="R28" s="82" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="S28" s="76"/>
       <c r="T28" s="85" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="U28" s="76"/>
       <c r="V28" s="76"/>
@@ -10557,33 +10552,33 @@
       <c r="H29" s="76"/>
       <c r="I29" s="76"/>
       <c r="J29" s="81" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K29" s="85" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="L29" s="76"/>
       <c r="M29" s="82" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="N29" s="83">
         <v>43</v>
       </c>
       <c r="O29" s="76" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="P29" s="76" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="Q29" s="83">
         <v>46</v>
       </c>
       <c r="R29" s="82" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="S29" s="76"/>
       <c r="T29" s="85" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="U29" s="76"/>
       <c r="V29" s="76"/>
@@ -10616,27 +10611,27 @@
       <c r="I30" s="84"/>
       <c r="J30" s="84"/>
       <c r="K30" s="84"/>
-      <c r="L30" s="162" t="s">
+      <c r="L30" s="160" t="s">
         <v>466</v>
       </c>
-      <c r="M30" s="162"/>
-      <c r="N30" s="162"/>
+      <c r="M30" s="160"/>
+      <c r="N30" s="160"/>
       <c r="O30" s="84" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="P30" s="84" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Q30" s="83">
         <v>45</v>
       </c>
       <c r="R30" s="82" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="S30" s="84"/>
       <c r="T30" s="84"/>
       <c r="U30" s="87" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="V30" s="84"/>
       <c r="W30" s="84"/>
@@ -10675,27 +10670,27 @@
       <c r="H31" s="84"/>
       <c r="I31" s="84"/>
       <c r="J31" s="87" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K31" s="84"/>
       <c r="L31" s="84"/>
       <c r="M31" s="90" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="N31" s="83">
         <v>44</v>
       </c>
       <c r="O31" s="84" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="P31" s="76" t="s">
-        <v>586</v>
-      </c>
-      <c r="Q31" s="162" t="s">
-        <v>494</v>
-      </c>
-      <c r="R31" s="162"/>
-      <c r="S31" s="162"/>
+        <v>585</v>
+      </c>
+      <c r="Q31" s="160" t="s">
+        <v>493</v>
+      </c>
+      <c r="R31" s="160"/>
+      <c r="S31" s="160"/>
       <c r="T31" s="84"/>
       <c r="U31" s="84"/>
       <c r="V31" s="84"/>
@@ -10756,7 +10751,7 @@
       <c r="M33" s="77"/>
       <c r="N33" s="77"/>
       <c r="O33" s="76" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="P33" s="77"/>
       <c r="Q33" s="77"/>
@@ -10796,19 +10791,19 @@
       </c>
       <c r="L34" s="76"/>
       <c r="M34" s="52" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N34" s="93">
         <v>52</v>
       </c>
       <c r="O34" s="76"/>
       <c r="P34" s="76"/>
-      <c r="Q34" s="163" t="s">
+      <c r="Q34" s="161" t="s">
         <v>466</v>
       </c>
-      <c r="R34" s="163"/>
-      <c r="S34" s="163"/>
-      <c r="T34" s="163"/>
+      <c r="R34" s="161"/>
+      <c r="S34" s="161"/>
+      <c r="T34" s="161"/>
       <c r="U34" s="76"/>
       <c r="V34" s="76"/>
       <c r="W34" s="76"/>
@@ -10840,7 +10835,7 @@
       </c>
       <c r="L35" s="76"/>
       <c r="M35" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="N35" s="93">
         <v>53</v>
@@ -10851,14 +10846,14 @@
         <v>50</v>
       </c>
       <c r="R35" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="S35" s="76"/>
       <c r="T35" s="94" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="U35" s="95" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="V35" s="76"/>
       <c r="W35" s="76"/>
@@ -10893,12 +10888,12 @@
       <c r="H36" s="76"/>
       <c r="I36" s="76"/>
       <c r="J36" s="95" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K36" s="76"/>
       <c r="L36" s="76"/>
       <c r="M36" s="52" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="N36" s="93">
         <v>54</v>
@@ -10908,12 +10903,12 @@
         <v>49</v>
       </c>
       <c r="R36" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="S36" s="76"/>
       <c r="T36" s="76"/>
       <c r="U36" s="95" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="V36" s="76"/>
       <c r="W36" s="76"/>
@@ -10943,27 +10938,27 @@
       <c r="I37" s="76"/>
       <c r="J37" s="76"/>
       <c r="K37" s="76"/>
-      <c r="L37" s="162" t="s">
-        <v>494</v>
-      </c>
-      <c r="M37" s="162"/>
-      <c r="N37" s="162"/>
+      <c r="L37" s="160" t="s">
+        <v>493</v>
+      </c>
+      <c r="M37" s="160"/>
+      <c r="N37" s="160"/>
       <c r="O37" s="76"/>
       <c r="P37" s="76" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="Q37" s="93">
         <v>51</v>
       </c>
       <c r="R37" s="52" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="S37" s="76"/>
       <c r="T37" s="76"/>
       <c r="U37" s="76"/>
       <c r="V37" s="76"/>
       <c r="W37" s="96" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="X37" s="76"/>
       <c r="Y37" s="76"/>
@@ -11031,19 +11026,19 @@
       </c>
       <c r="L39" s="76"/>
       <c r="M39" s="52" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N39" s="93">
         <v>52</v>
       </c>
       <c r="O39" s="76"/>
       <c r="P39" s="76"/>
-      <c r="Q39" s="163" t="s">
+      <c r="Q39" s="161" t="s">
         <v>466</v>
       </c>
-      <c r="R39" s="163"/>
-      <c r="S39" s="163"/>
-      <c r="T39" s="163"/>
+      <c r="R39" s="161"/>
+      <c r="S39" s="161"/>
+      <c r="T39" s="161"/>
       <c r="U39" s="76"/>
       <c r="V39" s="76"/>
       <c r="W39" s="76"/>
@@ -11075,7 +11070,7 @@
       </c>
       <c r="L40" s="76"/>
       <c r="M40" s="52" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="N40" s="93">
         <v>53</v>
@@ -11086,14 +11081,14 @@
         <v>50</v>
       </c>
       <c r="R40" s="52" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="S40" s="76"/>
       <c r="T40" s="94" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="U40" s="95" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="V40" s="76"/>
       <c r="W40" s="76"/>
@@ -11128,12 +11123,12 @@
       <c r="H41" s="76"/>
       <c r="I41" s="76"/>
       <c r="J41" s="95" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K41" s="76"/>
       <c r="L41" s="76"/>
       <c r="M41" s="52" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="N41" s="93">
         <v>54</v>
@@ -11144,12 +11139,12 @@
         <v>49</v>
       </c>
       <c r="R41" s="52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="S41" s="76"/>
       <c r="T41" s="76"/>
       <c r="U41" s="95" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="V41" s="76"/>
       <c r="W41" s="76"/>
@@ -11179,24 +11174,24 @@
       <c r="I42" s="76"/>
       <c r="J42" s="76"/>
       <c r="K42" s="76"/>
-      <c r="L42" s="162" t="s">
-        <v>494</v>
-      </c>
-      <c r="M42" s="162"/>
-      <c r="N42" s="162"/>
+      <c r="L42" s="160" t="s">
+        <v>493</v>
+      </c>
+      <c r="M42" s="160"/>
+      <c r="N42" s="160"/>
       <c r="O42" s="76"/>
       <c r="P42" s="76" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="Q42" s="93">
         <v>48</v>
       </c>
       <c r="R42" s="52" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="S42" s="76"/>
       <c r="T42" s="92" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="U42" s="76"/>
       <c r="V42" s="76"/>

</xml_diff>

<commit_message>
SDCard pins can be used for Wire1
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7DBC01-141D-4042-AB3F-3F06F9088D41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B402A9-F177-4591-AC86-05D7A69C0A9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="0" windowWidth="23655" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="15555" yWindow="45" windowWidth="23655" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2587" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2591" uniqueCount="630">
   <si>
     <t>Column1</t>
   </si>
@@ -1947,7 +1947,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2029,6 +2029,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -2316,7 +2322,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2652,6 +2658,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3428,7 +3437,7 @@
   <dimension ref="A1:M44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5067,7 +5076,7 @@
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T21" sqref="T21"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6686,7 +6695,9 @@
       <c r="G30" s="147">
         <v>5</v>
       </c>
-      <c r="H30" s="150"/>
+      <c r="H30" s="162" t="s">
+        <v>495</v>
+      </c>
       <c r="I30" s="150"/>
       <c r="J30" s="154" t="s">
         <v>578</v>
@@ -6761,7 +6772,9 @@
       <c r="G32" s="156">
         <v>4</v>
       </c>
-      <c r="H32" s="135"/>
+      <c r="H32" s="162" t="s">
+        <v>497</v>
+      </c>
       <c r="I32" s="135"/>
       <c r="J32" s="154" t="s">
         <v>579</v>
@@ -6990,8 +7003,8 @@
   <dimension ref="A1:M59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8876,7 +8889,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomLeft" activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10634,7 +10647,9 @@
         <v>579</v>
       </c>
       <c r="V30" s="84"/>
-      <c r="W30" s="84"/>
+      <c r="W30" s="162" t="s">
+        <v>497</v>
+      </c>
       <c r="X30" s="88">
         <v>4</v>
       </c>
@@ -10667,7 +10682,9 @@
       <c r="G31" s="80">
         <v>5</v>
       </c>
-      <c r="H31" s="84"/>
+      <c r="H31" s="162" t="s">
+        <v>495</v>
+      </c>
       <c r="I31" s="84"/>
       <c r="J31" s="87" t="s">
         <v>578</v>

</xml_diff>

<commit_message>
Add VBat, 3.3... pin marking on T4 card as well
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73B4F7A-3BDD-442A-A2FE-0F4EA86A56E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE33384A-8CDE-4E35-9130-3D463EC61F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="360" windowWidth="23655" windowHeight="20415" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="4185" yWindow="2130" windowWidth="18615" windowHeight="17235" activeTab="3" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -2830,8 +2830,8 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>791026</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2859,8 +2859,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="3811101" y="997845"/>
-          <a:ext cx="2806211" cy="1308753"/>
+          <a:off x="4124617" y="997459"/>
+          <a:ext cx="2808910" cy="1312224"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2968,6 +2968,89 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>215564</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>120316</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1080937" cy="233205"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F33DF9D-3526-42A7-B8E7-B9673BAD85E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4998117" y="2987842"/>
+          <a:ext cx="1080937" cy="233205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="800">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>VB</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>  3V </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="900" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>GND PG  ON</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="900">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3325,9 +3408,9 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>194369</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>121861</xdr:rowOff>
+      <xdr:rowOff>119743</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="264560" cy="447558"/>
+    <xdr:ext cx="264560" cy="449676"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="14" name="TextBox 13">
@@ -3341,8 +3424,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="5505450" y="4034790"/>
-          <a:ext cx="447558" cy="264560"/>
+          <a:off x="5490240" y="4033187"/>
+          <a:ext cx="449676" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3364,7 +3447,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -5496,9 +5579,9 @@
   </sheetPr>
   <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9311,7 +9394,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q47" sqref="Q47"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M20:Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Update T4.1 CSI pins
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC0B77C-70A7-4E26-8361-EE065BD7EBA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C611B3F7-F7F4-4251-8514-110023058D91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="1410" windowWidth="19365" windowHeight="17565" activeTab="5" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="1035" yWindow="1290" windowWidth="19365" windowHeight="17565" activeTab="5" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2654" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="573">
   <si>
     <t/>
   </si>
@@ -1765,7 +1765,7 @@
     <t>CSI_D9</t>
   </si>
   <si>
-    <t>CSD_D8</t>
+    <t>CSI_D8</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2504,6 +2504,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -7157,7 +7160,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomLeft" activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10970,7 +10973,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12925,7 +12928,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AB6" sqref="AB6"/>
+      <selection pane="bottomLeft" activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13259,7 +13262,7 @@
       <c r="AB5" s="40" t="s">
         <v>145</v>
       </c>
-      <c r="AC5" s="40" t="s">
+      <c r="AC5" s="169" t="s">
         <v>572</v>
       </c>
       <c r="AD5" s="40" t="s">
@@ -13325,7 +13328,7 @@
       <c r="AB6" s="40" t="s">
         <v>140</v>
       </c>
-      <c r="AC6" s="40" t="s">
+      <c r="AC6" s="169" t="s">
         <v>571</v>
       </c>
       <c r="AD6" s="40"/>
@@ -13388,7 +13391,7 @@
       <c r="AB7" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="AC7" s="40" t="s">
+      <c r="AC7" s="169" t="s">
         <v>548</v>
       </c>
       <c r="AD7" s="40" t="s">
@@ -13455,7 +13458,7 @@
       <c r="AB8" s="40" t="s">
         <v>130</v>
       </c>
-      <c r="AC8" s="40" t="s">
+      <c r="AC8" s="169" t="s">
         <v>549</v>
       </c>
       <c r="AD8" s="40" t="s">
@@ -13656,7 +13659,7 @@
       <c r="AB11" s="40" t="s">
         <v>115</v>
       </c>
-      <c r="AC11" s="40" t="s">
+      <c r="AC11" s="169" t="s">
         <v>551</v>
       </c>
       <c r="AD11" s="40"/>
@@ -13715,7 +13718,7 @@
       <c r="AB12" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="AC12" s="40" t="s">
+      <c r="AC12" s="169" t="s">
         <v>552</v>
       </c>
       <c r="AD12" s="40"/>
@@ -14013,7 +14016,7 @@
       <c r="AB17" s="40" t="s">
         <v>431</v>
       </c>
-      <c r="AC17" s="40" t="s">
+      <c r="AC17" s="169" t="s">
         <v>553</v>
       </c>
       <c r="AD17" s="40"/>
@@ -14071,12 +14074,14 @@
       <c r="AB18" s="40" t="s">
         <v>430</v>
       </c>
-      <c r="AC18" s="40"/>
+      <c r="AC18" s="169" t="s">
+        <v>550</v>
+      </c>
       <c r="AD18" s="40"/>
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="40"/>
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="169" t="s">
         <v>545</v>
       </c>
       <c r="C19" s="40" t="s">
@@ -14128,14 +14133,14 @@
       <c r="AB19" s="40" t="s">
         <v>429</v>
       </c>
-      <c r="AC19" s="40" t="s">
+      <c r="AC19" s="169" t="s">
         <v>546</v>
       </c>
       <c r="AD19" s="40"/>
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="40"/>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="169" t="s">
         <v>544</v>
       </c>
       <c r="C20" s="40" t="s">
@@ -14187,7 +14192,7 @@
       <c r="AB20" s="40" t="s">
         <v>428</v>
       </c>
-      <c r="AC20" s="40" t="s">
+      <c r="AC20" s="169" t="s">
         <v>547</v>
       </c>
       <c r="AD20" s="40"/>
@@ -14355,7 +14360,7 @@
       <c r="AB23" s="40" t="s">
         <v>425</v>
       </c>
-      <c r="AC23" s="40" t="s">
+      <c r="AC23" s="169" t="s">
         <v>550</v>
       </c>
       <c r="AD23" s="40"/>
@@ -14413,7 +14418,7 @@
       <c r="AB24" s="40" t="s">
         <v>424</v>
       </c>
-      <c r="AC24" s="40" t="s">
+      <c r="AC24" s="169" t="s">
         <v>551</v>
       </c>
       <c r="AD24" s="40"/>

</xml_diff>

<commit_message>
T4.1 Add MUX page...
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038236A4-5614-4F58-BE0C-F26D7CF78D8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405B0BE6-6F0C-42FC-819B-5073A8786844}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="225" windowWidth="20745" windowHeight="19695" activeTab="5" xr2:uid="{157985FD-D6B7-4AEF-8AFE-EA864123C2AA}"/>
+    <workbookView xWindow="14160" yWindow="2130" windowWidth="20520" windowHeight="17745" activeTab="6" xr2:uid="{7909E9C6-F02A-4F53-B5AB-976DAA1030D4}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
     <sheet name="T4 - GPIO " sheetId="10" r:id="rId2"/>
     <sheet name="T4 card like" sheetId="8" r:id="rId3"/>
     <sheet name="T4.1" sheetId="6" r:id="rId4"/>
-    <sheet name="T4.1 - GPIO" sheetId="11" r:id="rId5"/>
-    <sheet name="T4.1 card like" sheetId="7" r:id="rId6"/>
-    <sheet name="Micromod" sheetId="12" r:id="rId7"/>
-    <sheet name="MicroMod - GPIO" sheetId="13" r:id="rId8"/>
+    <sheet name="T4.1 MUX" sheetId="14" r:id="rId5"/>
+    <sheet name="T4.1 - GPIO" sheetId="11" r:id="rId6"/>
+    <sheet name="T4.1 card like" sheetId="7" r:id="rId7"/>
+    <sheet name="Micromod" sheetId="12" r:id="rId8"/>
+    <sheet name="MicroMod - GPIO" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3681" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4270" uniqueCount="1020">
   <si>
     <t/>
   </si>
@@ -1918,6 +1919,1197 @@
   </si>
   <si>
     <t>CSID8</t>
+  </si>
+  <si>
+    <t>F2A_SSO_B</t>
+  </si>
+  <si>
+    <t>F2A_D1</t>
+  </si>
+  <si>
+    <t>F2A_D0</t>
+  </si>
+  <si>
+    <t>F2A_SCLK</t>
+  </si>
+  <si>
+    <t>F2A_D2</t>
+  </si>
+  <si>
+    <t>F2A_D3</t>
+  </si>
+  <si>
+    <t>F2A_SS1_B</t>
+  </si>
+  <si>
+    <t>ALT0</t>
+  </si>
+  <si>
+    <t>ALt1</t>
+  </si>
+  <si>
+    <t>ALT2</t>
+  </si>
+  <si>
+    <t>ALT3</t>
+  </si>
+  <si>
+    <t>ALT4</t>
+  </si>
+  <si>
+    <t>Alt5</t>
+  </si>
+  <si>
+    <t>ALT6</t>
+  </si>
+  <si>
+    <t>ALT7</t>
+  </si>
+  <si>
+    <t>ALT8</t>
+  </si>
+  <si>
+    <t>ALT9</t>
+  </si>
+  <si>
+    <t>FLEXCAN2_RX</t>
+  </si>
+  <si>
+    <t>FLEXCAN2_TX</t>
+  </si>
+  <si>
+    <t>LPUART6_RX</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT17</t>
+  </si>
+  <si>
+    <t>USB_OTG1_OC</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMX01</t>
+  </si>
+  <si>
+    <t>GPIO1_IO03</t>
+  </si>
+  <si>
+    <t>REF_CLK_24M</t>
+  </si>
+  <si>
+    <t>LPSPI3_PCS0</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT16</t>
+  </si>
+  <si>
+    <t>LPUART6_TX</t>
+  </si>
+  <si>
+    <t>USB_OTG1_PWR</t>
+  </si>
+  <si>
+    <t>LEXPWM1_PWMX0</t>
+  </si>
+  <si>
+    <t>GPIO1_IO02</t>
+  </si>
+  <si>
+    <t>LPI2C1_HREQ</t>
+  </si>
+  <si>
+    <t>LPSPI3_SDI</t>
+  </si>
+  <si>
+    <t>LPI2C4_SCL</t>
+  </si>
+  <si>
+    <t>CCM_PMIC_READY</t>
+  </si>
+  <si>
+    <t>LPUART1_TX</t>
+  </si>
+  <si>
+    <t>WDOG2_WDOG_B</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMX02</t>
+  </si>
+  <si>
+    <t>GPIO1_IO12</t>
+  </si>
+  <si>
+    <t>ENET_1588_EVENT1_OUT</t>
+  </si>
+  <si>
+    <t>NMI_GLUE_NMI</t>
+  </si>
+  <si>
+    <t>LPI2C4_SDA</t>
+  </si>
+  <si>
+    <t>LPUART1_RX</t>
+  </si>
+  <si>
+    <t>EWM_OUT_B</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMX03</t>
+  </si>
+  <si>
+    <t>GPIO1_IO13</t>
+  </si>
+  <si>
+    <t>ENET_1588_EVENT1_IN</t>
+  </si>
+  <si>
+    <t>USB_OTG2_ID</t>
+  </si>
+  <si>
+    <t>QTIMER3_TIMER0</t>
+  </si>
+  <si>
+    <t>LPUART2_CTS_B</t>
+  </si>
+  <si>
+    <t>LPI2C1_SCL</t>
+  </si>
+  <si>
+    <t>WDOG1_B</t>
+  </si>
+  <si>
+    <t>GPIO1_IO16</t>
+  </si>
+  <si>
+    <t>QTIMER3_TIMER1</t>
+  </si>
+  <si>
+    <t>LPUART2_RTS_B</t>
+  </si>
+  <si>
+    <t>LPI2C1_SDA</t>
+  </si>
+  <si>
+    <t>GPIO1_IO17</t>
+  </si>
+  <si>
+    <t>USDHC1_VSELECT</t>
+  </si>
+  <si>
+    <t>USDHC1_W</t>
+  </si>
+  <si>
+    <t>KPP_ROW07</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT0_OUT</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO00</t>
+  </si>
+  <si>
+    <t>KPP_COL07</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT0_IN</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO01</t>
+  </si>
+  <si>
+    <t>USB_OTG1_ID</t>
+  </si>
+  <si>
+    <t>QTIMER3_TIMER2</t>
+  </si>
+  <si>
+    <t>LPUART2_TX</t>
+  </si>
+  <si>
+    <t>ENET_1588_EVENT2_OUT</t>
+  </si>
+  <si>
+    <t>GPIO1_IO18</t>
+  </si>
+  <si>
+    <t>USDHC1_CD_B</t>
+  </si>
+  <si>
+    <t>KPP_ROW06</t>
+  </si>
+  <si>
+    <t>GPT2_CLK</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO02</t>
+  </si>
+  <si>
+    <t>QTIMER3_TIMER3</t>
+  </si>
+  <si>
+    <t>LPUART2_RX</t>
+  </si>
+  <si>
+    <t>ENET_1588_EVENT2_IN</t>
+  </si>
+  <si>
+    <t>GPIO1_IO19</t>
+  </si>
+  <si>
+    <t>USDHC2_CD_B</t>
+  </si>
+  <si>
+    <t>KPP_COL06</t>
+  </si>
+  <si>
+    <t>GPT2_CAPTURE1</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO03</t>
+  </si>
+  <si>
+    <t>FLEXSPIB_DATA03</t>
+  </si>
+  <si>
+    <t>ENET_MDC</t>
+  </si>
+  <si>
+    <t>LPUART3_CTS_B</t>
+  </si>
+  <si>
+    <t>SPDIF_SR_CLK</t>
+  </si>
+  <si>
+    <t>GPIO1_IO20</t>
+  </si>
+  <si>
+    <t>KPP_ROW05</t>
+  </si>
+  <si>
+    <t>GPT2_CAPTURE2</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO04</t>
+  </si>
+  <si>
+    <t>FLEXSPIB_DATA02</t>
+  </si>
+  <si>
+    <t>ENET_MDIO</t>
+  </si>
+  <si>
+    <t>LPUART3_RTS_B</t>
+  </si>
+  <si>
+    <t>GPIO1_IO21</t>
+  </si>
+  <si>
+    <t>KPP_COL05</t>
+  </si>
+  <si>
+    <t>GPT2_COMPARE1</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO05</t>
+  </si>
+  <si>
+    <t>FLEXSPIB_DATA01</t>
+  </si>
+  <si>
+    <t>LPI2C3_SDA</t>
+  </si>
+  <si>
+    <t>LPUART3_TX</t>
+  </si>
+  <si>
+    <t>GPIO1_IO22</t>
+  </si>
+  <si>
+    <t>KPP_ROW04</t>
+  </si>
+  <si>
+    <t>GPT2_COMPARE2</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO06</t>
+  </si>
+  <si>
+    <t>FLEXSPIB_DATA00</t>
+  </si>
+  <si>
+    <t>LPI2C3_SCL</t>
+  </si>
+  <si>
+    <t>LPUART3_RX</t>
+  </si>
+  <si>
+    <t>SPDIF_EXT_CLK</t>
+  </si>
+  <si>
+    <t>GPIO1_IO23</t>
+  </si>
+  <si>
+    <t>KPP_COL04</t>
+  </si>
+  <si>
+    <t>GPT2_COMPARE3</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO07</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_SS1_B</t>
+  </si>
+  <si>
+    <t>FLEXPWM4_PWMA00</t>
+  </si>
+  <si>
+    <t>FLEXCAN1_TX</t>
+  </si>
+  <si>
+    <t>CSI_DATA09</t>
+  </si>
+  <si>
+    <t>GPIO1_IO24</t>
+  </si>
+  <si>
+    <t>KPP_ROW03</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO08</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_DQS</t>
+  </si>
+  <si>
+    <t>FLEXPWM4_PWMA01</t>
+  </si>
+  <si>
+    <t>FLEXCAN1_RX</t>
+  </si>
+  <si>
+    <t>SAI1_MCLK</t>
+  </si>
+  <si>
+    <t>CSI_DATA08</t>
+  </si>
+  <si>
+    <t>GPIO1_IO25</t>
+  </si>
+  <si>
+    <t>KPP_COL03</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO09</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_DATA03</t>
+  </si>
+  <si>
+    <t>LPUART8_TX</t>
+  </si>
+  <si>
+    <t>SAI1_RX_SYNC</t>
+  </si>
+  <si>
+    <t>CSI_DATA07</t>
+  </si>
+  <si>
+    <t>GPIO1_IO26</t>
+  </si>
+  <si>
+    <t>USDHC2_WP</t>
+  </si>
+  <si>
+    <t>KPP_ROW02</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT1_OUT</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO10</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_DATA02</t>
+  </si>
+  <si>
+    <t>LPUART8_RX</t>
+  </si>
+  <si>
+    <t>SAI1_RX_BCL</t>
+  </si>
+  <si>
+    <t>CSI_DATA06</t>
+  </si>
+  <si>
+    <t>GPIO1_IO27</t>
+  </si>
+  <si>
+    <t>USDHC2_RESET_B</t>
+  </si>
+  <si>
+    <t>KPP_COL02</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT1_IN</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO11</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_DATA01</t>
+  </si>
+  <si>
+    <t>ACMP_OUT00</t>
+  </si>
+  <si>
+    <t>SAI1_RX_DATA00</t>
+  </si>
+  <si>
+    <t>CSI_DATA05</t>
+  </si>
+  <si>
+    <t>GPIO1_IO28</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA4</t>
+  </si>
+  <si>
+    <t>KPP_ROW01</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT2_OUT</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO12</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_DATA00</t>
+  </si>
+  <si>
+    <t>ACMP_OUT01</t>
+  </si>
+  <si>
+    <t>SAI1_TX_DATA00</t>
+  </si>
+  <si>
+    <t>CSI_DATA04</t>
+  </si>
+  <si>
+    <t>GPIO1_IO29</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA5</t>
+  </si>
+  <si>
+    <t>KPP_COL01</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT2_IN</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO13</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_SCLK</t>
+  </si>
+  <si>
+    <t>ACMP_OUT02</t>
+  </si>
+  <si>
+    <t>LPSPI3_SDO</t>
+  </si>
+  <si>
+    <t>SAI1_TX_BCLK</t>
+  </si>
+  <si>
+    <t>CSI_DATA03</t>
+  </si>
+  <si>
+    <t>GPIO1_IO30</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA6</t>
+  </si>
+  <si>
+    <t>KPP_ROW00</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT3_OUT</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO14</t>
+  </si>
+  <si>
+    <t>FLEXSPIA_SS0_B</t>
+  </si>
+  <si>
+    <t>ACMP_OUT03</t>
+  </si>
+  <si>
+    <t>LPSPI3_SCK</t>
+  </si>
+  <si>
+    <t>SAI1_TX_SYNC</t>
+  </si>
+  <si>
+    <t>CSI_DATA02</t>
+  </si>
+  <si>
+    <t>GPIO1_IO31</t>
+  </si>
+  <si>
+    <t>USDHC2_DATA7</t>
+  </si>
+  <si>
+    <t>KPP_COL00</t>
+  </si>
+  <si>
+    <t>ENET2_1588_EVENT3_IN</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO15</t>
+  </si>
+  <si>
+    <t>QTIMER1_TIMER0</t>
+  </si>
+  <si>
+    <t>LPSPI4_PCS0</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO00</t>
+  </si>
+  <si>
+    <t>GPIO2_IO00</t>
+  </si>
+  <si>
+    <t>SEMC_CSX01</t>
+  </si>
+  <si>
+    <t>ENET2_MDC</t>
+  </si>
+  <si>
+    <t>QTIMER1_TIMER1</t>
+  </si>
+  <si>
+    <t>LPSPI4_SDI</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO01</t>
+  </si>
+  <si>
+    <t>GPIO2_IO01</t>
+  </si>
+  <si>
+    <t>SEMC_CSX02</t>
+  </si>
+  <si>
+    <t>ENET2_MDIO</t>
+  </si>
+  <si>
+    <t>QTIMER1_TIMER2</t>
+  </si>
+  <si>
+    <t>LPSPI4_SDO</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO02</t>
+  </si>
+  <si>
+    <t>GPIO2_IO02</t>
+  </si>
+  <si>
+    <t>SEMC_CSX03</t>
+  </si>
+  <si>
+    <t>QTIMER2_TIMER0</t>
+  </si>
+  <si>
+    <t>LPSPI4_SCK</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO03</t>
+  </si>
+  <si>
+    <t>GPIO2_IO03</t>
+  </si>
+  <si>
+    <t>WDOG2_RESET_B_DEB</t>
+  </si>
+  <si>
+    <t>LCD_DATA06</t>
+  </si>
+  <si>
+    <t>QTIMER4_TIMER1</t>
+  </si>
+  <si>
+    <t>FLEXPWM2_PWMA02</t>
+  </si>
+  <si>
+    <t>SAI1_TX_DATA03</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO10</t>
+  </si>
+  <si>
+    <t>GPIO2_IO10</t>
+  </si>
+  <si>
+    <t>SRC_BOOT_CFG06</t>
+  </si>
+  <si>
+    <t>ENET2_CRS</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO11</t>
+  </si>
+  <si>
+    <t>GPIO2_IO11</t>
+  </si>
+  <si>
+    <t>LCD_DATA07</t>
+  </si>
+  <si>
+    <t>QTIMER4_TIMER2</t>
+  </si>
+  <si>
+    <t>FLEXPWM2_PWMB02</t>
+  </si>
+  <si>
+    <t>SAI1_TX_DATA02</t>
+  </si>
+  <si>
+    <t>SRC_BOOT_CFG07</t>
+  </si>
+  <si>
+    <t>ENET2_COL</t>
+  </si>
+  <si>
+    <t>LCD_DATA08</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT10</t>
+  </si>
+  <si>
+    <t>ARM_TRACE_CLK</t>
+  </si>
+  <si>
+    <t>SAI1_TX_DATA01</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO12</t>
+  </si>
+  <si>
+    <t>GPIO2_IO12</t>
+  </si>
+  <si>
+    <t>SRC_BOOT_CFG08</t>
+  </si>
+  <si>
+    <t>ENET2_TDATA00</t>
+  </si>
+  <si>
+    <t>LCD_DATA12</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT14</t>
+  </si>
+  <si>
+    <t>LPUART4_TX</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO16</t>
+  </si>
+  <si>
+    <t>GPIO2_IO16</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMA03</t>
+  </si>
+  <si>
+    <t>ENET2_RX_ER</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO16</t>
+  </si>
+  <si>
+    <t>LCD_DATA13</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT15</t>
+  </si>
+  <si>
+    <t>LPUART4_RX</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO17</t>
+  </si>
+  <si>
+    <t>GPIO2_IO17</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMB03</t>
+  </si>
+  <si>
+    <t>ENET2_RDATA00</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO17</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO18</t>
+  </si>
+  <si>
+    <t>ENET2_RDATA01</t>
+  </si>
+  <si>
+    <t>GPIO2_IO18</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO18</t>
+  </si>
+  <si>
+    <t>LCD_DATA14</t>
+  </si>
+  <si>
+    <t>LPSPI4_PCS2</t>
+  </si>
+  <si>
+    <t>FLEXPWM2_PWMA03</t>
+  </si>
+  <si>
+    <t>LCD_DATA15</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO19</t>
+  </si>
+  <si>
+    <t>GPIO2_IO19</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO19</t>
+  </si>
+  <si>
+    <t>ENET2_RX_EN</t>
+  </si>
+  <si>
+    <t>FLEXPWM2_PWMB03</t>
+  </si>
+  <si>
+    <t>LPSPI4_PCS1</t>
+  </si>
+  <si>
+    <t>LPUART5_TX</t>
+  </si>
+  <si>
+    <t>ENET_1588_EVENT0_IN</t>
+  </si>
+  <si>
+    <t>GPIO2_IO28</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO28</t>
+  </si>
+  <si>
+    <t>LPUART5_RX</t>
+  </si>
+  <si>
+    <t>ENET_1588_EVENT0_OUT</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO28</t>
+  </si>
+  <si>
+    <t>FLEXIO2_FLEXIO29</t>
+  </si>
+  <si>
+    <t>GPIO2_IO29</t>
+  </si>
+  <si>
+    <t>USDHC1_WP</t>
+  </si>
+  <si>
+    <t>SEMC_DQS4</t>
+  </si>
+  <si>
+    <t>FLEXIO3_FLEXIO29</t>
+  </si>
+  <si>
+    <t>SEMC_DATA04</t>
+  </si>
+  <si>
+    <t>FLEXPWM4_PWMA02</t>
+  </si>
+  <si>
+    <t>SAI2_TX_DATA</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT06</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO04</t>
+  </si>
+  <si>
+    <t>GPIO4_IO04</t>
+  </si>
+  <si>
+    <t>SEMC_DATA05</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT07</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO05</t>
+  </si>
+  <si>
+    <t>GPIO4_IO05</t>
+  </si>
+  <si>
+    <t>FLEXPWM4_PWMB0</t>
+  </si>
+  <si>
+    <t>SAI2_TX_SYNC</t>
+  </si>
+  <si>
+    <t>SEMC_DATA06</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO06</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT08</t>
+  </si>
+  <si>
+    <t>SAI2_TX_BCLK</t>
+  </si>
+  <si>
+    <t>FLEXPWM2_PWMA00</t>
+  </si>
+  <si>
+    <t>SEMC_DATA07</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT09</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO07</t>
+  </si>
+  <si>
+    <t>GPIO4_IO06</t>
+  </si>
+  <si>
+    <t>GPIO4_IO07</t>
+  </si>
+  <si>
+    <t>FLEXPWM2_PWMB00</t>
+  </si>
+  <si>
+    <t>SAI2_MCLK</t>
+  </si>
+  <si>
+    <t>SEMC_DM00</t>
+  </si>
+  <si>
+    <t>FLEXPWM2_PWMA01</t>
+  </si>
+  <si>
+    <t>SAI2_RX_DATA</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO08</t>
+  </si>
+  <si>
+    <t>GPIO4_IO08</t>
+  </si>
+  <si>
+    <t>SEMC_BA1</t>
+  </si>
+  <si>
+    <t>FLEXPWM3_PWMB03</t>
+  </si>
+  <si>
+    <t>ENET_TDATA00</t>
+  </si>
+  <si>
+    <t>QTIMER2_TIMER3</t>
+  </si>
+  <si>
+    <t>GPIO4_IO22</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_SS1_B of</t>
+  </si>
+  <si>
+    <t>SEMC_CAS</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMB00</t>
+  </si>
+  <si>
+    <t>ENET_TX_EN</t>
+  </si>
+  <si>
+    <t>GPT1_CAPTURE1</t>
+  </si>
+  <si>
+    <t>SEMC_RAS</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMA01</t>
+  </si>
+  <si>
+    <t>ENET_TX_CLK</t>
+  </si>
+  <si>
+    <t>ENET_REF_CLK</t>
+  </si>
+  <si>
+    <t>GPIO4_IO24</t>
+  </si>
+  <si>
+    <t>GPIO4_IO25</t>
+  </si>
+  <si>
+    <t>GPIO4_IO27</t>
+  </si>
+  <si>
+    <t>SEMC_CLK</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMB01</t>
+  </si>
+  <si>
+    <t>ENET_RX_ER</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO12</t>
+  </si>
+  <si>
+    <t>GPIO4_IO26</t>
+  </si>
+  <si>
+    <t>GPIO4_IO28</t>
+  </si>
+  <si>
+    <t>GPIO4_IO29</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_DATA01</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO13</t>
+  </si>
+  <si>
+    <t>LPSPI1_SCK</t>
+  </si>
+  <si>
+    <t>LPUART5_RTS_B</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMA02</t>
+  </si>
+  <si>
+    <t>SEMC_CKE</t>
+  </si>
+  <si>
+    <t>SEMC_WE</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMB02</t>
+  </si>
+  <si>
+    <t>LPUART5_CTS_B</t>
+  </si>
+  <si>
+    <t>LPSPI1_SDO</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO14</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_DATA02</t>
+  </si>
+  <si>
+    <t>FLEXSPI2_A_DATA03</t>
+  </si>
+  <si>
+    <t>FLEXIO1_FLEXIO15</t>
+  </si>
+  <si>
+    <t>SEMC_CS0</t>
+  </si>
+  <si>
+    <t>FLEXPWM3_PWMA00</t>
+  </si>
+  <si>
+    <t>LPUART6_RTS_B</t>
+  </si>
+  <si>
+    <t>LPSPI1_SDI</t>
+  </si>
+  <si>
+    <t>SEMC_DATA09</t>
+  </si>
+  <si>
+    <t>FLEXPWM3_PWMA01</t>
+  </si>
+  <si>
+    <t>LPUART7_TX</t>
+  </si>
+  <si>
+    <t>LPSPI1_PCS1</t>
+  </si>
+  <si>
+    <t>CSI_DATA22</t>
+  </si>
+  <si>
+    <t>GPIO4_IO31</t>
+  </si>
+  <si>
+    <t>ENET2_TDATA01</t>
+  </si>
+  <si>
+    <t>SEMC_DATA10</t>
+  </si>
+  <si>
+    <t>FLEXPWM3_PWMB01</t>
+  </si>
+  <si>
+    <t>LPUART7_RX</t>
+  </si>
+  <si>
+    <t>CCM_PMIC_RDY</t>
+  </si>
+  <si>
+    <t>CSI_DATA21</t>
+  </si>
+  <si>
+    <t>GPIO3_IO18</t>
+  </si>
+  <si>
+    <t>ENET2_TX_EN</t>
+  </si>
+  <si>
+    <t>SEMC_DATA14</t>
+  </si>
+  <si>
+    <t>XBAR1_IN22</t>
+  </si>
+  <si>
+    <t>GPT1_COMPARE2</t>
+  </si>
+  <si>
+    <t>SAI3_TX_DATA</t>
+  </si>
+  <si>
+    <t>CSI_DATA17</t>
+  </si>
+  <si>
+    <t>GPIO3_IO22</t>
+  </si>
+  <si>
+    <t>FLEXCAN3_TX</t>
+  </si>
+  <si>
+    <t>SEMC_DATA15</t>
+  </si>
+  <si>
+    <t>XBAR1_IN23</t>
+  </si>
+  <si>
+    <t>GPT1_COMPARE3</t>
+  </si>
+  <si>
+    <t>SAI3_MCLK</t>
+  </si>
+  <si>
+    <t>CSI_DATA16</t>
+  </si>
+  <si>
+    <t>GPIO3_IO23</t>
+  </si>
+  <si>
+    <t>FLEXCAN3_RX</t>
+  </si>
+  <si>
+    <t>USDHC1_CMD</t>
+  </si>
+  <si>
+    <t>FLEXPWM1_PWMA00</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT04</t>
+  </si>
+  <si>
+    <t>GPIO3_IO12</t>
+  </si>
+  <si>
+    <t>USDHC1_CLK</t>
+  </si>
+  <si>
+    <t>XBAR1_INOUT05</t>
+  </si>
+  <si>
+    <t>LPSPI1_PCS0</t>
+  </si>
+  <si>
+    <t>GPIO3_IO13</t>
+  </si>
+  <si>
+    <t>FLEXSPIB_SS1_B</t>
+  </si>
+  <si>
+    <t>ENET2_TX_CLK</t>
+  </si>
+  <si>
+    <t>ENET2_REF_CLK2</t>
+  </si>
+  <si>
+    <t>USDHC1_DATA0</t>
+  </si>
+  <si>
+    <t>LPUART8_CTS_B</t>
+  </si>
+  <si>
+    <t>GPIO3_IO14</t>
+  </si>
+  <si>
+    <t>SEMC_CLK5</t>
+  </si>
+  <si>
+    <t>USDHC1_DATA1</t>
+  </si>
+  <si>
+    <t>LPUART8_RTS_B</t>
+  </si>
+  <si>
+    <t>GPIO3_IO15</t>
+  </si>
+  <si>
+    <t>SEMC_CLK6</t>
+  </si>
+  <si>
+    <t>USDHC1_DATA2</t>
+  </si>
+  <si>
+    <t>GPIO3_IO16</t>
+  </si>
+  <si>
+    <t>FLEXSPIB_SS0_B</t>
+  </si>
+  <si>
+    <t>CCM_CLKO1</t>
+  </si>
+  <si>
+    <t>CCM_CLKO2</t>
+  </si>
+  <si>
+    <t>GPIO3_IO17</t>
+  </si>
+  <si>
+    <t>FLEXSPIB_DQS</t>
+  </si>
+  <si>
+    <t>USDHC1_DATA3</t>
   </si>
 </sst>
 </file>
@@ -2032,7 +3224,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2231,6 +3423,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF339933"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFF33"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -2317,7 +3551,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2654,6 +3888,9 @@
     <xf numFmtId="0" fontId="9" fillId="33" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2666,15 +3903,69 @@
     <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B33FA5B1-4CE6-4A8A-BADE-2FB8021A9AC4}"/>
   </cellStyles>
-  <dxfs count="60">
+  <dxfs count="74">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -2859,6 +4150,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCCFF33"/>
+      <color rgb="FF339933"/>
+      <color rgb="FFCCECFF"/>
+      <color rgb="FFFF7C80"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FFF97F8B"/>
       <color rgb="FF61D6FF"/>
@@ -3845,94 +5140,118 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M59" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M59" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
   <autoFilter ref="A1:M59" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{F9478000-D09D-4158-8962-151C792B9115}" name="GPIO" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{EEB23B63-7C82-4BC1-80FE-826F4A02B99D}" name="Serial" dataDxfId="54"/>
-    <tableColumn id="5" xr3:uid="{1D7F4122-4922-476A-8C8E-378628CB944B}" name="I2C" dataDxfId="53"/>
-    <tableColumn id="6" xr3:uid="{8B2BA30D-AD74-4591-9119-1A5E4B5E627D}" name="SPI" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{50F13DDA-AECC-4873-B8BF-BF29B9FA3A1D}" name="PWM" dataDxfId="51"/>
-    <tableColumn id="8" xr3:uid="{99EA318C-72FB-4EFD-9E14-9B5211643911}" name="CAN" dataDxfId="50"/>
-    <tableColumn id="9" xr3:uid="{DC6B9277-B97B-4891-B766-22B3DE725408}" name="Audio" dataDxfId="49"/>
-    <tableColumn id="10" xr3:uid="{1446B065-9F8B-426F-A535-611F882183B3}" name="XBAR" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{DC1C2DEB-A4BD-44FE-B52D-E7ABF3D565E7}" name="FlexIO" dataDxfId="47"/>
-    <tableColumn id="12" xr3:uid="{2A37AD20-1A78-4C16-9F5C-DBB6ECB30C3F}" name="Analog" dataDxfId="46"/>
-    <tableColumn id="13" xr3:uid="{E0FD363E-BD42-46D9-8D08-5AE1FF584E61}" name="SD/CSI/LCD" dataDxfId="45"/>
+    <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="71"/>
+    <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="70"/>
+    <tableColumn id="3" xr3:uid="{F9478000-D09D-4158-8962-151C792B9115}" name="GPIO" dataDxfId="69"/>
+    <tableColumn id="4" xr3:uid="{EEB23B63-7C82-4BC1-80FE-826F4A02B99D}" name="Serial" dataDxfId="68"/>
+    <tableColumn id="5" xr3:uid="{1D7F4122-4922-476A-8C8E-378628CB944B}" name="I2C" dataDxfId="67"/>
+    <tableColumn id="6" xr3:uid="{8B2BA30D-AD74-4591-9119-1A5E4B5E627D}" name="SPI" dataDxfId="66"/>
+    <tableColumn id="7" xr3:uid="{50F13DDA-AECC-4873-B8BF-BF29B9FA3A1D}" name="PWM" dataDxfId="65"/>
+    <tableColumn id="8" xr3:uid="{99EA318C-72FB-4EFD-9E14-9B5211643911}" name="CAN" dataDxfId="64"/>
+    <tableColumn id="9" xr3:uid="{DC6B9277-B97B-4891-B766-22B3DE725408}" name="Audio" dataDxfId="63"/>
+    <tableColumn id="10" xr3:uid="{1446B065-9F8B-426F-A535-611F882183B3}" name="XBAR" dataDxfId="62"/>
+    <tableColumn id="11" xr3:uid="{DC1C2DEB-A4BD-44FE-B52D-E7ABF3D565E7}" name="FlexIO" dataDxfId="61"/>
+    <tableColumn id="12" xr3:uid="{2A37AD20-1A78-4C16-9F5C-DBB6ECB30C3F}" name="Analog" dataDxfId="60"/>
+    <tableColumn id="13" xr3:uid="{E0FD363E-BD42-46D9-8D08-5AE1FF584E61}" name="SD/CSI/LCD" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FBF0D35-2CE8-4056-99C9-8BA06E84A4F2}" name="Table44" displayName="Table44" ref="A1:M57" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
-  <autoFilter ref="A1:M57" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M57">
-    <sortCondition ref="C2:C57"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F6923B6-4F50-44A0-85F6-B6E706E61BCE}" name="Table46" displayName="Table46" ref="A1:L56" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+  <autoFilter ref="A1:L56" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L56">
+    <sortCondition ref="A2:A56"/>
   </sortState>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{1F964F0D-83A4-459C-9496-6A1229BDD1CA}" name="Pin" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{29F07050-DC12-4F4A-93C9-84EA4D24FC14}" name="Name" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{2491D004-6B1F-44DA-9E9A-E599F694FEC5}" name="GPIO" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{3AF6E798-9147-4AB4-936B-73FB56DAADDC}" name="Serial" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{F90CC261-4748-4F6F-84BC-1F4507953F2B}" name="I2C" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{1228CC1B-8420-4510-8B20-1B5A755F93F4}" name="SPI" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{B5235724-C934-4085-BA21-9D87B83403F0}" name="PWM" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{E6A78068-999F-4EB1-BC47-E0339ADDEB19}" name="CAN" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{676FF9FA-1D40-4E7E-9217-0AB090DAD93E}" name="Audio" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{B75CFCB1-0F3D-4A48-B9FB-BE8C97A0D331}" name="XBAR" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{B6165631-5DF9-46E6-AFC1-E89804AF65C9}" name="FlexIO" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{0A677E09-F667-440D-83B9-6B28A7D0361A}" name="Analog" dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{CACC907E-B7D3-4542-AA4D-60AA34159A4E}" name="SD/CSI/LCD" dataDxfId="30"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{2FF2926D-76AF-4A43-864C-1929BFD0A68A}" name="Pin" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{DBD9783C-68D1-4579-8AC6-92B0E31BC1E2}" name="Name" dataDxfId="56"/>
+    <tableColumn id="14" xr3:uid="{76C17CD9-2E7D-4846-9BD8-D8AF2AEDA0DE}" name="ALT0" dataDxfId="55"/>
+    <tableColumn id="15" xr3:uid="{BE004B08-9CAD-42A6-BD65-6B48419A2E82}" name="ALt1" dataDxfId="54"/>
+    <tableColumn id="16" xr3:uid="{98599106-77C1-42F5-919C-AAB320F80A47}" name="ALT2" dataDxfId="53"/>
+    <tableColumn id="17" xr3:uid="{32C3D940-EA13-46FC-A402-814E1B152721}" name="ALT3" dataDxfId="52"/>
+    <tableColumn id="18" xr3:uid="{B2EC6B0E-2511-4B8C-A8E1-A6F7BBE97AA4}" name="ALT4" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{7AC3B94D-0445-4DF5-9989-6936927A50E1}" name="Alt5" dataDxfId="0"/>
+    <tableColumn id="20" xr3:uid="{CCFEC2C2-FBF1-474A-92CD-A58A299FF456}" name="ALT6" dataDxfId="1"/>
+    <tableColumn id="21" xr3:uid="{B108228D-000D-4A0C-82EF-0E977A0DF892}" name="ALT7" dataDxfId="51"/>
+    <tableColumn id="22" xr3:uid="{A38F3C31-4856-4D35-AA59-6E24E6DECC0C}" name="ALT8" dataDxfId="50"/>
+    <tableColumn id="23" xr3:uid="{C86B93AE-1D5F-4DE8-A58A-8219019947DF}" name="ALT9" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A31209C-0744-40DF-BEA2-51480749F938}" name="Table42" displayName="Table42" ref="A1:M50" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:M50" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FBF0D35-2CE8-4056-99C9-8BA06E84A4F2}" name="Table44" displayName="Table44" ref="A1:M57" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+  <autoFilter ref="A1:M57" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M57">
+    <sortCondition ref="C2:C57"/>
+  </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{1FA4817C-7344-4B9E-9BD4-442E849ED7E8}" name="Pin" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{4AD2AB58-241E-4CFC-A1C5-16943CF49E13}" name="Name" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{F71AF128-9344-4146-AFB8-763C46188B4F}" name="GPIO" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{09C9E89C-BD40-41CD-BCD9-FBFAF33CB6D8}" name="Serial" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{3E815C42-FCE2-489B-91D3-683FE184F105}" name="I2C" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{FEEE2127-D6CF-4F96-819F-1B287988C35D}" name="SPI" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{73226C5A-CBE1-49F8-9481-E18F0FD235CE}" name="PWM" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{9F8D0763-B9D7-4C0A-AED0-834476CC37CA}" name="CAN" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{FB55AA45-516A-4120-8948-A5AF8C8A54DD}" name="Audio" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{FE9C4536-9536-418C-8C69-E56A803D4E2B}" name="XBAR" dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{80808062-5E4F-4FCA-BB01-53A3D23512F9}" name="FlexIO" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{CC4496D7-52BC-4F94-AA69-73D82D9E163E}" name="Analog" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{F42DD222-DD94-4C47-A5E3-AAB2345C9AEB}" name="SD/CSI/LCD" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{1F964F0D-83A4-459C-9496-6A1229BDD1CA}" name="Pin" dataDxfId="46"/>
+    <tableColumn id="2" xr3:uid="{29F07050-DC12-4F4A-93C9-84EA4D24FC14}" name="Name" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{2491D004-6B1F-44DA-9E9A-E599F694FEC5}" name="GPIO" dataDxfId="44"/>
+    <tableColumn id="4" xr3:uid="{3AF6E798-9147-4AB4-936B-73FB56DAADDC}" name="Serial" dataDxfId="43"/>
+    <tableColumn id="5" xr3:uid="{F90CC261-4748-4F6F-84BC-1F4507953F2B}" name="I2C" dataDxfId="42"/>
+    <tableColumn id="6" xr3:uid="{1228CC1B-8420-4510-8B20-1B5A755F93F4}" name="SPI" dataDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{B5235724-C934-4085-BA21-9D87B83403F0}" name="PWM" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{E6A78068-999F-4EB1-BC47-E0339ADDEB19}" name="CAN" dataDxfId="39"/>
+    <tableColumn id="9" xr3:uid="{676FF9FA-1D40-4E7E-9217-0AB090DAD93E}" name="Audio" dataDxfId="38"/>
+    <tableColumn id="10" xr3:uid="{B75CFCB1-0F3D-4A48-B9FB-BE8C97A0D331}" name="XBAR" dataDxfId="37"/>
+    <tableColumn id="11" xr3:uid="{B6165631-5DF9-46E6-AFC1-E89804AF65C9}" name="FlexIO" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{0A677E09-F667-440D-83B9-6B28A7D0361A}" name="Analog" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{CACC907E-B7D3-4542-AA4D-60AA34159A4E}" name="SD/CSI/LCD" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A83D5ACF-E653-4DB3-8FE2-1B01953FA219}" name="Table423" displayName="Table423" ref="A1:M47" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A31209C-0744-40DF-BEA2-51480749F938}" name="Table42" displayName="Table42" ref="A1:M50" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+  <autoFilter ref="A1:M50" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{1FA4817C-7344-4B9E-9BD4-442E849ED7E8}" name="Pin" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{4AD2AB58-241E-4CFC-A1C5-16943CF49E13}" name="Name" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{F71AF128-9344-4146-AFB8-763C46188B4F}" name="GPIO" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{09C9E89C-BD40-41CD-BCD9-FBFAF33CB6D8}" name="Serial" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{3E815C42-FCE2-489B-91D3-683FE184F105}" name="I2C" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{FEEE2127-D6CF-4F96-819F-1B287988C35D}" name="SPI" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{73226C5A-CBE1-49F8-9481-E18F0FD235CE}" name="PWM" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{9F8D0763-B9D7-4C0A-AED0-834476CC37CA}" name="CAN" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{FB55AA45-516A-4120-8948-A5AF8C8A54DD}" name="Audio" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{FE9C4536-9536-418C-8C69-E56A803D4E2B}" name="XBAR" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{80808062-5E4F-4FCA-BB01-53A3D23512F9}" name="FlexIO" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{CC4496D7-52BC-4F94-AA69-73D82D9E163E}" name="Analog" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{F42DD222-DD94-4C47-A5E3-AAB2345C9AEB}" name="SD/CSI/LCD" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A83D5ACF-E653-4DB3-8FE2-1B01953FA219}" name="Table423" displayName="Table423" ref="A1:M47" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:M47" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M47">
     <sortCondition ref="C1:C47"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E235028C-ACE8-4A1F-98BD-F9271F19A1D2}" name="Pin" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{1F222945-3BCF-4053-98AF-648BD8687B08}" name="Name" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D441F102-0187-41C3-A599-5422C2DA8755}" name="GPIO" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{06DF530B-4B4E-44C9-8DDE-3AD326E1E14F}" name="Serial" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{FAD43D46-EB5B-473B-91C4-485BEB1E341A}" name="I2C" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{167987D0-794F-449D-A9C6-10A4C507490A}" name="SPI" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{FA011A7B-F201-400A-9944-07B86FDE3CC8}" name="PWM" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{2C77510B-E776-4A66-8E95-E299D8840634}" name="CAN" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{23957E32-3ECD-4002-9B52-2A6AC70592CA}" name="Audio" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{9E86FA4C-0EE4-4197-8193-1D2D26419192}" name="XBAR" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{91907E0A-BB1E-4AD4-A578-4E156B00B089}" name="FlexIO" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{B5129136-343E-4C0E-B257-CC80A2575D2C}" name="Analog" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{018BA245-1B76-45AD-BE6D-82A0CBAC04E3}" name="SD/CSI/LCD" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E235028C-ACE8-4A1F-98BD-F9271F19A1D2}" name="Pin" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{1F222945-3BCF-4053-98AF-648BD8687B08}" name="Name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{D441F102-0187-41C3-A599-5422C2DA8755}" name="GPIO" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{06DF530B-4B4E-44C9-8DDE-3AD326E1E14F}" name="Serial" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{FAD43D46-EB5B-473B-91C4-485BEB1E341A}" name="I2C" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{167987D0-794F-449D-A9C6-10A4C507490A}" name="SPI" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{FA011A7B-F201-400A-9944-07B86FDE3CC8}" name="PWM" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{2C77510B-E776-4A66-8E95-E299D8840634}" name="CAN" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{23957E32-3ECD-4002-9B52-2A6AC70592CA}" name="Audio" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{9E86FA4C-0EE4-4197-8193-1D2D26419192}" name="XBAR" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{91907E0A-BB1E-4AD4-A578-4E156B00B089}" name="FlexIO" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{B5129136-343E-4C0E-B257-CC80A2575D2C}" name="Analog" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{018BA245-1B76-45AD-BE6D-82A0CBAC04E3}" name="SD/CSI/LCD" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4237,9 +5556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B4A98D7-59ED-43A9-B01B-8AE7AF7474EA}">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -5872,9 +7189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A35696-03D0-445C-9164-20930A935361}">
   <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7456,10 +8771,7 @@
   </sheetPr>
   <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V32" sqref="V32"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7597,19 +8909,19 @@
       <c r="I2" s="111"/>
       <c r="J2" s="111"/>
       <c r="K2" s="111"/>
-      <c r="L2" s="167" t="s">
+      <c r="L2" s="168" t="s">
         <v>379</v>
       </c>
-      <c r="M2" s="167"/>
-      <c r="N2" s="167"/>
+      <c r="M2" s="168"/>
+      <c r="N2" s="168"/>
       <c r="O2" s="114"/>
       <c r="P2" s="114"/>
-      <c r="Q2" s="166" t="s">
+      <c r="Q2" s="167" t="s">
         <v>380</v>
       </c>
-      <c r="R2" s="166"/>
-      <c r="S2" s="166"/>
-      <c r="T2" s="166"/>
+      <c r="R2" s="167"/>
+      <c r="S2" s="167"/>
+      <c r="T2" s="167"/>
       <c r="U2" s="111"/>
       <c r="V2" s="111"/>
       <c r="W2" s="111"/>
@@ -7656,12 +8968,12 @@
       </c>
       <c r="O3" s="114"/>
       <c r="P3" s="114"/>
-      <c r="Q3" s="166" t="s">
+      <c r="Q3" s="167" t="s">
         <v>379</v>
       </c>
-      <c r="R3" s="166"/>
-      <c r="S3" s="166"/>
-      <c r="T3" s="166"/>
+      <c r="R3" s="167"/>
+      <c r="S3" s="167"/>
+      <c r="T3" s="167"/>
       <c r="U3" s="111"/>
       <c r="V3" s="111"/>
       <c r="W3" s="111"/>
@@ -7710,12 +9022,12 @@
       </c>
       <c r="O4" s="114"/>
       <c r="P4" s="114"/>
-      <c r="Q4" s="166" t="s">
+      <c r="Q4" s="167" t="s">
         <v>383</v>
       </c>
-      <c r="R4" s="166"/>
-      <c r="S4" s="166"/>
-      <c r="T4" s="166"/>
+      <c r="R4" s="167"/>
+      <c r="S4" s="167"/>
+      <c r="T4" s="167"/>
       <c r="U4" s="111"/>
       <c r="V4" s="111"/>
       <c r="W4" s="111"/>
@@ -9035,11 +10347,11 @@
       <c r="I29" s="143"/>
       <c r="J29" s="143"/>
       <c r="K29" s="143"/>
-      <c r="L29" s="167" t="s">
+      <c r="L29" s="168" t="s">
         <v>379</v>
       </c>
-      <c r="M29" s="167"/>
-      <c r="N29" s="167"/>
+      <c r="M29" s="168"/>
+      <c r="N29" s="168"/>
       <c r="O29" s="143" t="s">
         <v>494</v>
       </c>
@@ -9116,12 +10428,12 @@
     <row r="31" spans="1:30">
       <c r="A31" s="128"/>
       <c r="B31" s="128"/>
-      <c r="L31" s="166" t="s">
+      <c r="L31" s="167" t="s">
         <v>383</v>
       </c>
-      <c r="M31" s="166"/>
-      <c r="N31" s="166"/>
-      <c r="O31" s="166"/>
+      <c r="M31" s="167"/>
+      <c r="N31" s="167"/>
+      <c r="O31" s="167"/>
       <c r="P31" s="128"/>
       <c r="Q31" s="128"/>
       <c r="R31" s="128"/>
@@ -9384,10 +10696,7 @@
   </sheetPr>
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K31" sqref="K31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -10504,7 +11813,7 @@
       <c r="L29" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="M29" s="170" t="s">
+      <c r="M29" s="166" t="s">
         <v>543</v>
       </c>
     </row>
@@ -10545,7 +11854,7 @@
       <c r="L30" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="M30" s="170" t="s">
+      <c r="M30" s="166" t="s">
         <v>542</v>
       </c>
     </row>
@@ -11281,16 +12590,1904 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E95FA3BF-4836-4E18-902A-73F96A8CFB1A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:L56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="D2" s="177" t="s">
+        <v>643</v>
+      </c>
+      <c r="E2" s="173" t="s">
+        <v>642</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="G2" s="172" t="s">
+        <v>645</v>
+      </c>
+      <c r="H2" s="174" t="s">
+        <v>646</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="J2" s="175" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="D3" s="177" t="s">
+        <v>649</v>
+      </c>
+      <c r="E3" s="173" t="s">
+        <v>650</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="G3" s="172" t="s">
+        <v>652</v>
+      </c>
+      <c r="H3" s="174" t="s">
+        <v>653</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="J3" s="175" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="D4" s="172" t="s">
+        <v>895</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>896</v>
+      </c>
+      <c r="F4" s="177" t="s">
+        <v>897</v>
+      </c>
+      <c r="G4" s="171" t="s">
+        <v>898</v>
+      </c>
+      <c r="H4" s="174" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="D5" s="172" t="s">
+        <v>904</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>905</v>
+      </c>
+      <c r="F5" s="177" t="s">
+        <v>901</v>
+      </c>
+      <c r="G5" s="171" t="s">
+        <v>902</v>
+      </c>
+      <c r="H5" s="174" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>906</v>
+      </c>
+      <c r="D6" s="172" t="s">
+        <v>910</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>909</v>
+      </c>
+      <c r="F6" s="177" t="s">
+        <v>908</v>
+      </c>
+      <c r="G6" s="171" t="s">
+        <v>907</v>
+      </c>
+      <c r="H6" s="174" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>918</v>
+      </c>
+      <c r="D7" s="172" t="s">
+        <v>919</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>920</v>
+      </c>
+      <c r="F7" s="177" t="s">
+        <v>643</v>
+      </c>
+      <c r="G7" s="171" t="s">
+        <v>921</v>
+      </c>
+      <c r="H7" s="174" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="E8" s="172" t="s">
+        <v>830</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="G8" s="171" t="s">
+        <v>832</v>
+      </c>
+      <c r="H8" s="174" t="s">
+        <v>833</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="D9" s="177" t="s">
+        <v>861</v>
+      </c>
+      <c r="E9" s="173" t="s">
+        <v>862</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G9" s="171" t="s">
+        <v>863</v>
+      </c>
+      <c r="H9" s="174" t="s">
+        <v>864</v>
+      </c>
+      <c r="I9" s="172" t="s">
+        <v>865</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="L9" s="171" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>852</v>
+      </c>
+      <c r="D10" s="177" t="s">
+        <v>853</v>
+      </c>
+      <c r="E10" s="173" t="s">
+        <v>854</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="G10" s="171" t="s">
+        <v>855</v>
+      </c>
+      <c r="H10" s="174" t="s">
+        <v>856</v>
+      </c>
+      <c r="I10" s="172" t="s">
+        <v>857</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="L10" s="171" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>838</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>839</v>
+      </c>
+      <c r="E11" s="172" t="s">
+        <v>840</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>841</v>
+      </c>
+      <c r="G11" s="171" t="s">
+        <v>836</v>
+      </c>
+      <c r="H11" s="174" t="s">
+        <v>837</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>842</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="D12" s="172" t="s">
+        <v>806</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="175" t="s">
+        <v>807</v>
+      </c>
+      <c r="G12" s="171" t="s">
+        <v>808</v>
+      </c>
+      <c r="H12" s="174" t="s">
+        <v>809</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="D13" s="172" t="s">
+        <v>818</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="F13" s="175" t="s">
+        <v>819</v>
+      </c>
+      <c r="G13" s="171" t="s">
+        <v>820</v>
+      </c>
+      <c r="H13" s="174" t="s">
+        <v>821</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="D14" s="172" t="s">
+        <v>812</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" s="175" t="s">
+        <v>813</v>
+      </c>
+      <c r="G14" s="171" t="s">
+        <v>814</v>
+      </c>
+      <c r="H14" s="174" t="s">
+        <v>815</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="D15" s="172" t="s">
+        <v>823</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="F15" s="175" t="s">
+        <v>824</v>
+      </c>
+      <c r="G15" s="171" t="s">
+        <v>825</v>
+      </c>
+      <c r="H15" s="174" t="s">
+        <v>826</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="D16" s="172" t="s">
+        <v>689</v>
+      </c>
+      <c r="E16" s="173" t="s">
+        <v>690</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="H16" s="174" t="s">
+        <v>692</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="L16" s="171" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="D17" s="172" t="s">
+        <v>697</v>
+      </c>
+      <c r="E17" s="173" t="s">
+        <v>698</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="H17" s="174" t="s">
+        <v>700</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="L17" s="171" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="D18" s="176" t="s">
+        <v>728</v>
+      </c>
+      <c r="E18" s="173" t="s">
+        <v>729</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="G18" s="178" t="s">
+        <v>550</v>
+      </c>
+      <c r="H18" s="174" t="s">
+        <v>731</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="L18" s="171" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="D19" s="176" t="s">
+        <v>721</v>
+      </c>
+      <c r="E19" s="173" t="s">
+        <v>722</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G19" s="178" t="s">
+        <v>549</v>
+      </c>
+      <c r="H19" s="174" t="s">
+        <v>723</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="L19" s="171" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="D20" s="172" t="s">
+        <v>676</v>
+      </c>
+      <c r="E20" s="173" t="s">
+        <v>677</v>
+      </c>
+      <c r="F20" s="176" t="s">
+        <v>678</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="H20" s="174" t="s">
+        <v>679</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>680</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="L20" s="171" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="D21" s="172" t="s">
+        <v>671</v>
+      </c>
+      <c r="E21" s="173" t="s">
+        <v>672</v>
+      </c>
+      <c r="F21" s="176" t="s">
+        <v>673</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="H21" s="174" t="s">
+        <v>675</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="L21" s="171" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="E22" s="173" t="s">
+        <v>751</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="G22" s="178" t="s">
+        <v>753</v>
+      </c>
+      <c r="H22" s="174" t="s">
+        <v>754</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="L22" s="171" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="E23" s="173" t="s">
+        <v>760</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="G23" s="178" t="s">
+        <v>762</v>
+      </c>
+      <c r="H23" s="174" t="s">
+        <v>763</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="L23" s="171" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="D24" s="172" t="s">
+        <v>736</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="G24" s="178" t="s">
+        <v>738</v>
+      </c>
+      <c r="H24" s="174" t="s">
+        <v>739</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="L24" s="171" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="D25" s="172" t="s">
+        <v>743</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>745</v>
+      </c>
+      <c r="G25" s="178" t="s">
+        <v>746</v>
+      </c>
+      <c r="H25" s="174" t="s">
+        <v>747</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="L25" s="171" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="176" t="s">
+        <v>656</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="E26" s="173" t="s">
+        <v>658</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="G26" s="172" t="s">
+        <v>660</v>
+      </c>
+      <c r="H26" s="174" t="s">
+        <v>661</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C27" s="176" t="s">
+        <v>664</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E27" s="173" t="s">
+        <v>665</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="G27" s="172" t="s">
+        <v>667</v>
+      </c>
+      <c r="H27" s="174" t="s">
+        <v>668</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="E28" s="175" t="s">
+        <v>788</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G28" s="178" t="s">
+        <v>790</v>
+      </c>
+      <c r="H28" s="174" t="s">
+        <v>791</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>793</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>794</v>
+      </c>
+      <c r="L28" s="171" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>796</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="E29" s="175" t="s">
+        <v>798</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="G29" s="178" t="s">
+        <v>800</v>
+      </c>
+      <c r="H29" s="174" t="s">
+        <v>801</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>802</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>803</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="L29" s="171" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>972</v>
+      </c>
+      <c r="D30" s="172" t="s">
+        <v>973</v>
+      </c>
+      <c r="E30" s="173" t="s">
+        <v>974</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>975</v>
+      </c>
+      <c r="G30" s="179" t="s">
+        <v>976</v>
+      </c>
+      <c r="H30" s="174" t="s">
+        <v>977</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>965</v>
+      </c>
+      <c r="D31" s="172" t="s">
+        <v>966</v>
+      </c>
+      <c r="E31" s="173" t="s">
+        <v>967</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>968</v>
+      </c>
+      <c r="G31" s="179" t="s">
+        <v>969</v>
+      </c>
+      <c r="H31" s="174" t="s">
+        <v>970</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>986</v>
+      </c>
+      <c r="D32" s="177" t="s">
+        <v>987</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>988</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>989</v>
+      </c>
+      <c r="G32" s="179" t="s">
+        <v>990</v>
+      </c>
+      <c r="H32" s="174" t="s">
+        <v>991</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>979</v>
+      </c>
+      <c r="D33" s="177" t="s">
+        <v>980</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>981</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="G33" s="179" t="s">
+        <v>983</v>
+      </c>
+      <c r="H33" s="174" t="s">
+        <v>984</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>844</v>
+      </c>
+      <c r="D34" s="177" t="s">
+        <v>845</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>846</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>847</v>
+      </c>
+      <c r="G34" s="171" t="s">
+        <v>848</v>
+      </c>
+      <c r="H34" s="174" t="s">
+        <v>849</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>850</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>911</v>
+      </c>
+      <c r="D35" s="172" t="s">
+        <v>916</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>917</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="G35" s="171" t="s">
+        <v>913</v>
+      </c>
+      <c r="H35" s="174" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="D36" s="173" t="s">
+        <v>886</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>887</v>
+      </c>
+      <c r="G36" s="171" t="s">
+        <v>889</v>
+      </c>
+      <c r="H36" s="174" t="s">
+        <v>890</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>892</v>
+      </c>
+      <c r="L36" s="171" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="D37" s="173" t="s">
+        <v>882</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>883</v>
+      </c>
+      <c r="G37" s="171" t="s">
+        <v>888</v>
+      </c>
+      <c r="H37" s="174" t="s">
+        <v>884</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="L37" s="171" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>872</v>
+      </c>
+      <c r="D38" s="177" t="s">
+        <v>649</v>
+      </c>
+      <c r="E38" s="175" t="s">
+        <v>873</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>789</v>
+      </c>
+      <c r="G38" s="171" t="s">
+        <v>871</v>
+      </c>
+      <c r="H38" s="174" t="s">
+        <v>870</v>
+      </c>
+      <c r="I38" s="172" t="s">
+        <v>874</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>869</v>
+      </c>
+      <c r="L38" s="171" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>875</v>
+      </c>
+      <c r="D39" s="177" t="s">
+        <v>643</v>
+      </c>
+      <c r="E39" s="175" t="s">
+        <v>881</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>799</v>
+      </c>
+      <c r="G39" s="171" t="s">
+        <v>876</v>
+      </c>
+      <c r="H39" s="174" t="s">
+        <v>877</v>
+      </c>
+      <c r="I39" s="172" t="s">
+        <v>880</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>879</v>
+      </c>
+      <c r="L39" s="171" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="E40" s="175" t="s">
+        <v>648</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="G40" s="178" t="s">
+        <v>771</v>
+      </c>
+      <c r="H40" s="174" t="s">
+        <v>772</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="L40" s="171" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="E41" s="175" t="s">
+        <v>655</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G41" s="178" t="s">
+        <v>780</v>
+      </c>
+      <c r="H41" s="174" t="s">
+        <v>781</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="L41" s="171" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="E42" s="173" t="s">
+        <v>707</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="G42" s="178" t="s">
+        <v>548</v>
+      </c>
+      <c r="H42" s="174" t="s">
+        <v>709</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>710</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="L42" s="171" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="E43" s="173" t="s">
+        <v>715</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G43" s="178" t="s">
+        <v>551</v>
+      </c>
+      <c r="H43" s="174" t="s">
+        <v>716</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="L43" s="171" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D44" s="172" t="s">
+        <v>941</v>
+      </c>
+      <c r="E44" s="173" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F44" s="177" t="s">
+        <v>901</v>
+      </c>
+      <c r="G44" s="175" t="s">
+        <v>964</v>
+      </c>
+      <c r="H44" s="174" t="s">
+        <v>1010</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>866</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D45" s="172" t="s">
+        <v>934</v>
+      </c>
+      <c r="E45" s="173" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F45" s="177" t="s">
+        <v>897</v>
+      </c>
+      <c r="G45" s="175" t="s">
+        <v>956</v>
+      </c>
+      <c r="H45" s="174" t="s">
+        <v>1006</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>858</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>997</v>
+      </c>
+      <c r="D46" s="172" t="s">
+        <v>930</v>
+      </c>
+      <c r="E46" s="176" t="s">
+        <v>721</v>
+      </c>
+      <c r="F46" s="177" t="s">
+        <v>998</v>
+      </c>
+      <c r="G46" s="175" t="s">
+        <v>999</v>
+      </c>
+      <c r="H46" s="174" t="s">
+        <v>1000</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>1001</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>1002</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>993</v>
+      </c>
+      <c r="D47" s="172" t="s">
+        <v>994</v>
+      </c>
+      <c r="E47" s="176" t="s">
+        <v>728</v>
+      </c>
+      <c r="F47" s="177" t="s">
+        <v>995</v>
+      </c>
+      <c r="G47" s="175" t="s">
+        <v>949</v>
+      </c>
+      <c r="H47" s="174" t="s">
+        <v>996</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>978</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D48" s="172" t="s">
+        <v>954</v>
+      </c>
+      <c r="E48" s="173" t="s">
+        <v>760</v>
+      </c>
+      <c r="F48" s="177" t="s">
+        <v>912</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H48" s="174" t="s">
+        <v>1017</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>1016</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D49" s="172" t="s">
+        <v>951</v>
+      </c>
+      <c r="E49" s="173" t="s">
+        <v>751</v>
+      </c>
+      <c r="F49" s="177" t="s">
+        <v>908</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="H49" s="174" t="s">
+        <v>1013</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>1015</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>929</v>
+      </c>
+      <c r="D50" s="172" t="s">
+        <v>930</v>
+      </c>
+      <c r="E50" s="173" t="s">
+        <v>886</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>931</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>932</v>
+      </c>
+      <c r="H50" s="174" t="s">
+        <v>937</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>952</v>
+      </c>
+      <c r="D51" s="172" t="s">
+        <v>951</v>
+      </c>
+      <c r="E51" s="173" t="s">
+        <v>950</v>
+      </c>
+      <c r="F51" s="175" t="s">
+        <v>949</v>
+      </c>
+      <c r="G51" s="171" t="s">
+        <v>948</v>
+      </c>
+      <c r="H51" s="174" t="s">
+        <v>939</v>
+      </c>
+      <c r="K51" s="2" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>953</v>
+      </c>
+      <c r="D52" s="172" t="s">
+        <v>954</v>
+      </c>
+      <c r="E52" s="173" t="s">
+        <v>955</v>
+      </c>
+      <c r="F52" s="175" t="s">
+        <v>956</v>
+      </c>
+      <c r="G52" s="171" t="s">
+        <v>957</v>
+      </c>
+      <c r="H52" s="174" t="s">
+        <v>945</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>923</v>
+      </c>
+      <c r="D53" s="172" t="s">
+        <v>924</v>
+      </c>
+      <c r="E53" s="176" t="s">
+        <v>728</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>925</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="H53" s="174" t="s">
+        <v>927</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>940</v>
+      </c>
+      <c r="D54" s="172" t="s">
+        <v>941</v>
+      </c>
+      <c r="E54" s="173" t="s">
+        <v>642</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>942</v>
+      </c>
+      <c r="G54" s="171" t="s">
+        <v>943</v>
+      </c>
+      <c r="H54" s="174" t="s">
+        <v>944</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>933</v>
+      </c>
+      <c r="D55" s="172" t="s">
+        <v>934</v>
+      </c>
+      <c r="E55" s="173" t="s">
+        <v>650</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>935</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>936</v>
+      </c>
+      <c r="H55" s="174" t="s">
+        <v>938</v>
+      </c>
+      <c r="K55" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>961</v>
+      </c>
+      <c r="D56" s="172" t="s">
+        <v>962</v>
+      </c>
+      <c r="E56" s="173" t="s">
+        <v>963</v>
+      </c>
+      <c r="F56" s="175" t="s">
+        <v>964</v>
+      </c>
+      <c r="G56" s="171" t="s">
+        <v>960</v>
+      </c>
+      <c r="H56" s="174" t="s">
+        <v>946</v>
+      </c>
+      <c r="K56" s="2" t="s">
+        <v>959</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="69" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA45D5F-33C6-4661-A5C7-F4257CE9578E}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13235,22 +16432,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{946B382E-0C83-4AA1-A09A-F99110E70DA1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" bestFit="1" customWidth="1"/>
@@ -13276,7 +16470,7 @@
     <col min="26" max="26" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="4.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="3.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13383,19 +16577,19 @@
       <c r="I2" s="40"/>
       <c r="J2" s="40"/>
       <c r="K2" s="40"/>
-      <c r="L2" s="168" t="s">
+      <c r="L2" s="169" t="s">
         <v>379</v>
       </c>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
+      <c r="M2" s="169"/>
+      <c r="N2" s="169"/>
       <c r="O2" s="41"/>
       <c r="P2" s="41"/>
-      <c r="Q2" s="169" t="s">
+      <c r="Q2" s="170" t="s">
         <v>380</v>
       </c>
-      <c r="R2" s="169"/>
-      <c r="S2" s="169"/>
-      <c r="T2" s="169"/>
+      <c r="R2" s="170"/>
+      <c r="S2" s="170"/>
+      <c r="T2" s="170"/>
       <c r="U2" s="40"/>
       <c r="V2" s="40"/>
       <c r="W2" s="40"/>
@@ -13442,12 +16636,12 @@
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
-      <c r="Q3" s="169" t="s">
+      <c r="Q3" s="170" t="s">
         <v>379</v>
       </c>
-      <c r="R3" s="169"/>
-      <c r="S3" s="169"/>
-      <c r="T3" s="169"/>
+      <c r="R3" s="170"/>
+      <c r="S3" s="170"/>
+      <c r="T3" s="170"/>
       <c r="U3" s="40"/>
       <c r="V3" s="40"/>
       <c r="W3" s="40"/>
@@ -13496,12 +16690,12 @@
       </c>
       <c r="O4" s="41"/>
       <c r="P4" s="41"/>
-      <c r="Q4" s="169" t="s">
+      <c r="Q4" s="170" t="s">
         <v>383</v>
       </c>
-      <c r="R4" s="169"/>
-      <c r="S4" s="169"/>
-      <c r="T4" s="169"/>
+      <c r="R4" s="170"/>
+      <c r="S4" s="170"/>
+      <c r="T4" s="170"/>
       <c r="U4" s="40"/>
       <c r="V4" s="40"/>
       <c r="W4" s="40"/>
@@ -14253,19 +17447,19 @@
       <c r="I16" s="40"/>
       <c r="J16" s="40"/>
       <c r="K16" s="40"/>
-      <c r="L16" s="168" t="s">
+      <c r="L16" s="169" t="s">
         <v>406</v>
       </c>
-      <c r="M16" s="168"/>
-      <c r="N16" s="168"/>
+      <c r="M16" s="169"/>
+      <c r="N16" s="169"/>
       <c r="O16" s="41"/>
       <c r="P16" s="41"/>
-      <c r="Q16" s="169" t="s">
+      <c r="Q16" s="170" t="s">
         <v>379</v>
       </c>
-      <c r="R16" s="169"/>
-      <c r="S16" s="169"/>
-      <c r="T16" s="169"/>
+      <c r="R16" s="170"/>
+      <c r="S16" s="170"/>
+      <c r="T16" s="170"/>
       <c r="U16" s="40"/>
       <c r="V16" s="40"/>
       <c r="W16" s="40"/>
@@ -15009,11 +18203,11 @@
       <c r="I30" s="77"/>
       <c r="J30" s="77"/>
       <c r="K30" s="77"/>
-      <c r="L30" s="168" t="s">
+      <c r="L30" s="169" t="s">
         <v>379</v>
       </c>
-      <c r="M30" s="168"/>
-      <c r="N30" s="168"/>
+      <c r="M30" s="169"/>
+      <c r="N30" s="169"/>
       <c r="O30" s="77" t="s">
         <v>494</v>
       </c>
@@ -15088,11 +18282,11 @@
       <c r="P31" s="69" t="s">
         <v>498</v>
       </c>
-      <c r="Q31" s="168" t="s">
+      <c r="Q31" s="169" t="s">
         <v>406</v>
       </c>
-      <c r="R31" s="168"/>
-      <c r="S31" s="168"/>
+      <c r="R31" s="169"/>
+      <c r="S31" s="169"/>
       <c r="T31" s="77"/>
       <c r="U31" s="77"/>
       <c r="V31" s="77"/>
@@ -15173,7 +18367,9 @@
     </row>
     <row r="34" spans="1:30">
       <c r="A34" s="69"/>
-      <c r="B34" s="69"/>
+      <c r="B34" s="74" t="s">
+        <v>625</v>
+      </c>
       <c r="C34" s="69" t="s">
         <v>322</v>
       </c>
@@ -15200,12 +18396,12 @@
       </c>
       <c r="O34" s="69"/>
       <c r="P34" s="69"/>
-      <c r="Q34" s="169" t="s">
+      <c r="Q34" s="170" t="s">
         <v>379</v>
       </c>
-      <c r="R34" s="169"/>
-      <c r="S34" s="169"/>
-      <c r="T34" s="169"/>
+      <c r="R34" s="170"/>
+      <c r="S34" s="170"/>
+      <c r="T34" s="170"/>
       <c r="U34" s="69"/>
       <c r="V34" s="69"/>
       <c r="W34" s="69"/>
@@ -15219,7 +18415,9 @@
     </row>
     <row r="35" spans="1:30">
       <c r="A35" s="69"/>
-      <c r="B35" s="69"/>
+      <c r="B35" s="74" t="s">
+        <v>626</v>
+      </c>
       <c r="C35" s="69" t="s">
         <v>321</v>
       </c>
@@ -15270,12 +18468,16 @@
       <c r="AB35" s="69" t="s">
         <v>324</v>
       </c>
-      <c r="AC35" s="70"/>
+      <c r="AC35" s="74" t="s">
+        <v>627</v>
+      </c>
       <c r="AD35" s="70"/>
     </row>
     <row r="36" spans="1:30">
       <c r="A36" s="69"/>
-      <c r="B36" s="69"/>
+      <c r="B36" s="74" t="s">
+        <v>628</v>
+      </c>
       <c r="C36" s="69" t="s">
         <v>325</v>
       </c>
@@ -15325,7 +18527,9 @@
       <c r="AB36" s="69" t="s">
         <v>323</v>
       </c>
-      <c r="AC36" s="70"/>
+      <c r="AC36" s="74" t="s">
+        <v>624</v>
+      </c>
       <c r="AD36" s="70"/>
     </row>
     <row r="37" spans="1:30">
@@ -15340,11 +18544,11 @@
       <c r="I37" s="69"/>
       <c r="J37" s="69"/>
       <c r="K37" s="69"/>
-      <c r="L37" s="168" t="s">
+      <c r="L37" s="169" t="s">
         <v>406</v>
       </c>
-      <c r="M37" s="168"/>
-      <c r="N37" s="168"/>
+      <c r="M37" s="169"/>
+      <c r="N37" s="169"/>
       <c r="O37" s="69"/>
       <c r="P37" s="69" t="s">
         <v>483</v>
@@ -15371,7 +18575,9 @@
       <c r="AB37" s="69" t="s">
         <v>320</v>
       </c>
-      <c r="AC37" s="70"/>
+      <c r="AC37" s="74" t="s">
+        <v>629</v>
+      </c>
       <c r="AD37" s="70"/>
     </row>
     <row r="38" spans="1:30">
@@ -15403,12 +18609,14 @@
       <c r="Z38" s="69"/>
       <c r="AA38" s="79"/>
       <c r="AB38" s="69"/>
-      <c r="AC38" s="70"/>
+      <c r="AC38" s="69"/>
       <c r="AD38" s="70"/>
     </row>
     <row r="39" spans="1:30">
       <c r="A39" s="69"/>
-      <c r="B39" s="69"/>
+      <c r="B39" s="74" t="s">
+        <v>625</v>
+      </c>
       <c r="C39" s="69" t="s">
         <v>322</v>
       </c>
@@ -15435,12 +18643,12 @@
       </c>
       <c r="O39" s="69"/>
       <c r="P39" s="69"/>
-      <c r="Q39" s="169" t="s">
+      <c r="Q39" s="170" t="s">
         <v>379</v>
       </c>
-      <c r="R39" s="169"/>
-      <c r="S39" s="169"/>
-      <c r="T39" s="169"/>
+      <c r="R39" s="170"/>
+      <c r="S39" s="170"/>
+      <c r="T39" s="170"/>
       <c r="U39" s="69"/>
       <c r="V39" s="69"/>
       <c r="W39" s="69"/>
@@ -15449,12 +18657,14 @@
       <c r="Z39" s="69"/>
       <c r="AA39" s="79"/>
       <c r="AB39" s="69"/>
-      <c r="AC39" s="70"/>
+      <c r="AC39" s="69"/>
       <c r="AD39" s="70"/>
     </row>
     <row r="40" spans="1:30">
       <c r="A40" s="69"/>
-      <c r="B40" s="69"/>
+      <c r="B40" s="74" t="s">
+        <v>626</v>
+      </c>
       <c r="C40" s="69" t="s">
         <v>321</v>
       </c>
@@ -15505,12 +18715,16 @@
       <c r="AB40" s="69" t="s">
         <v>324</v>
       </c>
-      <c r="AC40" s="70"/>
+      <c r="AC40" s="74" t="s">
+        <v>627</v>
+      </c>
       <c r="AD40" s="70"/>
     </row>
     <row r="41" spans="1:30">
       <c r="A41" s="69"/>
-      <c r="B41" s="69"/>
+      <c r="B41" s="74" t="s">
+        <v>628</v>
+      </c>
       <c r="C41" s="69" t="s">
         <v>325</v>
       </c>
@@ -15561,7 +18775,9 @@
       <c r="AB41" s="69" t="s">
         <v>323</v>
       </c>
-      <c r="AC41" s="70"/>
+      <c r="AC41" s="74" t="s">
+        <v>624</v>
+      </c>
       <c r="AD41" s="70"/>
     </row>
     <row r="42" spans="1:30">
@@ -15576,11 +18792,11 @@
       <c r="I42" s="69"/>
       <c r="J42" s="69"/>
       <c r="K42" s="69"/>
-      <c r="L42" s="168" t="s">
+      <c r="L42" s="169" t="s">
         <v>406</v>
       </c>
-      <c r="M42" s="168"/>
-      <c r="N42" s="168"/>
+      <c r="M42" s="169"/>
+      <c r="N42" s="169"/>
       <c r="O42" s="69"/>
       <c r="P42" s="69" t="s">
         <v>483</v>
@@ -15607,7 +18823,9 @@
       <c r="AB42" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="AC42" s="70"/>
+      <c r="AC42" s="74" t="s">
+        <v>623</v>
+      </c>
       <c r="AD42" s="70"/>
     </row>
   </sheetData>
@@ -15627,22 +18845,19 @@
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="70" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="68" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6218514E-45F9-4D23-9618-624D84C32829}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -17337,17 +20552,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85C3E308-4111-46EA-8E1C-A70B7BA29816}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M22" sqref="M22:M27"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
More MM pin info
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E20A553-08B7-4741-B002-78DA86B91147}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C97FBD8-ED2A-4867-A1B5-DD707BAA11A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="0" windowWidth="38430" windowHeight="19335" activeTab="6" xr2:uid="{42D65D2A-8D1C-4D07-8E53-DE4B585A6847}"/>
+    <workbookView xWindow="6480" yWindow="450" windowWidth="24900" windowHeight="20220" firstSheet="3" activeTab="6" xr2:uid="{42D65D2A-8D1C-4D07-8E53-DE4B585A6847}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Micromod" sheetId="12" r:id="rId8"/>
     <sheet name="MicroMod - Mux" sheetId="15" r:id="rId9"/>
     <sheet name="MicroMod - GPIO" sheetId="13" r:id="rId10"/>
+    <sheet name="Micromod - MM Pin" sheetId="16" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5330" uniqueCount="1113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5957" uniqueCount="1148">
   <si>
     <t/>
   </si>
@@ -3390,6 +3391,111 @@
   </si>
   <si>
     <t>LPI2C2_SDA</t>
+  </si>
+  <si>
+    <t>MM Pin</t>
+  </si>
+  <si>
+    <t>USB Pins</t>
+  </si>
+  <si>
+    <t>HUSB D+</t>
+  </si>
+  <si>
+    <t>USB D+</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>USB D-</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>HUSB D-</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -4246,27 +4352,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B33FA5B1-4CE6-4A8A-BADE-2FB8021A9AC4}"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="119">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -4312,6 +4400,75 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -5596,163 +5753,190 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M59" totalsRowShown="0" headerRowDxfId="101" dataDxfId="100">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ECA8428E-B0AF-455D-8C53-27C78090EA97}" name="Table4" displayName="Table4" ref="A1:M59" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
   <autoFilter ref="A1:M59" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="99"/>
-    <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="98"/>
-    <tableColumn id="3" xr3:uid="{F9478000-D09D-4158-8962-151C792B9115}" name="GPIO" dataDxfId="97"/>
-    <tableColumn id="4" xr3:uid="{EEB23B63-7C82-4BC1-80FE-826F4A02B99D}" name="Serial" dataDxfId="96"/>
-    <tableColumn id="5" xr3:uid="{1D7F4122-4922-476A-8C8E-378628CB944B}" name="I2C" dataDxfId="95"/>
-    <tableColumn id="6" xr3:uid="{8B2BA30D-AD74-4591-9119-1A5E4B5E627D}" name="SPI" dataDxfId="94"/>
-    <tableColumn id="7" xr3:uid="{50F13DDA-AECC-4873-B8BF-BF29B9FA3A1D}" name="PWM" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{99EA318C-72FB-4EFD-9E14-9B5211643911}" name="CAN" dataDxfId="92"/>
-    <tableColumn id="9" xr3:uid="{DC6B9277-B97B-4891-B766-22B3DE725408}" name="Audio" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{1446B065-9F8B-426F-A535-611F882183B3}" name="XBAR" dataDxfId="90"/>
-    <tableColumn id="11" xr3:uid="{DC1C2DEB-A4BD-44FE-B52D-E7ABF3D565E7}" name="FlexIO" dataDxfId="89"/>
-    <tableColumn id="12" xr3:uid="{2A37AD20-1A78-4C16-9F5C-DBB6ECB30C3F}" name="Analog" dataDxfId="88"/>
-    <tableColumn id="13" xr3:uid="{E0FD363E-BD42-46D9-8D08-5AE1FF584E61}" name="SD/CSI/LCD" dataDxfId="87"/>
+    <tableColumn id="1" xr3:uid="{A16C6DF5-C3BD-4138-ACBB-ACE061AC5443}" name="Pin" dataDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{CC5B6B65-7928-436A-BED0-58A0574EBBC6}" name="Name" dataDxfId="115"/>
+    <tableColumn id="3" xr3:uid="{F9478000-D09D-4158-8962-151C792B9115}" name="GPIO" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{EEB23B63-7C82-4BC1-80FE-826F4A02B99D}" name="Serial" dataDxfId="113"/>
+    <tableColumn id="5" xr3:uid="{1D7F4122-4922-476A-8C8E-378628CB944B}" name="I2C" dataDxfId="112"/>
+    <tableColumn id="6" xr3:uid="{8B2BA30D-AD74-4591-9119-1A5E4B5E627D}" name="SPI" dataDxfId="111"/>
+    <tableColumn id="7" xr3:uid="{50F13DDA-AECC-4873-B8BF-BF29B9FA3A1D}" name="PWM" dataDxfId="110"/>
+    <tableColumn id="8" xr3:uid="{99EA318C-72FB-4EFD-9E14-9B5211643911}" name="CAN" dataDxfId="109"/>
+    <tableColumn id="9" xr3:uid="{DC6B9277-B97B-4891-B766-22B3DE725408}" name="Audio" dataDxfId="108"/>
+    <tableColumn id="10" xr3:uid="{1446B065-9F8B-426F-A535-611F882183B3}" name="XBAR" dataDxfId="107"/>
+    <tableColumn id="11" xr3:uid="{DC1C2DEB-A4BD-44FE-B52D-E7ABF3D565E7}" name="FlexIO" dataDxfId="106"/>
+    <tableColumn id="12" xr3:uid="{2A37AD20-1A78-4C16-9F5C-DBB6ECB30C3F}" name="Analog" dataDxfId="105"/>
+    <tableColumn id="13" xr3:uid="{E0FD363E-BD42-46D9-8D08-5AE1FF584E61}" name="SD/CSI/LCD" dataDxfId="104"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F6923B6-4F50-44A0-85F6-B6E706E61BCE}" name="Table46" displayName="Table46" ref="A1:L56" totalsRowShown="0" headerRowDxfId="86" dataDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{1F6923B6-4F50-44A0-85F6-B6E706E61BCE}" name="Table46" displayName="Table46" ref="A1:L56" totalsRowShown="0" headerRowDxfId="103" dataDxfId="102">
   <autoFilter ref="A1:L56" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L56">
     <sortCondition ref="A2:A56"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{2FF2926D-76AF-4A43-864C-1929BFD0A68A}" name="Pin" dataDxfId="84"/>
-    <tableColumn id="2" xr3:uid="{DBD9783C-68D1-4579-8AC6-92B0E31BC1E2}" name="Name" dataDxfId="83"/>
-    <tableColumn id="14" xr3:uid="{76C17CD9-2E7D-4846-9BD8-D8AF2AEDA0DE}" name="ALT0" dataDxfId="82"/>
-    <tableColumn id="15" xr3:uid="{BE004B08-9CAD-42A6-BD65-6B48419A2E82}" name="ALt1" dataDxfId="81"/>
-    <tableColumn id="16" xr3:uid="{98599106-77C1-42F5-919C-AAB320F80A47}" name="ALT2" dataDxfId="80"/>
-    <tableColumn id="17" xr3:uid="{32C3D940-EA13-46FC-A402-814E1B152721}" name="ALT3" dataDxfId="79"/>
-    <tableColumn id="18" xr3:uid="{B2EC6B0E-2511-4B8C-A8E1-A6F7BBE97AA4}" name="ALT4" dataDxfId="78"/>
-    <tableColumn id="19" xr3:uid="{7AC3B94D-0445-4DF5-9989-6936927A50E1}" name="Alt5" dataDxfId="77"/>
-    <tableColumn id="20" xr3:uid="{CCFEC2C2-FBF1-474A-92CD-A58A299FF456}" name="ALT6" dataDxfId="76"/>
-    <tableColumn id="21" xr3:uid="{B108228D-000D-4A0C-82EF-0E977A0DF892}" name="ALT7" dataDxfId="75"/>
-    <tableColumn id="22" xr3:uid="{A38F3C31-4856-4D35-AA59-6E24E6DECC0C}" name="ALT8" dataDxfId="74"/>
-    <tableColumn id="23" xr3:uid="{C86B93AE-1D5F-4DE8-A58A-8219019947DF}" name="ALT9" dataDxfId="73"/>
+    <tableColumn id="1" xr3:uid="{2FF2926D-76AF-4A43-864C-1929BFD0A68A}" name="Pin" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{DBD9783C-68D1-4579-8AC6-92B0E31BC1E2}" name="Name" dataDxfId="100"/>
+    <tableColumn id="14" xr3:uid="{76C17CD9-2E7D-4846-9BD8-D8AF2AEDA0DE}" name="ALT0" dataDxfId="99"/>
+    <tableColumn id="15" xr3:uid="{BE004B08-9CAD-42A6-BD65-6B48419A2E82}" name="ALt1" dataDxfId="98"/>
+    <tableColumn id="16" xr3:uid="{98599106-77C1-42F5-919C-AAB320F80A47}" name="ALT2" dataDxfId="97"/>
+    <tableColumn id="17" xr3:uid="{32C3D940-EA13-46FC-A402-814E1B152721}" name="ALT3" dataDxfId="96"/>
+    <tableColumn id="18" xr3:uid="{B2EC6B0E-2511-4B8C-A8E1-A6F7BBE97AA4}" name="ALT4" dataDxfId="95"/>
+    <tableColumn id="19" xr3:uid="{7AC3B94D-0445-4DF5-9989-6936927A50E1}" name="Alt5" dataDxfId="94"/>
+    <tableColumn id="20" xr3:uid="{CCFEC2C2-FBF1-474A-92CD-A58A299FF456}" name="ALT6" dataDxfId="93"/>
+    <tableColumn id="21" xr3:uid="{B108228D-000D-4A0C-82EF-0E977A0DF892}" name="ALT7" dataDxfId="92"/>
+    <tableColumn id="22" xr3:uid="{A38F3C31-4856-4D35-AA59-6E24E6DECC0C}" name="ALT8" dataDxfId="91"/>
+    <tableColumn id="23" xr3:uid="{C86B93AE-1D5F-4DE8-A58A-8219019947DF}" name="ALT9" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D58B21B-5C22-4FA1-A362-68DAB3B97BB9}" name="Table6" displayName="Table6" ref="A60:L114" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{9D58B21B-5C22-4FA1-A362-68DAB3B97BB9}" name="Table6" displayName="Table6" ref="A60:L114" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="A60:L114" xr:uid="{2169E4F2-D9D8-454C-A0D1-E6674FA9DAD9}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B7A125DB-8197-4137-927D-01B57F6D2DB8}" name="Column1" dataDxfId="70"/>
-    <tableColumn id="2" xr3:uid="{27772364-1ECB-4022-9501-5B18CACBEEB9}" name="Column2" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{F7D07088-D82A-40E7-8DE6-9364D8606B68}" name="Column3" dataDxfId="68"/>
-    <tableColumn id="4" xr3:uid="{DB82474D-E7C1-4AE9-86FB-D179BABB9BA5}" name="Column4" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{CD08E255-64CB-483F-B70A-D94A461D1BB4}" name="Column5" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{581A2802-7807-41F6-B19C-50FB2EAB3F37}" name="Column6" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{4FAAAD73-A912-4138-A798-2F03FC0F267A}" name="Column7" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{A7D6005F-9DA2-4C22-A99C-8E33EE2A9F9E}" name="Column8" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{5488E0B9-52D2-4799-8B6F-2812F7462E6C}" name="Column9" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{031DDFB5-CE19-4B43-875F-E09137CA5FB1}" name="Column10" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{597C4812-2955-4E96-8267-9B6B0B972A3A}" name="Column11" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{E319C875-3FF9-4AB9-88BD-B1B921E6B585}" name="Column12" dataDxfId="59"/>
+    <tableColumn id="1" xr3:uid="{B7A125DB-8197-4137-927D-01B57F6D2DB8}" name="Column1" dataDxfId="87"/>
+    <tableColumn id="2" xr3:uid="{27772364-1ECB-4022-9501-5B18CACBEEB9}" name="Column2" dataDxfId="86"/>
+    <tableColumn id="3" xr3:uid="{F7D07088-D82A-40E7-8DE6-9364D8606B68}" name="Column3" dataDxfId="85"/>
+    <tableColumn id="4" xr3:uid="{DB82474D-E7C1-4AE9-86FB-D179BABB9BA5}" name="Column4" dataDxfId="84"/>
+    <tableColumn id="5" xr3:uid="{CD08E255-64CB-483F-B70A-D94A461D1BB4}" name="Column5" dataDxfId="83"/>
+    <tableColumn id="6" xr3:uid="{581A2802-7807-41F6-B19C-50FB2EAB3F37}" name="Column6" dataDxfId="82"/>
+    <tableColumn id="7" xr3:uid="{4FAAAD73-A912-4138-A798-2F03FC0F267A}" name="Column7" dataDxfId="81"/>
+    <tableColumn id="8" xr3:uid="{A7D6005F-9DA2-4C22-A99C-8E33EE2A9F9E}" name="Column8" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{5488E0B9-52D2-4799-8B6F-2812F7462E6C}" name="Column9" dataDxfId="79"/>
+    <tableColumn id="10" xr3:uid="{031DDFB5-CE19-4B43-875F-E09137CA5FB1}" name="Column10" dataDxfId="78"/>
+    <tableColumn id="11" xr3:uid="{597C4812-2955-4E96-8267-9B6B0B972A3A}" name="Column11" dataDxfId="77"/>
+    <tableColumn id="12" xr3:uid="{E319C875-3FF9-4AB9-88BD-B1B921E6B585}" name="Column12" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FBF0D35-2CE8-4056-99C9-8BA06E84A4F2}" name="Table44" displayName="Table44" ref="A1:M57" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0FBF0D35-2CE8-4056-99C9-8BA06E84A4F2}" name="Table44" displayName="Table44" ref="A1:M57" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="A1:M57" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M57">
     <sortCondition ref="C2:C57"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{1F964F0D-83A4-459C-9496-6A1229BDD1CA}" name="Pin" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{29F07050-DC12-4F4A-93C9-84EA4D24FC14}" name="Name" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{2491D004-6B1F-44DA-9E9A-E599F694FEC5}" name="GPIO" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{3AF6E798-9147-4AB4-936B-73FB56DAADDC}" name="Serial" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{F90CC261-4748-4F6F-84BC-1F4507953F2B}" name="I2C" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{1228CC1B-8420-4510-8B20-1B5A755F93F4}" name="SPI" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{B5235724-C934-4085-BA21-9D87B83403F0}" name="PWM" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{E6A78068-999F-4EB1-BC47-E0339ADDEB19}" name="CAN" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{676FF9FA-1D40-4E7E-9217-0AB090DAD93E}" name="Audio" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{B75CFCB1-0F3D-4A48-B9FB-BE8C97A0D331}" name="XBAR" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{B6165631-5DF9-46E6-AFC1-E89804AF65C9}" name="FlexIO" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{0A677E09-F667-440D-83B9-6B28A7D0361A}" name="Analog" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{CACC907E-B7D3-4542-AA4D-60AA34159A4E}" name="SD/CSI/LCD" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{1F964F0D-83A4-459C-9496-6A1229BDD1CA}" name="Pin" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{29F07050-DC12-4F4A-93C9-84EA4D24FC14}" name="Name" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{2491D004-6B1F-44DA-9E9A-E599F694FEC5}" name="GPIO" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{3AF6E798-9147-4AB4-936B-73FB56DAADDC}" name="Serial" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{F90CC261-4748-4F6F-84BC-1F4507953F2B}" name="I2C" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{1228CC1B-8420-4510-8B20-1B5A755F93F4}" name="SPI" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{B5235724-C934-4085-BA21-9D87B83403F0}" name="PWM" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{E6A78068-999F-4EB1-BC47-E0339ADDEB19}" name="CAN" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{676FF9FA-1D40-4E7E-9217-0AB090DAD93E}" name="Audio" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{B75CFCB1-0F3D-4A48-B9FB-BE8C97A0D331}" name="XBAR" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{B6165631-5DF9-46E6-AFC1-E89804AF65C9}" name="FlexIO" dataDxfId="63"/>
+    <tableColumn id="12" xr3:uid="{0A677E09-F667-440D-83B9-6B28A7D0361A}" name="Analog" dataDxfId="62"/>
+    <tableColumn id="13" xr3:uid="{CACC907E-B7D3-4542-AA4D-60AA34159A4E}" name="SD/CSI/LCD" dataDxfId="61"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A31209C-0744-40DF-BEA2-51480749F938}" name="Table42" displayName="Table42" ref="A1:M50" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:M50" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
-  <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{1FA4817C-7344-4B9E-9BD4-442E849ED7E8}" name="Pin" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{4AD2AB58-241E-4CFC-A1C5-16943CF49E13}" name="Name" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{F71AF128-9344-4146-AFB8-763C46188B4F}" name="GPIO" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{09C9E89C-BD40-41CD-BCD9-FBFAF33CB6D8}" name="Serial" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{3E815C42-FCE2-489B-91D3-683FE184F105}" name="I2C" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{FEEE2127-D6CF-4F96-819F-1B287988C35D}" name="SPI" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{73226C5A-CBE1-49F8-9481-E18F0FD235CE}" name="PWM" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{9F8D0763-B9D7-4C0A-AED0-834476CC37CA}" name="CAN" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{FB55AA45-516A-4120-8948-A5AF8C8A54DD}" name="Audio" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{FE9C4536-9536-418C-8C69-E56A803D4E2B}" name="XBAR" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{80808062-5E4F-4FCA-BB01-53A3D23512F9}" name="FlexIO" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{CC4496D7-52BC-4F94-AA69-73D82D9E163E}" name="Analog" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{F42DD222-DD94-4C47-A5E3-AAB2345C9AEB}" name="SD/CSI/LCD" dataDxfId="29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{9A31209C-0744-40DF-BEA2-51480749F938}" name="Table42" displayName="Table42" ref="A1:N55" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
+  <autoFilter ref="A1:N55" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{1FA4817C-7344-4B9E-9BD4-442E849ED7E8}" name="Pin" dataDxfId="58"/>
+    <tableColumn id="14" xr3:uid="{D04EE676-F5DF-4C67-A077-D3541E71989D}" name="MM Pin" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{4AD2AB58-241E-4CFC-A1C5-16943CF49E13}" name="Name" dataDxfId="57"/>
+    <tableColumn id="3" xr3:uid="{F71AF128-9344-4146-AFB8-763C46188B4F}" name="GPIO" dataDxfId="56"/>
+    <tableColumn id="4" xr3:uid="{09C9E89C-BD40-41CD-BCD9-FBFAF33CB6D8}" name="Serial" dataDxfId="55"/>
+    <tableColumn id="5" xr3:uid="{3E815C42-FCE2-489B-91D3-683FE184F105}" name="I2C" dataDxfId="54"/>
+    <tableColumn id="6" xr3:uid="{FEEE2127-D6CF-4F96-819F-1B287988C35D}" name="SPI" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{73226C5A-CBE1-49F8-9481-E18F0FD235CE}" name="PWM" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{9F8D0763-B9D7-4C0A-AED0-834476CC37CA}" name="CAN" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{FB55AA45-516A-4120-8948-A5AF8C8A54DD}" name="Audio" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{FE9C4536-9536-418C-8C69-E56A803D4E2B}" name="XBAR" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{80808062-5E4F-4FCA-BB01-53A3D23512F9}" name="FlexIO" dataDxfId="48"/>
+    <tableColumn id="12" xr3:uid="{CC4496D7-52BC-4F94-AA69-73D82D9E163E}" name="Analog" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{F42DD222-DD94-4C47-A5E3-AAB2345C9AEB}" name="SD/CSI/LCD" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BFF0D0DE-E703-498E-803F-134DCC0D2DF8}" name="Table468" displayName="Table468" ref="A1:L49" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{BFF0D0DE-E703-498E-803F-134DCC0D2DF8}" name="Table468" displayName="Table468" ref="A1:L49" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
   <autoFilter ref="A1:L49" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L49">
     <sortCondition ref="A2:A49"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{097CAC07-ACCE-443D-94A7-419C66E4E3C3}" name="Pin" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{5A846C30-C7ED-4854-BD00-BEAC4E2718CC}" name="Name" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{90E2F772-E066-4194-91FF-2DC2496A8214}" name="ALT0" dataDxfId="9"/>
-    <tableColumn id="15" xr3:uid="{39A2F77B-1C42-48FD-8856-5612AC205AB8}" name="ALt1" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{456EFAA6-A7BA-4400-8AE0-E1091C7520F8}" name="ALT2" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{1612AABD-9788-4905-AE0F-27CF7F79F402}" name="ALT3" dataDxfId="6"/>
-    <tableColumn id="18" xr3:uid="{C0AF6905-CE1B-4C10-ACC0-ECD3B61A08C6}" name="ALT4" dataDxfId="5"/>
-    <tableColumn id="19" xr3:uid="{DCD0F4A0-37B0-423C-B04C-3D3B377F8511}" name="Alt5" dataDxfId="4"/>
-    <tableColumn id="20" xr3:uid="{186BE6AA-F7E6-4E55-8E78-A4AE5C15635C}" name="ALT6" dataDxfId="3"/>
-    <tableColumn id="21" xr3:uid="{66A339C3-DD04-416C-9DFB-90EB0C4212B2}" name="ALT7" dataDxfId="2"/>
-    <tableColumn id="22" xr3:uid="{4D745D3A-F911-40A2-9BC8-AA687438894C}" name="ALT8" dataDxfId="1"/>
-    <tableColumn id="23" xr3:uid="{27E14851-7939-422A-8CF4-8CA3F0574DB5}" name="ALT9" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{097CAC07-ACCE-443D-94A7-419C66E4E3C3}" name="Pin" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{5A846C30-C7ED-4854-BD00-BEAC4E2718CC}" name="Name" dataDxfId="42"/>
+    <tableColumn id="14" xr3:uid="{90E2F772-E066-4194-91FF-2DC2496A8214}" name="ALT0" dataDxfId="41"/>
+    <tableColumn id="15" xr3:uid="{39A2F77B-1C42-48FD-8856-5612AC205AB8}" name="ALt1" dataDxfId="40"/>
+    <tableColumn id="16" xr3:uid="{456EFAA6-A7BA-4400-8AE0-E1091C7520F8}" name="ALT2" dataDxfId="39"/>
+    <tableColumn id="17" xr3:uid="{1612AABD-9788-4905-AE0F-27CF7F79F402}" name="ALT3" dataDxfId="38"/>
+    <tableColumn id="18" xr3:uid="{C0AF6905-CE1B-4C10-ACC0-ECD3B61A08C6}" name="ALT4" dataDxfId="37"/>
+    <tableColumn id="19" xr3:uid="{DCD0F4A0-37B0-423C-B04C-3D3B377F8511}" name="Alt5" dataDxfId="36"/>
+    <tableColumn id="20" xr3:uid="{186BE6AA-F7E6-4E55-8E78-A4AE5C15635C}" name="ALT6" dataDxfId="35"/>
+    <tableColumn id="21" xr3:uid="{66A339C3-DD04-416C-9DFB-90EB0C4212B2}" name="ALT7" dataDxfId="34"/>
+    <tableColumn id="22" xr3:uid="{4D745D3A-F911-40A2-9BC8-AA687438894C}" name="ALT8" dataDxfId="33"/>
+    <tableColumn id="23" xr3:uid="{27E14851-7939-422A-8CF4-8CA3F0574DB5}" name="ALT9" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A83D5ACF-E653-4DB3-8FE2-1B01953FA219}" name="Table423" displayName="Table423" ref="A1:M47" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A83D5ACF-E653-4DB3-8FE2-1B01953FA219}" name="Table423" displayName="Table423" ref="A1:M47" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:M47" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M47">
     <sortCondition ref="C1:C47"/>
   </sortState>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{E235028C-ACE8-4A1F-98BD-F9271F19A1D2}" name="Pin" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{1F222945-3BCF-4053-98AF-648BD8687B08}" name="Name" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{D441F102-0187-41C3-A599-5422C2DA8755}" name="GPIO" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{06DF530B-4B4E-44C9-8DDE-3AD326E1E14F}" name="Serial" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{FAD43D46-EB5B-473B-91C4-485BEB1E341A}" name="I2C" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{167987D0-794F-449D-A9C6-10A4C507490A}" name="SPI" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{FA011A7B-F201-400A-9944-07B86FDE3CC8}" name="PWM" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{2C77510B-E776-4A66-8E95-E299D8840634}" name="CAN" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{23957E32-3ECD-4002-9B52-2A6AC70592CA}" name="Audio" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{9E86FA4C-0EE4-4197-8193-1D2D26419192}" name="XBAR" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{91907E0A-BB1E-4AD4-A578-4E156B00B089}" name="FlexIO" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{B5129136-343E-4C0E-B257-CC80A2575D2C}" name="Analog" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{018BA245-1B76-45AD-BE6D-82A0CBAC04E3}" name="SD/CSI/LCD" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{E235028C-ACE8-4A1F-98BD-F9271F19A1D2}" name="Pin" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{1F222945-3BCF-4053-98AF-648BD8687B08}" name="Name" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{D441F102-0187-41C3-A599-5422C2DA8755}" name="GPIO" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{06DF530B-4B4E-44C9-8DDE-3AD326E1E14F}" name="Serial" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{FAD43D46-EB5B-473B-91C4-485BEB1E341A}" name="I2C" dataDxfId="25"/>
+    <tableColumn id="6" xr3:uid="{167987D0-794F-449D-A9C6-10A4C507490A}" name="SPI" dataDxfId="24"/>
+    <tableColumn id="7" xr3:uid="{FA011A7B-F201-400A-9944-07B86FDE3CC8}" name="PWM" dataDxfId="23"/>
+    <tableColumn id="8" xr3:uid="{2C77510B-E776-4A66-8E95-E299D8840634}" name="CAN" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{23957E32-3ECD-4002-9B52-2A6AC70592CA}" name="Audio" dataDxfId="21"/>
+    <tableColumn id="10" xr3:uid="{9E86FA4C-0EE4-4197-8193-1D2D26419192}" name="XBAR" dataDxfId="20"/>
+    <tableColumn id="11" xr3:uid="{91907E0A-BB1E-4AD4-A578-4E156B00B089}" name="FlexIO" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{B5129136-343E-4C0E-B257-CC80A2575D2C}" name="Analog" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{018BA245-1B76-45AD-BE6D-82A0CBAC04E3}" name="SD/CSI/LCD" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2F41AECC-5712-4BCA-A596-9C0CB1293C3C}" name="Table429" displayName="Table429" ref="A1:N55" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N55" xr:uid="{2C4157B9-E38B-485C-A285-A102A142EA99}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N55">
+    <sortCondition ref="B2:B55"/>
+  </sortState>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{37ED9441-AADD-45A5-9B8A-66F6628F8231}" name="Pin" dataDxfId="13"/>
+    <tableColumn id="14" xr3:uid="{09562C75-1038-4785-B8A3-8DAFBAFB30B3}" name="MM Pin" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{29631A29-5E49-4960-8F77-1258826E97D5}" name="Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{E952EDD8-4192-4D61-A812-8240B62D5B81}" name="GPIO" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{9E640BBA-D605-49E5-9A21-5217214971DE}" name="Serial" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{D3FE2504-C0B1-49F9-8DA7-539544C4C0F2}" name="I2C" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{1DEA927C-E26E-4F66-9175-F56020C92232}" name="SPI" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{37FF36DC-3436-40BD-82FA-D695E413BB22}" name="PWM" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{747496B3-BC07-4D95-9679-D89F36304C4A}" name="CAN" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{3CE5B864-8FD7-4D08-B650-9908E11A92F2}" name="Audio" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{B1DE82DD-6EF5-4255-A071-D1D816FC455A}" name="XBAR" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{700AFAFF-A2D6-46AE-B456-2DE96305B686}" name="FlexIO" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{D9A0BB67-82F6-462F-A31C-3DF1CBE7F3A7}" name="Analog" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{2B30549A-F3EF-4AEA-A629-039D03297FA8}" name="SD/CSI/LCD" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9377,6 +9561,1921 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DC7C86E-1B9F-4431-A4B3-3BF96BDF1992}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N55"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1117</v>
+      </c>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1119</v>
+      </c>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="2">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="N13" s="30" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="N14" s="30" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C20" t="s">
+        <v>578</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3.23</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D23" s="2">
+        <v>3.22</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="N28" s="30" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="2">
+        <v>8</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14">
+      <c r="A34" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
+      <c r="A35" s="2">
+        <v>7</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14">
+      <c r="A36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="N37" s="30" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
+      <c r="A38" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
+      <c r="A39" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="K41" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
+      <c r="A42" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N43" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
+      <c r="A44" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
+      <c r="A45" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
+      <c r="A46" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14">
+      <c r="A47" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N47" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
+      <c r="A48" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="A49" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="A50" s="2">
+        <v>6</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K52" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="N55" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="69" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A35696-03D0-445C-9164-20930A935361}">
   <dimension ref="A1:M42"/>
@@ -22995,10 +25094,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:B50"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23016,138 +25115,150 @@
     <col min="11" max="11" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.85546875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="J2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="L2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="M2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="J3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="L3" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="M3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E4" s="2" t="s">
         <v>0</v>
       </c>
@@ -23155,37 +25266,41 @@
         <v>0</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="L4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="M4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
@@ -23193,37 +25308,41 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="M5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
@@ -23231,37 +25350,41 @@
         <v>0</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="M6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E7" s="2" t="s">
         <v>0</v>
       </c>
@@ -23269,37 +25392,41 @@
         <v>0</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="M7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
       </c>
@@ -23307,101 +25434,112 @@
         <v>0</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14">
       <c r="A9" s="2">
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="2">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E11" s="2" t="s">
         <v>0</v>
       </c>
@@ -23409,277 +25547,300 @@
         <v>0</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="L11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="M12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14">
       <c r="A13" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="J13" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L13" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="M13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14">
       <c r="A14" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="M14" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14">
       <c r="A15" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="J15" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="M15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14">
       <c r="A16" s="2" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F16" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="J16" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F17" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="J17" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="G18" s="2" t="s">
         <v>0</v>
       </c>
@@ -23687,40 +25848,43 @@
         <v>0</v>
       </c>
       <c r="I18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J18" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="M18" s="30" t="s">
+      <c r="N18" s="30" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:14">
       <c r="A19" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="G19" s="2" t="s">
         <v>0</v>
       </c>
@@ -23728,46 +25892,49 @@
         <v>0</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="J19" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K19" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="N19" s="30" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:14">
       <c r="A20" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="G20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I20" s="2" t="s">
         <v>0</v>
       </c>
@@ -23775,37 +25942,41 @@
         <v>0</v>
       </c>
       <c r="K20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>1123</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="G21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I21" s="2" t="s">
         <v>0</v>
       </c>
@@ -23813,28 +25984,32 @@
         <v>0</v>
       </c>
       <c r="K21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="M21" s="2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F22" s="2" t="s">
         <v>0</v>
       </c>
@@ -23845,34 +26020,38 @@
         <v>0</v>
       </c>
       <c r="I22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="J22" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K22" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="L22" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F23" s="2" t="s">
         <v>0</v>
       </c>
@@ -23883,31 +26062,35 @@
         <v>0</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J23" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="L23" s="2" t="s">
+      <c r="M23" s="2" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="24" spans="1:13">
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E24" s="2" t="s">
         <v>0</v>
       </c>
@@ -23915,40 +26098,43 @@
         <v>0</v>
       </c>
       <c r="G24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="I24" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="J24" s="2" t="s">
         <v>0</v>
       </c>
       <c r="K24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="L24" s="2" t="s">
+      <c r="M24" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="M24" s="30" t="s">
+      <c r="N24" s="30" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:14">
       <c r="A25" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E25" s="2" t="s">
         <v>0</v>
       </c>
@@ -23956,42 +26142,42 @@
         <v>0</v>
       </c>
       <c r="G25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="I25" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="J25" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="J25" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L25" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="L25" s="2" t="s">
+      <c r="M25" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="N25" s="30" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:14">
       <c r="A26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="C26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>13</v>
@@ -24003,43 +26189,47 @@
         <v>13</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:13">
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="G27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I27" s="2" t="s">
         <v>0</v>
       </c>
@@ -24050,37 +26240,41 @@
         <v>0</v>
       </c>
       <c r="L27" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="28" spans="1:13">
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="2" t="s">
         <v>156</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="G28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="H28" s="2" t="s">
+      <c r="I28" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="J28" s="2" t="s">
         <v>0</v>
       </c>
@@ -24088,110 +26282,122 @@
         <v>0</v>
       </c>
       <c r="L28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" s="2" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="29" spans="1:13">
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="H29" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K29" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="L29" s="2" t="s">
+      <c r="M29" s="2" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="30" spans="1:13">
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="2" t="s">
         <v>167</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>1146</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="H30" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J30" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="J30" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="K30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="L30" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="L30" s="2" t="s">
+      <c r="M30" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="31" spans="1:13">
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="2" t="s">
         <v>172</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F31" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I31" s="2" t="s">
         <v>0</v>
       </c>
@@ -24204,32 +26410,36 @@
       <c r="L31" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="M31" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="2" t="s">
         <v>176</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="E32" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="H32" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I32" s="2" t="s">
         <v>0</v>
       </c>
@@ -24242,90 +26452,102 @@
       <c r="L32" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:13">
+      <c r="M32" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" s="2" t="s">
         <v>180</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C33" s="2">
+      <c r="D33" s="2">
         <v>3.23</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F33" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="I33" s="2" t="s">
+      <c r="J33" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="K33" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="K33" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="L33" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:13">
+      <c r="M33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C34" s="2">
+      <c r="D34" s="2">
         <v>3.22</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="F34" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="J34" s="2" t="s">
+      <c r="K34" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="K34" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="L34" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:13">
+      <c r="M34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E35" s="2" t="s">
         <v>0</v>
       </c>
@@ -24339,34 +26561,37 @@
         <v>0</v>
       </c>
       <c r="I35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J35" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="J35" s="2" t="s">
+      <c r="K35" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="K35" s="2" t="s">
+      <c r="L35" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="L35" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="M35" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N35" s="2" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:14">
       <c r="A36" s="2" t="s">
         <v>192</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>1145</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="2">
+      <c r="D36" s="2">
         <v>4.7</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E36" s="2" t="s">
         <v>0</v>
       </c>
@@ -24374,315 +26599,401 @@
         <v>0</v>
       </c>
       <c r="G36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H36" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="I36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J36" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J36" s="2" t="s">
+      <c r="K36" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K36" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="L36" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13">
+      <c r="M36" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" s="4" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="38" spans="1:13">
+      <c r="B37" s="4"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" s="2" t="s">
         <v>210</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="E38" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="G38" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="J38" s="2" t="s">
+      <c r="K38" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="M38" s="2" t="s">
+      <c r="N38" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:14">
       <c r="A39" s="2" t="s">
         <v>211</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>1129</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="J39" s="2" t="s">
+      <c r="K39" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M39" s="2" t="s">
+      <c r="N39" s="2" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:14">
       <c r="A40" s="2" t="s">
         <v>317</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="H40" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="J40" s="2" t="s">
+      <c r="K40" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="M40" s="2" t="s">
+      <c r="N40" s="2" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:14">
       <c r="A41" s="2" t="s">
         <v>318</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="H41" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="J41" s="2" t="s">
+      <c r="K41" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="M41" s="2" t="s">
+      <c r="N41" s="2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:14">
       <c r="A42" s="2" t="s">
         <v>574</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="J42" s="2" t="s">
+      <c r="K42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M42" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:14">
       <c r="A43" s="2" t="s">
         <v>575</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="J43" s="2" t="s">
+      <c r="K43" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M43" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:14">
       <c r="A44" s="4" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="45" spans="1:13">
+      <c r="B44" s="4"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="C45" t="s">
         <v>578</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="K45" s="2" t="s">
+      <c r="L45" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="M45" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:14">
       <c r="A46" s="2" t="s">
         <v>577</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="K46" s="2" t="s">
+      <c r="L46" s="2" t="s">
         <v>596</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:14">
       <c r="A47" s="2" t="s">
         <v>347</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>580</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K47" s="2" t="s">
+      <c r="L47" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="M47" s="2" t="s">
+      <c r="N47" s="2" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:14">
       <c r="A48" s="2" t="s">
         <v>348</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>581</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="H48" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K48" s="2" t="s">
+      <c r="L48" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:14">
       <c r="A49" s="2" t="s">
         <v>349</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="G49" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="K49" s="2" t="s">
+      <c r="L49" s="2" t="s">
         <v>600</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="N49" s="2" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:14">
       <c r="A50" s="2" t="s">
         <v>350</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="G50" s="2" t="s">
+      <c r="H50" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="K50" s="2" t="s">
+      <c r="L50" s="2" t="s">
         <v>598</v>
       </c>
-      <c r="M50" s="2" t="s">
+      <c r="N50" s="2" t="s">
         <v>618</v>
       </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="A51" s="4" t="s">
+        <v>1114</v>
+      </c>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="A52" s="2" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="A53" s="2" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="A54" s="2" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>1117</v>
+      </c>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="1:14">
+      <c r="A55" s="2" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>1119</v>
+      </c>
+      <c r="N55" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>

<commit_message>
MMOD pins 0 and 1
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38298AEA-DB28-446D-9037-53CD2131B58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA21581-1EEB-492E-8EA3-92E5949C6F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3990" yWindow="1665" windowWidth="24810" windowHeight="18975" firstSheet="2" activeTab="7" xr2:uid="{42D65D2A-8D1C-4D07-8E53-DE4B585A6847}"/>
+    <workbookView xWindow="5025" yWindow="885" windowWidth="26850" windowHeight="18975" firstSheet="3" activeTab="6" xr2:uid="{42D65D2A-8D1C-4D07-8E53-DE4B585A6847}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -9820,7 +9820,7 @@
   <dimension ref="A1:Q55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10215,43 +10215,43 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>1134</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>0</v>
@@ -10314,43 +10314,43 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>1135</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="O12" s="2" t="s">
         <v>0</v>
@@ -23220,7 +23220,7 @@
   </sheetPr>
   <dimension ref="A1:AD42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -25636,7 +25636,7 @@
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
TMMOD Fix pins 38, 39, where reversed
</commit_message>
<xml_diff>
--- a/Teensy4 Pins.xlsx
+++ b/Teensy4 Pins.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TeensyDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA21581-1EEB-492E-8EA3-92E5949C6F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C96ABAF-0DF3-485A-81F3-0BBF34849BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="885" windowWidth="26850" windowHeight="18975" firstSheet="3" activeTab="6" xr2:uid="{42D65D2A-8D1C-4D07-8E53-DE4B585A6847}"/>
+    <workbookView xWindow="6990" yWindow="690" windowWidth="26850" windowHeight="18975" firstSheet="3" activeTab="6" xr2:uid="{42D65D2A-8D1C-4D07-8E53-DE4B585A6847}"/>
   </bookViews>
   <sheets>
     <sheet name="T4" sheetId="3" r:id="rId1"/>
@@ -8126,8 +8126,8 @@
   </sheetPr>
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9399,7 +9399,7 @@
     </row>
     <row r="37" spans="1:13">
       <c r="A37" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>223</v>
@@ -9430,7 +9430,7 @@
     </row>
     <row r="38" spans="1:13" s="160" customFormat="1">
       <c r="A38" s="5" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>224</v>
@@ -9819,8 +9819,8 @@
   </sheetPr>
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11769,28 +11769,28 @@
         <v>1128</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1207</v>
+        <v>1215</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="Q47" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="48" spans="1:17">
@@ -11842,28 +11842,28 @@
         <v>1123</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1215</v>
+        <v>1207</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:17">
@@ -25636,8 +25636,8 @@
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27292,25 +27292,25 @@
         <v>1128</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -27321,25 +27321,25 @@
         <v>1123</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -27552,8 +27552,8 @@
   </sheetPr>
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -28884,31 +28884,31 @@
         <v>574</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C41" s="190" t="s">
-        <v>1016</v>
+        <v>1009</v>
       </c>
       <c r="D41" s="167" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="E41" s="168" t="s">
-        <v>757</v>
+        <v>748</v>
       </c>
       <c r="F41" s="174" t="s">
-        <v>909</v>
+        <v>905</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>1015</v>
+        <v>1011</v>
       </c>
       <c r="H41" s="169" t="s">
-        <v>1014</v>
+        <v>1010</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>876</v>
+        <v>866</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -28916,31 +28916,31 @@
         <v>575</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C42" s="190" t="s">
-        <v>1009</v>
+        <v>1016</v>
       </c>
       <c r="D42" s="167" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="E42" s="168" t="s">
-        <v>748</v>
+        <v>757</v>
       </c>
       <c r="F42" s="174" t="s">
-        <v>905</v>
+        <v>909</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>1011</v>
+        <v>1015</v>
       </c>
       <c r="H42" s="169" t="s">
-        <v>1010</v>
+        <v>1014</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>866</v>
+        <v>876</v>
       </c>
     </row>
     <row r="43" spans="1:12">

</xml_diff>